<commit_message>
Too much thing for one commit
</commit_message>
<xml_diff>
--- a/data/02_intermediate/cleaned_1PLIKÉ140_songs.xlsx
+++ b/data/02_intermediate/cleaned_1PLIKÉ140_songs.xlsx
@@ -463,7 +463,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Gang, gang J'perds pas mon temps sur des plans qui rapportent nada poh, poh Tu dis qu't'es un vrai, mais dans l'tier-quar, tu fais nada poh, poh Ça vient d'où ? J'aime bien ta Canada brr, brr J'me suis levé à onze heures, j'ai visser Fernando brr J'connais ma cité par cur, j'peux baroder les yeux bandés wouh Midi, c'est calme sur l'rrain-te wouh, seize heures, j'suis grave débordé wouh J'connais des mecs gantés qui peuvent soul'ver ton max-T paw Le ient-cli sort du boulot poh, direct, il vient acheter wouh On t'chouara, ça t'fume ta mère, si tu veux pas lâcher paw Un seul faux pas et ta vie s'ra gâchée paw J'découpe l'instru' comme la 'quette han, j'fais les choses précis han, han J'mets deux grammes cinq, c'est normal que l'ient-cli apprécie wouh Mettre les gants ou tenir la sacoche wouh ? J'suis grave indécis wouh Y a les keufs dans l'secteur, mes négros parlent en langage des signes Elle veut que j'pense à elle, j'ai la tête dans les chiffres paw L'instrumentale, j'lui mets que des gifles J'mets harbat, j'oublie pas qu'les bacqueux, ils sont vifs paw Trop d'pédés, trop d'salopes, putain, dans quel monde on vit paw ? On t'dépouille, on s'en bat les couilles de ton avis brr Pour soulever ton scoot' brr, j'me promenais avec un tournevis brr You might also like Le te-shi est vert comme Piccolo paw, la BAC, c'est des connards, ils font que d'me coller paw Ça crie pu sur le r, cache le tail-dé paw, paw, ton terrain est miné donc tes chiffres sont minables paw J'aime quand elle a un gros cul genre Nicki Minaj brr, j'ai d'la monnaie, elle demande pas mon âge brr, brr Parfois, on dirait qu'mes phrases son interminables brr, y a des mes-ar cachées à l'étage Y a les condés au tier-quar, faut alerter Si tu veux pas donner ton cul, tu dégages J'ai pas le temps de blablater, les ients-clis veulent pas quitter ma tête paw J'sais qu'tu l'as compris dans mes textes paw, on trafique, même si les passants, ils guettent brr Si y a les condés, on met les gaz brr, j'voulais finir au casino à Las Vegas han Pour un gros billet minimum, je me déplace han et en temps de guerre, j'me promène avec un schlass Ils sont pas opé' mais ils font les mecs en place, c'est des bonhommes que devant la glace 9.2.1.4.0, 140BRICKS, si y a un problème, t'as mon adresse salope Rentre dans la cité, on t'agresse salope, rentre dans la cité, on t'agresse paw J'fais grossir la sse-lia sous le matelas paw askip, y a brouille-em paw, est-c'que, demain, t'es là paw ? J'vais te bouillave dans le bloc salope, sale pute, tu mérites pas le tel-hô paw Ces tiagas me trouvent insolent wouh pas mé-cra, j'enchaîne les plavons solo wouh Y a plus d'pocheton, alors, on met le cello' wouh il a parlé, alors, on l'mêle aussitôt wouh Y a la batman qui tourne dans la cité paw, 9.2..1.4.0 sur le pocheton paw Le ient-cli prend son bout, il a halluciné brr, merci pour la qualité Netflix brr Au quartier, c'est réel, c'est pas du ciné wouh, elle a vu le buzz, la miss, elle veut m'câliner salope Pour les éteindre, même pas b'soin d'être calibré paw, paw, sortir un opinel, c'est mon plan B paw Les porcs, ils veulent nous voir tomber paw, ils veulent nous démanteler wouh Ils contrôlent tous les shlags qu'on a ravitaillé poh Vaut mieux être seul que mal accompagné, pourtant, on déboule à dix devant ton palier wouh T'inquiète, on n'est pas venus cambrioler wouh, on écrase ta tête dans les escaliers paw Et toi, t'as cru qu'on rigolait bâtard Toute la journée à chercher le fric, j'ai la tête dans les chiffres bâtard J'veux pas finir bloqué dans la street paw, j'me sens obligé d'tuer l'instru' paw Tu t'es fait accoster par des négros sombres wouh, tu t'sens obligé d'donner les thunes wouh Aquarium dans l'bâtiment, tout l'monde s'enfume Y a la mumu au quartier, tout l'monde s'en fout Y a la mumu au quartier, tout l'monde s'en fout salope Comme d'habitude, y a d'l'argent à faire dans le four paw On n'est pas méchants dans le fond paw, mais à tout moment on peut te faire wouh J'ai tenu la sacoche en hiver, en été han, le terrain, c'est moi qui l'a ouvert han Passe à Nila si tu veux un truc wouh, mais t'auras jamais d'barrette offerte wouh J'entends les sirènes dans le tieks, j'ai pas perdu mon temps, j'me suis déjà coffré paw J'suis un vrai laud-sa, j'peux pas trahir mon reufré paw Et si le plavon, il marche, ne t'étonne pas si on l'refait J'fais partir les stupéfiants, l'ient-cli revient, il a kiffé les effets paw J'marche dans la ville, j'pense qu'à chiffrer paw, y a un plavon, j'y vais y a un plavon, j'y vais, y a un plavon, j'y vais 9.2.1.4.0 sur le pocheton paw Tu peux appeler tous tes potos, dans tout les cas, ils vont tous faire le marathon paw2</t>
+          <t>Gang, gang J'perds pas mon temps sur des plans qui rapportent nada poh, poh Tu dis qu't'es un vrai, mais dans l'tier-quar, tu fais nada poh, poh Ça vient d'où ? J'aime bien ta Canada brr, brr J'me suis levé à onze heures, j'ai visser Fernando brr J'connais ma cité par cur, j'peux baroder les yeux bandés wouh Midi, c'est calme sur l'rrain-te wouh, seize heures, j'suis grave débordé wouh J'connais des mecs gantés qui peuvent soul'ver ton max-T paw Le ient-cli sort du boulot poh, direct, il vient acheter wouh On t'chouara, ça t'fume ta mère, si tu veux pas lâcher paw Un seul faux pas et ta vie s'ra gâchée paw J'découpe l'instru' comme la 'quette han, j'fais les choses précis han, han J'mets deux grammes cinq, c'est normal que l'ient-cli apprécie wouh Mettre les gants ou tenir la sacoche wouh ? J'suis grave indécis wouh Y a les keufs dans l'secteur, mes négros parlent en langage des signes Elle veut que j'pense à elle, j'ai la tête dans les chiffres paw L'instrumentale, j'lui mets que des gifles J'mets harbat, j'oublie pas qu'les bacqueux, ils sont vifs paw Trop d'pédés, trop d'salopes, putain, dans quel monde on vit paw ? On t'dépouille, on s'en bat les couilles de ton avis brr Pour soulever ton scoot' brr, j'me promenais avec un tournevis brr Le te-shi est vert comme Piccolo paw, la BAC, c'est des connards, ils font que d'me coller paw Ça crie pu sur le r, cache le tail-dé paw, paw, ton terrain est miné donc tes chiffres sont minables paw J'aime quand elle a un gros cul genre Nicki Minaj brr, j'ai d'la monnaie, elle demande pas mon âge brr, brr Parfois, on dirait qu'mes phrases son interminables brr, y a des mes-ar cachées à l'étage Y a les condés au tier-quar, faut alerter Si tu veux pas donner ton cul, tu dégages J'ai pas le temps de blablater, les ients-clis veulent pas quitter ma tête paw J'sais qu'tu l'as compris dans mes textes paw, on trafique, même si les passants, ils guettent brr Si y a les condés, on met les gaz brr, j'voulais finir au casino à Las Vegas han Pour un gros billet minimum, je me déplace han et en temps de guerre, j'me promène avec un schlass Ils sont pas opé' mais ils font les mecs en place, c'est des bonhommes que devant la glace 9.2.1.4.0, 140BRICKS, si y a un problème, t'as mon adresse salope Rentre dans la cité, on t'agresse salope, rentre dans la cité, on t'agresse paw J'fais grossir la sse-lia sous le matelas paw askip, y a brouille-em paw, est-c'que, demain, t'es là paw ? J'vais te bouillave dans le bloc salope, sale pute, tu mérites pas le tel-hô paw Ces tiagas me trouvent insolent wouh pas mé-cra, j'enchaîne les plavons solo wouh Y a plus d'pocheton, alors, on met le cello' wouh il a parlé, alors, on l'mêle aussitôt wouh Y a la batman qui tourne dans la cité paw, 9.2..1.4.0 sur le pocheton paw Le ient-cli prend son bout, il a halluciné brr, merci pour la qualité Netflix brr Au quartier, c'est réel, c'est pas du ciné wouh, elle a vu le buzz, la miss, elle veut m'câliner salope Pour les éteindre, même pas b'soin d'être calibré paw, paw, sortir un opinel, c'est mon plan B paw Les porcs, ils veulent nous voir tomber paw, ils veulent nous démanteler wouh Ils contrôlent tous les shlags qu'on a ravitaillé poh Vaut mieux être seul que mal accompagné, pourtant, on déboule à dix devant ton palier wouh T'inquiète, on n'est pas venus cambrioler wouh, on écrase ta tête dans les escaliers paw Et toi, t'as cru qu'on rigolait bâtard Toute la journée à chercher le fric, j'ai la tête dans les chiffres bâtard J'veux pas finir bloqué dans la street paw, j'me sens obligé d'tuer l'instru' paw Tu t'es fait accoster par des négros sombres wouh, tu t'sens obligé d'donner les thunes wouh Aquarium dans l'bâtiment, tout l'monde s'enfume Y a la mumu au quartier, tout l'monde s'en fout Y a la mumu au quartier, tout l'monde s'en fout salope Comme d'habitude, y a d'l'argent à faire dans le four paw On n'est pas méchants dans le fond paw, mais à tout moment on peut te faire wouh J'ai tenu la sacoche en hiver, en été han, le terrain, c'est moi qui l'a ouvert han Passe à Nila si tu veux un truc wouh, mais t'auras jamais d'barrette offerte wouh J'entends les sirènes dans le tieks, j'ai pas perdu mon temps, j'me suis déjà coffré paw J'suis un vrai laud-sa, j'peux pas trahir mon reufré paw Et si le plavon, il marche, ne t'étonne pas si on l'refait J'fais partir les stupéfiants, l'ient-cli revient, il a kiffé les effets paw J'marche dans la ville, j'pense qu'à chiffrer paw, y a un plavon, j'y vais y a un plavon, j'y vais, y a un plavon, j'y vais 9.2.1.4.0 sur le pocheton paw Tu peux appeler tous tes potos, dans tout les cas, ils vont tous faire le marathon paw2</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Mmh, mmh, mmh, mmh Mmh, mmh, mmh L'habit ne fait pas le moine, en Prada, le Diable est habillé Deux-trois coups d'couteau bien placés, impossible qu'ils reviennent comme le mec de Nabilla D'la vida loca, j'ai rêvassé, t'es prêt à faire quoi pour avoir cette vie-là han ? J'perds la mémoire mais han j'me rappelle de cette nuit-là poh Impossible d'effacer le passé, j'ai la poisse, mais j'ai pas gué-lar la C poh J'débite sur l'instru' comme si j'suis pressé alors qu'j'ai tout mon temps j'ai tout mon temps Mes couplts, j'vous laisse apprécier, profitez bin, j'compte pas rapper longtemps J'le fais pour les mapé', j'avance sans ma peur, conduite sans mis-per, j'baraude comme un kidnappeur Faut te pointer à l'heure si l'billet, tu veux l'faire La frappe dans l'pantalon pour tous les anciens et les jeunes consommateurs Elle m'trouvait différent, j'ai joué avec son cur Aujourd'hui, elle m'dit qu'j'suis comme ces menteurs ah bon ? Et elle a pas tort, ouais, j'suis un menteur ah bon ?, pendant l'audition, aucune vérité sort han Si on t'monte en l'air, ton alcool redescend, j'me suis calmé, dans ma tête, c'était le désordre J'suis sous Absolut pas sous Martini J'suis écouté jusqu'à Gwada Martinique Ça t'enlève ta tunique et on reste unis Le flow est unique, dis-moi, pourquoi tu nies ? Dommage que tu pues trop d'la schneck Sale pute, tu n'auras jamais de cunni' poh, poh T'es en train d'khleh, t'inquiète, le massacre est bientôt fini You might also like What you gonna do si mes gars prennent ta Canada mmh ? Location toute l'année, mais t'as walou mmh, en vrai, t'as nada mmh, mmh On coupe, on décale, on coupe, on décale comme Saga Douk comme Saga Douk C'est les quartiers d'France, ça s'la fout pour un ça vient d'où ? pour un ça vient d'où ? What you gonna do si mes gars prennent ta Canada mmh ? Location toute l'année, mais t'as walou mmh, en vrai, t'as nada mmh, mmh On coupe, on décale, on coupe, on décale comme Saga Douk poh, poh C'est les quartiers d'France, ça s'la fout pour un Ça vient d'où ? poh, poh À quinze ans, j'arrivais même plus à mi-dor, étant mineur, j'courais après la mine d'or Pourquoi tu cala pas ceux qui veulent ton bien ? Pourquoi tu t'attaches à tous ceux qui t'ignorent ? Pour des sentiments, y en a qui sont morts, y en a qui bé-tom pour pas un centime 9 millimètres, on l'achète en deux-deux, Opinel 13, 22 centimètres Toujours le majeur levé aux 22-2 han, ces flocos, ils pètent rien et ils sont étonnés han Ils arrêteront jamais le bénéf' du teu-teu le bénéf' du teu-teu Ta veste, tu veux la retourner, tu vas m'la donner, bâtard, ton heure peut sonner Nan, j'suis pas son ex, pas b'soin d'kichta pour l'impressionner La roue va tourner brr, quand le bosseur n'est pas payé brr, brr, il se met à détourner brr Flûte, t'as le tournis, j'ai des barrettes gées-char, les tiennes, elles sont skinny J'm'en bat les c' de briller, j'traîne dans des coins sinistres J'suis sous Absolut pas sous Martini J'suis écouté jusqu'à Gwada Martinique Ça t'enlève ta tunique et on reste unis Le flow est unique, dis-moi, pourquoi tu nies ? Dommage que tu pues trop d'la schneck Sale pute, tu n'auras jamais de cunni' poh, poh T'es en train d'khleh, t'inquiète, le massacre est bientôt fini What you gonna do si mes gars prennent ta Canada mmh ? Location toute l'année, mais t'as walou mmh, en vrai, t'as nada mmh, mmh On coupe, on décale, on coupe, on décale comme Saga Douk comme Saga Douk C'est les quartiers d'France, ça s'la fout pour un ça vient d'où ? pour un ça vient d'où ? What you gonna do si mes gars prennent ta Canada mmh ? Location toute l'année, mais t'as walou mmh, en vrai, t'as nada mmh, mmh On coupe, on décale, on coupe, on décale comme Saga Douk poh, poh C'est les quartiers d'France, ça s'la fout pour un Ça vient d'où ? poh, poh</t>
+          <t>Mmh, mmh, mmh, mmh Mmh, mmh, mmh L'habit ne fait pas le moine, en Prada, le Diable est habillé Deux-trois coups d'couteau bien placés, impossible qu'ils reviennent comme le mec de Nabilla D'la vida loca, j'ai rêvassé, t'es prêt à faire quoi pour avoir cette vie-là han ? J'perds la mémoire mais han j'me rappelle de cette nuit-là poh Impossible d'effacer le passé, j'ai la poisse, mais j'ai pas gué-lar la C poh J'débite sur l'instru' comme si j'suis pressé alors qu'j'ai tout mon temps j'ai tout mon temps Mes couplts, j'vous laisse apprécier, profitez bin, j'compte pas rapper longtemps J'le fais pour les mapé', j'avance sans ma peur, conduite sans mis-per, j'baraude comme un kidnappeur Faut te pointer à l'heure si l'billet, tu veux l'faire La frappe dans l'pantalon pour tous les anciens et les jeunes consommateurs Elle m'trouvait différent, j'ai joué avec son cur Aujourd'hui, elle m'dit qu'j'suis comme ces menteurs ah bon ? Et elle a pas tort, ouais, j'suis un menteur ah bon ?, pendant l'audition, aucune vérité sort han Si on t'monte en l'air, ton alcool redescend, j'me suis calmé, dans ma tête, c'était le désordre J'suis sous Absolut pas sous Martini J'suis écouté jusqu'à Gwada Martinique Ça t'enlève ta tunique et on reste unis Le flow est unique, dis-moi, pourquoi tu nies ? Dommage que tu pues trop d'la schneck Sale pute, tu n'auras jamais de cunni' poh, poh T'es en train d'khleh, t'inquiète, le massacre est bientôt fini What you gonna do si mes gars prennent ta Canada mmh ? Location toute l'année, mais t'as walou mmh, en vrai, t'as nada mmh, mmh On coupe, on décale, on coupe, on décale comme Saga Douk comme Saga Douk C'est les quartiers d'France, ça s'la fout pour un ça vient d'où ? pour un ça vient d'où ? What you gonna do si mes gars prennent ta Canada mmh ? Location toute l'année, mais t'as walou mmh, en vrai, t'as nada mmh, mmh On coupe, on décale, on coupe, on décale comme Saga Douk poh, poh C'est les quartiers d'France, ça s'la fout pour un Ça vient d'où ? poh, poh À quinze ans, j'arrivais même plus à mi-dor, étant mineur, j'courais après la mine d'or Pourquoi tu cala pas ceux qui veulent ton bien ? Pourquoi tu t'attaches à tous ceux qui t'ignorent ? Pour des sentiments, y en a qui sont morts, y en a qui bé-tom pour pas un centime 9 millimètres, on l'achète en deux-deux, Opinel 13, 22 centimètres Toujours le majeur levé aux 22-2 han, ces flocos, ils pètent rien et ils sont étonnés han Ils arrêteront jamais le bénéf' du teu-teu le bénéf' du teu-teu Ta veste, tu veux la retourner, tu vas m'la donner, bâtard, ton heure peut sonner Nan, j'suis pas son ex, pas b'soin d'kichta pour l'impressionner La roue va tourner brr, quand le bosseur n'est pas payé brr, brr, il se met à détourner brr Flûte, t'as le tournis, j'ai des barrettes gées-char, les tiennes, elles sont skinny J'm'en bat les c' de briller, j'traîne dans des coins sinistres J'suis sous Absolut pas sous Martini J'suis écouté jusqu'à Gwada Martinique Ça t'enlève ta tunique et on reste unis Le flow est unique, dis-moi, pourquoi tu nies ? Dommage que tu pues trop d'la schneck Sale pute, tu n'auras jamais de cunni' poh, poh T'es en train d'khleh, t'inquiète, le massacre est bientôt fini What you gonna do si mes gars prennent ta Canada mmh ? Location toute l'année, mais t'as walou mmh, en vrai, t'as nada mmh, mmh On coupe, on décale, on coupe, on décale comme Saga Douk comme Saga Douk C'est les quartiers d'France, ça s'la fout pour un ça vient d'où ? pour un ça vient d'où ? What you gonna do si mes gars prennent ta Canada mmh ? Location toute l'année, mais t'as walou mmh, en vrai, t'as nada mmh, mmh On coupe, on décale, on coupe, on décale comme Saga Douk poh, poh C'est les quartiers d'France, ça s'la fout pour un Ça vient d'où ? poh, poh</t>
         </is>
       </c>
     </row>
@@ -497,7 +497,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Partie 1 Beaucoup d'rappeurs, j'suis obligé d'faire la diff' Et vu que j'dois rester actif, j'la que-n' j'oublie pas l'préservatif Paw Le week-end on fait pas la te-fê On augmente le bénéfice Brr J'aime bien voir ma cité en HD, c'est l'deuxième épisode de la série Merci pour la qualité Netflix 92140 sur le pocheton, le te-shi est vert donc le ent-cli vient acheter Fais partir la bonbonne sans qu'les condés te chopent Fais belek où tu caches ton taille-dé Wouh J'entends les sirènes sur l'terrain c'est trop miné Tant qu'il y a des ents-cli le match va pas s'terminer Ah bon ? Fais belek à qui tu fais la passe, les vils-ci ils sont determinés C'est pas pour rien qu'on te chope par le col bâtard, tu vas donner la somme En vrai, j'm'en balek que tu baises pas, sale pute ce soir, tu vas lahsa Je rap pour ceux qui s'reconnaissent dans mes sons J'perds mon sang froid, c'est toi qui finis en sang Salope Et toi t'es qu'une salope Bow T'as cru qu'on finirait ensemble J'suis gé-char, j'me mets pas sur le côté J'arrête pas d'courir donc j'ai un point de côté J'm'arrête pas d'vi'-ser donc j'arrête pas de compter C'est des acteurs, ils ont peur de nous affronter Bow Sur l'terrain j'dois rester actif, j'la que-n' j'oublie pas l'préservatif Ton poto t'a que-arna mais t'es trop naïf Opinel 12 si vous êtes trop massifs J'peux rajouter des trous dans ton jeans Jcrie, Nique les keufs, j'espère qu'ils m'ont entendu Y a la batman dans le secteur, c'est tendu J'avais plus d'cardio mais je me suis pas rendu Et j'avoue la vie est cruelle Quand mes gars te disent d'enlever ton iCloud Enlève ta sacoche, le débat est clos T'es une balance donc tu traînes pas avec nous Jeune négro dans les bails noirs Maman m'a dit Sors pas la nuit, y a des jnouns J'suis sur l'terrain depuis midi pile, j'ai oublié mon p'tit déj'ner Mourir dans une villa comme Tony Montana, la fin est tragique C'est tragique, c'est tragique J'ai les mains faites pour l'or mais elles sont dans le shit Dans le shit, dans le shit Pour ve-esqui les keufs, faut être agile J'monte sur Paname pour plus d'cent balles Cent balles C'est pas pour rien qu'on fait le trajet Les tits-pe, ils s'attaquent aux personnes âgées À minuit dans l'tier-quar, y a personne à jeun C'est des menteurs, ils s'inventent des personnages Tu t'fais dépouiller à la Plaine c'est le jeu Le son il est lourd, t'oses me dire que c'est léger ? On veut pas brûler mais on enchaîne les péchés Sale pute, j'suis dans l'bâtiment, pour faire des sous la con de tes morts On a la BAC dans notre ligne de mire, car ils nous ont mis contre le mur Fuck la BAC et tous les keufs j'suis dans l'binks, y a mes reufs On calcule pas les meufs que des lovés, pas d'love T'as mal fini t'es dans l'coffre J'encaisse des sous faut que j'coffre, j'encaisse des sous faut que j'coffre You might also likePartie 2 Jcoffre, faut qu'j'encaisse des sous J'pète une kichta et les condés sont jaloux, et les condés sont jaloux J'coffre, faut qu'j'encaisse des sous J'pète une kichta et les condés sont jaloux, et les condés sont jaloux 9.2.1.4.0 sur le pocheton J'en remets une couche, tas pas compris la leçon Tu t'fais accoster par des négros sombres Elle veut rien faire donc elle sort de la bre-cham J'voulais cricket et personne m'a incité, et toi tu te caches parce que des blases t'as cité Faut peter ce cash et pas posé des teilles J'suis plus du genre à posé ldétail Ça fait 20 minutes qu'on te piste J'suis à 2 doigts d'enfiler l'gator Après l'plavon j'm'achète un truc Alligator C'est possible que j'visser un collègue à toi Et sous teu-shi on fait les gamins Le ffre-chi, ouais j'l'ai fais ilégalement J'marche dans la ville, les keufs veulent me Ferragamo Comme d'hab' devant l'OPJ, on dit pas un mot paw J'aime quand le yen-cli prend sa dose Juste en me serrant la main La vrai moula ne se coupe pas en lamelles Il ressemble à un condé mais j'vais quand même lui mettre, c'est bien d'parler d'calibre mais gros faut allumer Et les shmits veulent rentrer dans la planque, que d'l'argent sale, me parles pas de compte en banque J'peux pas m'arrêter tant qu'il y a des ients-cli en manque J'ai trop les mains dans la résine, envers les condés, igo j'ai d'la haine en moi J'crois qu'ils veulent pas m'voir dans la limousine ah bon J'fais pas de feats, j'suis au régime Elle, elle veut savoir mes origines Moi, tout c'que je veux c'est voir ients-cli qui défilent, tout c'que je veux, c'est voir ients-cli qui défilent Pas d'négociations, les prix, c'est moi qui les fixe</t>
+          <t>Partie 1 Beaucoup d'rappeurs, j'suis obligé d'faire la diff' Et vu que j'dois rester actif, j'la que-n' j'oublie pas l'préservatif Paw Le week-end on fait pas la te-fê On augmente le bénéfice Brr J'aime bien voir ma cité en HD, c'est l'deuxième épisode de la série Merci pour la qualité Netflix 92140 sur le pocheton, le te-shi est vert donc le ent-cli vient acheter Fais partir la bonbonne sans qu'les condés te chopent Fais belek où tu caches ton taille-dé Wouh J'entends les sirènes sur l'terrain c'est trop miné Tant qu'il y a des ents-cli le match va pas s'terminer Ah bon ? Fais belek à qui tu fais la passe, les vils-ci ils sont determinés C'est pas pour rien qu'on te chope par le col bâtard, tu vas donner la somme En vrai, j'm'en balek que tu baises pas, sale pute ce soir, tu vas lahsa Je rap pour ceux qui s'reconnaissent dans mes sons J'perds mon sang froid, c'est toi qui finis en sang Salope Et toi t'es qu'une salope Bow T'as cru qu'on finirait ensemble J'suis gé-char, j'me mets pas sur le côté J'arrête pas d'courir donc j'ai un point de côté J'm'arrête pas d'vi'-ser donc j'arrête pas de compter C'est des acteurs, ils ont peur de nous affronter Bow Sur l'terrain j'dois rester actif, j'la que-n' j'oublie pas l'préservatif Ton poto t'a que-arna mais t'es trop naïf Opinel 12 si vous êtes trop massifs J'peux rajouter des trous dans ton jeans Jcrie, Nique les keufs, j'espère qu'ils m'ont entendu Y a la batman dans le secteur, c'est tendu J'avais plus d'cardio mais je me suis pas rendu Et j'avoue la vie est cruelle Quand mes gars te disent d'enlever ton iCloud Enlève ta sacoche, le débat est clos T'es une balance donc tu traînes pas avec nous Jeune négro dans les bails noirs Maman m'a dit Sors pas la nuit, y a des jnouns J'suis sur l'terrain depuis midi pile, j'ai oublié mon p'tit déj'ner Mourir dans une villa comme Tony Montana, la fin est tragique C'est tragique, c'est tragique J'ai les mains faites pour l'or mais elles sont dans le shit Dans le shit, dans le shit Pour ve-esqui les keufs, faut être agile J'monte sur Paname pour plus d'cent balles Cent balles C'est pas pour rien qu'on fait le trajet Les tits-pe, ils s'attaquent aux personnes âgées À minuit dans l'tier-quar, y a personne à jeun C'est des menteurs, ils s'inventent des personnages Tu t'fais dépouiller à la Plaine c'est le jeu Le son il est lourd, t'oses me dire que c'est léger ? On veut pas brûler mais on enchaîne les péchés Sale pute, j'suis dans l'bâtiment, pour faire des sous la con de tes morts On a la BAC dans notre ligne de mire, car ils nous ont mis contre le mur Fuck la BAC et tous les keufs j'suis dans l'binks, y a mes reufs On calcule pas les meufs que des lovés, pas d'love T'as mal fini t'es dans l'coffre J'encaisse des sous faut que j'coffre, j'encaisse des sous faut que j'coffre Partie 2 Jcoffre, faut qu'j'encaisse des sous J'pète une kichta et les condés sont jaloux, et les condés sont jaloux J'coffre, faut qu'j'encaisse des sous J'pète une kichta et les condés sont jaloux, et les condés sont jaloux 9.2.1.4.0 sur le pocheton J'en remets une couche, tas pas compris la leçon Tu t'fais accoster par des négros sombres Elle veut rien faire donc elle sort de la bre-cham J'voulais cricket et personne m'a incité, et toi tu te caches parce que des blases t'as cité Faut peter ce cash et pas posé des teilles J'suis plus du genre à posé ldétail Ça fait 20 minutes qu'on te piste J'suis à 2 doigts d'enfiler l'gator Après l'plavon j'm'achète un truc Alligator C'est possible que j'visser un collègue à toi Et sous teu-shi on fait les gamins Le ffre-chi, ouais j'l'ai fais ilégalement J'marche dans la ville, les keufs veulent me Ferragamo Comme d'hab' devant l'OPJ, on dit pas un mot paw J'aime quand le yen-cli prend sa dose Juste en me serrant la main La vrai moula ne se coupe pas en lamelles Il ressemble à un condé mais j'vais quand même lui mettre, c'est bien d'parler d'calibre mais gros faut allumer Et les shmits veulent rentrer dans la planque, que d'l'argent sale, me parles pas de compte en banque J'peux pas m'arrêter tant qu'il y a des ients-cli en manque J'ai trop les mains dans la résine, envers les condés, igo j'ai d'la haine en moi J'crois qu'ils veulent pas m'voir dans la limousine ah bon J'fais pas de feats, j'suis au régime Elle, elle veut savoir mes origines Moi, tout c'que je veux c'est voir ients-cli qui défilent, tout c'que je veux, c'est voir ients-cli qui défilent Pas d'négociations, les prix, c'est moi qui les fixe</t>
         </is>
       </c>
     </row>
@@ -514,7 +514,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Comme dhabitude jai la bonbonne sur moi Donc jai les couilles qui me démangent Jallais voler pour arrondir la fin du mois J'sais qu'les condés, ça les dérange Je veux des talbins, nan, je veux pas attendre Je suis un lossa, si je prends tes sous, je vais pas t'les rendre On s'connait à peine Comment tu veux que j't'arrange Laisse-moi un million et j'me range Dis-moi pourquoi ils font les fous à les entendre c'est eux qui ravitaillent le four J'suis un vrai négro alors j'm'écarte des faux Je connais personne qu'à zero défaut Je cours apres l'argent donc souvent j'me fais sé-cour Mais j'oublie pas q'la vie est courte Parfois j'suis sous adrenaline Quand j'vois quatre bacqueux dans un vehicule Et à chaque fois que t'écoutes mes sons T'entends la haine que je véhicule La miss elle m'a donné son coeur, l'instru elle m'a donné son cul J'casse la démarche dans ta cité Pourtant jai 0 sécu Igo qu'est-ce que tu viens nous raconter Moi j'sais très bien que t'as zero vécu On demande, ça vient d'où ou bien tu veux quoi En détail ou en gros, igo j'te laisse le choix J'ai caché plus de cent grammes de beuh dans la ve-ca Elle fait semblant mais en vrai moi je sais qu'elle veut ken Sur la bécane si tu casses il faut que tu payes Y a les condés si t'es gé-char il faut que tu partes J'ai l'impression que les bacqueux sont tout-par Ils déboulent au moment opportun J'me suis fait courser, j'ai fait tomber mon portable Mais j'vais quand même pas me retourner J'veux voir la tchop de la mumu faire des tonneaux Fais belek, sur le terrain y'a des détourneurs On me dit 1pliké, attends un peu T'inquiète pas elle viendra ton heure Après la pluie y'a le beau temps Après le beau temps y'a le tonnerre Si t'es pas pret, il faut que t'abandonnes Et si y'a un plavon faut que tu te la donnes Non j'évite pas les sujets tabous Sale pute, sale pute y'a ma queue dans ta bouche Fuck les condés, fuck la caméra J't'le redirai à jamais En vrai j'm'arrêterais jamais d'visser Même si j'ai le bras à Jamel J'aime bien voir les keufs qui se gamellent Toi tu m'appelles quand t'es en galère Bizarrement j'te vois pas quand j'suis en galère J'marche dans la ville odeur de stupéfiant Mais pourtant j'l'ai bien emballé Dans mes textes j'ai pas tout devoilé J'laisse pas mes empreintes sur le scooter volé T'as fumé la frappe et tu t'es envolé You might also like Fuck les condés, fuck la caméra J't'le redirai à jamais En vrai j'm'arrêterais jamais d'visser Même si j'ai le bras à Jamel Fuck les condés, fuck la caméra J't'le redirai à jamais En vrai j'm'arrêterai jamais d'visser Même si j'ai le bras à Jamel Fuck les condés fuck la caméra J't'le redirai à jamais En vrai j'm'arrêterai jamais d'visser Même si j'ai le bras à Jamel Et le pilon c'est nous on l'ramène 92140 sur le pocheton Et le pilon c'est nous ont l'ramènent Askip t'a une me-ar dans l'caleçon C'est dommage que t'a pas les couilles C'est des salopes tout ces ennemis donc ont les canne Toute la journée j'ai mangé des sous Après minuit j'ai encore la dalle J'suis un salaud j'aime le racket comme Nadal Fais belek où tu caches ton détail J'fais pas de chrome l'argent il faut qu'tu m'le donnes J'aime bien quand la beuh elle vient d'Meda Le cricket vient pécho son médoc Y'a des ien-cli dans mon agenda Faut que l'argent rentre dans ma poche Faut que la lame rentre dans ton corps Les condés ils ont mis les lampes torches Dommage à minuit ils nous cherchent encore Toi dis moi pourquoi t'as une sacoche T'es qu'un acteur pendant que tu dors nous on bosse Et nous on vend la mort même si elle approche Paw Paw A six heure sa toque Toi tu parles mal parce que t'as bu En descente normal on remplit le bus J'me sens obligé de remplir ma puce Faut qu'j'enfile la capuche j'ai vu la focus En vérité j'm'en balek des conséquences On caillasse la première tchop et on s'casse On esquive la remontada Ça vient d'où j'aime bien ta Canada Batard si t'essaies de nous rot-ca On revient cagoulés comme Sin Cara J'veux des kichtas salope moi j'veux pas d'calin Ien-cli qui m'appelle j'suis obligé de décaler J'suis posé au tiéquar y'a une descente de keufs Trop tard le bosseur à détaler Beaucoup d'rappeur mais très peu ont du talent On t'encule ta mère si t'a pas tenu ta langue Et si tu parles pas monnaie Enculé tu parles pas ma langue Et si tu parles pas monnaie Enculé tu parles pas ma langue1</t>
+          <t>Comme dhabitude jai la bonbonne sur moi Donc jai les couilles qui me démangent Jallais voler pour arrondir la fin du mois J'sais qu'les condés, ça les dérange Je veux des talbins, nan, je veux pas attendre Je suis un lossa, si je prends tes sous, je vais pas t'les rendre On s'connait à peine Comment tu veux que j't'arrange Laisse-moi un million et j'me range Dis-moi pourquoi ils font les fous à les entendre c'est eux qui ravitaillent le four J'suis un vrai négro alors j'm'écarte des faux Je connais personne qu'à zero défaut Je cours apres l'argent donc souvent j'me fais sé-cour Mais j'oublie pas q'la vie est courte Parfois j'suis sous adrenaline Quand j'vois quatre bacqueux dans un vehicule Et à chaque fois que t'écoutes mes sons T'entends la haine que je véhicule La miss elle m'a donné son coeur, l'instru elle m'a donné son cul J'casse la démarche dans ta cité Pourtant jai 0 sécu Igo qu'est-ce que tu viens nous raconter Moi j'sais très bien que t'as zero vécu On demande, ça vient d'où ou bien tu veux quoi En détail ou en gros, igo j'te laisse le choix J'ai caché plus de cent grammes de beuh dans la ve-ca Elle fait semblant mais en vrai moi je sais qu'elle veut ken Sur la bécane si tu casses il faut que tu payes Y a les condés si t'es gé-char il faut que tu partes J'ai l'impression que les bacqueux sont tout-par Ils déboulent au moment opportun J'me suis fait courser, j'ai fait tomber mon portable Mais j'vais quand même pas me retourner J'veux voir la tchop de la mumu faire des tonneaux Fais belek, sur le terrain y'a des détourneurs On me dit 1pliké, attends un peu T'inquiète pas elle viendra ton heure Après la pluie y'a le beau temps Après le beau temps y'a le tonnerre Si t'es pas pret, il faut que t'abandonnes Et si y'a un plavon faut que tu te la donnes Non j'évite pas les sujets tabous Sale pute, sale pute y'a ma queue dans ta bouche Fuck les condés, fuck la caméra J't'le redirai à jamais En vrai j'm'arrêterais jamais d'visser Même si j'ai le bras à Jamel J'aime bien voir les keufs qui se gamellent Toi tu m'appelles quand t'es en galère Bizarrement j'te vois pas quand j'suis en galère J'marche dans la ville odeur de stupéfiant Mais pourtant j'l'ai bien emballé Dans mes textes j'ai pas tout devoilé J'laisse pas mes empreintes sur le scooter volé T'as fumé la frappe et tu t'es envolé Fuck les condés, fuck la caméra J't'le redirai à jamais En vrai j'm'arrêterais jamais d'visser Même si j'ai le bras à Jamel Fuck les condés, fuck la caméra J't'le redirai à jamais En vrai j'm'arrêterai jamais d'visser Même si j'ai le bras à Jamel Fuck les condés fuck la caméra J't'le redirai à jamais En vrai j'm'arrêterai jamais d'visser Même si j'ai le bras à Jamel Et le pilon c'est nous on l'ramène 92140 sur le pocheton Et le pilon c'est nous ont l'ramènent Askip t'a une me-ar dans l'caleçon C'est dommage que t'a pas les couilles C'est des salopes tout ces ennemis donc ont les canne Toute la journée j'ai mangé des sous Après minuit j'ai encore la dalle J'suis un salaud j'aime le racket comme Nadal Fais belek où tu caches ton détail J'fais pas de chrome l'argent il faut qu'tu m'le donnes J'aime bien quand la beuh elle vient d'Meda Le cricket vient pécho son médoc Y'a des ien-cli dans mon agenda Faut que l'argent rentre dans ma poche Faut que la lame rentre dans ton corps Les condés ils ont mis les lampes torches Dommage à minuit ils nous cherchent encore Toi dis moi pourquoi t'as une sacoche T'es qu'un acteur pendant que tu dors nous on bosse Et nous on vend la mort même si elle approche Paw Paw A six heure sa toque Toi tu parles mal parce que t'as bu En descente normal on remplit le bus J'me sens obligé de remplir ma puce Faut qu'j'enfile la capuche j'ai vu la focus En vérité j'm'en balek des conséquences On caillasse la première tchop et on s'casse On esquive la remontada Ça vient d'où j'aime bien ta Canada Batard si t'essaies de nous rot-ca On revient cagoulés comme Sin Cara J'veux des kichtas salope moi j'veux pas d'calin Ien-cli qui m'appelle j'suis obligé de décaler J'suis posé au tiéquar y'a une descente de keufs Trop tard le bosseur à détaler Beaucoup d'rappeur mais très peu ont du talent On t'encule ta mère si t'a pas tenu ta langue Et si tu parles pas monnaie Enculé tu parles pas ma langue Et si tu parles pas monnaie Enculé tu parles pas ma langue1</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Binks Beatz Il reste du te-shi sur le couteau Si j'l'enfonce dans ton corps, combien ça va t'coûter ? Et si t'enfiles les gants, gros, tu peux plus douter Tu fumes la frappe, tu t'envoles, tu sais plus où t'es Y a toujours mon gang avec moi en cas d'embrouille Même quand c'est chaud, faut porter ses couilles J'ai encore eu d'la chance, j'ai v'-esqui la patrouille La bonbonne est gée-char, ce soir, y aura pas d'fouille Y a d'la frappe dans l'pochtar, le ient-cli devient fou J'suis rentré tard mais j'ai fait plus de sous Les poucaves, les pédales, nan, on veut pas d'vous Askip, t'es un chaud mais bon, on t'voit pas d'vant Midi-minuit, j'suis à l'affût des bacqueux J'cache le tail-dé, j'ai vu les shtars qui débarquent Nan, j'laisse pas l'couteau dans la kitchen J'découpe la 'quette, la frappe te couche comme Jackie Chan À midi pile, le guetteur se positionne Askip, t'as poucave, j'veux voir ta déposition J'rentre cagoulé, j'suis dans l'action Y a des ients-cli, j'visser dans l'axe Y a des mes-ar dans le sac à dos Si on vient dans ton tier-quar, on f'ra pas d'cadeau Si on rentre dans l'appart', on va tout saccager Beaucoup qui font les fous, en vrai, personne agit You might also like J'sors, j'fais trois passes, jretourne nehess J'aime bien ta bouche, tu vas mlehess Comme d'hab', j'ai enfumé la pièce J'peux t'ambiancer en t'racontant la vie dla tess Pour niquer linstru', jai pas bsoin dvider la teille Jveux pas ber-tom donc jserre mes lacets Jai la dalle des sous, jveux des liasses dans mon assiette Jai la dalle des sous, jveux des liasses dans mon assiette J'sors, j'fais trois passes, jretourne nehess J'aime bien ta bouche, tu vas mlehess Comme d'hab', j'ai enfumé la pièce J'peux t'ambiancer en t'racontant la vie dla tess Pour niquer linstru jai pas bsoin dvider la teille Jveux pas ber-tom donc jserre mes lacets Jai la dalle des sous, jveux des liasses dans mon assiette Jai la dalle des sous, jveux des liasses dans mon assiette On vient dniquer un mec, jvois la BAC qui ne-tour Jviens dallumer lpét, jai djà la tête qui ne-tour Désolé, ma belle, si jme suis éloigné dtoi La monnaie mappelle, jrecompte mes billets le soir Jai caché lOpinel si y a embrouille, jle sors Avec un trou dans la jambe, comment tu ten sors ? Cest pour faire des sous si tu mvois traîner dehors Jfais que dtartiner pour avoir les couilles en or On court après la vida loca Jsuis bloqué, jvois mon bonheur dans lillégal Parfois la vie est paradoxale Pour shabiller propre, normal, on tfait du sale Dix négros dans ton tieks, cest toi qui va finir au sol Rentrer dans ma cité, jte déconseille Quand jsuis triste, y a qules billets qui me consolent Pour oublier sa meuf, le pilon, il consomme Calcule pas les raclis, elles vont rien tapporter Y a les condés dans lbat, les voisins, ils ont alerté Avant lplavon, moi et mes gars on sest bien concertés Ce soir, jrepars avec le butin, jen suis certain Le bosseur, il a enchaîné la troisième mi-temps Il lâchera pas la sacoche même avec les yeux cernés Jconnais ma cité par cur, jgué-lar les keufs les yeux fermés Jconnais ma cité par cur, jgué-lar les keufs les yeux fermés J'sors, j'fais trois passes, jretourne nehess J'aime bien ta bouche, tu vas mlehess Comme d'hab', j'ai enfumé la pièce J'peux t'ambiancer en t'racontant la vie dla tess Pour niquer linstru, jai pas bsoin dvider la teille Jveux pas ber-tom donc jserre mes lacets Jai la dalle des sous, jveux des liasses dans mon assiette Jai la dalle des sous, jveux des liasses dans mon assiette J'sors, j'fais trois passes, jretourne nehess J'aime bien ta bouche, tu vas mlehess Comme d'hab', j'ai enfumé la pièce J'peux t'ambiancer en t'racontant la vie dla tess Pour niquer linstru, jai pas bsoin dvider la teille Jveux pas ber-tom donc jserre mes lacets Jai la dalle des sous, jveux des liasses dans mon assiette Jai la dalle des sous, jveux des liasses dans mon assiette2</t>
+          <t>Binks Beatz Il reste du te-shi sur le couteau Si j'l'enfonce dans ton corps, combien ça va t'coûter ? Et si t'enfiles les gants, gros, tu peux plus douter Tu fumes la frappe, tu t'envoles, tu sais plus où t'es Y a toujours mon gang avec moi en cas d'embrouille Même quand c'est chaud, faut porter ses couilles J'ai encore eu d'la chance, j'ai v'-esqui la patrouille La bonbonne est gée-char, ce soir, y aura pas d'fouille Y a d'la frappe dans l'pochtar, le ient-cli devient fou J'suis rentré tard mais j'ai fait plus de sous Les poucaves, les pédales, nan, on veut pas d'vous Askip, t'es un chaud mais bon, on t'voit pas d'vant Midi-minuit, j'suis à l'affût des bacqueux J'cache le tail-dé, j'ai vu les shtars qui débarquent Nan, j'laisse pas l'couteau dans la kitchen J'découpe la 'quette, la frappe te couche comme Jackie Chan À midi pile, le guetteur se positionne Askip, t'as poucave, j'veux voir ta déposition J'rentre cagoulé, j'suis dans l'action Y a des ients-cli, j'visser dans l'axe Y a des mes-ar dans le sac à dos Si on vient dans ton tier-quar, on f'ra pas d'cadeau Si on rentre dans l'appart', on va tout saccager Beaucoup qui font les fous, en vrai, personne agit J'sors, j'fais trois passes, jretourne nehess J'aime bien ta bouche, tu vas mlehess Comme d'hab', j'ai enfumé la pièce J'peux t'ambiancer en t'racontant la vie dla tess Pour niquer linstru', jai pas bsoin dvider la teille Jveux pas ber-tom donc jserre mes lacets Jai la dalle des sous, jveux des liasses dans mon assiette Jai la dalle des sous, jveux des liasses dans mon assiette J'sors, j'fais trois passes, jretourne nehess J'aime bien ta bouche, tu vas mlehess Comme d'hab', j'ai enfumé la pièce J'peux t'ambiancer en t'racontant la vie dla tess Pour niquer linstru jai pas bsoin dvider la teille Jveux pas ber-tom donc jserre mes lacets Jai la dalle des sous, jveux des liasses dans mon assiette Jai la dalle des sous, jveux des liasses dans mon assiette On vient dniquer un mec, jvois la BAC qui ne-tour Jviens dallumer lpét, jai djà la tête qui ne-tour Désolé, ma belle, si jme suis éloigné dtoi La monnaie mappelle, jrecompte mes billets le soir Jai caché lOpinel si y a embrouille, jle sors Avec un trou dans la jambe, comment tu ten sors ? Cest pour faire des sous si tu mvois traîner dehors Jfais que dtartiner pour avoir les couilles en or On court après la vida loca Jsuis bloqué, jvois mon bonheur dans lillégal Parfois la vie est paradoxale Pour shabiller propre, normal, on tfait du sale Dix négros dans ton tieks, cest toi qui va finir au sol Rentrer dans ma cité, jte déconseille Quand jsuis triste, y a qules billets qui me consolent Pour oublier sa meuf, le pilon, il consomme Calcule pas les raclis, elles vont rien tapporter Y a les condés dans lbat, les voisins, ils ont alerté Avant lplavon, moi et mes gars on sest bien concertés Ce soir, jrepars avec le butin, jen suis certain Le bosseur, il a enchaîné la troisième mi-temps Il lâchera pas la sacoche même avec les yeux cernés Jconnais ma cité par cur, jgué-lar les keufs les yeux fermés Jconnais ma cité par cur, jgué-lar les keufs les yeux fermés J'sors, j'fais trois passes, jretourne nehess J'aime bien ta bouche, tu vas mlehess Comme d'hab', j'ai enfumé la pièce J'peux t'ambiancer en t'racontant la vie dla tess Pour niquer linstru, jai pas bsoin dvider la teille Jveux pas ber-tom donc jserre mes lacets Jai la dalle des sous, jveux des liasses dans mon assiette Jai la dalle des sous, jveux des liasses dans mon assiette J'sors, j'fais trois passes, jretourne nehess J'aime bien ta bouche, tu vas mlehess Comme d'hab', j'ai enfumé la pièce J'peux t'ambiancer en t'racontant la vie dla tess Pour niquer linstru, jai pas bsoin dvider la teille Jveux pas ber-tom donc jserre mes lacets Jai la dalle des sous, jveux des liasses dans mon assiette Jai la dalle des sous, jveux des liasses dans mon assiette2</t>
         </is>
       </c>
     </row>
@@ -548,7 +548,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Elle utilise son corps comme si c'était un jouet Avoir une maxi kichta, c'est aussi son plus grand souhait Au fond elle est comme toi elle a la dalle des sous Au début elle voulait d'l'amour, mais tous les gars l'ont déçue Au début elle voulait d'l'amour, mais tous les gars l'ont déçue han Elle aussi, elle veut s'ranger, mais son démon prend ldessus oh Elle renie son passé, elle aime pas quand on parle de ça Elle passe inaperçue, ell peut cacher des trucs dans son c-sa Ell encaisse les thunes, elle va dans l'sud pour fêter ça Elle a un gros tarma, mais mon gars, tu vas jamais péter ça brr Tu peux t'faire tacler en deuspi, donc vérifie tes srabs han Elle peut t'faire les poches pendant qu'tu dors, donc vérifie tes sapes han Tu crois pouvoir l'oublier, en vrai, c'est elle qui te zappe hmm T'es pas tout seul sur ses côtes, tous les jours, on lui d'mande son snap hmm Enfoiré, tu crois qu'elle est comme ça juste avec oi-t ? Pour te la mettre, elle attend l'moment adéquat Elle a pas besoin d'toi pour passer à la douane, elle veut les anneaux sur la gova, s'en fout de la bague au doigt ah bon ? Pour faire son seille-o, elle utilise ses vices, et si elle donne le go, tu rembourses c'que tu dois ah bon ? Elle t'fait les yeux doux, négro, crois pas qu'elle t'aime Avant d'rentrer dans ton porte-monnaie, faut qu'elle rentre dans ta tête pow, pow Ça fait bien longtemps que t'essaies de la tej', si tu peux rien lui donner, envoie-la aux grands d'la tess You might also like Elle sait c'qu'elle veut elle veut monter en gamos brr Suffit d'un appel, un SMS et une équipe t'arrose brr Si tu la trompes, elle peut rayer toute ta carrosserie ah bon ? Tu rentres tard, elle rentre tard aussi ah bon ? Elle croit connaître la rue, elle a un reuf au placard Elle veut ton oseille, à quoi bon lui raconter tous tes bobards ? Bâtard, tes son plan B, ça sert à rien d'flamber pow En un seul regard, tous les mecs, elle les fait tomber Elle sait c'qu'elle veut elle veut monter en gamos brr Suffit d'un appel, un SMS et une équipe t'arrose brr Si tu la trompes, elle peut rayer toute ta carrosserie ah bon ? Tu rentres tard, elle rentre tard aussi ah bon ? Elle croit connaître la rue, elle a un reuf au placard Elle veut ton oseille, à quoi bon lui raconter tous tes bobards ? Bâtard, tes son plan B, ça sert à rien d'flamber pow En un seul regard, tous les mecs, elle les fait tomber Elle séduit même les hommes mariés, le chantage, elle trouve ça marrant En temps normal, c'est une pétasse, c'est une meuf bien quand ça l'arrange Méfie-toi des apparences, elle tient jamais ses paroles Tu veux qu'elle t'obéisse, mais est-ce qu'elle écoute ses parents ? Même si t'es attentionné, pour elle c'est pareil Une fois qu'elle a gratté un bon billet, elle veut se séparer Une heure avant la soirée elle est d'jà préparée Elle habite en banlieue, elle aime faire la meuf de Paris Elle s'en bat les couilles d'ta vie et de tes conseils De base elle est détendue, avec toi, elle fait la meuf coincée ah bon ? Lui donner ton cur, négro, j'te déconseille ah bon ? Zéro sentiment, le chemin est corsé ah ah bon ? Elle t'fait les yeux doux, négro, crois pas qu'elle t'aime Avant d'rentrer dans ton porte-monnaie, faut qu'elle rentre dans ta tête Ça fait bien longtemps que t'essaies de la tej', si tu peux rien lui donner, envoie-la aux grands d'la tess Elle sait c'qu'elle veut elle veut monter en gamos brr Suffit d'un appel, un SMS et une équipe t'arrose brr Si tu la trompes, elle peut rayer toute ta carrosserie ah bon ? Tu rentres tard, elle rentre tard aussi ah bon ? Elle croit connaître la rue, elle a un reuf au placard Elle veut ton oseille, à quoi bon lui raconter tous tes bobards ? Bâtard, tes son plan B, ça sert à rien d'flamber pow En un seul regard, tous les mecs, elle les fait tomber Tous les mecs, elle les fait tomber En un seul regard, tous les mecs, elle les fait tomber1</t>
+          <t>Elle utilise son corps comme si c'était un jouet Avoir une maxi kichta, c'est aussi son plus grand souhait Au fond elle est comme toi elle a la dalle des sous Au début elle voulait d'l'amour, mais tous les gars l'ont déçue Au début elle voulait d'l'amour, mais tous les gars l'ont déçue han Elle aussi, elle veut s'ranger, mais son démon prend ldessus oh Elle renie son passé, elle aime pas quand on parle de ça Elle passe inaperçue, ell peut cacher des trucs dans son c-sa Ell encaisse les thunes, elle va dans l'sud pour fêter ça Elle a un gros tarma, mais mon gars, tu vas jamais péter ça brr Tu peux t'faire tacler en deuspi, donc vérifie tes srabs han Elle peut t'faire les poches pendant qu'tu dors, donc vérifie tes sapes han Tu crois pouvoir l'oublier, en vrai, c'est elle qui te zappe hmm T'es pas tout seul sur ses côtes, tous les jours, on lui d'mande son snap hmm Enfoiré, tu crois qu'elle est comme ça juste avec oi-t ? Pour te la mettre, elle attend l'moment adéquat Elle a pas besoin d'toi pour passer à la douane, elle veut les anneaux sur la gova, s'en fout de la bague au doigt ah bon ? Pour faire son seille-o, elle utilise ses vices, et si elle donne le go, tu rembourses c'que tu dois ah bon ? Elle t'fait les yeux doux, négro, crois pas qu'elle t'aime Avant d'rentrer dans ton porte-monnaie, faut qu'elle rentre dans ta tête pow, pow Ça fait bien longtemps que t'essaies de la tej', si tu peux rien lui donner, envoie-la aux grands d'la tess Elle sait c'qu'elle veut elle veut monter en gamos brr Suffit d'un appel, un SMS et une équipe t'arrose brr Si tu la trompes, elle peut rayer toute ta carrosserie ah bon ? Tu rentres tard, elle rentre tard aussi ah bon ? Elle croit connaître la rue, elle a un reuf au placard Elle veut ton oseille, à quoi bon lui raconter tous tes bobards ? Bâtard, tes son plan B, ça sert à rien d'flamber pow En un seul regard, tous les mecs, elle les fait tomber Elle sait c'qu'elle veut elle veut monter en gamos brr Suffit d'un appel, un SMS et une équipe t'arrose brr Si tu la trompes, elle peut rayer toute ta carrosserie ah bon ? Tu rentres tard, elle rentre tard aussi ah bon ? Elle croit connaître la rue, elle a un reuf au placard Elle veut ton oseille, à quoi bon lui raconter tous tes bobards ? Bâtard, tes son plan B, ça sert à rien d'flamber pow En un seul regard, tous les mecs, elle les fait tomber Elle séduit même les hommes mariés, le chantage, elle trouve ça marrant En temps normal, c'est une pétasse, c'est une meuf bien quand ça l'arrange Méfie-toi des apparences, elle tient jamais ses paroles Tu veux qu'elle t'obéisse, mais est-ce qu'elle écoute ses parents ? Même si t'es attentionné, pour elle c'est pareil Une fois qu'elle a gratté un bon billet, elle veut se séparer Une heure avant la soirée elle est d'jà préparée Elle habite en banlieue, elle aime faire la meuf de Paris Elle s'en bat les couilles d'ta vie et de tes conseils De base elle est détendue, avec toi, elle fait la meuf coincée ah bon ? Lui donner ton cur, négro, j'te déconseille ah bon ? Zéro sentiment, le chemin est corsé ah ah bon ? Elle t'fait les yeux doux, négro, crois pas qu'elle t'aime Avant d'rentrer dans ton porte-monnaie, faut qu'elle rentre dans ta tête Ça fait bien longtemps que t'essaies de la tej', si tu peux rien lui donner, envoie-la aux grands d'la tess Elle sait c'qu'elle veut elle veut monter en gamos brr Suffit d'un appel, un SMS et une équipe t'arrose brr Si tu la trompes, elle peut rayer toute ta carrosserie ah bon ? Tu rentres tard, elle rentre tard aussi ah bon ? Elle croit connaître la rue, elle a un reuf au placard Elle veut ton oseille, à quoi bon lui raconter tous tes bobards ? Bâtard, tes son plan B, ça sert à rien d'flamber pow En un seul regard, tous les mecs, elle les fait tomber Tous les mecs, elle les fait tomber En un seul regard, tous les mecs, elle les fait tomber1</t>
         </is>
       </c>
     </row>
@@ -565,7 +565,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Ouais Quel bail ? Quel bail ? Eh, de la B Quel bail ? Quel bail ? G.A Paris, c'est magique Hein, le bendo, le rrain-te, le hazi Hein 1PLIKÉ, faut brouiller le réseau Hein, cents-quarante mmes-gra sur la pesette Hein Obligé d'faire passer les colis Hein, ton équipe à toi, c'est des comiques Oui Apparemment, c'est pas du solide Nan, apparemment, c'est pas du solide Jamais Ils ont fouillé mais n'ont rien trouvé Non, y a plusieurs cachettes dans le bolide Bou-bou-bou-bouh Tu fais que bosser à perte, tes clients t'évitent et tu dis qu'c'est le COVID Oui Cinq-cents euros pour la passe, elle passe à la casse, elle a refait le tigné Tigné La selha, ça porte la guigne Guigne, d'toute façon, la ne-zo est minée Boumi Paris, c'est magique, la banlieue, c'est danger Ouh, y a rien d'sympathique, les tits-pe veulent manger Viens, on parle en gros, le détail, c'est long, si y a rien à grailler, j'peux pas rester là Oui Attention aux folles, c'est le Sheitan Sheitan, ils fument trop de shit, ils sont chés-tou La vie de César ou de Zidane ? J'mets la famille avant comme un Rital Eh 9.1 9.1, cent moins huit Oui, viens pas ici, faut écouter les gens Jamais Dis-moi Dis-moi, à ton avis Hein ?, est-ce que les mecs que j'ai fait écoutaient mes sons ? Évry De la B, Clamart-zoo Ouh, viens pas ici, faut écouter les gens Dis-moi Dis-moi, à ton avis Oui, est-ce que les mecs que j'ai fait écoutaient mes sons ? You might also like Paris, c'est magique Hein, le bendo, le rrain-te, le hazi Hein 1PLIKÉ, faut brouiller le réseau Hein, cents-quarante mmes-gra sur la pesette Hein Obligé d'faire passer les colis Hein, ton équipe à toi, c'est des comiques Oui Apparemment, c'est pas du solide Nan, apparemment, c'est pas du solide Brr, brr, brr, jamais Paris, c'est magique Hein, le bendo, le rrain-te, le hazi Hein 1PLIKÉ, faut brouiller le réseau Hein, cents-quarante mmes-gra sur la pesette Bou-bou-bou-bouh Obligé d'faire passer les colis Hein, ton équipe à toi, c'est des comiques Oui, méchant, méchant Apparemment, c'est pas du solide Nan, apparemment, c'est pas du solide Brr, brr, brr, jamais J'sais que ce soir, j'empoche, j'me frotte déjà les mains Poh, est-ce que t'éteins l'moteur si on t'démarre Poh ? Est-ce que t'éteins l'moteur si on t'démarre ? Est-ce que tu donnes des blases si on t'demande Drr ? 140 défouraille, c'est trop méchant Han, j'suis boosté, j'crois qu'y a des djinns dans ma jambe Han J'm'accroche aux loves, j'aurai moins d'mal en lâchant, j'fais du ffre-chi, ça fait du mal à l'agent Drr Aucun regret à part ces putes que j'ai baisées Uh, j'ai buzzé grâce aux instru' que j'ai baisées Uh Grâce à ma voix et mon flow de baisé Uh, j'rêvais d'voler quand j'regardais DBZ Uh Pourquoi j'l'ai fait autrement ? En si peu d'temps, j'suis devenu un stre-mon 1PLIKÉ J'aime quand j'me défoule sur l'instrument' 1PLIKÉ en tac-tac, juste pour leur trer-mon 1PLIKÉ A c'qui-p', c'est toi qui as les outils Brr, brr, brr mais c'est ta meuf qui veut qu'on la démonte Bâtard, ton pardon inutile, mon cur Han, j'le répare pas avec des mots Salope Que des coups, des pensées macabres Jamais, flashback des schmitts qui retournent ma cave Jamais Qui golent-ri quand j'suis dans l'fond d'la G.A.V Jamais, quand-quand j'suis dans l'fond d'la G.A.V Brr Paris, c'est magique Hein, le bendo, le rrain-te, le hazi Hein 1PLIKÉ, faut brouiller le réseau Hein, cents-quarante mmes-gra sur la pesette Hein, bou-bou-bou-bouh Obligé d'faire passer les colis Hein, ton équipe à toi, c'est des comiques Oui, méchant, méchant Apparemment, c'est pas du solide Nan, apparemment, c'est pas du solide Brr, brr, brr, jamais Paris, c'est magique Hein, le bendo, le rrain-te, le hazi Hein 1PLIKÉ, faut brouiller le réseau Hein, cents-quarante mmes-gra sur la pesette Bou-bou-bou-bouh Obligé d'faire passer les colis Hein, ton équipe à toi, c'est des comiques Oui, méchant, méchant Apparemment, c'est pas du solide Nan, apparemment, c'est pas du solide Brr, brr, brr, jamais Paris, c'est magique 1PLIKÉ 1PLIKÉ, faut brouiller le réseau Brr, brr, brr Obligé d'faire passer les colis</t>
+          <t>Ouais Quel bail ? Quel bail ? Eh, de la B Quel bail ? Quel bail ? G.A Paris, c'est magique Hein, le bendo, le rrain-te, le hazi Hein 1PLIKÉ, faut brouiller le réseau Hein, cents-quarante mmes-gra sur la pesette Hein Obligé d'faire passer les colis Hein, ton équipe à toi, c'est des comiques Oui Apparemment, c'est pas du solide Nan, apparemment, c'est pas du solide Jamais Ils ont fouillé mais n'ont rien trouvé Non, y a plusieurs cachettes dans le bolide Bou-bou-bou-bouh Tu fais que bosser à perte, tes clients t'évitent et tu dis qu'c'est le COVID Oui Cinq-cents euros pour la passe, elle passe à la casse, elle a refait le tigné Tigné La selha, ça porte la guigne Guigne, d'toute façon, la ne-zo est minée Boumi Paris, c'est magique, la banlieue, c'est danger Ouh, y a rien d'sympathique, les tits-pe veulent manger Viens, on parle en gros, le détail, c'est long, si y a rien à grailler, j'peux pas rester là Oui Attention aux folles, c'est le Sheitan Sheitan, ils fument trop de shit, ils sont chés-tou La vie de César ou de Zidane ? J'mets la famille avant comme un Rital Eh 9.1 9.1, cent moins huit Oui, viens pas ici, faut écouter les gens Jamais Dis-moi Dis-moi, à ton avis Hein ?, est-ce que les mecs que j'ai fait écoutaient mes sons ? Évry De la B, Clamart-zoo Ouh, viens pas ici, faut écouter les gens Dis-moi Dis-moi, à ton avis Oui, est-ce que les mecs que j'ai fait écoutaient mes sons ? Paris, c'est magique Hein, le bendo, le rrain-te, le hazi Hein 1PLIKÉ, faut brouiller le réseau Hein, cents-quarante mmes-gra sur la pesette Hein Obligé d'faire passer les colis Hein, ton équipe à toi, c'est des comiques Oui Apparemment, c'est pas du solide Nan, apparemment, c'est pas du solide Brr, brr, brr, jamais Paris, c'est magique Hein, le bendo, le rrain-te, le hazi Hein 1PLIKÉ, faut brouiller le réseau Hein, cents-quarante mmes-gra sur la pesette Bou-bou-bou-bouh Obligé d'faire passer les colis Hein, ton équipe à toi, c'est des comiques Oui, méchant, méchant Apparemment, c'est pas du solide Nan, apparemment, c'est pas du solide Brr, brr, brr, jamais J'sais que ce soir, j'empoche, j'me frotte déjà les mains Poh, est-ce que t'éteins l'moteur si on t'démarre Poh ? Est-ce que t'éteins l'moteur si on t'démarre ? Est-ce que tu donnes des blases si on t'demande Drr ? 140 défouraille, c'est trop méchant Han, j'suis boosté, j'crois qu'y a des djinns dans ma jambe Han J'm'accroche aux loves, j'aurai moins d'mal en lâchant, j'fais du ffre-chi, ça fait du mal à l'agent Drr Aucun regret à part ces putes que j'ai baisées Uh, j'ai buzzé grâce aux instru' que j'ai baisées Uh Grâce à ma voix et mon flow de baisé Uh, j'rêvais d'voler quand j'regardais DBZ Uh Pourquoi j'l'ai fait autrement ? En si peu d'temps, j'suis devenu un stre-mon 1PLIKÉ J'aime quand j'me défoule sur l'instrument' 1PLIKÉ en tac-tac, juste pour leur trer-mon 1PLIKÉ A c'qui-p', c'est toi qui as les outils Brr, brr, brr mais c'est ta meuf qui veut qu'on la démonte Bâtard, ton pardon inutile, mon cur Han, j'le répare pas avec des mots Salope Que des coups, des pensées macabres Jamais, flashback des schmitts qui retournent ma cave Jamais Qui golent-ri quand j'suis dans l'fond d'la G.A.V Jamais, quand-quand j'suis dans l'fond d'la G.A.V Brr Paris, c'est magique Hein, le bendo, le rrain-te, le hazi Hein 1PLIKÉ, faut brouiller le réseau Hein, cents-quarante mmes-gra sur la pesette Hein, bou-bou-bou-bouh Obligé d'faire passer les colis Hein, ton équipe à toi, c'est des comiques Oui, méchant, méchant Apparemment, c'est pas du solide Nan, apparemment, c'est pas du solide Brr, brr, brr, jamais Paris, c'est magique Hein, le bendo, le rrain-te, le hazi Hein 1PLIKÉ, faut brouiller le réseau Hein, cents-quarante mmes-gra sur la pesette Bou-bou-bou-bouh Obligé d'faire passer les colis Hein, ton équipe à toi, c'est des comiques Oui, méchant, méchant Apparemment, c'est pas du solide Nan, apparemment, c'est pas du solide Brr, brr, brr, jamais Paris, c'est magique 1PLIKÉ 1PLIKÉ, faut brouiller le réseau Brr, brr, brr Obligé d'faire passer les colis</t>
         </is>
       </c>
     </row>
@@ -582,7 +582,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Wouh, wouh Poh, poh Il m'faut une montagne de kichta, pas une montagne de coke comme Tony Montana poh Si j'pète le million, j'finis à Punta Cana poh, t'as fait l'canard donc cette pute, elle t'a carna poh 9-2-1-4-0, tu m'reconnais, sur l'terrain, j'dis aux ients-cli d'aller s'abonner brr Si t'es pas prêt pour la guerre, bâtard brr, j'te conseille d'abandonner brr Y a un mec à faire donc j'enfile le bandana, y a plus d'bédo, t'inquiète, j'te rappelle quand y en a J'm'éloigne des putes, j'me rapproche d'la marijuana poh, j'me rapproche d'la marijuana poh Faut v'-esqui les keufs, faut v'-esqui le corona et même quand c'est chaud, faut porter ses cojones Et pour régler une embrouille, des négros cagoulés devant ton adresse Des mmes-gra d'pilon dans la saisie han, igo, comment veux-tu qu'j'sois honnête han ? On revient pas le lendemain poh, on t'encule ta race même si tu fais deux mètres poh J'aime voir les billets dans ma pocket brr Attiré par l'argent haram pourtant brr, j'suis conscient qu'tous les jours, la mort me guette brr Tous les jours brr, la mort me guette brr J'crois en Dieu, j'peux pas t'ôter la vie, dans la street, on survit J'fume, j'oublie tous mes souvenirs han, j'reste à l'affût, j'aperçois les condés venir han Si t'as fauté, on va t'punir poh, j't'aimais bien, guette comment t'es devenu poh T'as donné des blases, tu traînes plus avec nous mmh, après ça, la vie continue mmh J'aime quand les billets s'entassent dans mon lit, gros, j'm'en bats les couilles de son tinié salope T'es tombé love, t'as fini ruiné salope, me promène avec l'opinel poh J'attends le premier qui vient chiffonner poh, j'lève un doigt à l'OPJ qui vient mauditionner han Des mmes-gra d'pilon dans la saisie han, igo, comment veux-tu qu'j'sois honnête han ? On revient pas le lendemain poh, on t'encule ta race même si tu fais deux mètres wouh J'croise la que-ba sur le chemin wouh, si j'me fais ser-cour, jamais j'm'arrête J'ai d'la moula, ton te-shi, il colle Non, j'suis pas v'nu pour chanter, l'instrumentale, j'l'ai attrapée par le col poh J'l'ai attrapée par le col poh You might also like Le rap, ça vient d'la ue-r la ue-r alors tu veux qu'j'te parle de quoi han ? Ça vient d'où si t'es un mec d'ailleurs poh ? Pour les loss-bo, on t'dit, tu veux quoi poh ? Et si t'as pas mis les gants sur le plan, j'espère que t'as un bon avocat brr Toi, t'es un chaud quand tu parles dans en vocal brr, y a du doré emballé dans le local brr Y a trop d'tiaga, j'ai pas l'temps d'les cala, toi, quand y a guenda, tu fais semblant qu't'es pas là On fonce dans l'tas, on s'en fout d'avoir des balafres, la BAC qui tourne au quartier, ouais, c'est banal Comme d'hab', on piétine le premier qui parle mal poh J'trouve ça pas mal poh Y a rien a faire au quartier donc on carna poh, si on descend chez eux poh, on fait un carnage poh On démarre ton scoot', on enlève les carénage, Opinel sorti en moins d'deux secondes, ils font la Macarena Les bacqueux m'ont suivi carrément, j'suis à l'affût juste avant d'rentrer chez moi han J'représente 140 BRIKS précisément Regarde derrière toi quand tu ches-mar poh, j'ai tordu l'instru comme le neiman J'cours après les thunes mais maman en a marre brr L'argent tombe pas du ciel pourtant, faut qu'j'ramasse brr J'aime quand les ients-cli sont hmar brr Même pas besoin de les rabattre ils sont attirés par l'odeur du kamas Bâtard, tu veux faire la guerre, on commence wouh Et c'est jamais fini à tout moment, gros, l'instru' elle recommence poh Pas besoin d'hausser le ton, gros han Opinel sorti en moins d'deux secondes han, ils s'mettent à danser le tango brr J'ai pas encore chouara, j'attends l'go brr, j'vais pas finir menotté dans la Kangoo brr J'ai retiré mon cur, j'ai mis la cagoule poh Hors-série, c'est juste un avant-goût poh, hors-série, c'est juste un avant-goût poh Pas besoin d'hausser le ton, gros han Opinel sorti en moins d'deux secondes han, ils s'mettent à danser le tango brr J'ai pas encore chouara, j'attends l'go brr, j'vais pas finir menotté dans la Kangoo brr J'ai retiré mon cur, j'ai mis la cagoule poh Hors-série, c'est juste un avant-goût poh, hors-série, c'est juste un avant-goût poh</t>
+          <t>Wouh, wouh Poh, poh Il m'faut une montagne de kichta, pas une montagne de coke comme Tony Montana poh Si j'pète le million, j'finis à Punta Cana poh, t'as fait l'canard donc cette pute, elle t'a carna poh 9-2-1-4-0, tu m'reconnais, sur l'terrain, j'dis aux ients-cli d'aller s'abonner brr Si t'es pas prêt pour la guerre, bâtard brr, j'te conseille d'abandonner brr Y a un mec à faire donc j'enfile le bandana, y a plus d'bédo, t'inquiète, j'te rappelle quand y en a J'm'éloigne des putes, j'me rapproche d'la marijuana poh, j'me rapproche d'la marijuana poh Faut v'-esqui les keufs, faut v'-esqui le corona et même quand c'est chaud, faut porter ses cojones Et pour régler une embrouille, des négros cagoulés devant ton adresse Des mmes-gra d'pilon dans la saisie han, igo, comment veux-tu qu'j'sois honnête han ? On revient pas le lendemain poh, on t'encule ta race même si tu fais deux mètres poh J'aime voir les billets dans ma pocket brr Attiré par l'argent haram pourtant brr, j'suis conscient qu'tous les jours, la mort me guette brr Tous les jours brr, la mort me guette brr J'crois en Dieu, j'peux pas t'ôter la vie, dans la street, on survit J'fume, j'oublie tous mes souvenirs han, j'reste à l'affût, j'aperçois les condés venir han Si t'as fauté, on va t'punir poh, j't'aimais bien, guette comment t'es devenu poh T'as donné des blases, tu traînes plus avec nous mmh, après ça, la vie continue mmh J'aime quand les billets s'entassent dans mon lit, gros, j'm'en bats les couilles de son tinié salope T'es tombé love, t'as fini ruiné salope, me promène avec l'opinel poh J'attends le premier qui vient chiffonner poh, j'lève un doigt à l'OPJ qui vient mauditionner han Des mmes-gra d'pilon dans la saisie han, igo, comment veux-tu qu'j'sois honnête han ? On revient pas le lendemain poh, on t'encule ta race même si tu fais deux mètres wouh J'croise la que-ba sur le chemin wouh, si j'me fais ser-cour, jamais j'm'arrête J'ai d'la moula, ton te-shi, il colle Non, j'suis pas v'nu pour chanter, l'instrumentale, j'l'ai attrapée par le col poh J'l'ai attrapée par le col poh Le rap, ça vient d'la ue-r la ue-r alors tu veux qu'j'te parle de quoi han ? Ça vient d'où si t'es un mec d'ailleurs poh ? Pour les loss-bo, on t'dit, tu veux quoi poh ? Et si t'as pas mis les gants sur le plan, j'espère que t'as un bon avocat brr Toi, t'es un chaud quand tu parles dans en vocal brr, y a du doré emballé dans le local brr Y a trop d'tiaga, j'ai pas l'temps d'les cala, toi, quand y a guenda, tu fais semblant qu't'es pas là On fonce dans l'tas, on s'en fout d'avoir des balafres, la BAC qui tourne au quartier, ouais, c'est banal Comme d'hab', on piétine le premier qui parle mal poh J'trouve ça pas mal poh Y a rien a faire au quartier donc on carna poh, si on descend chez eux poh, on fait un carnage poh On démarre ton scoot', on enlève les carénage, Opinel sorti en moins d'deux secondes, ils font la Macarena Les bacqueux m'ont suivi carrément, j'suis à l'affût juste avant d'rentrer chez moi han J'représente 140 BRIKS précisément Regarde derrière toi quand tu ches-mar poh, j'ai tordu l'instru comme le neiman J'cours après les thunes mais maman en a marre brr L'argent tombe pas du ciel pourtant, faut qu'j'ramasse brr J'aime quand les ients-cli sont hmar brr Même pas besoin de les rabattre ils sont attirés par l'odeur du kamas Bâtard, tu veux faire la guerre, on commence wouh Et c'est jamais fini à tout moment, gros, l'instru' elle recommence poh Pas besoin d'hausser le ton, gros han Opinel sorti en moins d'deux secondes han, ils s'mettent à danser le tango brr J'ai pas encore chouara, j'attends l'go brr, j'vais pas finir menotté dans la Kangoo brr J'ai retiré mon cur, j'ai mis la cagoule poh Hors-série, c'est juste un avant-goût poh, hors-série, c'est juste un avant-goût poh Pas besoin d'hausser le ton, gros han Opinel sorti en moins d'deux secondes han, ils s'mettent à danser le tango brr J'ai pas encore chouara, j'attends l'go brr, j'vais pas finir menotté dans la Kangoo brr J'ai retiré mon cur, j'ai mis la cagoule poh Hors-série, c'est juste un avant-goût poh, hors-série, c'est juste un avant-goût poh</t>
         </is>
       </c>
     </row>
@@ -599,7 +599,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Chacun son métier, le mien, c'est d'ravitailler, brr, on rafale tous tes négros vont tailler Comment tu veux qu'j't'arrange si t'es un mec d'ailleurs ? Soit tu paies, soit on t'fume, mieux vaut tard que jamais J'suis bloqué l'implication m'a condamné, j'me d'mande je vais penser comme ça combien d'années J'ouvrais l'terrain à midi c'est moi qui donnait, j'en ai mis des buts avec la main d'Maradona Si tu trahis l'tieks, on pourra pas t'pardonner, pas b'soin d'leur force pour envoyer l'genkidama han Dans ton tieks, beaucoup d'gens qui dorment, dans la ve-ca, les los-ki dorment Baraude, capuché dans l'secteur et fais tes thunes, devant les keufs, ne change pas ton attitude Faut qu'tu ramasses mais n'oublie jamais les études, les p'tits ont grandi trop vite, poto, laisse ber-tom Nan, je perds pas mon temps sur le bitume, j'pull up en North Face j'm'en bats les c' de Louis Vuitton Chez nous, tous les jours, les shtars, nous évitons, mon son dans la tchop, obligé d'rouler vite Combien d'fois j'ai rêvé d'la Dolce Vita ? L'amour, ça te tue, l'argent, c'est vital ah bon ? Combien d'fois j'ai rêvé d'la Dolce Vita ? L'amour, ça te tue, l'argent, c'est vital ah bon ? Nan, je perds pas mon temps sur le bitume, j'pull up en North Face j'm'en bats les c' de Louis Vuitton Chez nous, tous les jours, les shtars, nous évitons, mon son dans la tchop, obligé d'rouler vite Combien d'fois j'ai rêvé d'la Dolce Vita ? L'amour, ça te tue, l'argent, c'est vital ah bon ? Combien d'fois j'ai rêvé d'la Dolce Vita ? L'amour, ça te tue, l'argent, c'est vital ah bon ? Ils m'donnent pas la force, ils m'demandent des feats, le pe-ra, c'est vicieux, t'inquiète, j'me méfie d'eux J'm'éloigne des chickens, j'm'éloigne des fils de, j'me rapproche du bénéfice De la beugueuh, pour cent meuj, il faut qu'tu sortes six deux, toujours La Mala ou Bizon qui m'assiste J'la baise même si son père, c'est un raciste, j'ai, peut-être vi-ser ta sista Ta copine t'a raconté du baratin, elle fait la sainte mais mes négros, ils l'ont cata' Faut encaisser brasser comme le Qatar, si j'finis locataire, re-noi, c'est la cata' Une bonbonne dans l'cavu, elle veut connaître ma vie, salope casse toi d'ma vue J'chouara, j'pète une somme en ni vu ni connu, comme Kobe, j'veux pas finir en hélico J'veux pas mourir dans une villa comme Tony, tu peux t'faire perquis' alors cache rien sous ton lit Avant d'donner l'argent vérifie le colis, ça fait bien longtemps qu'j'suis plus écolier brr J'ai commencé l'vol, j'rentrais avec des colliers brr, j'ai arrêté l'vol mais l'ient-cli j'fais décoller brr Au début, c'était pour déconner, mon but c'est d'me barrer, arrêter les conneries Elle a vu la sse-lia donc elle croit qu'j'suis che-ri, j'veux juste la doro, elle veut qu'j'sois son chéri Si j'cours après une fille, c'est pour la cher-ra, j'en place une pour les charbonneurs qui lâchent rien pow, pow J'détaille des savonnettes, j'ai les mains sales, une voix dans ma tête m'dit 1PLIKÉ termine ça Mes négros vi-sser des Blancs à Château d'Versailles, est-ce que Louis XIV avait pensé à ça ? You might also like Nan, je perds pas mon temps sur le bitume, j'pull up en North Face j'm'en bats les c' de Louis Vuitton Chez nous, tous les jours, les shtars, nous évitons, mon son dans la tchop, obligé d'rouler vite Combien d'fois j'ai rêvé d'la Dolce Vita ? L'amour, ça te tue, l'argent, c'est vital ah bon ? Combien d'fois j'ai rêvé d'la Dolce Vita ? L'amour, ça te tue, l'argent, c'est vital ah bon ? Nan, je perds pas mon temps sur le bitume, j'pull up en North Face j'm'en bats les c' de Louis Vuitton Chez nous, tous les jours, les shtars, nous évitons, mon son dans la tchop, obligé d'rouler vite Combien d'fois j'ai rêvé d'la Dolce Vita ? L'amour, ça te tue, l'argent, c'est vital ah bon ? Combien d'fois j'ai rêvé d'la Dolce Vita ? L'amour, ça te tue, l'argent, c'est vital ah bon ?1</t>
+          <t>Chacun son métier, le mien, c'est d'ravitailler, brr, on rafale tous tes négros vont tailler Comment tu veux qu'j't'arrange si t'es un mec d'ailleurs ? Soit tu paies, soit on t'fume, mieux vaut tard que jamais J'suis bloqué l'implication m'a condamné, j'me d'mande je vais penser comme ça combien d'années J'ouvrais l'terrain à midi c'est moi qui donnait, j'en ai mis des buts avec la main d'Maradona Si tu trahis l'tieks, on pourra pas t'pardonner, pas b'soin d'leur force pour envoyer l'genkidama han Dans ton tieks, beaucoup d'gens qui dorment, dans la ve-ca, les los-ki dorment Baraude, capuché dans l'secteur et fais tes thunes, devant les keufs, ne change pas ton attitude Faut qu'tu ramasses mais n'oublie jamais les études, les p'tits ont grandi trop vite, poto, laisse ber-tom Nan, je perds pas mon temps sur le bitume, j'pull up en North Face j'm'en bats les c' de Louis Vuitton Chez nous, tous les jours, les shtars, nous évitons, mon son dans la tchop, obligé d'rouler vite Combien d'fois j'ai rêvé d'la Dolce Vita ? L'amour, ça te tue, l'argent, c'est vital ah bon ? Combien d'fois j'ai rêvé d'la Dolce Vita ? L'amour, ça te tue, l'argent, c'est vital ah bon ? Nan, je perds pas mon temps sur le bitume, j'pull up en North Face j'm'en bats les c' de Louis Vuitton Chez nous, tous les jours, les shtars, nous évitons, mon son dans la tchop, obligé d'rouler vite Combien d'fois j'ai rêvé d'la Dolce Vita ? L'amour, ça te tue, l'argent, c'est vital ah bon ? Combien d'fois j'ai rêvé d'la Dolce Vita ? L'amour, ça te tue, l'argent, c'est vital ah bon ? Ils m'donnent pas la force, ils m'demandent des feats, le pe-ra, c'est vicieux, t'inquiète, j'me méfie d'eux J'm'éloigne des chickens, j'm'éloigne des fils de, j'me rapproche du bénéfice De la beugueuh, pour cent meuj, il faut qu'tu sortes six deux, toujours La Mala ou Bizon qui m'assiste J'la baise même si son père, c'est un raciste, j'ai, peut-être vi-ser ta sista Ta copine t'a raconté du baratin, elle fait la sainte mais mes négros, ils l'ont cata' Faut encaisser brasser comme le Qatar, si j'finis locataire, re-noi, c'est la cata' Une bonbonne dans l'cavu, elle veut connaître ma vie, salope casse toi d'ma vue J'chouara, j'pète une somme en ni vu ni connu, comme Kobe, j'veux pas finir en hélico J'veux pas mourir dans une villa comme Tony, tu peux t'faire perquis' alors cache rien sous ton lit Avant d'donner l'argent vérifie le colis, ça fait bien longtemps qu'j'suis plus écolier brr J'ai commencé l'vol, j'rentrais avec des colliers brr, j'ai arrêté l'vol mais l'ient-cli j'fais décoller brr Au début, c'était pour déconner, mon but c'est d'me barrer, arrêter les conneries Elle a vu la sse-lia donc elle croit qu'j'suis che-ri, j'veux juste la doro, elle veut qu'j'sois son chéri Si j'cours après une fille, c'est pour la cher-ra, j'en place une pour les charbonneurs qui lâchent rien pow, pow J'détaille des savonnettes, j'ai les mains sales, une voix dans ma tête m'dit 1PLIKÉ termine ça Mes négros vi-sser des Blancs à Château d'Versailles, est-ce que Louis XIV avait pensé à ça ? Nan, je perds pas mon temps sur le bitume, j'pull up en North Face j'm'en bats les c' de Louis Vuitton Chez nous, tous les jours, les shtars, nous évitons, mon son dans la tchop, obligé d'rouler vite Combien d'fois j'ai rêvé d'la Dolce Vita ? L'amour, ça te tue, l'argent, c'est vital ah bon ? Combien d'fois j'ai rêvé d'la Dolce Vita ? L'amour, ça te tue, l'argent, c'est vital ah bon ? Nan, je perds pas mon temps sur le bitume, j'pull up en North Face j'm'en bats les c' de Louis Vuitton Chez nous, tous les jours, les shtars, nous évitons, mon son dans la tchop, obligé d'rouler vite Combien d'fois j'ai rêvé d'la Dolce Vita ? L'amour, ça te tue, l'argent, c'est vital ah bon ? Combien d'fois j'ai rêvé d'la Dolce Vita ? L'amour, ça te tue, l'argent, c'est vital ah bon ?1</t>
         </is>
       </c>
     </row>
@@ -616,7 +616,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Si tu veux larsa, mets-toi à g'noux, y a d'la moula et d'la beuh au menu poh Tu sais pourquoi on est venus, on est gentils poh, on t'a fumé à mains nues poh, poh Nan, j'suis pas dans les I love you brr, j'suis dans des plavons avec mes you-v' brr J'aime voir les schmitts brûler dans la Kangoo brr, pour v'-esqui les caméras, on met la cagoule Devant l'OPJ, j'réponds pas aux questions, 9-2-1-4-0 sur le pochton wouh J'ai sorti un truc et j'lui ai foutu les j'tons, salope, il faut que tu lèches tout salope J'avoue, la vie est cruelle, après le Ça vient d'où ? Faut qu'tu lâches tout poh Non, on pourra jamais lâcher nos couilles, mais on peut t'chouara si t'as trop de chaînes au cou han Y a du bon doré comme les ch'veux de Son Goku, j'veux des billets, j'm'en bats les couilles de son gros cul ouh J'viens tout baiser, j'm'en bats les couilles de la concu', j'aime quand l'pe-ra me rapporte des gues-shla en plus wouh Et si on rentre en embrouille poh, on t'encule ta mère si on te croise dans le bus salope Faut que j'm'occupe de ma Lebara salope, j'calcule pas ces putes, igo, j'pense qu'à ma puce han J'viens kicker l'instru', j'ai pas de frein han, comme d'habitude, j'la fais sans refrain Même si tu brasses des thunes, gros, tu meurs à la fin han T'es trop con, j'vais pas t'faire un dessin han Il veut t'rotte-ca et toi, tu mords à l'hameçon, même en descente, toujours du shit dans le caleçon Pourquoi faire la mala ? Gros, c'est qu'une location, j'ai la haine quand j'reçois une convocation brr, brr, brr Impliqué dans les bails bre-som wouh, mauvaises fréquentations, j'fais ça pour l'argent wouh Ne crois pas qu'c'est ma passion, j'ai rempli mes poches, donc j'ai rempli ma mission J'veux un gamos garé juste devant ma maison brr, après la guerre, y aura pas d'réconciliation brr On n'est pas sociables, on peut t'enculer à six, j'peux pas devenir chelou à cause d'une racli wouh You might also like Et ces rappeurs, ils font les racailles poh mais dans leurs sons, ces salauds, ils disent de la caille poh T'es un chaud seulement quand tu prends une 'teille de sky, j'suis un vrai négro, alors j'peux pas faire de zgar Y a les condés à pattes, alors faut qu'tu bombardes, j'ai la main dans l'sac et y a personne qui m'regarde Tu t'fais planter même si tu fais du krav-maga poh, passe au quartier, gros, y a toujours du bon taga Passe au quartier, gros, y a toujours du bon taga, on peut t'racketter si on n'aime pas trop ta gueule Tu t'es fait contrôler, igo, t'as baissé ta garde poh, sous le rrain-té, c'est l'odeur d'la frappe qui t'accueille Et c'est bien beau d'avoir un gun, mais faut les couilles qui vont avec C'est l'heure de manger, j'veux des liasses dans mon assiette, j'crois bien qu'j'ai grandi dans le mauvais tieks Après l'agression, tu te remémores la scène mmh, on allume les condés à la chaîne mmh Même si c'est pas le 14, la lame pénètre ton corps poh, pourquoi bomber le torse ? poh Croco, dinero, sors le matos brr, j'ai l'sourire quand le ient-cli y vient prendre sa cons' brr J'tape une gestu' en survêt' Lacoste, pour te dépouiller, on t'attend devant l'tacos brr1</t>
+          <t>Si tu veux larsa, mets-toi à g'noux, y a d'la moula et d'la beuh au menu poh Tu sais pourquoi on est venus, on est gentils poh, on t'a fumé à mains nues poh, poh Nan, j'suis pas dans les I love you brr, j'suis dans des plavons avec mes you-v' brr J'aime voir les schmitts brûler dans la Kangoo brr, pour v'-esqui les caméras, on met la cagoule Devant l'OPJ, j'réponds pas aux questions, 9-2-1-4-0 sur le pochton wouh J'ai sorti un truc et j'lui ai foutu les j'tons, salope, il faut que tu lèches tout salope J'avoue, la vie est cruelle, après le Ça vient d'où ? Faut qu'tu lâches tout poh Non, on pourra jamais lâcher nos couilles, mais on peut t'chouara si t'as trop de chaînes au cou han Y a du bon doré comme les ch'veux de Son Goku, j'veux des billets, j'm'en bats les couilles de son gros cul ouh J'viens tout baiser, j'm'en bats les couilles de la concu', j'aime quand l'pe-ra me rapporte des gues-shla en plus wouh Et si on rentre en embrouille poh, on t'encule ta mère si on te croise dans le bus salope Faut que j'm'occupe de ma Lebara salope, j'calcule pas ces putes, igo, j'pense qu'à ma puce han J'viens kicker l'instru', j'ai pas de frein han, comme d'habitude, j'la fais sans refrain Même si tu brasses des thunes, gros, tu meurs à la fin han T'es trop con, j'vais pas t'faire un dessin han Il veut t'rotte-ca et toi, tu mords à l'hameçon, même en descente, toujours du shit dans le caleçon Pourquoi faire la mala ? Gros, c'est qu'une location, j'ai la haine quand j'reçois une convocation brr, brr, brr Impliqué dans les bails bre-som wouh, mauvaises fréquentations, j'fais ça pour l'argent wouh Ne crois pas qu'c'est ma passion, j'ai rempli mes poches, donc j'ai rempli ma mission J'veux un gamos garé juste devant ma maison brr, après la guerre, y aura pas d'réconciliation brr On n'est pas sociables, on peut t'enculer à six, j'peux pas devenir chelou à cause d'une racli wouh Et ces rappeurs, ils font les racailles poh mais dans leurs sons, ces salauds, ils disent de la caille poh T'es un chaud seulement quand tu prends une 'teille de sky, j'suis un vrai négro, alors j'peux pas faire de zgar Y a les condés à pattes, alors faut qu'tu bombardes, j'ai la main dans l'sac et y a personne qui m'regarde Tu t'fais planter même si tu fais du krav-maga poh, passe au quartier, gros, y a toujours du bon taga Passe au quartier, gros, y a toujours du bon taga, on peut t'racketter si on n'aime pas trop ta gueule Tu t'es fait contrôler, igo, t'as baissé ta garde poh, sous le rrain-té, c'est l'odeur d'la frappe qui t'accueille Et c'est bien beau d'avoir un gun, mais faut les couilles qui vont avec C'est l'heure de manger, j'veux des liasses dans mon assiette, j'crois bien qu'j'ai grandi dans le mauvais tieks Après l'agression, tu te remémores la scène mmh, on allume les condés à la chaîne mmh Même si c'est pas le 14, la lame pénètre ton corps poh, pourquoi bomber le torse ? poh Croco, dinero, sors le matos brr, j'ai l'sourire quand le ient-cli y vient prendre sa cons' brr J'tape une gestu' en survêt' Lacoste, pour te dépouiller, on t'attend devant l'tacos brr1</t>
         </is>
       </c>
     </row>
@@ -633,7 +633,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Louis, ah, ah Insolent, depuis minot Insolent, depuis minot Poh, poh, poh 9.2, 1.4.0 sur le pocheton 9.2, 1.4.0 sur le pocheton Poh, poh, poh 9.2, 1.4.0 sur le pocheton, si l'argent rend beau, on t'enlève ta beauté Brr T'es un chaud quand tu bois la pisse du diable Brr, brr, qu'est-ce tu fais si on t'enlève ta bouteille ? Cagoulé à chaque fois qu'j'tenais l'sac pour pas glisser sur l'terrain comme Boateng Ah bon ? On s'promène chez eux avec des béquilles, ce soir, tous les ennemis vont boîter Ah bon ? Fin d'G.A.V, on m'dit Fais pas d'bêtise, nique ta grand-mère, j'ressors et j'fais d'la D Poh Pour un cent meuj de beuh, il faut qu'tu cotises Poh, poh, on a toujours la ppe-fra qui t'fait bader Poh Gros, ça vise pas les bes-j', ça vise ton cochi, si on t'hagar, on hagar ton pote aussi Brr Que des liasses dans mon assiette, j'ai bien grossi Brr, brr, le cur noirci, le mal nous amochi Brr C'est une kakala devant toi, elle fait la timide Uh, faut sortir la kichta pour la faire gémir Uh Bâtard, j'vais pas quitter l'trône comme Vladimir, tu vas cracher les tales, j'te l'ai d'jà dit, mec Opinel 13, j'cours même pas devant dix mecs, Byakugan, j'rodave les vingt-deux à dix mètres Skalape en moins d'une heure, me fait changer d'humeur, mmh, faut qu'ça pète comme les tours jumelles Brr J'repense au passé, j'avais zéro pitié, est-ce que j'vais rembourser les curs que j'ai cassés ? La haine, j'ai attisé Tout va bien tant qu'la puce est activée, sur ma mère que j'vais jamais pactiser Négro, bois pas si tu sais pas tiser, la 'teille, j'la bois cul sec Que des têtes cramées sur l'banc des accusés, c'est pas en tenant l'sac que t'auras un Q7 Bâtard, la brigade canine, elle veut péter mon shit, belek, ta frangine veut péter mon chibre Han J'vide la Cristalline et je remplis mon 'she, les porcs, ils veulent péter mon chiffre Zéro démocratie, c'est la voyoucratie Salope Si j'mélange vodka-cassis Salope, c'est toi qui vas payer les pots cassés Poh, poh Charbon, argent sale, j'suis bon qu'à ça Poh Ceux qui descendent ne veulent plus repasser, j'traîne avec des 3arbi, que des gueules cassées Mali, Côte d'Ivoire, Congo, Kinshasa Brr, tous mes Comoriens, j'viens dédicacer Brr On va te gonfler si t'es trop kassa, j'fais gonfler ma liasse, j'v'-esqui la casa J'aime trop l'argent, donc j'esquive le cazin', j'aime pas trop les jeux d'hasard You might also like Insolent depuis minot, fuck l'amour Fuck Juliette et Roméo, fuck Zemmour et toutes ses idéaux Le regard est froid, viens t'per-ta si t'es chaud, hendek, ça peut t'quer-cho J'suis pas seul dans la bine-ca, mon cerveau, il chauffe Mmh Comme d'habitude, le guetteur, il chouffe Poh On fait la guerre, protège bien tes abdominaux Poh, poh Rafale, poh, impossible qu'on échoue Poh Ils savent pas s'per-ta mais ils s'croient dans Ong-bak 2 Uh, Ong-bak 2 Uh J'ai rêvé qu'j'me faisais courser par onze bacqueux Uh, onze bacqueux Uh Nique la juge, elle joue trop avec ma queue Salope, elle joue trop avec ma queue Salope J'représente le quatre-vingt douze, ma gueule Le quatre-vingt douze, ma gueule</t>
+          <t>Louis, ah, ah Insolent, depuis minot Insolent, depuis minot Poh, poh, poh 9.2, 1.4.0 sur le pocheton 9.2, 1.4.0 sur le pocheton Poh, poh, poh 9.2, 1.4.0 sur le pocheton, si l'argent rend beau, on t'enlève ta beauté Brr T'es un chaud quand tu bois la pisse du diable Brr, brr, qu'est-ce tu fais si on t'enlève ta bouteille ? Cagoulé à chaque fois qu'j'tenais l'sac pour pas glisser sur l'terrain comme Boateng Ah bon ? On s'promène chez eux avec des béquilles, ce soir, tous les ennemis vont boîter Ah bon ? Fin d'G.A.V, on m'dit Fais pas d'bêtise, nique ta grand-mère, j'ressors et j'fais d'la D Poh Pour un cent meuj de beuh, il faut qu'tu cotises Poh, poh, on a toujours la ppe-fra qui t'fait bader Poh Gros, ça vise pas les bes-j', ça vise ton cochi, si on t'hagar, on hagar ton pote aussi Brr Que des liasses dans mon assiette, j'ai bien grossi Brr, brr, le cur noirci, le mal nous amochi Brr C'est une kakala devant toi, elle fait la timide Uh, faut sortir la kichta pour la faire gémir Uh Bâtard, j'vais pas quitter l'trône comme Vladimir, tu vas cracher les tales, j'te l'ai d'jà dit, mec Opinel 13, j'cours même pas devant dix mecs, Byakugan, j'rodave les vingt-deux à dix mètres Skalape en moins d'une heure, me fait changer d'humeur, mmh, faut qu'ça pète comme les tours jumelles Brr J'repense au passé, j'avais zéro pitié, est-ce que j'vais rembourser les curs que j'ai cassés ? La haine, j'ai attisé Tout va bien tant qu'la puce est activée, sur ma mère que j'vais jamais pactiser Négro, bois pas si tu sais pas tiser, la 'teille, j'la bois cul sec Que des têtes cramées sur l'banc des accusés, c'est pas en tenant l'sac que t'auras un Q7 Bâtard, la brigade canine, elle veut péter mon shit, belek, ta frangine veut péter mon chibre Han J'vide la Cristalline et je remplis mon 'she, les porcs, ils veulent péter mon chiffre Zéro démocratie, c'est la voyoucratie Salope Si j'mélange vodka-cassis Salope, c'est toi qui vas payer les pots cassés Poh, poh Charbon, argent sale, j'suis bon qu'à ça Poh Ceux qui descendent ne veulent plus repasser, j'traîne avec des 3arbi, que des gueules cassées Mali, Côte d'Ivoire, Congo, Kinshasa Brr, tous mes Comoriens, j'viens dédicacer Brr On va te gonfler si t'es trop kassa, j'fais gonfler ma liasse, j'v'-esqui la casa J'aime trop l'argent, donc j'esquive le cazin', j'aime pas trop les jeux d'hasard Insolent depuis minot, fuck l'amour Fuck Juliette et Roméo, fuck Zemmour et toutes ses idéaux Le regard est froid, viens t'per-ta si t'es chaud, hendek, ça peut t'quer-cho J'suis pas seul dans la bine-ca, mon cerveau, il chauffe Mmh Comme d'habitude, le guetteur, il chouffe Poh On fait la guerre, protège bien tes abdominaux Poh, poh Rafale, poh, impossible qu'on échoue Poh Ils savent pas s'per-ta mais ils s'croient dans Ong-bak 2 Uh, Ong-bak 2 Uh J'ai rêvé qu'j'me faisais courser par onze bacqueux Uh, onze bacqueux Uh Nique la juge, elle joue trop avec ma queue Salope, elle joue trop avec ma queue Salope J'représente le quatre-vingt douze, ma gueule Le quatre-vingt douze, ma gueule</t>
         </is>
       </c>
     </row>
@@ -650,7 +650,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Binks Beatz J'ai pas perdu mon temps sur des plans Ramène pas d'couteau si t'es pas cap de ter-plan Sale fils de pute, les vrais négros n'ont pas de tarpé à blanc Ça porte malheur alors touche pas à la blanche Tu peux t'faire trahir comme dans Blow Ils m'ont pris une kichta, j'ai le blues Donc j'suis prêt à faire couler le blood T'es une pute, mon pote il m'a dit ça, après le Ça vient d'où ?, tu donnes tes mapessas On s'en fout d'où tu viens, personne nous impressionne, les keufs vont descendre et c'est pas qu'une impression Ça vient d'Chicago, toutes nos ruelles sont bre-som Tu partages pas, mais tu bouges la tête sur le son Après l'agression t'es sous le choc, l'instru, elle est sale donc je la choque Askip, dormir, c'est pour les riches, on rentre chez toi, on casse ta porte pendant qu'tu dors On t'encule ta mère si t'as lé-par de la mif', la rue c'est pas Rap Contenders J'fais plus d'600 sur la 'quette, en vrai, j'ai l'diplôme pour détailler Perquisition, j'ai trop d'émotions, j'souhaite la mort au condé qui met le coup d'bélier Pour un gros billet, j'remue l'couteau dans la plaie, si tu meurs, c'est la fin, la vie c'est pas la Play' Tu m'parles de plavons qu'j'ai déjà faits, si y a pas cinq chiffres c'est pas la peine Si t'as chikem, viens pas m'tchequer, j'suis un vrai lossa, moi j'veux pas quitter l'tier-quar 9-2-1-4-0, la bicrave dans ma tess, devenue une tradition Si j'fais des aller-retours, gros c'est pas pour rien, kichta dans la poche, c'est pas les sous du terrain Ma liasse monte d'un étage, j'détaille dans l'sous-terrain, en vrai la vie est cruelle sans les sous, t'es rien Tire sur la frappe, tu t'envoles, jamais t'atteris, tu veux voler une bonbonne, gros c'est à tes risques On a niqué ton pote, viens l'récupérer, j'entends beaucoup d'acteurs qui se mettent à pe-ra On est venus les mains vides et t'es apeuré, on veut juste te masser, igo t'as chaud pour rien J'suis sur l'terrain depuis 13 heures pow, pow, et t'oses me dire que y a déjà plus rien Bécane achetée avec argent sale, donc c'est normal si j'bé-tom avec J'veux pas quitter la tess, j'me fait qué-'bar dans la cave, j'ai gants en latex J'ai entendu les tits-pe réciter mes textes, mais j'veux pas les influencer Tous les jours encaisser, j'fais en sorte T'es mon reuf si on plavonne ensemble, t'es une miss mais on sort pas ensemble À 15 ans, j'avais la main dans le sac, à 16 ans, comme Gaara, souvent la main dans le sable, le vol ou la drogue ? J't'avoue j'suis trop indécis ah bon ? Y a plus d'bédo mais y a des plavons, si y a plus de plavons, on vient voler ton bédo Et toi tu penses pouvoir nous la mettre, igo tu vas tomber de haut Cagoulé, ganté pendant l'action, alors y aura pas d'portrait robot La miss c'est une marocaine, pourtant elle m'dit qu'elle est pas trop rebeux Il a les yeux rouges, faut le rabattre, j'crois qu'je me fais filoche par la BAC, tu peux t'faire remplir par la bague J'suis en train d'bicrave, j't'appelle après, askip, t'es pas rodave mais ils t'ont pris en flag' Fermeture à 2 heures, j'pète la forme, passe à Nilla si tu veux un truc Mais viens pas demander des infos T'es pas un vrai, tu t'habilles en faux, des billets, billets tous les jours il en faut Elle veux ma bite, c'est une nympho, elle veux ma bite, c'est une nympho La mala sur le tecs', c'est l'heure du sale boulot, à midi, un clicos, j'ai fait le sale boulot J'fais que d'la tamponner, elle a un sale boulard Elle m'larsa, elle me regarde dans les yeux J'visser un ien-cli et j'le regarde dans les yeux, on t'arrache ton sac et on reste pas dans les lieux La BAC ils ner-tour, mais ils risquent pas d'aller loin, et parfois, des questions j'me pose Si j'rabats le ien-cli à l'entrée, j'peux vider la bonbonne dans ta fête J'veux des sous mais j'veux pas taffer, j'traîne avec des vrais négros Nan, j'tolère pas les tafioles, souvent envie d'braquer l'État Regarde tu finis dans quel état, j'avoue, la drogue c'est rentable, mais faut pas sauter les étapes J'graille des rappeurs à l'apéro, j'rentre dans le pe-ra, j'fais des dommages collatéraux, j'vais jamais trahir mes khos You might also like J'encaisse un billet à chaque fois que le ient-cli serre ma main Et à chaque fois j'compte le bénéf, j'me rappelle que j'suis proche de la mort Étant petit, j'ai perdu mon temps, la miss, elle s'accroche, j'crois qu'elle a kiffé mon 'tard Rien n'a changé, mes négros enfilent le Gator Et pour allumer les keufs, bâtard, on n'attend pas le 14 J'veux les voir brûler dans leur uniforme J'dédicace les lossas qui m'donnent la force, j'dédicace les lossas qui m'donnent la force J'encaisse un billet à chaque fois que le ient-cli serre ma main Et à chaque fois j'compte le bénéf, j'me rappelle que j'suis proche de la mort Étant petit, j'ai perdu mon temps, la miss, elle s'accroche, j'crois qu'elle a kiffé mon 'tard Rien n'a changé, mes négros enfilent le Gator Et pour allumer les keufs, bâtard, on n'attend pas le 14 J'veux les voir brûler dans leur uniforme J'dédicace les lossas qui m'donnent la force, j'dédicace les lossas qui m'donnent la force 9-2-1-4-0 sur le pocheton, la bicrave dans ma tess, devenue une tradition J'vais pas t'pousser un pain, toi, t'es pas un mec d'ici Le bacqueux, il a la calvitie Avant l'plavon, je vide ma vessie, tu peux pas rentrer, tu fais l'tour de la té-ci Le bacqueux, il a la calvitie Avant l'plavon, je vide ma vessie, tu peux pas rentrer, tu fais l'tour de la té-ci Avant l'plavon, je vide ma vessie, tu peux pas rentrer, tu fais l'tour de la té-ci</t>
+          <t>Binks Beatz J'ai pas perdu mon temps sur des plans Ramène pas d'couteau si t'es pas cap de ter-plan Sale fils de pute, les vrais négros n'ont pas de tarpé à blanc Ça porte malheur alors touche pas à la blanche Tu peux t'faire trahir comme dans Blow Ils m'ont pris une kichta, j'ai le blues Donc j'suis prêt à faire couler le blood T'es une pute, mon pote il m'a dit ça, après le Ça vient d'où ?, tu donnes tes mapessas On s'en fout d'où tu viens, personne nous impressionne, les keufs vont descendre et c'est pas qu'une impression Ça vient d'Chicago, toutes nos ruelles sont bre-som Tu partages pas, mais tu bouges la tête sur le son Après l'agression t'es sous le choc, l'instru, elle est sale donc je la choque Askip, dormir, c'est pour les riches, on rentre chez toi, on casse ta porte pendant qu'tu dors On t'encule ta mère si t'as lé-par de la mif', la rue c'est pas Rap Contenders J'fais plus d'600 sur la 'quette, en vrai, j'ai l'diplôme pour détailler Perquisition, j'ai trop d'émotions, j'souhaite la mort au condé qui met le coup d'bélier Pour un gros billet, j'remue l'couteau dans la plaie, si tu meurs, c'est la fin, la vie c'est pas la Play' Tu m'parles de plavons qu'j'ai déjà faits, si y a pas cinq chiffres c'est pas la peine Si t'as chikem, viens pas m'tchequer, j'suis un vrai lossa, moi j'veux pas quitter l'tier-quar 9-2-1-4-0, la bicrave dans ma tess, devenue une tradition Si j'fais des aller-retours, gros c'est pas pour rien, kichta dans la poche, c'est pas les sous du terrain Ma liasse monte d'un étage, j'détaille dans l'sous-terrain, en vrai la vie est cruelle sans les sous, t'es rien Tire sur la frappe, tu t'envoles, jamais t'atteris, tu veux voler une bonbonne, gros c'est à tes risques On a niqué ton pote, viens l'récupérer, j'entends beaucoup d'acteurs qui se mettent à pe-ra On est venus les mains vides et t'es apeuré, on veut juste te masser, igo t'as chaud pour rien J'suis sur l'terrain depuis 13 heures pow, pow, et t'oses me dire que y a déjà plus rien Bécane achetée avec argent sale, donc c'est normal si j'bé-tom avec J'veux pas quitter la tess, j'me fait qué-'bar dans la cave, j'ai gants en latex J'ai entendu les tits-pe réciter mes textes, mais j'veux pas les influencer Tous les jours encaisser, j'fais en sorte T'es mon reuf si on plavonne ensemble, t'es une miss mais on sort pas ensemble À 15 ans, j'avais la main dans le sac, à 16 ans, comme Gaara, souvent la main dans le sable, le vol ou la drogue ? J't'avoue j'suis trop indécis ah bon ? Y a plus d'bédo mais y a des plavons, si y a plus de plavons, on vient voler ton bédo Et toi tu penses pouvoir nous la mettre, igo tu vas tomber de haut Cagoulé, ganté pendant l'action, alors y aura pas d'portrait robot La miss c'est une marocaine, pourtant elle m'dit qu'elle est pas trop rebeux Il a les yeux rouges, faut le rabattre, j'crois qu'je me fais filoche par la BAC, tu peux t'faire remplir par la bague J'suis en train d'bicrave, j't'appelle après, askip, t'es pas rodave mais ils t'ont pris en flag' Fermeture à 2 heures, j'pète la forme, passe à Nilla si tu veux un truc Mais viens pas demander des infos T'es pas un vrai, tu t'habilles en faux, des billets, billets tous les jours il en faut Elle veux ma bite, c'est une nympho, elle veux ma bite, c'est une nympho La mala sur le tecs', c'est l'heure du sale boulot, à midi, un clicos, j'ai fait le sale boulot J'fais que d'la tamponner, elle a un sale boulard Elle m'larsa, elle me regarde dans les yeux J'visser un ien-cli et j'le regarde dans les yeux, on t'arrache ton sac et on reste pas dans les lieux La BAC ils ner-tour, mais ils risquent pas d'aller loin, et parfois, des questions j'me pose Si j'rabats le ien-cli à l'entrée, j'peux vider la bonbonne dans ta fête J'veux des sous mais j'veux pas taffer, j'traîne avec des vrais négros Nan, j'tolère pas les tafioles, souvent envie d'braquer l'État Regarde tu finis dans quel état, j'avoue, la drogue c'est rentable, mais faut pas sauter les étapes J'graille des rappeurs à l'apéro, j'rentre dans le pe-ra, j'fais des dommages collatéraux, j'vais jamais trahir mes khos J'encaisse un billet à chaque fois que le ient-cli serre ma main Et à chaque fois j'compte le bénéf, j'me rappelle que j'suis proche de la mort Étant petit, j'ai perdu mon temps, la miss, elle s'accroche, j'crois qu'elle a kiffé mon 'tard Rien n'a changé, mes négros enfilent le Gator Et pour allumer les keufs, bâtard, on n'attend pas le 14 J'veux les voir brûler dans leur uniforme J'dédicace les lossas qui m'donnent la force, j'dédicace les lossas qui m'donnent la force J'encaisse un billet à chaque fois que le ient-cli serre ma main Et à chaque fois j'compte le bénéf, j'me rappelle que j'suis proche de la mort Étant petit, j'ai perdu mon temps, la miss, elle s'accroche, j'crois qu'elle a kiffé mon 'tard Rien n'a changé, mes négros enfilent le Gator Et pour allumer les keufs, bâtard, on n'attend pas le 14 J'veux les voir brûler dans leur uniforme J'dédicace les lossas qui m'donnent la force, j'dédicace les lossas qui m'donnent la force 9-2-1-4-0 sur le pocheton, la bicrave dans ma tess, devenue une tradition J'vais pas t'pousser un pain, toi, t'es pas un mec d'ici Le bacqueux, il a la calvitie Avant l'plavon, je vide ma vessie, tu peux pas rentrer, tu fais l'tour de la té-ci Le bacqueux, il a la calvitie Avant l'plavon, je vide ma vessie, tu peux pas rentrer, tu fais l'tour de la té-ci Avant l'plavon, je vide ma vessie, tu peux pas rentrer, tu fais l'tour de la té-ci</t>
         </is>
       </c>
     </row>
@@ -667,7 +667,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Mais nan ? Poh Le métal en béton, j'suis tout seul à ma table poh, j'serai seul dans ma tombe poh Ici, personne n'est imbattable, ça s'pull up, ça s'bagarre plus avec des bâtons brr On fait les choses, on vient pas débattre brr, si on t'attrape, est-ce que tu peux t'débattre ? brr Ça sort les mes-ar en pagaille, mes gavas sont réels, ne sont pas dans l'théâtre ah bon ? Elle fait la miss, elle est trop atroce, bowling, elle prend par les trois trous ah bon ? Attends, pause, tu mérites pas l'carrosse, sorry, j'la ramène dans l'bât', j'la tamponne salope J'la fais crier comme Kakarot, j'entends leurs sons, on dirait 1PLIKÉ140 salope Quand j'les écoute, j'entends 1PLIKÉ140 paw, comment s'en sortir sans leur mettre de carotte ? paw C'est pour son cavu qu'j'la cala, j'rêve de kichta, kalash, si t'as mal t'as qu'à lâcher han Ça commence souvent par des han, mais ça t'encule ta mère han J'en place une pour tous mes skaters qui fument du shit hmm, si j'm'éloigne de toutes ces bitches hmm C'est pour finir en Mitsubishi donc j'enfile le gator comme Kakashi Si on baraude dans ton tieks, mon négro, qué pasa ? eh Au début, c'était ma meuf, c'est devenu ma pétasse eh J'reçois pas des je t'aime, j'reçois des est-ce que t'as ça ? poh Tu veux faire la guerre avec nous, est-ce que t'assumes ? poh-poh Si on baraude dans ton tieks, mon négro, qué pasa ? eh Au début, c'était ma meuf, c'est devenu ma pétasse eh J'reçois pas des je t'aime, j'reçois des est-ce que t'as ça ? poh Tu veux faire la guerre avec nous, est-ce que t'assumes ? poh-poh You might also like Bébé, bouge ton booty, c'est à midi qu'on ouvre la boutique brr Ils veulent s'habiller en Gucci mais dans la vie, ils ont rien abouti brr Rien abouti, ta meuf vient me voir pour un bout d'shit pa-paw Pour un bout d'shit, quand tu la galoches, y a un goût d'chibre pa-paw Bébé, bouge ton booty, c'est à midi qu'on ouvre la boutique brr Ils veulent s'habiller en Gucci mais dans la vie, ils ont rien abouti brr Rien abouti, ta meuf vient me voir pour un bout d'shit pa-paw Pour un bout d'shit, quand tu la galoches, y a un goût d'chibre pa-paw Pas pour rien qu'on sort les outils, Opinel sorti, pour me rendre utile On peut s'faire la guerre comme dans Call Of Duty, ça pull up pour de vrai, c'est pas pour le style han Insolent, j'me sens bien en milieu hostile, ils veulent le conflit, mais comment osent-ils ? hmm On descend, on baise tout, après ça, on s'tire, on descend, on baise tout, après ça, on s'tire Askip, les vrais yous-voy sont en costume ou bien lacostés ah bon ? À deux doigts d'baiser les coutumes quand on s'attaque au bosseur qu'est posté ah bon ? Y avait heja, tu t'es téléporté, même si j'm'en bats les couilles, j'oublie pas d'les porter brr Mauvais payeur finira toujours par payer, le passé est passé mais peut te rattraper brr, brr Si on baraude dans ton tieks, mon négro, qué pasa ? eh Au début, c'était ma meuf, c'est devenu ma pétasse eh J'reçois pas des je t'aime, j'reçois des est-ce que t'as ça ? poh Tu veux faire la guerre avec nous, est-ce que t'assumes ? poh-poh Si on baraude dans ton tieks, mon négro, qué pasa ? eh Au début, c'était ma meuf, c'est devenu ma pétasse eh J'reçois pas des je t'aime, j'reçois des est-ce que t'as ça ? poh Tu veux faire la guerre avec nous, est-ce que t'assumes ? poh-poh On baraude dans ton tieks, qué pasa, cache les mes-ar, y a le Focus qui passe C'était ma meuf, c'est devenu ma pétasse, c'était ma meuf, c'est devenu ma pétasse J'reçois zéro je t'aime sur mon tél', j'reçois que des est-ce que t'as ca ?Renoi, tu veux faire la guerre mais en vrai, est-ce que t'assumes ? Renoi, tu veux faire la guerre mais en vrai, est-ce que t'assumes ?</t>
+          <t>Mais nan ? Poh Le métal en béton, j'suis tout seul à ma table poh, j'serai seul dans ma tombe poh Ici, personne n'est imbattable, ça s'pull up, ça s'bagarre plus avec des bâtons brr On fait les choses, on vient pas débattre brr, si on t'attrape, est-ce que tu peux t'débattre ? brr Ça sort les mes-ar en pagaille, mes gavas sont réels, ne sont pas dans l'théâtre ah bon ? Elle fait la miss, elle est trop atroce, bowling, elle prend par les trois trous ah bon ? Attends, pause, tu mérites pas l'carrosse, sorry, j'la ramène dans l'bât', j'la tamponne salope J'la fais crier comme Kakarot, j'entends leurs sons, on dirait 1PLIKÉ140 salope Quand j'les écoute, j'entends 1PLIKÉ140 paw, comment s'en sortir sans leur mettre de carotte ? paw C'est pour son cavu qu'j'la cala, j'rêve de kichta, kalash, si t'as mal t'as qu'à lâcher han Ça commence souvent par des han, mais ça t'encule ta mère han J'en place une pour tous mes skaters qui fument du shit hmm, si j'm'éloigne de toutes ces bitches hmm C'est pour finir en Mitsubishi donc j'enfile le gator comme Kakashi Si on baraude dans ton tieks, mon négro, qué pasa ? eh Au début, c'était ma meuf, c'est devenu ma pétasse eh J'reçois pas des je t'aime, j'reçois des est-ce que t'as ça ? poh Tu veux faire la guerre avec nous, est-ce que t'assumes ? poh-poh Si on baraude dans ton tieks, mon négro, qué pasa ? eh Au début, c'était ma meuf, c'est devenu ma pétasse eh J'reçois pas des je t'aime, j'reçois des est-ce que t'as ça ? poh Tu veux faire la guerre avec nous, est-ce que t'assumes ? poh-poh Bébé, bouge ton booty, c'est à midi qu'on ouvre la boutique brr Ils veulent s'habiller en Gucci mais dans la vie, ils ont rien abouti brr Rien abouti, ta meuf vient me voir pour un bout d'shit pa-paw Pour un bout d'shit, quand tu la galoches, y a un goût d'chibre pa-paw Bébé, bouge ton booty, c'est à midi qu'on ouvre la boutique brr Ils veulent s'habiller en Gucci mais dans la vie, ils ont rien abouti brr Rien abouti, ta meuf vient me voir pour un bout d'shit pa-paw Pour un bout d'shit, quand tu la galoches, y a un goût d'chibre pa-paw Pas pour rien qu'on sort les outils, Opinel sorti, pour me rendre utile On peut s'faire la guerre comme dans Call Of Duty, ça pull up pour de vrai, c'est pas pour le style han Insolent, j'me sens bien en milieu hostile, ils veulent le conflit, mais comment osent-ils ? hmm On descend, on baise tout, après ça, on s'tire, on descend, on baise tout, après ça, on s'tire Askip, les vrais yous-voy sont en costume ou bien lacostés ah bon ? À deux doigts d'baiser les coutumes quand on s'attaque au bosseur qu'est posté ah bon ? Y avait heja, tu t'es téléporté, même si j'm'en bats les couilles, j'oublie pas d'les porter brr Mauvais payeur finira toujours par payer, le passé est passé mais peut te rattraper brr, brr Si on baraude dans ton tieks, mon négro, qué pasa ? eh Au début, c'était ma meuf, c'est devenu ma pétasse eh J'reçois pas des je t'aime, j'reçois des est-ce que t'as ça ? poh Tu veux faire la guerre avec nous, est-ce que t'assumes ? poh-poh Si on baraude dans ton tieks, mon négro, qué pasa ? eh Au début, c'était ma meuf, c'est devenu ma pétasse eh J'reçois pas des je t'aime, j'reçois des est-ce que t'as ça ? poh Tu veux faire la guerre avec nous, est-ce que t'assumes ? poh-poh On baraude dans ton tieks, qué pasa, cache les mes-ar, y a le Focus qui passe C'était ma meuf, c'est devenu ma pétasse, c'était ma meuf, c'est devenu ma pétasse J'reçois zéro je t'aime sur mon tél', j'reçois que des est-ce que t'as ca ?Renoi, tu veux faire la guerre mais en vrai, est-ce que t'assumes ? Renoi, tu veux faire la guerre mais en vrai, est-ce que t'assumes ?</t>
         </is>
       </c>
     </row>
@@ -684,7 +684,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Frosty J'ai serré deux-trois mains et j'ai déjà skalape paw, il veut m'checker, j'sais même pas c'est qui c'gars-là paw Elle a sucé des bites donc j'vais pas la galoche paw et quand ça court, j'aime bien voir les condés s'galope paw, paw Aucun sentiment quand on t'dépouille brr, tu portes la bonbonne mais tu portes même pas tes couilles brr J'entends la portière, j'suis prêt à m'évaporer, j'fais des aller-retours, j't'assure, c'est pas pour rien Et si tu dois des sous, on tournera pas la page han, jfais mes bails discrets histoire déviter la cage han On t'encule ta mère sur le parking, tu t'es fait poucave et tu sais même pas par qui paw T'es au dépôt, la suite, tu la connais par cur, t'es un ient-cli, pourquoi tu parle de los-ki ? Askip, tu tires mais bon, tu fais zéro kill, menotté devant les bleus, jpeux pas rester tranquille Hasba sur hasba, on n'est pas gentils wouh, couteau dans l'dos même s'il est argenté wouh Le temps, c'est d'l'argent, ne me fais pas patienter paw Le te-shi me nique la santé paw mais me donne des idées en tête wouh Ils ont mis les gants pour faire blerni, j'viens d'guer-lar la bac, j'canalise mon énergie J'viens d'guer-lar la bac, j'canalise mon énergie Tu vas rien faire, igo, même si on t'a carna brr, y a un ient-cli, j'vais jusqu'à la tour Montparnasse brr Jlève un doigt pour la mumu, la bac et la nat' paw J'pète une kichta sans me vanter, eux, cqui disent dans leurs textes, ils lont grave inventé han Là, j'suis venu kicker l'instru' han, non, j'suis pas v'nu pour chanter paw Même en été, tu peux nous voir gantés brr et si t'es pas prêt, ne viens pas nous fréquenter brr Et c'est pas en détaillant des 'quettes wouh que tu finiras en jet wouh Y a la Focus, les cailloux, on les jette paw parce que sur le terrain, ils nous gênent paw Le bosseur fait des trous, normal qu'on le remplace paw, ils sont v'nus massif, obligé d'sortir un schlass han Et tous les soirs, c'est toi qu'elle appelle ah bon ? mais pourtant, c'est moi qui la pine ah bon ? Nan, j'cache pas mes trucs chez la voisine salope et je touche pas à la cocaïne paw À c'qui paraît ça porte la poisse paw Tu fais le fou sur le réseau, bizarrement, igo, t'es gentil en face salope Tu veux pas per-cho, à quoi tu sers paw ? Pour un billet violet, normal, ton cou, j'le serre brr La roue, elle tourne et je le sais, donc faire tourner l'business, j'essaye wouh J'en ai marre d'avoir les mains sales mais j'aime l'argent facile paw Y a qu'les billets qui me fascinent, j'vais brasser à mort pour finir dans une piscine poh, poh Tu tombes quand tu cours, tout l'monde peut te piétine couteau dans la jambe, c'est normal que tu titubes wouh Et ouais, mon gars, c'est ça la vie brr, c'est en vendant la mort qu'on revit brr J'aime pas quand mon ex, elle revient, j'suis un vrai laud-sa, j'aime quand le ient-cli revient paw T'es pas sûr de t'réveiller demain wouh, fais belek quand t'es sur le chemin wouh Fuck la BAC qui déboule à tout moment pow, pour quatre chiffres, on débarque chez ta maman pow Et j'peux t'assurer qu'c'est pas marrant, le shit, il est vert, mon gars, il est pas marron brr Et ils font les gros en vrai ils ont pas un rond, 9.2.1.4.0 sur le pochton On arrache ton c-sa sur le passage piéton, ne les écoute pas, ils racontent du baratin wouh Ils ont jamais vu d'semi-auto, j'ai la haine quand les condés, ils fouillent les locaux J'ai la haine quand sur l'bigo, y a des échos bâtard, j'crois bien qu'ils m'ont mis sur écoute paw Fais belek si t'as une chaîne au cou, on t'laisse au sol, on t'finit avec les coudes, on t'laisse au sol paw You might also like J'me sens obligé de nier même si le vil-ci a bien reconnu ma tête brr Négros armés dans ton quartier, t'as bien reconnu ma tess paw J'm'en bats les couilles des élections wouh, dans mon tiekson, c'est le ient-cli qui vient voter han J'me fait couper par la bac, j'suis dégouté han, j'crois qu'les billets m'ont envoûté paw J'me sens obligé de nier même si le vil-ci a bien reconnu ma tête brr Négros armés dans ton quartier brr, t'as bien reconnu ma tess paw J'm'en bats les couilles des élections, dans mon tiekson, c'est le ient-cli qui vient voter han J'me fait couper par la bac, j'suis dégouté, j'crois qu'les billets m'ont envoûté</t>
+          <t>Frosty J'ai serré deux-trois mains et j'ai déjà skalape paw, il veut m'checker, j'sais même pas c'est qui c'gars-là paw Elle a sucé des bites donc j'vais pas la galoche paw et quand ça court, j'aime bien voir les condés s'galope paw, paw Aucun sentiment quand on t'dépouille brr, tu portes la bonbonne mais tu portes même pas tes couilles brr J'entends la portière, j'suis prêt à m'évaporer, j'fais des aller-retours, j't'assure, c'est pas pour rien Et si tu dois des sous, on tournera pas la page han, jfais mes bails discrets histoire déviter la cage han On t'encule ta mère sur le parking, tu t'es fait poucave et tu sais même pas par qui paw T'es au dépôt, la suite, tu la connais par cur, t'es un ient-cli, pourquoi tu parle de los-ki ? Askip, tu tires mais bon, tu fais zéro kill, menotté devant les bleus, jpeux pas rester tranquille Hasba sur hasba, on n'est pas gentils wouh, couteau dans l'dos même s'il est argenté wouh Le temps, c'est d'l'argent, ne me fais pas patienter paw Le te-shi me nique la santé paw mais me donne des idées en tête wouh Ils ont mis les gants pour faire blerni, j'viens d'guer-lar la bac, j'canalise mon énergie J'viens d'guer-lar la bac, j'canalise mon énergie Tu vas rien faire, igo, même si on t'a carna brr, y a un ient-cli, j'vais jusqu'à la tour Montparnasse brr Jlève un doigt pour la mumu, la bac et la nat' paw J'pète une kichta sans me vanter, eux, cqui disent dans leurs textes, ils lont grave inventé han Là, j'suis venu kicker l'instru' han, non, j'suis pas v'nu pour chanter paw Même en été, tu peux nous voir gantés brr et si t'es pas prêt, ne viens pas nous fréquenter brr Et c'est pas en détaillant des 'quettes wouh que tu finiras en jet wouh Y a la Focus, les cailloux, on les jette paw parce que sur le terrain, ils nous gênent paw Le bosseur fait des trous, normal qu'on le remplace paw, ils sont v'nus massif, obligé d'sortir un schlass han Et tous les soirs, c'est toi qu'elle appelle ah bon ? mais pourtant, c'est moi qui la pine ah bon ? Nan, j'cache pas mes trucs chez la voisine salope et je touche pas à la cocaïne paw À c'qui paraît ça porte la poisse paw Tu fais le fou sur le réseau, bizarrement, igo, t'es gentil en face salope Tu veux pas per-cho, à quoi tu sers paw ? Pour un billet violet, normal, ton cou, j'le serre brr La roue, elle tourne et je le sais, donc faire tourner l'business, j'essaye wouh J'en ai marre d'avoir les mains sales mais j'aime l'argent facile paw Y a qu'les billets qui me fascinent, j'vais brasser à mort pour finir dans une piscine poh, poh Tu tombes quand tu cours, tout l'monde peut te piétine couteau dans la jambe, c'est normal que tu titubes wouh Et ouais, mon gars, c'est ça la vie brr, c'est en vendant la mort qu'on revit brr J'aime pas quand mon ex, elle revient, j'suis un vrai laud-sa, j'aime quand le ient-cli revient paw T'es pas sûr de t'réveiller demain wouh, fais belek quand t'es sur le chemin wouh Fuck la BAC qui déboule à tout moment pow, pour quatre chiffres, on débarque chez ta maman pow Et j'peux t'assurer qu'c'est pas marrant, le shit, il est vert, mon gars, il est pas marron brr Et ils font les gros en vrai ils ont pas un rond, 9.2.1.4.0 sur le pochton On arrache ton c-sa sur le passage piéton, ne les écoute pas, ils racontent du baratin wouh Ils ont jamais vu d'semi-auto, j'ai la haine quand les condés, ils fouillent les locaux J'ai la haine quand sur l'bigo, y a des échos bâtard, j'crois bien qu'ils m'ont mis sur écoute paw Fais belek si t'as une chaîne au cou, on t'laisse au sol, on t'finit avec les coudes, on t'laisse au sol paw J'me sens obligé de nier même si le vil-ci a bien reconnu ma tête brr Négros armés dans ton quartier, t'as bien reconnu ma tess paw J'm'en bats les couilles des élections wouh, dans mon tiekson, c'est le ient-cli qui vient voter han J'me fait couper par la bac, j'suis dégouté han, j'crois qu'les billets m'ont envoûté paw J'me sens obligé de nier même si le vil-ci a bien reconnu ma tête brr Négros armés dans ton quartier brr, t'as bien reconnu ma tess paw J'm'en bats les couilles des élections, dans mon tiekson, c'est le ient-cli qui vient voter han J'me fait couper par la bac, j'suis dégouté, j'crois qu'les billets m'ont envoûté</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>J'peux pas arrêter d'plavonner, j'peux pas arrêter d'plavonner Binks Beatz J'peux pas arrêter d'plavonner, j'ai envie d'arrêter mais j'aime trop la monnaie J'peux pas arrêter d'plavonner, j'ai envie d'arrêter mais j'aime trop la monnaie J'retombe dedans à chaque fois qu'c'est la pénurie, j'retombe dedans à chaque fois qu'c'est la pénurie Mais pourquoi elle fait la ge-vier ? Moi, j'connais des mecs qui l'ont ken Et on n'a pas taffé les bras mais on peut soulever tes los-ki Ça vend la muerte pour voir la vida loca, comme un grand garçon, j'détaillais dans le local Ces négros, ils ont la boca, ils font genre qu'ils sont chauds mais en vrai, ils sont calmes J'ai pas l'temps d'capter des go', j'ai souvent des trucs dans le çon-cal' La miss, elle est conne, elle croit que j'veux son cur mais j'suis en train d'ter-ma son kah Bâtard, j'suis encore dans la ve-ca, ient-cli en manque donc j'lui demande il veut quoi On peut t'courir après si tu dois des tales, askip vous êtes chauds, vous êtes bons qu'à détale J'vi-sser un ient-cli, j'monte sur la capitale, t'arrives pas à la tenir, on coupera ta langue Y a du te-shi, d'la beuh, regarde le catalogue, 2 grammes 5, j'ai fait l'bon, j't'ai rajouté Les keufs, ils descendent, toute façon, j'm'en doutais et quand y a descente, on se demande où t'es J'ai vu les tes-schmi débouler des deux côtés, j'ai vu ma liasse qui grossit, alors j'suis content Y a des mecs qui ont la boule au ventre, d'autres qui ont perdu la boule J'aime faire des billets, j'aime quand ça rentre, si on t'arrache ton scoot', pas besoin d'faire la boule Et même si t'es un mec vif, tu pourras pas esquiver la balle Même si la sortie, c'est sûr, j'espère que j'irai pas là-bas Y en a qui cambu, ils s'en foutent que tu sois là, y en a qui reculent et ont peur d'aller che-arra J'arrache un collier et j'le donne pas à madame, si j'vais en soirée, c'est pour faire partir la came Les keufs nous traquent comme dans GTA, c'est dommage qu'on voit pas les tes-schmi sur la carte Tu bicraves pour t'acheter des sapes, c'est toi qui va finir au placard Sur un plavon, j'ai perdu mon cur mais la miss, elle a perdu sa carte À chaque fois, j'compte le bénéf', j'me rappelle que la vie est courte Parle pas harak sur mon téléphone, ils n'ont jamais détaille mais parlent de cellophane Fuck les poucaves, fuck l'OPJ qui questionne, tout c'qu'on dit c'est réel, tout c'qu'on dit c'est réel Et la vie est cruelle, quand ton corps finit dans une ruelle T'inquiète, on sait kicker l'instru, passe à Nilla si tu veux un truc Parfois y a les vils-ci dans le four, alors essaye de trouver l'intrus Si tu m'as vu dans l'métro, c'est que j'faisais gonfler ma puce You might also like Tu t'es fait mêler, c'est ça la vie, tu t'es fait mêler, c'est ça la vie La moitié des meufs sont des putes mais j'vais pas finir seul à vie Une seule bastos, ça va vite, j'fais que détailler donc mes mains sont sales à vie Et cette pute veut rentrer dans ma vie, elle a bégayé dès qu'elle m'a vu Tu t'es fait mêler, c'est ça la vie, tu t'es fait mêler, c'est ça la vie La moitié des meufs sont des putes mais j'vais pas finir seul à vie Une seule bastos, ça va vite, j'fais que détailler donc mes mains sont sales à vie Et cette pute veut rentrer dans ma vie, elle a bégayé dès qu'elle m'a vu Cagoulé, ganté, pour un plavon, j'monte, sur un plavon, j'raconte l'implication Capuché dans un hall avec mauvais garçons, mon rêve c'est faire des sous Brolique est dans l'caleçon, eh Eh, la vie, c'est avant la mort, la vue, c'est avant l'amour Depuis qu'j'ai vu les sous, j'calcule plus mi amor et si tu m'dois des sous, v'-esqui la mise à mort J'déboule dans ton tieks avec dix négros, eh Tu vas cracher mes dinero, j'suis dans l'bâtiment, j'fais des midi-minuit Faut qu'ma liasse elle grossit, faut pas qu'elle diminue Tu vas cracher du sang si t'as craché des noms, Opinel 12, c'est chacun ses démons On casse ta jambe si tu casses la démarche et pendant la descente y a l'adré' qui te-mon Tu t'es fait mêler, c'est ça la vie, tu t'es fait mêler, c'est ça la vie La moitié des meufs sont des putes mais j'vais pas finir seul à vie Une seule bastos, ça va vite, j'fais que détailler donc mes mains sont sales à vie Et cette pute veut rentrer dans ma vie, elle a bégayé dès qu'elle m'a vu Tu t'es fait mêler, c'est ça la vie, tu t'es fait mêler, c'est ça la vie La moitié des meufs sont des putes mais j'vais pas finir seul à vie Une seule bastos, ça va vite, j'fais que détailler donc mes mains sont sales à vie Et cette pute veut rentrer dans ma vie, elle a bégayé dès qu'elle m'a vu J'peux pas arrêter d'plavonner, j'peux pas arrêter d'plavonner J'peux pas arrêter d'plavonner, j'ai envie d'arrêter mais j'aime trop la monnaie J'peux pas arrêter d'plavonner, j'peux pas arrêter d'plavonner J'peux pas arrêter d'plavonner, j'ai envie d'arrêter mais j'aime trop la monnaie J'peux pas arrêter d'plavonner, j'ai envie d'arrêter mais j'aime trop la monnaie</t>
+          <t>J'peux pas arrêter d'plavonner, j'peux pas arrêter d'plavonner Binks Beatz J'peux pas arrêter d'plavonner, j'ai envie d'arrêter mais j'aime trop la monnaie J'peux pas arrêter d'plavonner, j'ai envie d'arrêter mais j'aime trop la monnaie J'retombe dedans à chaque fois qu'c'est la pénurie, j'retombe dedans à chaque fois qu'c'est la pénurie Mais pourquoi elle fait la ge-vier ? Moi, j'connais des mecs qui l'ont ken Et on n'a pas taffé les bras mais on peut soulever tes los-ki Ça vend la muerte pour voir la vida loca, comme un grand garçon, j'détaillais dans le local Ces négros, ils ont la boca, ils font genre qu'ils sont chauds mais en vrai, ils sont calmes J'ai pas l'temps d'capter des go', j'ai souvent des trucs dans le çon-cal' La miss, elle est conne, elle croit que j'veux son cur mais j'suis en train d'ter-ma son kah Bâtard, j'suis encore dans la ve-ca, ient-cli en manque donc j'lui demande il veut quoi On peut t'courir après si tu dois des tales, askip vous êtes chauds, vous êtes bons qu'à détale J'vi-sser un ient-cli, j'monte sur la capitale, t'arrives pas à la tenir, on coupera ta langue Y a du te-shi, d'la beuh, regarde le catalogue, 2 grammes 5, j'ai fait l'bon, j't'ai rajouté Les keufs, ils descendent, toute façon, j'm'en doutais et quand y a descente, on se demande où t'es J'ai vu les tes-schmi débouler des deux côtés, j'ai vu ma liasse qui grossit, alors j'suis content Y a des mecs qui ont la boule au ventre, d'autres qui ont perdu la boule J'aime faire des billets, j'aime quand ça rentre, si on t'arrache ton scoot', pas besoin d'faire la boule Et même si t'es un mec vif, tu pourras pas esquiver la balle Même si la sortie, c'est sûr, j'espère que j'irai pas là-bas Y en a qui cambu, ils s'en foutent que tu sois là, y en a qui reculent et ont peur d'aller che-arra J'arrache un collier et j'le donne pas à madame, si j'vais en soirée, c'est pour faire partir la came Les keufs nous traquent comme dans GTA, c'est dommage qu'on voit pas les tes-schmi sur la carte Tu bicraves pour t'acheter des sapes, c'est toi qui va finir au placard Sur un plavon, j'ai perdu mon cur mais la miss, elle a perdu sa carte À chaque fois, j'compte le bénéf', j'me rappelle que la vie est courte Parle pas harak sur mon téléphone, ils n'ont jamais détaille mais parlent de cellophane Fuck les poucaves, fuck l'OPJ qui questionne, tout c'qu'on dit c'est réel, tout c'qu'on dit c'est réel Et la vie est cruelle, quand ton corps finit dans une ruelle T'inquiète, on sait kicker l'instru, passe à Nilla si tu veux un truc Parfois y a les vils-ci dans le four, alors essaye de trouver l'intrus Si tu m'as vu dans l'métro, c'est que j'faisais gonfler ma puce Tu t'es fait mêler, c'est ça la vie, tu t'es fait mêler, c'est ça la vie La moitié des meufs sont des putes mais j'vais pas finir seul à vie Une seule bastos, ça va vite, j'fais que détailler donc mes mains sont sales à vie Et cette pute veut rentrer dans ma vie, elle a bégayé dès qu'elle m'a vu Tu t'es fait mêler, c'est ça la vie, tu t'es fait mêler, c'est ça la vie La moitié des meufs sont des putes mais j'vais pas finir seul à vie Une seule bastos, ça va vite, j'fais que détailler donc mes mains sont sales à vie Et cette pute veut rentrer dans ma vie, elle a bégayé dès qu'elle m'a vu Cagoulé, ganté, pour un plavon, j'monte, sur un plavon, j'raconte l'implication Capuché dans un hall avec mauvais garçons, mon rêve c'est faire des sous Brolique est dans l'caleçon, eh Eh, la vie, c'est avant la mort, la vue, c'est avant l'amour Depuis qu'j'ai vu les sous, j'calcule plus mi amor et si tu m'dois des sous, v'-esqui la mise à mort J'déboule dans ton tieks avec dix négros, eh Tu vas cracher mes dinero, j'suis dans l'bâtiment, j'fais des midi-minuit Faut qu'ma liasse elle grossit, faut pas qu'elle diminue Tu vas cracher du sang si t'as craché des noms, Opinel 12, c'est chacun ses démons On casse ta jambe si tu casses la démarche et pendant la descente y a l'adré' qui te-mon Tu t'es fait mêler, c'est ça la vie, tu t'es fait mêler, c'est ça la vie La moitié des meufs sont des putes mais j'vais pas finir seul à vie Une seule bastos, ça va vite, j'fais que détailler donc mes mains sont sales à vie Et cette pute veut rentrer dans ma vie, elle a bégayé dès qu'elle m'a vu Tu t'es fait mêler, c'est ça la vie, tu t'es fait mêler, c'est ça la vie La moitié des meufs sont des putes mais j'vais pas finir seul à vie Une seule bastos, ça va vite, j'fais que détailler donc mes mains sont sales à vie Et cette pute veut rentrer dans ma vie, elle a bégayé dès qu'elle m'a vu J'peux pas arrêter d'plavonner, j'peux pas arrêter d'plavonner J'peux pas arrêter d'plavonner, j'ai envie d'arrêter mais j'aime trop la monnaie J'peux pas arrêter d'plavonner, j'peux pas arrêter d'plavonner J'peux pas arrêter d'plavonner, j'ai envie d'arrêter mais j'aime trop la monnaie J'peux pas arrêter d'plavonner, j'ai envie d'arrêter mais j'aime trop la monnaie</t>
         </is>
       </c>
     </row>
@@ -718,7 +718,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Poh, poh, poh, poh Poh, poh, poh, poh Curt Bain has all the smoke, boy J'me fais solo dans la street, j'ai zéro tuteur han, on fait courir les bandits d'Twitter han T'as poucave quoi ? T'as poucave quoi ? T'as même pas fait 48 heures salope 9-2-1-4-0 sur le pocheton, comme dhab', de la ppe-fra, j'envoie aux auditeurs Y a pas qu'en été qu'on sort les motos le matin, le réveil, c'est le bruit du moteur Mon flow met ton cerveau en ébullition, tu rleh déjà, c'est que le début du son Tous les jours d'l'année, j'suis en noir comme Ardisson brr, brr, l'ange de la mort est ché-ca dans les munitions brr Pour faire des vues, j'ai pas eu b'soin d'Daymolition, c'était qu'une démo, là, c'est la démolition La miss, elle est belle mais son démon est cheum, pour des talbins, elle s'met direct en position Ici, quand on s'amuse, tu t'fais réveiller par les sirènes du SAMU poh Tous les vrais, j'les salue, les faux, on les salit, un penchant pour les thunes, les fimbis, nique sa mère L'gérant be-tom, le p'tit gère, les rôles s'inversent, à Clamart, ça t'arrache ton keus quand tu traverse Couteau papillon, y a pas qu'le Glock qui transperce, sors le liquide, négro, j'veux pas qu'tu transpires salope On t'fera pas d'mal si tu parles bien han, tu finis pas bien si tu parles mal han Des pesos, j'en voulais beaucoup, j'me levais, j'mettais des rottes-ca sur l'Bon Coin Toujours confiance en mon Opinel mais j'perds pas mes lles-coui, j'compte aussi sur mes poings Tu parles de rasba, en vrai, toi, t'en mets pas, j'monte sur l'instru', je sais qu't'entends mes basses C'est des menteurs, j'sais qu'ils s'inventent des talles, j'aimerais bien voir couler le sang d'l'État Tu touches un des miens donc fais bellek aux tiens, on règle les embrouilles avec la vendetta J'dédicace mes dealers, mes receleurs, la moitié des meufs sont des grosses catins Mais je sais qu'j'vais pas finir solo han, j'vais p't-être finir avec une catin Rien n'a changé dans mes sons, j'reste insolent poh, j'reste insolent, poh, j'reste insolent You might also like Rien n'a changé dans mes sons, j'reste insolent, ils viennent massifs, mais ils sont pas impressionnants Flow agressif donc augmente le niveau sonore, j'peux niquer l'instru' juste avec des assonances Et si les keufs sont lents, j'gué-lar en rigolant, de base, pas violent, j'ai volé avec violence T'occupe pas de tes clicos, ils sont khabat, en groupe t'es un mec chaud, mais tout seul tu harbat Le manque d'argent, ça tue, ne te laisse pas abattre, le bosseur fait des trous mais l'gérant est khabat J'étais sur le R, cette pute voulait que j'la capte charo, j'volais même chez les meufs que je captais L'argent facile, c'est pas si simple mais on s'adapte, pour te piétiner, toujours la paire adaptée Guette l'ascension, j'ai pas fini d'monter, là, j'suis dans l'ascenseur, c'est la reine des tiagas Elle veut que j'sois sincère, une bonbonne dans l'fut', c'est comme ça qu'on s'en sort, mon pilon, il sent fort T'as d'la selha dans l'nez, c'est maintenant qu'tu t'sens fort, un plavon qui marche, j'suis prêt à le faire 100 fois Comme Céline Dion, le guetteur, il casse sa voix, les pieds sur terre, tu vois tes rêves qui s'envolent Sur l'rrain-te comme R9, que d'la frappe qu'on envoie, normal que tous les criquets s'affolent Elle aime faire des sous alors surveille bien ta folle, un d'mes négros peut la faire taffer Fais pas la mala, raconte pas tout c'que t'as fait, ils jouent les Ze Pek' mais j'vois que des Buscapé Quand y a heja, ils sont bons qu'à snaper, j'freestylais dans l'bloc, maintenant, j'suis sur Booska-P Ça sort l'bécane, y a plus d'coco, mets la soupape, mon équipe dans ton tier-quar, tu kahalass ou pas ? Mes gavas s'évaporent une fois qu'le coup part, comme d'habitude, gros, y a zéro coupable Toi, tu rappes sur d'la drill mais tu découpes pas, j'vois que des copies, j'entends mon flow tout-par Derrière toi, les képis, négro, te retourne pas, négro, te retourne pas J'en ai mis des rottes-ca comme Cenoura brr, toi, tu bombes le torse devant les p'tits brr Tu fais moins l'malin quand c'est nous, hein brr ? Tu fais moins l'malin quand c'est nous, hein ? Même nos 03 éclatent leurs 01 heuu, éclatent leurs 01 heuu Y a des mecs qui montent sur des plans sans redescendre, j'ai té-cla mon pét' et j'ai fait tomber des cendres Que des négros cagoulés pendant la descente, t'as chaud même si on est en décembre1</t>
+          <t>Poh, poh, poh, poh Poh, poh, poh, poh Curt Bain has all the smoke, boy J'me fais solo dans la street, j'ai zéro tuteur han, on fait courir les bandits d'Twitter han T'as poucave quoi ? T'as poucave quoi ? T'as même pas fait 48 heures salope 9-2-1-4-0 sur le pocheton, comme dhab', de la ppe-fra, j'envoie aux auditeurs Y a pas qu'en été qu'on sort les motos le matin, le réveil, c'est le bruit du moteur Mon flow met ton cerveau en ébullition, tu rleh déjà, c'est que le début du son Tous les jours d'l'année, j'suis en noir comme Ardisson brr, brr, l'ange de la mort est ché-ca dans les munitions brr Pour faire des vues, j'ai pas eu b'soin d'Daymolition, c'était qu'une démo, là, c'est la démolition La miss, elle est belle mais son démon est cheum, pour des talbins, elle s'met direct en position Ici, quand on s'amuse, tu t'fais réveiller par les sirènes du SAMU poh Tous les vrais, j'les salue, les faux, on les salit, un penchant pour les thunes, les fimbis, nique sa mère L'gérant be-tom, le p'tit gère, les rôles s'inversent, à Clamart, ça t'arrache ton keus quand tu traverse Couteau papillon, y a pas qu'le Glock qui transperce, sors le liquide, négro, j'veux pas qu'tu transpires salope On t'fera pas d'mal si tu parles bien han, tu finis pas bien si tu parles mal han Des pesos, j'en voulais beaucoup, j'me levais, j'mettais des rottes-ca sur l'Bon Coin Toujours confiance en mon Opinel mais j'perds pas mes lles-coui, j'compte aussi sur mes poings Tu parles de rasba, en vrai, toi, t'en mets pas, j'monte sur l'instru', je sais qu't'entends mes basses C'est des menteurs, j'sais qu'ils s'inventent des talles, j'aimerais bien voir couler le sang d'l'État Tu touches un des miens donc fais bellek aux tiens, on règle les embrouilles avec la vendetta J'dédicace mes dealers, mes receleurs, la moitié des meufs sont des grosses catins Mais je sais qu'j'vais pas finir solo han, j'vais p't-être finir avec une catin Rien n'a changé dans mes sons, j'reste insolent poh, j'reste insolent, poh, j'reste insolent Rien n'a changé dans mes sons, j'reste insolent, ils viennent massifs, mais ils sont pas impressionnants Flow agressif donc augmente le niveau sonore, j'peux niquer l'instru' juste avec des assonances Et si les keufs sont lents, j'gué-lar en rigolant, de base, pas violent, j'ai volé avec violence T'occupe pas de tes clicos, ils sont khabat, en groupe t'es un mec chaud, mais tout seul tu harbat Le manque d'argent, ça tue, ne te laisse pas abattre, le bosseur fait des trous mais l'gérant est khabat J'étais sur le R, cette pute voulait que j'la capte charo, j'volais même chez les meufs que je captais L'argent facile, c'est pas si simple mais on s'adapte, pour te piétiner, toujours la paire adaptée Guette l'ascension, j'ai pas fini d'monter, là, j'suis dans l'ascenseur, c'est la reine des tiagas Elle veut que j'sois sincère, une bonbonne dans l'fut', c'est comme ça qu'on s'en sort, mon pilon, il sent fort T'as d'la selha dans l'nez, c'est maintenant qu'tu t'sens fort, un plavon qui marche, j'suis prêt à le faire 100 fois Comme Céline Dion, le guetteur, il casse sa voix, les pieds sur terre, tu vois tes rêves qui s'envolent Sur l'rrain-te comme R9, que d'la frappe qu'on envoie, normal que tous les criquets s'affolent Elle aime faire des sous alors surveille bien ta folle, un d'mes négros peut la faire taffer Fais pas la mala, raconte pas tout c'que t'as fait, ils jouent les Ze Pek' mais j'vois que des Buscapé Quand y a heja, ils sont bons qu'à snaper, j'freestylais dans l'bloc, maintenant, j'suis sur Booska-P Ça sort l'bécane, y a plus d'coco, mets la soupape, mon équipe dans ton tier-quar, tu kahalass ou pas ? Mes gavas s'évaporent une fois qu'le coup part, comme d'habitude, gros, y a zéro coupable Toi, tu rappes sur d'la drill mais tu découpes pas, j'vois que des copies, j'entends mon flow tout-par Derrière toi, les képis, négro, te retourne pas, négro, te retourne pas J'en ai mis des rottes-ca comme Cenoura brr, toi, tu bombes le torse devant les p'tits brr Tu fais moins l'malin quand c'est nous, hein brr ? Tu fais moins l'malin quand c'est nous, hein ? Même nos 03 éclatent leurs 01 heuu, éclatent leurs 01 heuu Y a des mecs qui montent sur des plans sans redescendre, j'ai té-cla mon pét' et j'ai fait tomber des cendres Que des négros cagoulés pendant la descente, t'as chaud même si on est en décembre1</t>
         </is>
       </c>
     </row>
@@ -735,7 +735,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Fumez The Engineer, plugged in Bow, bow, bow, bow, bow J'ai fini le taff, j'ai les mains sales, bâtard, après l'embrouille, y a des corps au sol La vie c'est pas un jeu, j'ai lâché la console pour faire rentrer des sommes colossales J'fume le doré, j'ai la tec' d'ailleurs, j'préfère être armé, j'connais pas la boxe thaï Devant l'que-tru, tu t'assoies en tailleur, en tailleur, par mon équipe tu t'fais entailler bow J'ai pas bossé pour acheter ton sac à main Quand j'ai une embrouille, j'appell pas des zinc' à moi, quand t'es en manqu de sous, tes problèmes s'accumulent À part tous ces billets, moi, y a rien qui m'stimule, elle est en manque, elle veut que j'la pine J'crache pas dedans mais j'lui fait prendre la pilule, j'crache pas dedans mais j'lui fait prendre la pilule J'crache pas dedans mais j'lui fait prendre la pilule, on augmente le score, on fait ça en rapide Y a zéro match nul salope, toutes mes promesses seront maintenues On part en guerre, les ennemis n'ont qu'à bien s'tenir On t'croise solo, tu t'fais bastonner, on t'croise en groupe, tu t'fais bastonner Tu prends en gros, j'te passe mon num' J'ai la haine quand le bigo, il veut pas sonner, la rue veut pas m'lâcher comme si j'étais son ex Pour cet argent, j'éprouve un amour passionnel, j'fais ma ce-pla solo, j'ai b'soin que personne m'aide Tu demandes combien j'peux ramasser par semaine, si on t'hagar tes affaires, y a rien d'personnel Tant qu'j'ai pas assez ramassé, j'ai pas sommeil, tant qu'j'ai pas assez ramassé, j'ai pas sommeil Tant qu'j'ai pas assez ramassé, j'ai pas sommeil, elle m'envoie des messages même si elle a son mec Ma-ma-matraque, shlass, extint, balle, dans ton quartier, à deux doigts de t'assommer Fils de pute, faut qu'tu sortes du bat', si t'es pas venu consommer Si ça touche un des nôtres, c'est normal qu'on s'en mêle, si ça touche un des nôtres, c'est normal qu'on s'en mêle Passe au tieks, y a des dealers tous les 200 mètres, les jaloux m'voient manger, normal qu'ils deviennent maigres On sort les mes-ar désormais, t'es pas en sécu' même à deux pas d'ta son-mai T'es pas en sécu' même à deux pas d'ta son-mai, c'est 140BRICKS, c'est pas les États-Unis Qu'est-ce que t'as ramassé tout ce temps qu't'as zoné ? You might also like Chouara, on s'arrache dans l'quartier mmh, mmh, désolé pour les dégâts occasionnés J'suis dans les bails noirs mmh, mmh, c'est l'bruit qu't'as fait quand on t'a bâillonné Elle fait la hlel mmh, mmh, mais t'as pas vu ses My Eyes Only Si elle veut tapiner, y a des postes disponibles, si elle veut tapiner, y a des places qui sont libres Chouara, on s'arrache dans l'quartier mmh, mmh, désolé pour les dégâts occasionnés J'suis dans les bails noirs mmh, mmh, c'est l'bruit qu't'as fait quand on t'a bâillonné Elle fait la hlel mmh, mmh, mais t'as pas vu ses My Eyes Only Si elle veut tapiner, y a des postes disponibles, si elle veut tapiner, y a des places qui sont libres J'fais que d'avancer, j'sais pas reculer, maman m'a dit ne parle pas aux inconnus Fils de pute, est-c'que on s'connaît ? Enculé, j'me mélange pas à ces comiques Inutile comme quand le baveux est commis, des délits j'ai commis, j'aurais du lire des livres J'l'ai fais pour mailler, j'l'ai pas fait pour l'délire, j'mélange mes billets, j'suis plutôt bordélique J'en connais qui font les Montana Tony, ils sont même pas bouillants, ils sont juste alcooliques Les vrais vaillants, on les connaît, toi, t'es qu'une salope, personne va tej' des colis J'aime voir la tête de l'ingé' en train d'décoller, si tu sais pas chiffrer, va à l'école Cette pute, comme mon pilon, elle fait que d'me coller, elle croit qu'j'vais la marier, putain, elle est conne Chouara, on s'arrache dans l'quartier mmh, mmh, désolé pour les dégâts occasionnés J'suis dans les bails noirs mmh, mmh, c'est l'bruit qu't'as fait quand on t'a bâillonné Elle fait la hlel mmh, mmh, mais t'as pas vu ses My Eyes Only Si elle veut tapiner, y a des postes disponibles, si elle veut tapiner, y a des places qui sont libres Brr, brr, mmh, mmh Fumez The Engineer Mmh, mmh Blood, don't know what he said in it, but it sounded fucking cold Fuck off1</t>
+          <t>Fumez The Engineer, plugged in Bow, bow, bow, bow, bow J'ai fini le taff, j'ai les mains sales, bâtard, après l'embrouille, y a des corps au sol La vie c'est pas un jeu, j'ai lâché la console pour faire rentrer des sommes colossales J'fume le doré, j'ai la tec' d'ailleurs, j'préfère être armé, j'connais pas la boxe thaï Devant l'que-tru, tu t'assoies en tailleur, en tailleur, par mon équipe tu t'fais entailler bow J'ai pas bossé pour acheter ton sac à main Quand j'ai une embrouille, j'appell pas des zinc' à moi, quand t'es en manqu de sous, tes problèmes s'accumulent À part tous ces billets, moi, y a rien qui m'stimule, elle est en manque, elle veut que j'la pine J'crache pas dedans mais j'lui fait prendre la pilule, j'crache pas dedans mais j'lui fait prendre la pilule J'crache pas dedans mais j'lui fait prendre la pilule, on augmente le score, on fait ça en rapide Y a zéro match nul salope, toutes mes promesses seront maintenues On part en guerre, les ennemis n'ont qu'à bien s'tenir On t'croise solo, tu t'fais bastonner, on t'croise en groupe, tu t'fais bastonner Tu prends en gros, j'te passe mon num' J'ai la haine quand le bigo, il veut pas sonner, la rue veut pas m'lâcher comme si j'étais son ex Pour cet argent, j'éprouve un amour passionnel, j'fais ma ce-pla solo, j'ai b'soin que personne m'aide Tu demandes combien j'peux ramasser par semaine, si on t'hagar tes affaires, y a rien d'personnel Tant qu'j'ai pas assez ramassé, j'ai pas sommeil, tant qu'j'ai pas assez ramassé, j'ai pas sommeil Tant qu'j'ai pas assez ramassé, j'ai pas sommeil, elle m'envoie des messages même si elle a son mec Ma-ma-matraque, shlass, extint, balle, dans ton quartier, à deux doigts de t'assommer Fils de pute, faut qu'tu sortes du bat', si t'es pas venu consommer Si ça touche un des nôtres, c'est normal qu'on s'en mêle, si ça touche un des nôtres, c'est normal qu'on s'en mêle Passe au tieks, y a des dealers tous les 200 mètres, les jaloux m'voient manger, normal qu'ils deviennent maigres On sort les mes-ar désormais, t'es pas en sécu' même à deux pas d'ta son-mai T'es pas en sécu' même à deux pas d'ta son-mai, c'est 140BRICKS, c'est pas les États-Unis Qu'est-ce que t'as ramassé tout ce temps qu't'as zoné ? Chouara, on s'arrache dans l'quartier mmh, mmh, désolé pour les dégâts occasionnés J'suis dans les bails noirs mmh, mmh, c'est l'bruit qu't'as fait quand on t'a bâillonné Elle fait la hlel mmh, mmh, mais t'as pas vu ses My Eyes Only Si elle veut tapiner, y a des postes disponibles, si elle veut tapiner, y a des places qui sont libres Chouara, on s'arrache dans l'quartier mmh, mmh, désolé pour les dégâts occasionnés J'suis dans les bails noirs mmh, mmh, c'est l'bruit qu't'as fait quand on t'a bâillonné Elle fait la hlel mmh, mmh, mais t'as pas vu ses My Eyes Only Si elle veut tapiner, y a des postes disponibles, si elle veut tapiner, y a des places qui sont libres J'fais que d'avancer, j'sais pas reculer, maman m'a dit ne parle pas aux inconnus Fils de pute, est-c'que on s'connaît ? Enculé, j'me mélange pas à ces comiques Inutile comme quand le baveux est commis, des délits j'ai commis, j'aurais du lire des livres J'l'ai fais pour mailler, j'l'ai pas fait pour l'délire, j'mélange mes billets, j'suis plutôt bordélique J'en connais qui font les Montana Tony, ils sont même pas bouillants, ils sont juste alcooliques Les vrais vaillants, on les connaît, toi, t'es qu'une salope, personne va tej' des colis J'aime voir la tête de l'ingé' en train d'décoller, si tu sais pas chiffrer, va à l'école Cette pute, comme mon pilon, elle fait que d'me coller, elle croit qu'j'vais la marier, putain, elle est conne Chouara, on s'arrache dans l'quartier mmh, mmh, désolé pour les dégâts occasionnés J'suis dans les bails noirs mmh, mmh, c'est l'bruit qu't'as fait quand on t'a bâillonné Elle fait la hlel mmh, mmh, mais t'as pas vu ses My Eyes Only Si elle veut tapiner, y a des postes disponibles, si elle veut tapiner, y a des places qui sont libres Brr, brr, mmh, mmh Fumez The Engineer Mmh, mmh Blood, don't know what he said in it, but it sounded fucking cold Fuck off1</t>
         </is>
       </c>
     </row>
@@ -752,7 +752,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>9-2-1-4-0 sur le pocheton, j'en place une pour tous les vrais lauds-sa du ghetto, les charbonneurs qui se lèvent tôt Pour péter le cross en été, qu'ils mettent des hassba pour pas finir endettés Les schmitts, ces batârds, ils sont bons qu'à enquêter mais arrivent pas à nous arrêter, mais arrivent pas à nous arrêter On monte sur un plan à deux, alors on partage à deux Tu dis qu'c'était ton pote, pourquoi tu lui as tourné l'dos ? batârd On est plus des ados, batârd, pour des sommes on va se battre J'suis à l'arrière de la tchop j'ai plus de batterie, mais y a une racli qui me fait une gâterie Tu critiques, ah bouge la tête, à la fin du bon-char j'redecoupe une plaquette À midi un ient-cli qui m'appelle sur le tel', ah bon ? attends deux trois minutes, j'ai pas quitté l'hôtel ah bon ? Elle est bonne, mais la bonne, c'est laquelle ? Dans le bat', le ient-cli, on accueille Il va jamais pécho si ton shit, c'est d'la caille Et en moins d'une minute j'ai mis tout l'monde d'accord On prend tes bijoux sans demander ton accord Si je sors le schlass j'vois plus personne au corps à corps J'lui visser dans la journée, mais à minuit il m'appelle encore Y a pas d'karaté, mes gars s'occupent de ton cas Ils sont pas armés, pourquoi ils parlent de toka ? salope Et ils font les Savastano, mais en vrai ils ont trop la boca 100 euros avant quatorze heures, c'est impeccable Les ients-cli qu'j'ai servis, ils ont pété un cable Et j'veux pas d'salope à ma table Et j'veux pas d'salope à ma table Ils ont pas les sous, c'est des coños On t'fume devant ta meuf à la Zé Pequeno J'suis plutôt violent, mais elle veut que j'continue Si j'pète une grosse somme, j'me barre de ce continent Si j'pète une grosse somme, j'me barre de ce continent Sous pilon on est tous maladroits J'ai fait des dingueries avec la main droite Faut pas être harag si t'as des détails sur oi-t J'coupe avec les mains donc il m'en reste sur les oid Chouara, on arrache ton sac, on est méconnaissables salope J'ai pas connu l'bac à sable, salope, j'rentre, j'pose une kichta sur la table paw Les kilogrammes bien cachés, fais belek où t'achètes, y a du teus-shi coupé Ils font les impliqués, mais c'est tous des mytho' quand j'ai besoin d'taille-dé Ils sont même pas opés donc j'vais les éviter Tant qu'les ients-cli seront là, les dealers seront là, igo, rien va bouger Tant qu'les ients-cli seront là, les dealers seront là, igo, rien va bouger Mama m'a donné la vie donc celui qui la touche, j'vais lui donner la mort Et j'ai pas besoin d'amour, j'visser toute la journée, j'suis trop généreux Les chtars, ils veulent peter, c'est trop tard pour eux, ces batârds sont venus pour rien Et si j'degaine un flingue en embrouille, j'sais qu'tous ces pédés vont crourir 22, 22, artena, ça rentre dans l'bat' J'suis à peine de té-cla, j'suis déjà khabat Et si ma liasse grossit pas, j'monte sur un plavon J'ai mis les gants, j'suis opé, j'fais mes choses à fond À midi pile j'suis à Mail, j'fais des sous, finir à Miami Avec ces p'tits batârds, j'fais pas ami ami Négro, tu crois en qui ? Même ton poto t'l'a mise Et à ma gauche un gue-shla J'veux une pétasse gée-char comme Fanny Neguesha Quand y a embrouille ils courent, ils font les négros chauds Ta meuf, elle en peut plus et j'ai même pas ché-cra La miss, j'la touche pas si elle est crade Pour un billet, ta tête, on écrase C'que j'veux, c'est ma tête à l'écran Ils ont mis boulette, c'est normal qu'ils ont les crampes You might also like Mama m'a donné la vie donc celui qui la touche, j'vais lui donner la mort Et j'ai pas besoin d'amour, j'visser toute la journée, j'suis trop généreux Les chtars, ils veulent péter, c'est trop tard pour eux Ces bâtards sont venus pour rien Et si j'degaine un flingue en embrouille, j'sais qu'tous ces pédés vont courir Mama m'a donné la vie donc celui qui la touche, j'vais lui donner la mort Et j'ai pas besoin d'amour, j'visser toute la journée, j'suis trop généreux Les chtars, ils veulent péter, c'est trop tard pour eux Ces bâtards sont venus pour rien Et si j'degaine un flingue en embrouille, j'sais qu'tous ces pédés vont courir</t>
+          <t>9-2-1-4-0 sur le pocheton, j'en place une pour tous les vrais lauds-sa du ghetto, les charbonneurs qui se lèvent tôt Pour péter le cross en été, qu'ils mettent des hassba pour pas finir endettés Les schmitts, ces batârds, ils sont bons qu'à enquêter mais arrivent pas à nous arrêter, mais arrivent pas à nous arrêter On monte sur un plan à deux, alors on partage à deux Tu dis qu'c'était ton pote, pourquoi tu lui as tourné l'dos ? batârd On est plus des ados, batârd, pour des sommes on va se battre J'suis à l'arrière de la tchop j'ai plus de batterie, mais y a une racli qui me fait une gâterie Tu critiques, ah bouge la tête, à la fin du bon-char j'redecoupe une plaquette À midi un ient-cli qui m'appelle sur le tel', ah bon ? attends deux trois minutes, j'ai pas quitté l'hôtel ah bon ? Elle est bonne, mais la bonne, c'est laquelle ? Dans le bat', le ient-cli, on accueille Il va jamais pécho si ton shit, c'est d'la caille Et en moins d'une minute j'ai mis tout l'monde d'accord On prend tes bijoux sans demander ton accord Si je sors le schlass j'vois plus personne au corps à corps J'lui visser dans la journée, mais à minuit il m'appelle encore Y a pas d'karaté, mes gars s'occupent de ton cas Ils sont pas armés, pourquoi ils parlent de toka ? salope Et ils font les Savastano, mais en vrai ils ont trop la boca 100 euros avant quatorze heures, c'est impeccable Les ients-cli qu'j'ai servis, ils ont pété un cable Et j'veux pas d'salope à ma table Et j'veux pas d'salope à ma table Ils ont pas les sous, c'est des coños On t'fume devant ta meuf à la Zé Pequeno J'suis plutôt violent, mais elle veut que j'continue Si j'pète une grosse somme, j'me barre de ce continent Si j'pète une grosse somme, j'me barre de ce continent Sous pilon on est tous maladroits J'ai fait des dingueries avec la main droite Faut pas être harag si t'as des détails sur oi-t J'coupe avec les mains donc il m'en reste sur les oid Chouara, on arrache ton sac, on est méconnaissables salope J'ai pas connu l'bac à sable, salope, j'rentre, j'pose une kichta sur la table paw Les kilogrammes bien cachés, fais belek où t'achètes, y a du teus-shi coupé Ils font les impliqués, mais c'est tous des mytho' quand j'ai besoin d'taille-dé Ils sont même pas opés donc j'vais les éviter Tant qu'les ients-cli seront là, les dealers seront là, igo, rien va bouger Tant qu'les ients-cli seront là, les dealers seront là, igo, rien va bouger Mama m'a donné la vie donc celui qui la touche, j'vais lui donner la mort Et j'ai pas besoin d'amour, j'visser toute la journée, j'suis trop généreux Les chtars, ils veulent peter, c'est trop tard pour eux, ces batârds sont venus pour rien Et si j'degaine un flingue en embrouille, j'sais qu'tous ces pédés vont crourir 22, 22, artena, ça rentre dans l'bat' J'suis à peine de té-cla, j'suis déjà khabat Et si ma liasse grossit pas, j'monte sur un plavon J'ai mis les gants, j'suis opé, j'fais mes choses à fond À midi pile j'suis à Mail, j'fais des sous, finir à Miami Avec ces p'tits batârds, j'fais pas ami ami Négro, tu crois en qui ? Même ton poto t'l'a mise Et à ma gauche un gue-shla J'veux une pétasse gée-char comme Fanny Neguesha Quand y a embrouille ils courent, ils font les négros chauds Ta meuf, elle en peut plus et j'ai même pas ché-cra La miss, j'la touche pas si elle est crade Pour un billet, ta tête, on écrase C'que j'veux, c'est ma tête à l'écran Ils ont mis boulette, c'est normal qu'ils ont les crampes Mama m'a donné la vie donc celui qui la touche, j'vais lui donner la mort Et j'ai pas besoin d'amour, j'visser toute la journée, j'suis trop généreux Les chtars, ils veulent péter, c'est trop tard pour eux Ces bâtards sont venus pour rien Et si j'degaine un flingue en embrouille, j'sais qu'tous ces pédés vont courir Mama m'a donné la vie donc celui qui la touche, j'vais lui donner la mort Et j'ai pas besoin d'amour, j'visser toute la journée, j'suis trop généreux Les chtars, ils veulent péter, c'est trop tard pour eux Ces bâtards sont venus pour rien Et si j'degaine un flingue en embrouille, j'sais qu'tous ces pédés vont courir</t>
         </is>
       </c>
     </row>
@@ -769,7 +769,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Chaque problème a sa solution, pourtant ma solution m'apporte des problèmes Renoi, t'es pas encore bon mais tu progresses, tu t'fais des ennemis si tu tiens pas tes promesses J'commence en dernier mais j'peux vite finir premier, j'montais sur Paname, ça puait l'herbe dans l'tro-mé On m'regardait comme si j'étais même pas humain, faire rentrer l'argent, c'est mon domaine Jamais aimé l'école mais j'ressors diplômé, j'ai charbonné toute la smaine Ce junkie j'l'aimais bin, mon blase il a donné, j'me demande il m'reste combien d'année à zoner Pour pas finir par terre, on s'est mis à voler et ce que je suis condamné ou j'peux m'faire pardonner ? Comme d'hab', on apparaît chaque fois que ça parle de nous, discret j'ai l'air heureux même quand j'suis malheureux Si j'te dis un secret ça reste entre nous, tes faux négros, ils ne font pas d'euros Si tu fais pas rentrer pourquoi tu traînes, ta copine m'imagine entrain d'la pénétrer Renoi c'est pas de ma faute pourquoi tu t'énerves, c'est soit tu ken ou bien tu t'fais kéni Soit tu dégaines ou tu t'fais guainer La nuit porte conseil, à minuit on marche dans ta tess À minuit deux mes négros ils marchent sur ta tête Pas mon délire de péter des 'teilles pour la frime, j'peux la péter sur ta tête On te dira pas tout c'qu'on a fait mais on l'a pas fait pour du Fendi C'est pas grave de perdre un tête, c'est grave si tu t'es pas défendu Elle est cheum mais elle a un gros boule, t'es prêt à lui faire croire qu'elle est belle Est-c'que je repose en paix si je m'endors calibré ? Jeune lossa fait son pain pense qu'à livrer T'es un bon rappeur mais est-c'que tu dis vrai ? Tu veux m'serrer la main mais est-c'que tu devrais ? Courir après la maille, pas pour acheter d'la marque, comment suivre le droit chemin en état d'ivresse ? J'bouge pas pour les meufs mais pour les tal j'y vais, j'quitte pas le quartier pour une niara comme Béné J'connais les vices d'la rue, tu vas rien m'enseigner, y a que quand tout va mal que tu pries le seigneur 1pliké 1.4.0 dans ton enceinte, la miss elle m'harcèle pourtant ça sonne occupé J'ai mis le peura en cloque, j'lui fais des enfants, j'ai pas l'temps d'm'en occuper Opinel sorti en moins de deux s'condes, tu danses décalé coupé Ils connaissent tous mes couplets, connaissent tous mes coupletsYou might also like</t>
+          <t>Chaque problème a sa solution, pourtant ma solution m'apporte des problèmes Renoi, t'es pas encore bon mais tu progresses, tu t'fais des ennemis si tu tiens pas tes promesses J'commence en dernier mais j'peux vite finir premier, j'montais sur Paname, ça puait l'herbe dans l'tro-mé On m'regardait comme si j'étais même pas humain, faire rentrer l'argent, c'est mon domaine Jamais aimé l'école mais j'ressors diplômé, j'ai charbonné toute la smaine Ce junkie j'l'aimais bin, mon blase il a donné, j'me demande il m'reste combien d'année à zoner Pour pas finir par terre, on s'est mis à voler et ce que je suis condamné ou j'peux m'faire pardonner ? Comme d'hab', on apparaît chaque fois que ça parle de nous, discret j'ai l'air heureux même quand j'suis malheureux Si j'te dis un secret ça reste entre nous, tes faux négros, ils ne font pas d'euros Si tu fais pas rentrer pourquoi tu traînes, ta copine m'imagine entrain d'la pénétrer Renoi c'est pas de ma faute pourquoi tu t'énerves, c'est soit tu ken ou bien tu t'fais kéni Soit tu dégaines ou tu t'fais guainer La nuit porte conseil, à minuit on marche dans ta tess À minuit deux mes négros ils marchent sur ta tête Pas mon délire de péter des 'teilles pour la frime, j'peux la péter sur ta tête On te dira pas tout c'qu'on a fait mais on l'a pas fait pour du Fendi C'est pas grave de perdre un tête, c'est grave si tu t'es pas défendu Elle est cheum mais elle a un gros boule, t'es prêt à lui faire croire qu'elle est belle Est-c'que je repose en paix si je m'endors calibré ? Jeune lossa fait son pain pense qu'à livrer T'es un bon rappeur mais est-c'que tu dis vrai ? Tu veux m'serrer la main mais est-c'que tu devrais ? Courir après la maille, pas pour acheter d'la marque, comment suivre le droit chemin en état d'ivresse ? J'bouge pas pour les meufs mais pour les tal j'y vais, j'quitte pas le quartier pour une niara comme Béné J'connais les vices d'la rue, tu vas rien m'enseigner, y a que quand tout va mal que tu pries le seigneur 1pliké 1.4.0 dans ton enceinte, la miss elle m'harcèle pourtant ça sonne occupé J'ai mis le peura en cloque, j'lui fais des enfants, j'ai pas l'temps d'm'en occuper Opinel sorti en moins de deux s'condes, tu danses décalé coupé Ils connaissent tous mes couplets, connaissent tous mes couplets</t>
         </is>
       </c>
     </row>
@@ -786,7 +786,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Ils parlent de los-ki, ils m'harcèlent pour du taga Belek, 1PLIKÉ fait bouger ta tchaga J't'envoie ma localisation si y a drah Belek, 1PLIKÉ fait bouger ta tchaga C'est pour les tales que j'me lève tous les tins-ma, sans claquer un rond, j'ai fait claquer son tarma Ça parle dans ton dos, ça mange dans ta main, sont pas là quand t'as mal, après ils font zarma Ces zemel croient pas en Dieu, mais au karma, j'te connais, mais bon j'peux quand même te karna poh J'en ai vu des guignols, c'était pas sur Canal, rien qu'tu parles de frappe, j'suis pas sûr que t'en as J'sais faire de l'oseille, j'suis pas un zonard brr, ça prend ta Canada, ça prend ta The North brr J'viens à peine de rentrer, c'est déjà l'sauna brr, brr, j'perdrai pas mes cojo' comme la nationale brr Tu veux 50 g ? J'coupe la diagonale poh, poh, t'as kiffé l'projet, tu vas rleh du bum-al poh Ils veulent pas qu'on bicrave, c'est pas pire que l'cool-al poh, bande de connards Est-ce que t'esquives le re-shta comme Nicolas ? uh J'voulais pas les cala, mais bon elles me collent Est-ce que sur l'argent sale, fallait qu'je mise ? Comme la moitié d'mes gavas qu'ont quitté l'école ? Mon nom, ils veulent le salir, rien qu'ça mythonne, on les baise, ils veulent s'allier, tu crois qu'ça m'étonne ? Cannabis sur mes billets, mais j'v-'esqui la taule, on nettoie pas l'argent crade avec Sanytol T'es là pour la gagne, mais t'enchaînes les échecs, on tabasse les ordures, on les laisse par terre Même si j'respecte ceux qui ramassent les déchets poh, les couilles remplies j'rentrais dans ta rée-soi poh Nan, j'allais pas ramasser des chiennes ah bon ?, j'suis sur écoute quand j'parle à cette tchaga Les 22 ils khleh comment j'lui mets des cheb ah bon ?, l'amour rend aveugle, tu vois pas qu'elle est cheum Ici, personne s'aime, que des balles dans l'dos, quand ton pote réussit, gros, pourquoi t'as le seum ? Toi, tu parles chinois quand il s'agit d'descendre, tu prends par les sentiments quand tu dois des sommes C'est après la guerre qu'ils savent qui nous sommes pah, c'est les prières de maman qui nous sauvent pah Et rien qu'ça encaisse à s'en arracher les veux-ch' han, tu t'fais soulever par un crâne chauve Il a pé-cho 50 balles, c'était pas un 'loss, belek, la CR, c'est pas des lol On l'boit pur, tu fais des mélanges han, pourtant, tu disais qu'l'alcool, c'est de l'eau Tu parles pour dire d'la merde, le silence, c'est de l'or uh, ils ont rien brassé à part brasser de l'air uh J'réponds pas à maman, j'entends crier l'tonnerre, quand c'était tendu, le sac, c'est qui qui l'tenait ? uh Nique sa mère la vie ou bien c'est elle qui te nique, j'te bicrave mon flow, gros, viens pé-cho ta gimmick Y a encore ton sang sur mon Sergio Tacchini, si on te taquine, tu t'réveilles à la clinique poh Je ne fais que courir, j'm'arrêterai quand j'pourrai pourrai, notre vie, ils veulent la pourrir Le , ils sont pas v'nu décorer, ils sont pas là pour rien, ils sont pas là pour rire Je sais d'où je viens, mes rêves, j'les poursuis, pocheton dans la nature pendant la poursuite Au contrôle juste après, y a aucun souci, belek, belek avec l'argent facile Tu peux foncer dans l'mur en cherchant l'raccourci, longue vie à mes lers-dea qui ont la frappe dans le jeans À cause des balances, y a que des peines alourdies, mort à tous les keufs, même ceux qui restent sur l'ordi' J'encaisse tous les jours, tu fuckes la fin du mois, tu fuckes la fin du mois À cette vie, tu t'attaches, qu'est-ce que t'emportes à la fin ? Dis-moi, transaction risquée à deux pas d'chez moi Si j'be-tom, personne prendra mes patins brr, c'est pas la patinoire Seigneur, ma haine, enlevez-la-moi brr Seigneur, ma haine, enlevez-la-moi brr, brr, brr Si tu touches à celle qui m'a donné la vida, j'serai complice avec l'ange de la mort mort Moi, bats les c' de sortir de l'ombre, dans la ve-ca, tous mes plans j'élabore 'bore Enculé, j'mérite bien ma place, j'suis rentré avant qu'ils m'ferment la porte porte, 1PLIKÉ On est gentils à la base, mais si on s'énerve, ça fait poh, poh J't'encule ta mère qui sait pas cuisiner, personne m'a incité, on m'a contaminé J'ai appris à bosser sur un terrain miné, quand tu commences le TP, faut le terminer Me-ar à la main, j'contrôle ta destinée, le flow est réel, ne crois pas halluciner Manque d'affection, ma kichta m'a câliné, c'est pas pour rien que le bitume, on le saigne 9-2-1-4-0 sur le pocheton, j'représente les Hauts-de-Seine Hauts-de-Seine Belek, 1PLIKÉ fait bouger ta tiaga bouger ta tiaga Belek, 1PLIKÉ fait bouger ta tiaga bouger ta tiaga You might also like Putain, 1PLIKÉ, encore toi T'as encore tout niqué Le laissez pas faire ça, ARRÊTEZ-LE ! Ils parlent de los-ki, ils m'harcèlent pour du taga Belek, 1PLIKÉ fait bouger ta tchaga J't'envoie ma localisation si y a drah Belek, 1PLIKÉ fait bouger ta tchaga</t>
+          <t>Ils parlent de los-ki, ils m'harcèlent pour du taga Belek, 1PLIKÉ fait bouger ta tchaga J't'envoie ma localisation si y a drah Belek, 1PLIKÉ fait bouger ta tchaga C'est pour les tales que j'me lève tous les tins-ma, sans claquer un rond, j'ai fait claquer son tarma Ça parle dans ton dos, ça mange dans ta main, sont pas là quand t'as mal, après ils font zarma Ces zemel croient pas en Dieu, mais au karma, j'te connais, mais bon j'peux quand même te karna poh J'en ai vu des guignols, c'était pas sur Canal, rien qu'tu parles de frappe, j'suis pas sûr que t'en as J'sais faire de l'oseille, j'suis pas un zonard brr, ça prend ta Canada, ça prend ta The North brr J'viens à peine de rentrer, c'est déjà l'sauna brr, brr, j'perdrai pas mes cojo' comme la nationale brr Tu veux 50 g ? J'coupe la diagonale poh, poh, t'as kiffé l'projet, tu vas rleh du bum-al poh Ils veulent pas qu'on bicrave, c'est pas pire que l'cool-al poh, bande de connards Est-ce que t'esquives le re-shta comme Nicolas ? uh J'voulais pas les cala, mais bon elles me collent Est-ce que sur l'argent sale, fallait qu'je mise ? Comme la moitié d'mes gavas qu'ont quitté l'école ? Mon nom, ils veulent le salir, rien qu'ça mythonne, on les baise, ils veulent s'allier, tu crois qu'ça m'étonne ? Cannabis sur mes billets, mais j'v-'esqui la taule, on nettoie pas l'argent crade avec Sanytol T'es là pour la gagne, mais t'enchaînes les échecs, on tabasse les ordures, on les laisse par terre Même si j'respecte ceux qui ramassent les déchets poh, les couilles remplies j'rentrais dans ta rée-soi poh Nan, j'allais pas ramasser des chiennes ah bon ?, j'suis sur écoute quand j'parle à cette tchaga Les 22 ils khleh comment j'lui mets des cheb ah bon ?, l'amour rend aveugle, tu vois pas qu'elle est cheum Ici, personne s'aime, que des balles dans l'dos, quand ton pote réussit, gros, pourquoi t'as le seum ? Toi, tu parles chinois quand il s'agit d'descendre, tu prends par les sentiments quand tu dois des sommes C'est après la guerre qu'ils savent qui nous sommes pah, c'est les prières de maman qui nous sauvent pah Et rien qu'ça encaisse à s'en arracher les veux-ch' han, tu t'fais soulever par un crâne chauve Il a pé-cho 50 balles, c'était pas un 'loss, belek, la CR, c'est pas des lol On l'boit pur, tu fais des mélanges han, pourtant, tu disais qu'l'alcool, c'est de l'eau Tu parles pour dire d'la merde, le silence, c'est de l'or uh, ils ont rien brassé à part brasser de l'air uh J'réponds pas à maman, j'entends crier l'tonnerre, quand c'était tendu, le sac, c'est qui qui l'tenait ? uh Nique sa mère la vie ou bien c'est elle qui te nique, j'te bicrave mon flow, gros, viens pé-cho ta gimmick Y a encore ton sang sur mon Sergio Tacchini, si on te taquine, tu t'réveilles à la clinique poh Je ne fais que courir, j'm'arrêterai quand j'pourrai pourrai, notre vie, ils veulent la pourrir Le , ils sont pas v'nu décorer, ils sont pas là pour rien, ils sont pas là pour rire Je sais d'où je viens, mes rêves, j'les poursuis, pocheton dans la nature pendant la poursuite Au contrôle juste après, y a aucun souci, belek, belek avec l'argent facile Tu peux foncer dans l'mur en cherchant l'raccourci, longue vie à mes lers-dea qui ont la frappe dans le jeans À cause des balances, y a que des peines alourdies, mort à tous les keufs, même ceux qui restent sur l'ordi' J'encaisse tous les jours, tu fuckes la fin du mois, tu fuckes la fin du mois À cette vie, tu t'attaches, qu'est-ce que t'emportes à la fin ? Dis-moi, transaction risquée à deux pas d'chez moi Si j'be-tom, personne prendra mes patins brr, c'est pas la patinoire Seigneur, ma haine, enlevez-la-moi brr Seigneur, ma haine, enlevez-la-moi brr, brr, brr Si tu touches à celle qui m'a donné la vida, j'serai complice avec l'ange de la mort mort Moi, bats les c' de sortir de l'ombre, dans la ve-ca, tous mes plans j'élabore 'bore Enculé, j'mérite bien ma place, j'suis rentré avant qu'ils m'ferment la porte porte, 1PLIKÉ On est gentils à la base, mais si on s'énerve, ça fait poh, poh J't'encule ta mère qui sait pas cuisiner, personne m'a incité, on m'a contaminé J'ai appris à bosser sur un terrain miné, quand tu commences le TP, faut le terminer Me-ar à la main, j'contrôle ta destinée, le flow est réel, ne crois pas halluciner Manque d'affection, ma kichta m'a câliné, c'est pas pour rien que le bitume, on le saigne 9-2-1-4-0 sur le pocheton, j'représente les Hauts-de-Seine Hauts-de-Seine Belek, 1PLIKÉ fait bouger ta tiaga bouger ta tiaga Belek, 1PLIKÉ fait bouger ta tiaga bouger ta tiaga Putain, 1PLIKÉ, encore toi T'as encore tout niqué Le laissez pas faire ça, ARRÊTEZ-LE ! Ils parlent de los-ki, ils m'harcèlent pour du taga Belek, 1PLIKÉ fait bouger ta tchaga J't'envoie ma localisation si y a drah Belek, 1PLIKÉ fait bouger ta tchaga</t>
         </is>
       </c>
     </row>
@@ -803,7 +803,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>This some plus four shit, man Les embrouilles, ça sert à rien mon gars Les embrouilles, les embrouilles, ça sert à rien mon gars Ça, cest cque tu dis quand on déboule à dix mon gars Vi-sser comme Tsonga Jai, j'ai j'ai séché lécole pour moccuper dma Lyca pow La rue, cest dur, y a rien ddélicat pow Appelle mes gars si y a un mec à niquer Tu sors un tarpé, mais tu vas canner qui ? pow Jsuis dans les diez, jsuis pas dans les polémiques Fuck le boule à Cardi, jpréfère celui dNicki brr Jai même plus bsoin dché-bran les meufs pour les niquer brr Lamende brr, tas pas payé brr, ne crois pas quon est quitte brr, brr Tu crois pas en toi, mais tu crois en ton équipe, tes con, marcher solo, cest bénéfique Pour moi, faire de largent, cest génétique, jdécale une fois qujai pris tout lbénéfice Transaction enchaînée sur un vélo, pour des pesos à 9 heures jsuis déjà vé-le ah bon ? Dun voyou elle est tombée love, il soccupe pas delle, il soccupe des losses ah bon ? Jai de linspi, donc je prends des notes Si tu touches un des nôtres, on te démonte On sbalade sur ta tête, on sait pas innover pow Jai toujours pas ltemps dclaquer pour des montres pow Eux, ils sont mignons, mais ils font les monstres, jen connais qui dégainent plus vite que leur ombre Après ça, il reste que les mauvaises nouvelles Après ça, il reste que les mauvaises nouvelles hmm Y a des escortes Lycamobile qui font plus de passes que tes dealers Jrentre tard la nuit, jrate tous les dîners, donc jme péta avec mes djinns jme péta avec mes djinns Trop dCamélia qui font les Kylie Jenner, des Fatou qui jouent les Rose Amber, les meufs daujourdhui se ressemblent Si elle pue dla chatte, jramène léléphant bleu Fuck tous ceux qui font bleh, fuck les uniformes bleus Si tas mal construit, tout seffondre pow, comme ta racli dans ma chambre pow Tu dois des sous, tes pas à lombre Tu tfais shlass, mais on nest pas à Londres Équipe déter qui vient devant ta porte, même si ta famille est nombreuse Linstrumental, jvoulais juste la té-plan, jai fini en massacre à la tronçonneuse Jm'arrête, j'souffle, jreprends 1pliké, il prend trop son aise Jarrive avec un flow assaisonné, fréquente pas le quartier à minuit, cest sombre mec Y a ceux qui coffrent largent sur le téco et toi, tas fumé ton bénef', tas sombré Tes un bon, mais le teu-chi, tas assombri Tes en liberté, mais la hess, cest ta son-pri J'pète une kichta, jme fais lehess en même temps sale pute Jrepense aux condés, tous les tals quils mont pris Eh renoi, tu connais, on srefait en despi Cest pas les pertes qui changeront mon état desprit Tu demandes comment jfais pour trouver linspi Les affaires marchent et nos ennemi, ils tapent des sprints Vodka Redbull, jsuis pas sous codéine Sprite et non, j'suis pas sous Despe On sbat pour du respect, menotté jparfume tout le 308 break En mode sommes alléchantes pour me faire vibrer, tas pris, t'as rotte-ca dans l140 bricks salope You might also like T'as rappliqué, tas tout niqué, tas tout niqué Tas baisé lpe-ra, arrête-toi enculé, arrêtez-le ! Plus four1</t>
+          <t>This some plus four shit, man Les embrouilles, ça sert à rien mon gars Les embrouilles, les embrouilles, ça sert à rien mon gars Ça, cest cque tu dis quand on déboule à dix mon gars Vi-sser comme Tsonga Jai, j'ai j'ai séché lécole pour moccuper dma Lyca pow La rue, cest dur, y a rien ddélicat pow Appelle mes gars si y a un mec à niquer Tu sors un tarpé, mais tu vas canner qui ? pow Jsuis dans les diez, jsuis pas dans les polémiques Fuck le boule à Cardi, jpréfère celui dNicki brr Jai même plus bsoin dché-bran les meufs pour les niquer brr Lamende brr, tas pas payé brr, ne crois pas quon est quitte brr, brr Tu crois pas en toi, mais tu crois en ton équipe, tes con, marcher solo, cest bénéfique Pour moi, faire de largent, cest génétique, jdécale une fois qujai pris tout lbénéfice Transaction enchaînée sur un vélo, pour des pesos à 9 heures jsuis déjà vé-le ah bon ? Dun voyou elle est tombée love, il soccupe pas delle, il soccupe des losses ah bon ? Jai de linspi, donc je prends des notes Si tu touches un des nôtres, on te démonte On sbalade sur ta tête, on sait pas innover pow Jai toujours pas ltemps dclaquer pour des montres pow Eux, ils sont mignons, mais ils font les monstres, jen connais qui dégainent plus vite que leur ombre Après ça, il reste que les mauvaises nouvelles Après ça, il reste que les mauvaises nouvelles hmm Y a des escortes Lycamobile qui font plus de passes que tes dealers Jrentre tard la nuit, jrate tous les dîners, donc jme péta avec mes djinns jme péta avec mes djinns Trop dCamélia qui font les Kylie Jenner, des Fatou qui jouent les Rose Amber, les meufs daujourdhui se ressemblent Si elle pue dla chatte, jramène léléphant bleu Fuck tous ceux qui font bleh, fuck les uniformes bleus Si tas mal construit, tout seffondre pow, comme ta racli dans ma chambre pow Tu dois des sous, tes pas à lombre Tu tfais shlass, mais on nest pas à Londres Équipe déter qui vient devant ta porte, même si ta famille est nombreuse Linstrumental, jvoulais juste la té-plan, jai fini en massacre à la tronçonneuse Jm'arrête, j'souffle, jreprends 1pliké, il prend trop son aise Jarrive avec un flow assaisonné, fréquente pas le quartier à minuit, cest sombre mec Y a ceux qui coffrent largent sur le téco et toi, tas fumé ton bénef', tas sombré Tes un bon, mais le teu-chi, tas assombri Tes en liberté, mais la hess, cest ta son-pri J'pète une kichta, jme fais lehess en même temps sale pute Jrepense aux condés, tous les tals quils mont pris Eh renoi, tu connais, on srefait en despi Cest pas les pertes qui changeront mon état desprit Tu demandes comment jfais pour trouver linspi Les affaires marchent et nos ennemi, ils tapent des sprints Vodka Redbull, jsuis pas sous codéine Sprite et non, j'suis pas sous Despe On sbat pour du respect, menotté jparfume tout le 308 break En mode sommes alléchantes pour me faire vibrer, tas pris, t'as rotte-ca dans l140 bricks salope T'as rappliqué, tas tout niqué, tas tout niqué Tas baisé lpe-ra, arrête-toi enculé, arrêtez-le ! Plus four1</t>
         </is>
       </c>
     </row>
@@ -820,7 +820,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Binks Beatz Pendant qu'tu perds ton temps, nous, on fait partir l'taga J'rappe pour ceux qui coffrent l'argent sale et dépensent rien pour ces tiaga J'marche dans l'tieks avec les gavas, j'vais recharger ma Lebara J'rappe pour ceux qui cricket la journée, le soir, ils vont chouara J'casse la vitre de ta tchop, pour 24 carats Y a mon négro qui m'assiste, y a les chickens, crie Arah Ils ont même pas d'deux roues, dans leurs textes, ils parlent de casques Arai Hier, t'étais mon reuf, aujourd'hui, j'te vois même plus pareil Pourquoi t'enfiles les gants, tu montes pas sur des plans Mes négros veulent péter des sommes Les keufs ils veulent péter des ploc' Au comico j'ai pas pété ma bouille J'ai mis la cagoule, le iencli voit plus ma bouche Et si on a niqué ton pote, c'est juste pour marquer l'embrouille Après l'avoir mêlé, on le dépouille J'détaille la quette', sur le couteau y a assez pour une seu-di On s'pète à 21 heures comme on s'est dit J'suis au charbon de lundi à lundi À la fin du plavon, bon appétit J'suis dans l'tieks, je quitte pas le bitume Envoie la bonbonne, t'inquiètes j'ai l'habitude, bâtard On te mêle et tu passes les thunes, bâtard On te mêle et tu passes les thunes J'ai pété une fortune Faut pas qu'j'écoute la voix du sheitan, cette voix qui m'dit de rentrer chez toi Cette voix qui m'dit d'arrêter les études J'perds le nord, j'veux m'barrer dans le sud Si j'suis pas sur l'terrain, j'suis dans le stud' J'suis pas sur l'terrain, j'suis dans le stud' You might also like Pendant qu'tu perds ton temps, nous, on fait partir l'taga J'rappe pour ceux qui coffrent l'argent sale et dépensent rien pour ces tiaga J'marche dans l'tieks avec les gavas, j'vais recharger ma Lebara J'rappe pour ceux qui cricket la journée, le soir, ils vont chouara J'casse la vitre de ta tchop, pour 24 carats Y a mon négro qui m'assiste, y a les chickens, crie Arah Ils ont même pas d'deux roues, dans leurs textes, ils parlent de casques Arai Hier, t'étais mon reuf, aujourd'hui, j'te vois même plus pareil J'aime faire des billets, j'aime quand ça rentre J'aime les étaler sur la table Moi mon pire ennemi c'est la taule Mon meilleur ami c'est les tales Et vu qu'ils vont pas ensemble, tous les jours les keufs se lèvent tôt C'est donc ça la loi du ghetto, qu'à péter des kilos pour venir soulever J'ai les bras à Popeye Pour gagner des tales, moi je perds mon sommeil On baraude dans la ville, des délits on commet Et tous les jours ça recommence, la rue, c'est pas un jeu Toi, tu joues avec la vérité Avec mes gars, on vi-sser des shlags everyday On rentre chez nous une fois qu'la bonbonne est vidée Après minuit, mes négros ont des sales idées Pendant qu'tu perds ton temps, nous, on fait partir l'taga J'rappe pour ceux qui coffrent l'argent sale et dépensent rien pour ces tiaga J'marche dans l'tieks avec les gavas, j'vais recharger ma Lebara J'rappe pour ceux qui cricket la journée, le soir, ils vont chouara J'casse la vitre de ta tchop, pour 24 carats Y a mon négro qui m'assiste, y a les chickens, crie Arah Ils ont même pas d'deux roues, dans leurs textes, ils parlent de casques Arai Hier, t'étais mon reuf, aujourd'hui, j'te vois même plus pareil Binks Beatz</t>
+          <t>Binks Beatz Pendant qu'tu perds ton temps, nous, on fait partir l'taga J'rappe pour ceux qui coffrent l'argent sale et dépensent rien pour ces tiaga J'marche dans l'tieks avec les gavas, j'vais recharger ma Lebara J'rappe pour ceux qui cricket la journée, le soir, ils vont chouara J'casse la vitre de ta tchop, pour 24 carats Y a mon négro qui m'assiste, y a les chickens, crie Arah Ils ont même pas d'deux roues, dans leurs textes, ils parlent de casques Arai Hier, t'étais mon reuf, aujourd'hui, j'te vois même plus pareil Pourquoi t'enfiles les gants, tu montes pas sur des plans Mes négros veulent péter des sommes Les keufs ils veulent péter des ploc' Au comico j'ai pas pété ma bouille J'ai mis la cagoule, le iencli voit plus ma bouche Et si on a niqué ton pote, c'est juste pour marquer l'embrouille Après l'avoir mêlé, on le dépouille J'détaille la quette', sur le couteau y a assez pour une seu-di On s'pète à 21 heures comme on s'est dit J'suis au charbon de lundi à lundi À la fin du plavon, bon appétit J'suis dans l'tieks, je quitte pas le bitume Envoie la bonbonne, t'inquiètes j'ai l'habitude, bâtard On te mêle et tu passes les thunes, bâtard On te mêle et tu passes les thunes J'ai pété une fortune Faut pas qu'j'écoute la voix du sheitan, cette voix qui m'dit de rentrer chez toi Cette voix qui m'dit d'arrêter les études J'perds le nord, j'veux m'barrer dans le sud Si j'suis pas sur l'terrain, j'suis dans le stud' J'suis pas sur l'terrain, j'suis dans le stud' Pendant qu'tu perds ton temps, nous, on fait partir l'taga J'rappe pour ceux qui coffrent l'argent sale et dépensent rien pour ces tiaga J'marche dans l'tieks avec les gavas, j'vais recharger ma Lebara J'rappe pour ceux qui cricket la journée, le soir, ils vont chouara J'casse la vitre de ta tchop, pour 24 carats Y a mon négro qui m'assiste, y a les chickens, crie Arah Ils ont même pas d'deux roues, dans leurs textes, ils parlent de casques Arai Hier, t'étais mon reuf, aujourd'hui, j'te vois même plus pareil J'aime faire des billets, j'aime quand ça rentre J'aime les étaler sur la table Moi mon pire ennemi c'est la taule Mon meilleur ami c'est les tales Et vu qu'ils vont pas ensemble, tous les jours les keufs se lèvent tôt C'est donc ça la loi du ghetto, qu'à péter des kilos pour venir soulever J'ai les bras à Popeye Pour gagner des tales, moi je perds mon sommeil On baraude dans la ville, des délits on commet Et tous les jours ça recommence, la rue, c'est pas un jeu Toi, tu joues avec la vérité Avec mes gars, on vi-sser des shlags everyday On rentre chez nous une fois qu'la bonbonne est vidée Après minuit, mes négros ont des sales idées Pendant qu'tu perds ton temps, nous, on fait partir l'taga J'rappe pour ceux qui coffrent l'argent sale et dépensent rien pour ces tiaga J'marche dans l'tieks avec les gavas, j'vais recharger ma Lebara J'rappe pour ceux qui cricket la journée, le soir, ils vont chouara J'casse la vitre de ta tchop, pour 24 carats Y a mon négro qui m'assiste, y a les chickens, crie Arah Ils ont même pas d'deux roues, dans leurs textes, ils parlent de casques Arai Hier, t'étais mon reuf, aujourd'hui, j'te vois même plus pareil Binks Beatz</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>11-0-1 Pas content quand jentends les sirènes, jpréfère entendre la sonnerie du bigo Debout avant que le jour se lève quand il s'agit de remplir mon frigo T'inquiète pas, en cas d'problème, y a tout c'quil faut, si on s'énerve trop, on passera aux infos T'as donné ton cur à une donneuse de go, t'es trop con, maintenant, assume tes fautes J'espère que t'as de l'argent de té-cô, tu sais qu'tu va khalass si la bonbonne, elle saute Dans ma tê-te, c'est trop ghetto, j'suis pas encore prêt à faire des sons commerciaux Qualité Netflix, toujours en immersion, on a pris tes affaires, on n'a pas dit merci Pendant l'audition, obligé d'changer d'version, tu me connais zéro déclaration Suffit d'une descente et on augmente le ratio, on s'bagarre avec toutes les générations Comme d'hab', maman s'inquiète pour son fiston, cagoule, gants, jsuis toujours dans laction Comme d'hab', tous les jours, jminquiète pour mon bifton donc si y a rien à faire, on monte sur un coup Comme dhab', tous les jours, il faut que le biz' tourne, lÉtat veut nous la mettre alors on baise tout salope Mes négros sont sans pitié comme la juge cette pute, elle veut pas nous voir manger Faut remplir ses poches sans remplir son casier, jallais voler, jrevendais à prix cassé Cest la loi du plus calibré, y a zéro démocratie Jsuis dans ma bulle, jcalcule pas ces ptites crasseuses, zéro sous-métier, lguetteur dédicacé La bibi, la bibi, mes gars sont bons quà ça, jconnais pas lRSA, jconnais pas les rées-soi Noyé dans linsomnie, jai des mauvais souvenirs, quand mes négros sénervent, vaut mieux rester chez soi Des me-cri jai commis, tu me connais, jai pas perdu la foi La victime qui agonise, jai oublié sa tête, jme rappelle de sa voix La bibi, la bibi, mes gars sont bons quà ça, j'connais pas lRSA, jconnais pas les rées-soi Jmenfonce dans linsomnie, jai des mauvais souvenirs, quand mes négros sénervent, vaut mieux rester chez soi Des me-cri jai commis, tu me connais, jai pas perdu la foi La victime qui agonise, jai oublié sa tête, jme rappelle de sa voix You might also like Jmets des disquettes même à lavocat, plutôt mourir que ouvrir la boca Jai activé mon flow, jrentre dans la bine-ca, sans pitié, ça thagar devant ta pine-co Johnny a allumé le fuego, jsuis venu allumer ces faux gars Jsuis dans le trafic, jrate pas mon service comme Wilfried Tsonga Linstru', jla piétine, nan, cest pas drôle de revendre la drogua À 15 ans, Marie-Jeanne ma dragué, jcrois quelle veut pas mlâcher, regarde le résultat Cest ton frérot mais tenvoies zéro mandat, y a pas que les chicken qui peuvent tamender Jtire un missile téléguidé, si jtenlève ton âme, jespère que Dieu me guidera Un an qujsuis dans lpe-ra, ça fait déjà trop longtemps, jsais que jaurais des regrets si demain, jmonte au ciel Le présent est précieux, le futur, incertain, jai à peine commencé et tu sens lpotentiel Tu sais qujme suis fait seul, jesquive le mauvais il, en quête dargent facile d'argent facile, d'argent facile Les flammes dici-bas ne sont que des étincelles des étincelles, des étincelles Même si tas vidé la Poliaka, igo, tes pas un dur On peut taper ton crâne comme une piñata, tu prends lmicro mais tas rien à dire En temps dguerre, y a des mes-ar dans la nature, jbig up mes vrais négros, jbig up le manager Avec paire de requins, jai appris à nager Y a des Camelia, y a des Fatoumata Jtabasse toutes les prods jusquà quils retiennent mon nom Jfais ça en deu-spi, après ça jretourne dans lombre 9-2-1-4-0 sur le pocheton, jy vais à mains nues, jdégaine s'ils sont en nombre Jdégaine s'ils sont en nombre Y a des Camelia, y a des Fatoumata</t>
+          <t>11-0-1 Pas content quand jentends les sirènes, jpréfère entendre la sonnerie du bigo Debout avant que le jour se lève quand il s'agit de remplir mon frigo T'inquiète pas, en cas d'problème, y a tout c'quil faut, si on s'énerve trop, on passera aux infos T'as donné ton cur à une donneuse de go, t'es trop con, maintenant, assume tes fautes J'espère que t'as de l'argent de té-cô, tu sais qu'tu va khalass si la bonbonne, elle saute Dans ma tê-te, c'est trop ghetto, j'suis pas encore prêt à faire des sons commerciaux Qualité Netflix, toujours en immersion, on a pris tes affaires, on n'a pas dit merci Pendant l'audition, obligé d'changer d'version, tu me connais zéro déclaration Suffit d'une descente et on augmente le ratio, on s'bagarre avec toutes les générations Comme d'hab', maman s'inquiète pour son fiston, cagoule, gants, jsuis toujours dans laction Comme d'hab', tous les jours, jminquiète pour mon bifton donc si y a rien à faire, on monte sur un coup Comme dhab', tous les jours, il faut que le biz' tourne, lÉtat veut nous la mettre alors on baise tout salope Mes négros sont sans pitié comme la juge cette pute, elle veut pas nous voir manger Faut remplir ses poches sans remplir son casier, jallais voler, jrevendais à prix cassé Cest la loi du plus calibré, y a zéro démocratie Jsuis dans ma bulle, jcalcule pas ces ptites crasseuses, zéro sous-métier, lguetteur dédicacé La bibi, la bibi, mes gars sont bons quà ça, jconnais pas lRSA, jconnais pas les rées-soi Noyé dans linsomnie, jai des mauvais souvenirs, quand mes négros sénervent, vaut mieux rester chez soi Des me-cri jai commis, tu me connais, jai pas perdu la foi La victime qui agonise, jai oublié sa tête, jme rappelle de sa voix La bibi, la bibi, mes gars sont bons quà ça, j'connais pas lRSA, jconnais pas les rées-soi Jmenfonce dans linsomnie, jai des mauvais souvenirs, quand mes négros sénervent, vaut mieux rester chez soi Des me-cri jai commis, tu me connais, jai pas perdu la foi La victime qui agonise, jai oublié sa tête, jme rappelle de sa voix Jmets des disquettes même à lavocat, plutôt mourir que ouvrir la boca Jai activé mon flow, jrentre dans la bine-ca, sans pitié, ça thagar devant ta pine-co Johnny a allumé le fuego, jsuis venu allumer ces faux gars Jsuis dans le trafic, jrate pas mon service comme Wilfried Tsonga Linstru', jla piétine, nan, cest pas drôle de revendre la drogua À 15 ans, Marie-Jeanne ma dragué, jcrois quelle veut pas mlâcher, regarde le résultat Cest ton frérot mais tenvoies zéro mandat, y a pas que les chicken qui peuvent tamender Jtire un missile téléguidé, si jtenlève ton âme, jespère que Dieu me guidera Un an qujsuis dans lpe-ra, ça fait déjà trop longtemps, jsais que jaurais des regrets si demain, jmonte au ciel Le présent est précieux, le futur, incertain, jai à peine commencé et tu sens lpotentiel Tu sais qujme suis fait seul, jesquive le mauvais il, en quête dargent facile d'argent facile, d'argent facile Les flammes dici-bas ne sont que des étincelles des étincelles, des étincelles Même si tas vidé la Poliaka, igo, tes pas un dur On peut taper ton crâne comme une piñata, tu prends lmicro mais tas rien à dire En temps dguerre, y a des mes-ar dans la nature, jbig up mes vrais négros, jbig up le manager Avec paire de requins, jai appris à nager Y a des Camelia, y a des Fatoumata Jtabasse toutes les prods jusquà quils retiennent mon nom Jfais ça en deu-spi, après ça jretourne dans lombre 9-2-1-4-0 sur le pocheton, jy vais à mains nues, jdégaine s'ils sont en nombre Jdégaine s'ils sont en nombre Y a des Camelia, y a des Fatoumata</t>
         </is>
       </c>
     </row>
@@ -854,7 +854,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Binks Beatz J'suis dans ta soirée mais j'suis pas venu danser Le premier ient-cli, j'l'ai ambiancé On remplit les demi, pas besoin des gants renforcés Pilon d'beuh, le mélange est corsé Après l'agression, tes négros bouleversés Le sang, ils ont versé C'est des ients-cli, les rôles, ils ont inversé En vérité, le pilon, il vient t'chercher Rallume la lumière d'la cave, j'vois même plus les chiffres sur la pesette Transaction, j'm'en ballek qu'les voisins me guettent Fais attention à qui tu veux hasba un kil' J'suis pisté avant d'rentrer, j'fais l'tour de la ville J'vois les tits-pe qui s'perdent dans le vol Et j'oublie pas les gants, faut éviter la taule Si t'as pookie, on te fait des hématomes Eux, ils font les fous, mais bon, c'est des amateurs Y a un plan sous, j'me suis levé tôt le matin On l'croise solo, il s'met à parler latin J'viens d'me réveiller, y'a un ient-cli qui m'attend J'suis rentré dans l'pe-ra en dérapant Rentre chez nous et tu repars en boîtant J'veux pas d'love, moi j'veux des chaînes en diamant La frappe arrive, le criquet attend patiemment J'ai suivi l'mauvais chemin inconsciemment Avant d'dormir, j'pense à la mort J'm'en ballek que ta racli, elle pense à moi Les keufs, ils appellent les renforts salope Dans l'équipe, personne qui parle chinois Perquisition, fallait rien laisser chez toi Et mon argent est sale, il faut que j'le nettoie J'te visser d'la frappe, tu fumes, tu deviens ché-tou You might also like Pour des raclis, les négros ils deviennent chelous Les ients-cli défilent, j'suis obligé d'enchaîner Et j'suis conscient qu'les condés, ils veulent m'enfermer Ils veulent mettre mon argent sous scellé Dans la cave, la plaquette est sous céllo' Ces rappeurs ils sont bons qu'à sucer mon flow Normal tu bouges la tête sur la mélo J'suis sur le terrain à midi, j'fais le sale boulot Pour des raclis, les négros ils deviennent chelous Les ients-cli défilent, j'suis obligé d'enchaîner Et j'suis conscient qu'les condés, ils veulent m'enfermer Ils veulent mettre mon argent sous scellé Dans la cave, la plaquette est sous céllo' Ces rappeurs ils sont bons qu'à sucer mon flow Normal tu bouges la tête sur la mélo J'suis sur le terrain à midi, j'fais le sale boulot Ici les cliquos on reconnaît Une dix ou une vingt ? Dis-moi tu veux quoi J'rappe pour les négros qui détaillent dans la ve-ca J'ai même pas commencé, et elle en veut encore J'entends la portière, normal que j'm'évapore La bicrave ou le vol, j'suis dans tout c'qui rapporte J'rappe pour le ghetto, qui fait des guêt-appens J'rappe pour les charbonneurs, prêts à midi tapant Les keufs, ils sont chauds, ils veulent nous mettre des tapages Et quand ils nous coursent, ils veulent nous mettent des plaquages Oublie pas que dans ce monde on est que d'passage J'ai le mort la que-ba, elle fait que de passer J'rappe pour ceux qui tartinent ensemble Lacosté Quand tu gères une meuf, pas besoin de l'accoster L'ennemi il a chaud, il veut pas riposter J'm'éloigne des hypocrites et des imposteurs Y a même des mecs qui viennent pécho en costard 9.2.1.4.0 sur le pochetard Ça m'appelle vers Paname alors ce soir j'rentre tard J'voulais pas qu'les keufs ils connaissent ma ronne-da S'il y a embrouille, bah on sort une armada, eh Tout d'un coup ces négros deviennent doux Pour niquer des instrus, t'inquiète pas que je suis dou-é J'ai pas b'soin d'un marabout Pour des raclis, les négros ils deviennent chelous Les ients-cli défilent, j'suis obligé d'enchaîner Et j'suis conscient qu'les condés, ils veulent m'enfermer Ils veulent mettre mon argent sous scellé Dans la cave, la plaquette est sous céllo' Ces rappeurs ils sont bons qu'à sucer mon flow Normal tu bouges la tête sur la mélo J'suis sur le terrain à midi, j'fais le sale boulot Pour des raclis, les négros ils deviennent chelous Les ients-cli défilent, j'suis obligé d'enchaîner Et j'suis conscient qu'les condés, ils veulent m'enfermer Ils veulent mettre mon argent sous scellé Dans la cave, la plaquette est sous céllo' Ces rappeurs ils sont bons qu'à sucer mon flow Normal tu bouges la tête sur la mélo J'suis sur le terrain à midi, j'fais le sale boulot</t>
+          <t>Binks Beatz J'suis dans ta soirée mais j'suis pas venu danser Le premier ient-cli, j'l'ai ambiancé On remplit les demi, pas besoin des gants renforcés Pilon d'beuh, le mélange est corsé Après l'agression, tes négros bouleversés Le sang, ils ont versé C'est des ients-cli, les rôles, ils ont inversé En vérité, le pilon, il vient t'chercher Rallume la lumière d'la cave, j'vois même plus les chiffres sur la pesette Transaction, j'm'en ballek qu'les voisins me guettent Fais attention à qui tu veux hasba un kil' J'suis pisté avant d'rentrer, j'fais l'tour de la ville J'vois les tits-pe qui s'perdent dans le vol Et j'oublie pas les gants, faut éviter la taule Si t'as pookie, on te fait des hématomes Eux, ils font les fous, mais bon, c'est des amateurs Y a un plan sous, j'me suis levé tôt le matin On l'croise solo, il s'met à parler latin J'viens d'me réveiller, y'a un ient-cli qui m'attend J'suis rentré dans l'pe-ra en dérapant Rentre chez nous et tu repars en boîtant J'veux pas d'love, moi j'veux des chaînes en diamant La frappe arrive, le criquet attend patiemment J'ai suivi l'mauvais chemin inconsciemment Avant d'dormir, j'pense à la mort J'm'en ballek que ta racli, elle pense à moi Les keufs, ils appellent les renforts salope Dans l'équipe, personne qui parle chinois Perquisition, fallait rien laisser chez toi Et mon argent est sale, il faut que j'le nettoie J'te visser d'la frappe, tu fumes, tu deviens ché-tou Pour des raclis, les négros ils deviennent chelous Les ients-cli défilent, j'suis obligé d'enchaîner Et j'suis conscient qu'les condés, ils veulent m'enfermer Ils veulent mettre mon argent sous scellé Dans la cave, la plaquette est sous céllo' Ces rappeurs ils sont bons qu'à sucer mon flow Normal tu bouges la tête sur la mélo J'suis sur le terrain à midi, j'fais le sale boulot Pour des raclis, les négros ils deviennent chelous Les ients-cli défilent, j'suis obligé d'enchaîner Et j'suis conscient qu'les condés, ils veulent m'enfermer Ils veulent mettre mon argent sous scellé Dans la cave, la plaquette est sous céllo' Ces rappeurs ils sont bons qu'à sucer mon flow Normal tu bouges la tête sur la mélo J'suis sur le terrain à midi, j'fais le sale boulot Ici les cliquos on reconnaît Une dix ou une vingt ? Dis-moi tu veux quoi J'rappe pour les négros qui détaillent dans la ve-ca J'ai même pas commencé, et elle en veut encore J'entends la portière, normal que j'm'évapore La bicrave ou le vol, j'suis dans tout c'qui rapporte J'rappe pour le ghetto, qui fait des guêt-appens J'rappe pour les charbonneurs, prêts à midi tapant Les keufs, ils sont chauds, ils veulent nous mettre des tapages Et quand ils nous coursent, ils veulent nous mettent des plaquages Oublie pas que dans ce monde on est que d'passage J'ai le mort la que-ba, elle fait que de passer J'rappe pour ceux qui tartinent ensemble Lacosté Quand tu gères une meuf, pas besoin de l'accoster L'ennemi il a chaud, il veut pas riposter J'm'éloigne des hypocrites et des imposteurs Y a même des mecs qui viennent pécho en costard 9.2.1.4.0 sur le pochetard Ça m'appelle vers Paname alors ce soir j'rentre tard J'voulais pas qu'les keufs ils connaissent ma ronne-da S'il y a embrouille, bah on sort une armada, eh Tout d'un coup ces négros deviennent doux Pour niquer des instrus, t'inquiète pas que je suis dou-é J'ai pas b'soin d'un marabout Pour des raclis, les négros ils deviennent chelous Les ients-cli défilent, j'suis obligé d'enchaîner Et j'suis conscient qu'les condés, ils veulent m'enfermer Ils veulent mettre mon argent sous scellé Dans la cave, la plaquette est sous céllo' Ces rappeurs ils sont bons qu'à sucer mon flow Normal tu bouges la tête sur la mélo J'suis sur le terrain à midi, j'fais le sale boulot Pour des raclis, les négros ils deviennent chelous Les ients-cli défilent, j'suis obligé d'enchaîner Et j'suis conscient qu'les condés, ils veulent m'enfermer Ils veulent mettre mon argent sous scellé Dans la cave, la plaquette est sous céllo' Ces rappeurs ils sont bons qu'à sucer mon flow Normal tu bouges la tête sur la mélo J'suis sur le terrain à midi, j'fais le sale boulot</t>
         </is>
       </c>
     </row>
@@ -871,7 +871,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Descente de shtars donc je file Y a un plavon, j'enfile les gants, jamais j'défile J'mets la pote-ca, j'suis pas prêt d'avoir un fils J'suis dans l'ghetto à la recherche du fric Plus j'me lève tôt, plus j'augmente le bénéfice Au début d'la journée, le que-sa est rempli J'écris mon texte, j'attends le prochain ient-cli Quand y a embrouille, y a tout l'monde qui s'équipe P't-être qu'ils sont massifs dans leurs clips Mais quand y a drah, y a tout l'monde qui s'éclipse Si tu poucaves, tu quittes le tieks sans revenir J'suis vé-nèr' quand l'ennemi, il a peur de venir Ça vient d'où ? Tu veux quoi ? Non, y a pas d'bienvenue T'étais un bon, regarde comment t'es devenu Les tes-shmi, ils font que de passer devant nous Ils font les chauds donc c'est normal qu'on les allume Les vrai négros qui font des sous, j'passe un salam Pour ceux qui guent-lar la BAC en f'sant des slaloms Y a un mec à faire, dans le quartier, chasse à l'homme Même s'ils sont armés, moi, j'sais qu'c'est des salopes Je perds pas mon temps, il est temps d'péter skalape J'fais couler le sang, tu fais couler l'mascara J'ai v-esqui' la que-ba, bon débarras Pour soul'ver tes litrons, pas besoin d'taffer les bras J'ai v'là les ients-cli sur ma ce-pu Lebara Si t'es un loss-bo, j'augmente le taro J'veux pas finir derrière les barreaux Si tu veux nous rotte-ca, c'est normal qu'on t'arrose J'viens kicker l'instru', dans le pe-ra, je m'impose Les keufs prennent des photos, j'vais pas taper la pose Détaille la moula, le te-shi se décompose Les bacqueux ils descendent, le bosseur quitte son poste J'suis un vrai laud-sa, j'pourrais pas trahir mon pote J'traîne dans la street à la recherche du jackpot Faut brasser des thunes à mort sans ber-tom Est-ce que t'es capable ? Calcule pas les meufs, c'est des catins J'rentre, j'pose une kichta sur la table Enchaîner plavons, dans l'tier-quar, fais pas mé-cra J'ai pas changé, batârd, j'fais pas d'me-chro J'fais que d'visser, tu m'as vu dans le métro Le clicos, il a fait un bad trip Tu bes-tom si dans le joint, t'en mets trop Si dans le joint, t'en mets trop T'es tombé amoureux d'une sale tain-p' On te nique ta mère si t'es une sale taupe salope Pas besoin d'avoir un flingue, devant l'Opinel, t'enlevais toutes tes fringues Parle pas mé-cra sur mon téléphone Cette pute veut rentrer dans ma vie, j'crois qu'elle est folle Côté Chicago, on t'hagar ton téléphone Mon réveil, c'est quand l'bigo, il sonne brr Les keufs, ils font que d'nous pister donc avant d'rentrer brr, j'fais l'tour de la zone J'suis prêt à serrer ton cou pour des sommes Ils ont pas les couilles, mais bon, ils s'prennent pour des hommes Dans tous les cas, y a qu'les billets qui m'soulagent Eux, ils font les gros, quand y a embrouille, personne agit J'ai tout nié, j'ressors de la GAV C'est des salopes, ils sont passés aux aveux J'sors la bonbonne et le ient-cli fait un vu J'rentre dans ta soirée, même si j'ai pas eu d'invit' À la fin d'la guenda, la bonbonne, elle est vide paw, paw Au quartier les keufs, ils nous espionnent par la vitre You might also like La nuit y a les chickens, v-esqui' la batman Si y a embrouille, mes négros déboulent en balle Sur l'tél,' un ient-cli, en deuspi, je m'habille Ça t'pull up ta mère, s'en fout d'comment tu t'appelles Est-ce que le lendemain, tu t'en rappelles ? Quand il faut chouara, fais les dièses en rapide Si tu veux per-cho, faut sortir le liquide Tu veux quelque chose, faut sortir le liquide La nuit y a les chickens, v-esqui' la batman Si y a embrouille, mes négros déboulent en balle Sur l'tél,' un ient-cli, en deuspi, je m'habille Ça t'pull up ta mère, s'en fout d'comment tu t'appelles Est-ce que le lendemain, tu t'en rappelles ? Quand il faut chouara, fais les dièses en rapide Si tu veux per-cho, faut sortir le liquide Tu veux quelque chose, faut sortir le liquide 9.2.1.4.0 sur le pochton pow, on écrase ta tête sur le béton pow Le bosseur, il enchaîne la troisième mi-temps pow, non, il a pas peur de ber-tom nan C'est pas pour rien qu'on s'est levés tôt, j'ai le M sur le front, comme Végéta J'ai toujours envie d'baiser l'état pow et les caméras, faut qu'on les casse pow J'prends un billet pow, et puis j'me casse brr 9.2.1.4.0 sur le pochton brr, y a que la ville que j'dédicace y a que la ville que j'dédicace Et les caméras, faut qu'on les casse J'prends un billet, et puis j'me casse La nuit y a les chickens, v-esqui' la batman Si y a embrouille, mes négros déboulent en balle Sur l'tél,' un ient-cli, en deuspi, je m'habille Ça t'pull up ta mère, s'en fout d'comment tu t'appelles Est-ce que le lendemain, tu t'en rappelles ? Quand il faut chouara, fais les dièses en rapide Si tu veux per-cho, faut sortir le liquide Tu veux quelque chose, faut sortir le liquide La nuit y a les chickens, v-esqui' la batman Si y a embrouille, mes négros déboulent en balle Sur l'tél,' un ient-cli, en deuspi, je m'habille Ça t'pull up ta mère, s'en fout d'comment tu t'appelles Est-ce que le lendemain, tu t'en rappelles ? Quand il faut chouara, fais les dièses en rapide Si tu veux per-cho, faut sortir le liquide Tu veux quelque chose, faut sortir le liquide3</t>
+          <t>Descente de shtars donc je file Y a un plavon, j'enfile les gants, jamais j'défile J'mets la pote-ca, j'suis pas prêt d'avoir un fils J'suis dans l'ghetto à la recherche du fric Plus j'me lève tôt, plus j'augmente le bénéfice Au début d'la journée, le que-sa est rempli J'écris mon texte, j'attends le prochain ient-cli Quand y a embrouille, y a tout l'monde qui s'équipe P't-être qu'ils sont massifs dans leurs clips Mais quand y a drah, y a tout l'monde qui s'éclipse Si tu poucaves, tu quittes le tieks sans revenir J'suis vé-nèr' quand l'ennemi, il a peur de venir Ça vient d'où ? Tu veux quoi ? Non, y a pas d'bienvenue T'étais un bon, regarde comment t'es devenu Les tes-shmi, ils font que de passer devant nous Ils font les chauds donc c'est normal qu'on les allume Les vrai négros qui font des sous, j'passe un salam Pour ceux qui guent-lar la BAC en f'sant des slaloms Y a un mec à faire, dans le quartier, chasse à l'homme Même s'ils sont armés, moi, j'sais qu'c'est des salopes Je perds pas mon temps, il est temps d'péter skalape J'fais couler le sang, tu fais couler l'mascara J'ai v-esqui' la que-ba, bon débarras Pour soul'ver tes litrons, pas besoin d'taffer les bras J'ai v'là les ients-cli sur ma ce-pu Lebara Si t'es un loss-bo, j'augmente le taro J'veux pas finir derrière les barreaux Si tu veux nous rotte-ca, c'est normal qu'on t'arrose J'viens kicker l'instru', dans le pe-ra, je m'impose Les keufs prennent des photos, j'vais pas taper la pose Détaille la moula, le te-shi se décompose Les bacqueux ils descendent, le bosseur quitte son poste J'suis un vrai laud-sa, j'pourrais pas trahir mon pote J'traîne dans la street à la recherche du jackpot Faut brasser des thunes à mort sans ber-tom Est-ce que t'es capable ? Calcule pas les meufs, c'est des catins J'rentre, j'pose une kichta sur la table Enchaîner plavons, dans l'tier-quar, fais pas mé-cra J'ai pas changé, batârd, j'fais pas d'me-chro J'fais que d'visser, tu m'as vu dans le métro Le clicos, il a fait un bad trip Tu bes-tom si dans le joint, t'en mets trop Si dans le joint, t'en mets trop T'es tombé amoureux d'une sale tain-p' On te nique ta mère si t'es une sale taupe salope Pas besoin d'avoir un flingue, devant l'Opinel, t'enlevais toutes tes fringues Parle pas mé-cra sur mon téléphone Cette pute veut rentrer dans ma vie, j'crois qu'elle est folle Côté Chicago, on t'hagar ton téléphone Mon réveil, c'est quand l'bigo, il sonne brr Les keufs, ils font que d'nous pister donc avant d'rentrer brr, j'fais l'tour de la zone J'suis prêt à serrer ton cou pour des sommes Ils ont pas les couilles, mais bon, ils s'prennent pour des hommes Dans tous les cas, y a qu'les billets qui m'soulagent Eux, ils font les gros, quand y a embrouille, personne agit J'ai tout nié, j'ressors de la GAV C'est des salopes, ils sont passés aux aveux J'sors la bonbonne et le ient-cli fait un vu J'rentre dans ta soirée, même si j'ai pas eu d'invit' À la fin d'la guenda, la bonbonne, elle est vide paw, paw Au quartier les keufs, ils nous espionnent par la vitre La nuit y a les chickens, v-esqui' la batman Si y a embrouille, mes négros déboulent en balle Sur l'tél,' un ient-cli, en deuspi, je m'habille Ça t'pull up ta mère, s'en fout d'comment tu t'appelles Est-ce que le lendemain, tu t'en rappelles ? Quand il faut chouara, fais les dièses en rapide Si tu veux per-cho, faut sortir le liquide Tu veux quelque chose, faut sortir le liquide La nuit y a les chickens, v-esqui' la batman Si y a embrouille, mes négros déboulent en balle Sur l'tél,' un ient-cli, en deuspi, je m'habille Ça t'pull up ta mère, s'en fout d'comment tu t'appelles Est-ce que le lendemain, tu t'en rappelles ? Quand il faut chouara, fais les dièses en rapide Si tu veux per-cho, faut sortir le liquide Tu veux quelque chose, faut sortir le liquide 9.2.1.4.0 sur le pochton pow, on écrase ta tête sur le béton pow Le bosseur, il enchaîne la troisième mi-temps pow, non, il a pas peur de ber-tom nan C'est pas pour rien qu'on s'est levés tôt, j'ai le M sur le front, comme Végéta J'ai toujours envie d'baiser l'état pow et les caméras, faut qu'on les casse pow J'prends un billet pow, et puis j'me casse brr 9.2.1.4.0 sur le pochton brr, y a que la ville que j'dédicace y a que la ville que j'dédicace Et les caméras, faut qu'on les casse J'prends un billet, et puis j'me casse La nuit y a les chickens, v-esqui' la batman Si y a embrouille, mes négros déboulent en balle Sur l'tél,' un ient-cli, en deuspi, je m'habille Ça t'pull up ta mère, s'en fout d'comment tu t'appelles Est-ce que le lendemain, tu t'en rappelles ? Quand il faut chouara, fais les dièses en rapide Si tu veux per-cho, faut sortir le liquide Tu veux quelque chose, faut sortir le liquide La nuit y a les chickens, v-esqui' la batman Si y a embrouille, mes négros déboulent en balle Sur l'tél,' un ient-cli, en deuspi, je m'habille Ça t'pull up ta mère, s'en fout d'comment tu t'appelles Est-ce que le lendemain, tu t'en rappelles ? Quand il faut chouara, fais les dièses en rapide Si tu veux per-cho, faut sortir le liquide Tu veux quelque chose, faut sortir le liquide3</t>
         </is>
       </c>
     </row>
@@ -888,7 +888,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>N'oublie pas que ce monde est éphémère han, que tu finis tout seul quand ca dégénère han Quand la mort arrive obligé d'te laisser faire ah bon ?, le charbon nous a laissé grave des cernes ah bon ? T'es bosseur à vie y'a pas d'intérimaires baw, j'en connais qui ont pris d'la prison ferme baw Tournent depuis des années des peines interminables baw, sur le droit chemin se trouve l'itinéraire baw, baw On garde la foi mais on reste vulnérabls, pour passer d'l'autre côté, il suffit d'une rreur baw On vit pour l'argent, on s'tue pour des dineros, tous les jours que Dieu fait essaye d'être le meilleur brr En vrai j'suis pas mieux qu'toi, j'ai trop glorifié le mal sous le feu des projecteurs brr Tu veux avancer parle pas des projets qu't'as brr, peuvent-ils m'arrêter avec une telle trajectoire ? brr, brr Si t'es encore en vie, la balle est dans ton camp han, parfois j'me demande han Si j'vais pouvoir m'arrêter juste à temps ? ah bon ? J'vais charbonner jusqu'à quand ? ah bon ? Charbonner jusqu'à quand ? mmh Parfois j'me demande mmh Si j'vais pouvoir m'arrêter juste à temps ? mmh, mmh Si t'es encore en vie, la balle est dans ton camp han, parfois j'me demande han Si j'vais pouvoir m'arrêter juste à temps ? ah bon ? J'vais charbonner jusqu'à quand ? ah bon ? Charbonner jusqu'à quand ? mmh Parfois j'me demande mmh Si j'vais pouvoir m'arrêter juste à temps ? mmh M'arrêter juste à temps mmh Et à chaque fois qu'on perd un proche baw, souvent on se demande c'est qui le prochain ? baw Au lieu d'se repentir et d'faire les bons choix woo, je n'pense qu'à mes poches woo Dans mon quartier c'est pas la joie, tu nous vois sourire seulement si on empoche Les p'tits appellent le bonheur, ça raccroche, pour ça qu'ils tiennent la sacoche baw L'ange de droite parle moins fort que l'ange de gauche, mes péchés font des ricochets baw Sur l'terrain sous pilon, souvent je cogite brr, j'repense à ce monde hypocrite brr Le client veut remplir son cochi woo, la te-pu veut remplir sa pussy woo Le gérant doit remplir le sac aussi woo, le bosseur fait partir le plus possible woo You might also like Si t'es encore en vie, la balle est dans ton camp han, parfois j'me demande han Si j'vais pouvoir m'arrêter juste à temps ? ah bon ? J'vais charbonner jusqu'à quand ? ah bon ? Charbonner jusqu'à quand ? mmh Parfois j'me demande mmh Si j'vais pouvoir m'arrêter juste à temps ? mmh, mmh Si t'es encore en vie, la balle est dans ton camp han, parfois j'me demande han Si j'vais pouvoir m'arrêter juste à temps ? ah bon ? J'vais charbonner jusqu'à quand ? ah bon ? Charbonner jusqu'à quand ? mmh Parfois j'me demande mmh Si j'vais pouvoir m'arrêter juste à temps ? mmh M'arrêter juste à temps temps, temps, temps</t>
+          <t>N'oublie pas que ce monde est éphémère han, que tu finis tout seul quand ca dégénère han Quand la mort arrive obligé d'te laisser faire ah bon ?, le charbon nous a laissé grave des cernes ah bon ? T'es bosseur à vie y'a pas d'intérimaires baw, j'en connais qui ont pris d'la prison ferme baw Tournent depuis des années des peines interminables baw, sur le droit chemin se trouve l'itinéraire baw, baw On garde la foi mais on reste vulnérabls, pour passer d'l'autre côté, il suffit d'une rreur baw On vit pour l'argent, on s'tue pour des dineros, tous les jours que Dieu fait essaye d'être le meilleur brr En vrai j'suis pas mieux qu'toi, j'ai trop glorifié le mal sous le feu des projecteurs brr Tu veux avancer parle pas des projets qu't'as brr, peuvent-ils m'arrêter avec une telle trajectoire ? brr, brr Si t'es encore en vie, la balle est dans ton camp han, parfois j'me demande han Si j'vais pouvoir m'arrêter juste à temps ? ah bon ? J'vais charbonner jusqu'à quand ? ah bon ? Charbonner jusqu'à quand ? mmh Parfois j'me demande mmh Si j'vais pouvoir m'arrêter juste à temps ? mmh, mmh Si t'es encore en vie, la balle est dans ton camp han, parfois j'me demande han Si j'vais pouvoir m'arrêter juste à temps ? ah bon ? J'vais charbonner jusqu'à quand ? ah bon ? Charbonner jusqu'à quand ? mmh Parfois j'me demande mmh Si j'vais pouvoir m'arrêter juste à temps ? mmh M'arrêter juste à temps mmh Et à chaque fois qu'on perd un proche baw, souvent on se demande c'est qui le prochain ? baw Au lieu d'se repentir et d'faire les bons choix woo, je n'pense qu'à mes poches woo Dans mon quartier c'est pas la joie, tu nous vois sourire seulement si on empoche Les p'tits appellent le bonheur, ça raccroche, pour ça qu'ils tiennent la sacoche baw L'ange de droite parle moins fort que l'ange de gauche, mes péchés font des ricochets baw Sur l'terrain sous pilon, souvent je cogite brr, j'repense à ce monde hypocrite brr Le client veut remplir son cochi woo, la te-pu veut remplir sa pussy woo Le gérant doit remplir le sac aussi woo, le bosseur fait partir le plus possible woo Si t'es encore en vie, la balle est dans ton camp han, parfois j'me demande han Si j'vais pouvoir m'arrêter juste à temps ? ah bon ? J'vais charbonner jusqu'à quand ? ah bon ? Charbonner jusqu'à quand ? mmh Parfois j'me demande mmh Si j'vais pouvoir m'arrêter juste à temps ? mmh, mmh Si t'es encore en vie, la balle est dans ton camp han, parfois j'me demande han Si j'vais pouvoir m'arrêter juste à temps ? ah bon ? J'vais charbonner jusqu'à quand ? ah bon ? Charbonner jusqu'à quand ? mmh Parfois j'me demande mmh Si j'vais pouvoir m'arrêter juste à temps ? mmh M'arrêter juste à temps temps, temps, temps</t>
         </is>
       </c>
     </row>
@@ -905,7 +905,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>This some plus four shit I-I-I-I love Chris Rich Ça t'envoie une équipe comme Sosa, le numéro d'ta porte peut régler mes soucis ah bon ? On a fait des sous sales enfermés dans nos blocs mais on veut s'en sortir ah bon ? Il est jamais trop tard pour s'repentir, pour te piétiner, j'ai la paire assortie poh Ils parlent d'embrouille mais ils sont pas dedans poh, tu dois des sous comment veux-tu qu'j'sois gentil ? Ennemis à l'hosto, j'tape mon dernier pas de danse, j'vais trop vite pour eux, il faut que j'ralentisse brr Pour ces putains, j'ai zéro galanterie, tu t'mets en mala, tu t'fais recal' à l'entrée brr Sur le terrain y a zéro plaisanterie, les keufs viennent de tout-par faut qu'tu restes concentré On sait faire des sous, on sait pas faire semblant et tous ces flocos, ils veulent nous ressembler han Y a un plan argent, on sait pas faire sans gants, suffit d'une minute, la concu' j'la fait trembler poh T'as pas un rond mais tu gratte des pains dans la rue, comment tu veux avancer sans blé poh ? Toujours des mes-ar en cas de pépin, que tu sois seul ou bien rassemblé eh Du comico je ressors innocenté, tu dis qu'c'est d'la frappe mais j'l'ai pas sentie eh Tout c'que j'fais c'est niquer ma santé, je sais que j'vais regretter juste avant de partir poh Si tu rentres en guerre avec mon équipe, igo, jamais tu t'en tires poh On visser on v'-esqui les tantines, j'ai jamais cru qu'j'allais faire ça étant p'tit Un TMax, une visière qui déboule un jeudi, après ça, c'est les coups d'feu qui retentissent Y a l'Opinel 12 si ils déboulent à 6, 9.2.1.4.0, tu sais qu'on maîtrise Quand un reuf bé-tom tu sais bien qu'on est tristes Les poucaves et les tres-traî, j'ai fait le tri Les tarifs sont fixés, les barrettes sont pesées, non tu peux pas marchander le prix Trop têtu, personne peut me commander donc tu peux pas contrôler mon esprit han You might also like Pour ma gue-dro, t'as succombé, j'ai vu des mecs tomber, jamais se relever mmh Couteau dans l'dos, j'le mets à tout l'monde sauf à mes res-fré mmh Trop souvent, j'oublie les refrains, comme mes sous, mes sentiments, j'les ai coffrés Hors-la-loi donc toutes les règles, on enfreint, normal que les chickens, on les effraie Sur la route du succès, j'avance prudemment, j'roule à fond c'est normal si j'me prends des amendes eh La vraie vie, c'est après la mort, si j'le fais, c'est pour les sous, j'veux pas qu'on m'adore eh Trop têtu, y a personne pour m'commander, les prix sont fixés, tu peux pas marchander poh J'détaille précis, les barrettes sont pesées poh, hmm, regarde comment je fais poh, poh Sur la route du succès, j'avance prudemment, j'roule à fond c'est normal si j'me prends des amendes eh La vraie vie, c'est après la mort, si j'le fais, c'est pour les sous, j'veux pas qu'on m'adore eh Trop têtu, y a personne pour m'commander, les prix sont fixés, tu peux pas marchander poh J'détaille précis, les barrettes sont pesées poh, hmm, regarde comment je fais poh, poh Ne te pose pas trop d'questions quand on baraude vers ton pavillon mmh Si tu veux pas payer, dans la coche-sa, y a l'couteau papillon mmh 9.2.1.4.0 sur le pocheton et encore, là, c'est juste un échantillon ah bon ? On est grave dans l'argent sale pourtant on veut éviter châtiment ah bon ? Lui il fait l'sisste-gro, j'sais qu'il ment salope, sisste-gros, j'sais qu'il ment salope J'lève un doigt au keuf qui veut mes économies, j'prends ma ce-pla dans l'pe-ra tranquillement Tranquillement, c'est qu'un freestyle, les punchlines j'les économise On a charbonné même pendant le confinement, même pendant le confinement Pour ma gue-dro, t'as succombé, j'ai vu des mecs tomber, jamais se relever eh Couteau dans l'dos, j'le mets à tout l'monde sauf à mes res-fré eh Trop souvent, j'oublie les refrains, comme mes sous, mes sentiments, j'les ai coffrés poh Hors-la-loi donc toutes les règles, on enfreint, normal que les chickens, on les effraie poh, poh Sur la route du succès, j'avance prudemment, j'roule à fond c'est normal si j'me prends des amendes eh La vraie vie, c'est après la mort, si j'le fais, c'est pour les sous, j'veux pas qu'on m'adore eh Trop têtu, y a personne pour m'commander, les prix sont fixés, tu peux pas marchander poh J'détaille précis, les barrettes sont pesées poh, hmm, regarde comment je fais poh, poh Sur la route du succès, j'avance prudemment, j'roule à fond c'est normal si j'me prends des amendes eh La vraie vie, c'est après la mort, si j'le fais, c'est pour les sous, j'veux pas qu'on m'adore eh Trop têtu, y a personne pour m'commander, les prix sont fixés, tu peux pas marchander poh J'détaille précis, les barrettes sont pesées poh, hmm, regarde comment je fais poh, poh Poh, poh, poh, poh</t>
+          <t>This some plus four shit I-I-I-I love Chris Rich Ça t'envoie une équipe comme Sosa, le numéro d'ta porte peut régler mes soucis ah bon ? On a fait des sous sales enfermés dans nos blocs mais on veut s'en sortir ah bon ? Il est jamais trop tard pour s'repentir, pour te piétiner, j'ai la paire assortie poh Ils parlent d'embrouille mais ils sont pas dedans poh, tu dois des sous comment veux-tu qu'j'sois gentil ? Ennemis à l'hosto, j'tape mon dernier pas de danse, j'vais trop vite pour eux, il faut que j'ralentisse brr Pour ces putains, j'ai zéro galanterie, tu t'mets en mala, tu t'fais recal' à l'entrée brr Sur le terrain y a zéro plaisanterie, les keufs viennent de tout-par faut qu'tu restes concentré On sait faire des sous, on sait pas faire semblant et tous ces flocos, ils veulent nous ressembler han Y a un plan argent, on sait pas faire sans gants, suffit d'une minute, la concu' j'la fait trembler poh T'as pas un rond mais tu gratte des pains dans la rue, comment tu veux avancer sans blé poh ? Toujours des mes-ar en cas de pépin, que tu sois seul ou bien rassemblé eh Du comico je ressors innocenté, tu dis qu'c'est d'la frappe mais j'l'ai pas sentie eh Tout c'que j'fais c'est niquer ma santé, je sais que j'vais regretter juste avant de partir poh Si tu rentres en guerre avec mon équipe, igo, jamais tu t'en tires poh On visser on v'-esqui les tantines, j'ai jamais cru qu'j'allais faire ça étant p'tit Un TMax, une visière qui déboule un jeudi, après ça, c'est les coups d'feu qui retentissent Y a l'Opinel 12 si ils déboulent à 6, 9.2.1.4.0, tu sais qu'on maîtrise Quand un reuf bé-tom tu sais bien qu'on est tristes Les poucaves et les tres-traî, j'ai fait le tri Les tarifs sont fixés, les barrettes sont pesées, non tu peux pas marchander le prix Trop têtu, personne peut me commander donc tu peux pas contrôler mon esprit han Pour ma gue-dro, t'as succombé, j'ai vu des mecs tomber, jamais se relever mmh Couteau dans l'dos, j'le mets à tout l'monde sauf à mes res-fré mmh Trop souvent, j'oublie les refrains, comme mes sous, mes sentiments, j'les ai coffrés Hors-la-loi donc toutes les règles, on enfreint, normal que les chickens, on les effraie Sur la route du succès, j'avance prudemment, j'roule à fond c'est normal si j'me prends des amendes eh La vraie vie, c'est après la mort, si j'le fais, c'est pour les sous, j'veux pas qu'on m'adore eh Trop têtu, y a personne pour m'commander, les prix sont fixés, tu peux pas marchander poh J'détaille précis, les barrettes sont pesées poh, hmm, regarde comment je fais poh, poh Sur la route du succès, j'avance prudemment, j'roule à fond c'est normal si j'me prends des amendes eh La vraie vie, c'est après la mort, si j'le fais, c'est pour les sous, j'veux pas qu'on m'adore eh Trop têtu, y a personne pour m'commander, les prix sont fixés, tu peux pas marchander poh J'détaille précis, les barrettes sont pesées poh, hmm, regarde comment je fais poh, poh Ne te pose pas trop d'questions quand on baraude vers ton pavillon mmh Si tu veux pas payer, dans la coche-sa, y a l'couteau papillon mmh 9.2.1.4.0 sur le pocheton et encore, là, c'est juste un échantillon ah bon ? On est grave dans l'argent sale pourtant on veut éviter châtiment ah bon ? Lui il fait l'sisste-gro, j'sais qu'il ment salope, sisste-gros, j'sais qu'il ment salope J'lève un doigt au keuf qui veut mes économies, j'prends ma ce-pla dans l'pe-ra tranquillement Tranquillement, c'est qu'un freestyle, les punchlines j'les économise On a charbonné même pendant le confinement, même pendant le confinement Pour ma gue-dro, t'as succombé, j'ai vu des mecs tomber, jamais se relever eh Couteau dans l'dos, j'le mets à tout l'monde sauf à mes res-fré eh Trop souvent, j'oublie les refrains, comme mes sous, mes sentiments, j'les ai coffrés poh Hors-la-loi donc toutes les règles, on enfreint, normal que les chickens, on les effraie poh, poh Sur la route du succès, j'avance prudemment, j'roule à fond c'est normal si j'me prends des amendes eh La vraie vie, c'est après la mort, si j'le fais, c'est pour les sous, j'veux pas qu'on m'adore eh Trop têtu, y a personne pour m'commander, les prix sont fixés, tu peux pas marchander poh J'détaille précis, les barrettes sont pesées poh, hmm, regarde comment je fais poh, poh Sur la route du succès, j'avance prudemment, j'roule à fond c'est normal si j'me prends des amendes eh La vraie vie, c'est après la mort, si j'le fais, c'est pour les sous, j'veux pas qu'on m'adore eh Trop têtu, y a personne pour m'commander, les prix sont fixés, tu peux pas marchander poh J'détaille précis, les barrettes sont pesées poh, hmm, regarde comment je fais poh, poh Poh, poh, poh, poh</t>
         </is>
       </c>
     </row>
@@ -922,7 +922,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Perds la sacoche Si tu perds la sacoche Si tu perds la sacoche Binks Beatz Si tu perds la sacoche, ça peut te laisser en sang Fils de pute, largent attire les suceurs de bite han Tas snappé ta kichta, tas perdu des thunes han Lil des gens, ça va vite han Tu casses ton tél', tu déchires ton survêt' Tu montes sur un plavon, ten rachètes, ça va vite poh, poh Zéro confiance en ces putes, j'la tamponne sans dire un mot poh Elle connaîtra pas ma vie Tu fais des trucs dans mon dos, tu quittes le navire Y a que pour les sos-pe que mon cur, il chavire Dans l'bâtiment, ça vire Sale con, tu sais pas rapper, tu veux qu'j'te donne mon avis ? Ressaisis-toi, tu dois prendre en main ton avenir Tu fais le gravon mais tu fais rien dans la ville, cruelle est la vie Le junkie prend son poison et il retourne à lasile Hasba, ouais, on ta boulé, bâtard uh Pas besoin de venir cagoulé, bâtard uh Quest-ce que tu vas faire si ton billet, on la pas ? Salope, tu baises pas, tu sors de lappart' La dalle des sous nous fait manger sur ta part Quand ça galérait, on allait rabattre Toutes les deux minutes, jsens la tate-pa Parano, ça paie pas d'bosser khabat eh eh eh eh Y a pas qu'les tes-schmi qui te retardent Ta pute de meuf tempêche de renta Elle veut s'poser mais jai pas l'temps Tous les jours, jsors tôt et je rentre tard Dans tes poches, y a pas un centime Tu rentres chez toi une fois qu'les armes sont sorties Non, jvais pas courir devant une extinct' Tu peux me laver, jvais rien sentir Pas détat dâme, on téteint, bâtard, si tu veux nous ralentir poh Et les histoires de terrain ne peuvent pas se régler sans tir po-poh Quand cétais tendu, tas disparu, pourtant, le quartier, tu revendiques Cest pas un jeu, arrête de faire la rue han, han, han Comment veux tu que je te prenne au sérieux ? On va les casser si on s'met sur tes côtes Ta vie tient quà un fil si on vient en découdre ah bon ? Enculé, tes un con, tas rien mis de té-cô Non, cest pas tes potos qui porteront tes lles-cou' ah bon ? Qui tassumera une fois qu'tes au trou ? Y a que maman qui trouve ton numéro d'écrou brr Les faux, j'les ai rodave comme les keufs en deux roues brr, brr J'étais sur le droit chemin, j'me suis trompé de route brr Dès midi dans l'bât', les bosseurs en train d'ler-rou On encaisse les oranges, on a virer les rouges Quand les p'tits volent ton sac et tes bijoux, y a personne pour jouer les superhéros mmh Et pour acheter des armes de l'Est sur un plavon, on est prêts à monter, négro Ça part en full , ramène tes négresses, mes gavas ont les crocs Dans ma teu-té, c'est comme dans ma tess, gros, on est trop massifs J'lève un doigt pour la schnek de la juge Même si elle m'a relaxé, y a que Dieu qu'j'remercie uh La guerre, c'est pour de vrai donc choisis bien ton camp Ça peut t'pull up si t'es trop laxiste poh Ils veulent pas voir un noir briller sauf si tu fais le con poh, poh Si tu fais gole-ri comme Omar Sy poh You might also like 500 ml, on te nettoie pch, pch, on fait le ménage Même si t'es taillé comme une armoire, le 9 millimètres te fait déménager Dans l'bloco, on est éméchés, les voisins croient tous qu'on est méchants J'veux l'bonheur, j'trouve rien, j'vais pas lâcher Comme les keufs qu'ont retourné ma chambre Comme les keufs qu'ont retourné ma chambre Mets ton pare-balles si tu dois plus d'un point C'est pas pour rien quand on sort le machin Tu peux bomber l'torse, faire des grands gestes On s'en bat les couilles, t'es même pas menaçant brr Ils font les mecs chauds mais c'est des glaçons brr J'reste sur mes gardes comme un vendeur de S brr, brr Ou une escorte en déplacement Tous tes plans tombent à l'eau, normal t'as coulé, nan Y a pas que l'alcool qui m'a saoulé Tous les jours, on m'contrôle à cause de ma couleur Touche un reuf, on r'vient à 1000 comme Metal Cooler Tu veux carotte ? T'as du culot ? Ça t'met des calottes, t'as une schnek escalope Combien d'grammes tu peux cacher dans ta culotte ? Combien d'grammes tu peux cacher dans ta culotte ? Pour kicker l'instru', j'attends pas qu'ça re-pull up Ça bombarde à mort dans la location full up Conduite criminelle et c'est Youska qui pilote Bâtard, même en jean j'suis harag Même si les tales du rap y'en a full up, j'oublie pas qu'ça reste d'l'argent haram 1PLIKÉ140, 150 BPM, arrêtez-le La voix dans ma tête crie Arrêtez-le Prêt à tout pour faire des sommes, belek, ça t'fait le coup du lapin, enculé oui Hasba, Clamart, t'y repense tous les matins, enculé oui Si j'sors la lame, t'apprends à parler latin, enculé oui Reste à l'affût, on envoie au parlu ta tain-p', enculé oui C'est cette putain qui t'a mytho han, cette putain qui t'a mytho Tu m'as vu sur l'rrain-te quand ça débitait pas, oui, je jouais les matchs amicaux 9.2.1.4.0 sur le pocheton, j'finis d'baiser l'rap, j'retourne en incognito 1PLIKÉ140, 150 BPM, arrêtez-le La voix dans ma tête crie Arrêtez-le 500 ml, on te nettoie pch, pch, on fait le ménage Même si t'es taillé comme une armoire, le 9 millimètres te fait déménager Dans l'bloco, on est éméchés, les voisins croient tous qu'on est méchants J'veux l'bonheur, j'trouve rien, j'vais pas lâcher Comme les keufs qu'ont retourné ma chambre Comme les keufs qu'ont retourné ma chambre Mets ton pare-balles si tu dois plus d'un point C'est pas pour rien quand on sort le machin Tu peux bomber l'torse, faire des grands gestes On s'en bat les couilles, t'es même pas menaçant brr Ils font les mecs chauds mais c'est des glaçons brr J'reste sur mes gardes comme un vendeur de S brr, brr Ou une escorte en déplacement1</t>
+          <t>Perds la sacoche Si tu perds la sacoche Si tu perds la sacoche Binks Beatz Si tu perds la sacoche, ça peut te laisser en sang Fils de pute, largent attire les suceurs de bite han Tas snappé ta kichta, tas perdu des thunes han Lil des gens, ça va vite han Tu casses ton tél', tu déchires ton survêt' Tu montes sur un plavon, ten rachètes, ça va vite poh, poh Zéro confiance en ces putes, j'la tamponne sans dire un mot poh Elle connaîtra pas ma vie Tu fais des trucs dans mon dos, tu quittes le navire Y a que pour les sos-pe que mon cur, il chavire Dans l'bâtiment, ça vire Sale con, tu sais pas rapper, tu veux qu'j'te donne mon avis ? Ressaisis-toi, tu dois prendre en main ton avenir Tu fais le gravon mais tu fais rien dans la ville, cruelle est la vie Le junkie prend son poison et il retourne à lasile Hasba, ouais, on ta boulé, bâtard uh Pas besoin de venir cagoulé, bâtard uh Quest-ce que tu vas faire si ton billet, on la pas ? Salope, tu baises pas, tu sors de lappart' La dalle des sous nous fait manger sur ta part Quand ça galérait, on allait rabattre Toutes les deux minutes, jsens la tate-pa Parano, ça paie pas d'bosser khabat eh eh eh eh Y a pas qu'les tes-schmi qui te retardent Ta pute de meuf tempêche de renta Elle veut s'poser mais jai pas l'temps Tous les jours, jsors tôt et je rentre tard Dans tes poches, y a pas un centime Tu rentres chez toi une fois qu'les armes sont sorties Non, jvais pas courir devant une extinct' Tu peux me laver, jvais rien sentir Pas détat dâme, on téteint, bâtard, si tu veux nous ralentir poh Et les histoires de terrain ne peuvent pas se régler sans tir po-poh Quand cétais tendu, tas disparu, pourtant, le quartier, tu revendiques Cest pas un jeu, arrête de faire la rue han, han, han Comment veux tu que je te prenne au sérieux ? On va les casser si on s'met sur tes côtes Ta vie tient quà un fil si on vient en découdre ah bon ? Enculé, tes un con, tas rien mis de té-cô Non, cest pas tes potos qui porteront tes lles-cou' ah bon ? Qui tassumera une fois qu'tes au trou ? Y a que maman qui trouve ton numéro d'écrou brr Les faux, j'les ai rodave comme les keufs en deux roues brr, brr J'étais sur le droit chemin, j'me suis trompé de route brr Dès midi dans l'bât', les bosseurs en train d'ler-rou On encaisse les oranges, on a virer les rouges Quand les p'tits volent ton sac et tes bijoux, y a personne pour jouer les superhéros mmh Et pour acheter des armes de l'Est sur un plavon, on est prêts à monter, négro Ça part en full , ramène tes négresses, mes gavas ont les crocs Dans ma teu-té, c'est comme dans ma tess, gros, on est trop massifs J'lève un doigt pour la schnek de la juge Même si elle m'a relaxé, y a que Dieu qu'j'remercie uh La guerre, c'est pour de vrai donc choisis bien ton camp Ça peut t'pull up si t'es trop laxiste poh Ils veulent pas voir un noir briller sauf si tu fais le con poh, poh Si tu fais gole-ri comme Omar Sy poh 500 ml, on te nettoie pch, pch, on fait le ménage Même si t'es taillé comme une armoire, le 9 millimètres te fait déménager Dans l'bloco, on est éméchés, les voisins croient tous qu'on est méchants J'veux l'bonheur, j'trouve rien, j'vais pas lâcher Comme les keufs qu'ont retourné ma chambre Comme les keufs qu'ont retourné ma chambre Mets ton pare-balles si tu dois plus d'un point C'est pas pour rien quand on sort le machin Tu peux bomber l'torse, faire des grands gestes On s'en bat les couilles, t'es même pas menaçant brr Ils font les mecs chauds mais c'est des glaçons brr J'reste sur mes gardes comme un vendeur de S brr, brr Ou une escorte en déplacement Tous tes plans tombent à l'eau, normal t'as coulé, nan Y a pas que l'alcool qui m'a saoulé Tous les jours, on m'contrôle à cause de ma couleur Touche un reuf, on r'vient à 1000 comme Metal Cooler Tu veux carotte ? T'as du culot ? Ça t'met des calottes, t'as une schnek escalope Combien d'grammes tu peux cacher dans ta culotte ? Combien d'grammes tu peux cacher dans ta culotte ? Pour kicker l'instru', j'attends pas qu'ça re-pull up Ça bombarde à mort dans la location full up Conduite criminelle et c'est Youska qui pilote Bâtard, même en jean j'suis harag Même si les tales du rap y'en a full up, j'oublie pas qu'ça reste d'l'argent haram 1PLIKÉ140, 150 BPM, arrêtez-le La voix dans ma tête crie Arrêtez-le Prêt à tout pour faire des sommes, belek, ça t'fait le coup du lapin, enculé oui Hasba, Clamart, t'y repense tous les matins, enculé oui Si j'sors la lame, t'apprends à parler latin, enculé oui Reste à l'affût, on envoie au parlu ta tain-p', enculé oui C'est cette putain qui t'a mytho han, cette putain qui t'a mytho Tu m'as vu sur l'rrain-te quand ça débitait pas, oui, je jouais les matchs amicaux 9.2.1.4.0 sur le pocheton, j'finis d'baiser l'rap, j'retourne en incognito 1PLIKÉ140, 150 BPM, arrêtez-le La voix dans ma tête crie Arrêtez-le 500 ml, on te nettoie pch, pch, on fait le ménage Même si t'es taillé comme une armoire, le 9 millimètres te fait déménager Dans l'bloco, on est éméchés, les voisins croient tous qu'on est méchants J'veux l'bonheur, j'trouve rien, j'vais pas lâcher Comme les keufs qu'ont retourné ma chambre Comme les keufs qu'ont retourné ma chambre Mets ton pare-balles si tu dois plus d'un point C'est pas pour rien quand on sort le machin Tu peux bomber l'torse, faire des grands gestes On s'en bat les couilles, t'es même pas menaçant brr Ils font les mecs chauds mais c'est des glaçons brr J'reste sur mes gardes comme un vendeur de S brr, brr Ou une escorte en déplacement1</t>
         </is>
       </c>
     </row>
@@ -939,7 +939,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Binks Beatz En vrai j'm'men ballek si t'as pété skal' On revend la came devant la cam' Elle a pas d'cul mais elle fait la Kim Si j'monte sur Paname habillé en jean, c'est pas pour faire la fête C'est juste pour éviter les schmitts, pendant que j'fais gonfler ma SIM Pendant que j'fais gonfler ma SIM J'ai écrit le texte sur le bigo à un schlag Et toi tu demandes comment on fait Tires sur l'kamas, tires sur l'kamas Et tu verras comment on fly J'lui donne ma beu-teu, j'lui offre pas des fleurs Vas-y, j'vais t'laisser copier mon flow C'est une descente ou une mission Commando ? Si on t'croise solo, dis-moi on fait comment gros ? En vérité, on fait comme on veut J'vais t'oublier vite, c'est un peu comme mon feu Pour niquer les keufs, mes lauds-sa sont en noir T'inquiètes on sait se camoufler Les condés vont repasser J'aime pas quand ils tournent à la Plaine On est venus pour te masser Putain j'ai encore oublié la crème You might also like 92140 sur le pocheton J'ai rempli mes poches donc j'ai rempli ma mission Faut jamais ler-par à l'audition Cagoulés, gantés, on s'incruste dans ta maison Et j'avoue qu'les femelles me lassent J'fais d'la prévention, pas des menaces Y a qu'les vrais lauds-sa que j'dédicace On rentre, on prend tout et on s'casse 92140 sur le pocheton J'ai rempli mes poches donc j'ai rempli ma mission Faut jamais ler-par à l'audition Cagoulés, gantés, on s'incruste dans ta maison Et j'avoue qu'les femelles me lassent J'fais d'la prévention, pas des menaces Y a qu'les vrais lauds-sa que j'dédicace On rentre, on prend tout et on s'casse Allez, fais tout c'qu'on t'as demandé Belek à toi, bâtard, ça peut t'amander Même si sur toi t'as pas le fric Igo, tu va décoffrer J'suis un salaud, elle trouve que j'suis frais Moi j'suis un laud-sa, j'pense qu'à chiffrer Si t'es mon reuf, pour toi j'y vais Dans ses yeux, d'la peur j'ai vu J'tire un ffeu-ta, j'perds la mémoire Est-ce que tu peux combattre la mort ? En vrai faut rien laisser dans l'armoire C'est pas sûr qu'elle va tenir, ta porte À part ton cavu, qu'est-ce que tu m'apportes ? Tu l'as tèj', elle a fini escorte Maintenant pour un llet-bi elle s'cambre J'cacherais jamais l'détail dans ma chambre Faus s'barrer à Las Vegas Au quartier le secteur il est trop quadrillé J'veux pas m'faire caner comme 2Pac J'ai vu l'ange de la mort rouler en Cadillac On rentre, on prend tout et on s'casse Eux ils font les fous mais ils se cachent La miss elle est conne, elle saura jamais y a quoi dans ma sacoche 92140 sur le pocheton J'ai rempli mes poches donc j'ai rempli ma mission Faut jamais ler-par à l'audition Cagoulés, gantés, on s'incruste dans ta maison Et j'avoue qu'les femelles me lassent J'fais d'la prévention, pas des menaces Y a qu'les vrais lauds-sa que j'dédicace On rentre, on prend tout et on s'casse 92140 sur le pocheton J'ai rempli mes poches donc j'ai rempli ma mission Faut jamais ler-par à l'audition Cagoulés, gantés, on s'incruste dans ta maison Et j'avoue qu'les femelles me lassent J'fais d'la prévention, pas des menaces Y a qu'les vrais lauds-sa que j'dédicace On rentre, on prend tout et on s'casse</t>
+          <t>Binks Beatz En vrai j'm'men ballek si t'as pété skal' On revend la came devant la cam' Elle a pas d'cul mais elle fait la Kim Si j'monte sur Paname habillé en jean, c'est pas pour faire la fête C'est juste pour éviter les schmitts, pendant que j'fais gonfler ma SIM Pendant que j'fais gonfler ma SIM J'ai écrit le texte sur le bigo à un schlag Et toi tu demandes comment on fait Tires sur l'kamas, tires sur l'kamas Et tu verras comment on fly J'lui donne ma beu-teu, j'lui offre pas des fleurs Vas-y, j'vais t'laisser copier mon flow C'est une descente ou une mission Commando ? Si on t'croise solo, dis-moi on fait comment gros ? En vérité, on fait comme on veut J'vais t'oublier vite, c'est un peu comme mon feu Pour niquer les keufs, mes lauds-sa sont en noir T'inquiètes on sait se camoufler Les condés vont repasser J'aime pas quand ils tournent à la Plaine On est venus pour te masser Putain j'ai encore oublié la crème 92140 sur le pocheton J'ai rempli mes poches donc j'ai rempli ma mission Faut jamais ler-par à l'audition Cagoulés, gantés, on s'incruste dans ta maison Et j'avoue qu'les femelles me lassent J'fais d'la prévention, pas des menaces Y a qu'les vrais lauds-sa que j'dédicace On rentre, on prend tout et on s'casse 92140 sur le pocheton J'ai rempli mes poches donc j'ai rempli ma mission Faut jamais ler-par à l'audition Cagoulés, gantés, on s'incruste dans ta maison Et j'avoue qu'les femelles me lassent J'fais d'la prévention, pas des menaces Y a qu'les vrais lauds-sa que j'dédicace On rentre, on prend tout et on s'casse Allez, fais tout c'qu'on t'as demandé Belek à toi, bâtard, ça peut t'amander Même si sur toi t'as pas le fric Igo, tu va décoffrer J'suis un salaud, elle trouve que j'suis frais Moi j'suis un laud-sa, j'pense qu'à chiffrer Si t'es mon reuf, pour toi j'y vais Dans ses yeux, d'la peur j'ai vu J'tire un ffeu-ta, j'perds la mémoire Est-ce que tu peux combattre la mort ? En vrai faut rien laisser dans l'armoire C'est pas sûr qu'elle va tenir, ta porte À part ton cavu, qu'est-ce que tu m'apportes ? Tu l'as tèj', elle a fini escorte Maintenant pour un llet-bi elle s'cambre J'cacherais jamais l'détail dans ma chambre Faus s'barrer à Las Vegas Au quartier le secteur il est trop quadrillé J'veux pas m'faire caner comme 2Pac J'ai vu l'ange de la mort rouler en Cadillac On rentre, on prend tout et on s'casse Eux ils font les fous mais ils se cachent La miss elle est conne, elle saura jamais y a quoi dans ma sacoche 92140 sur le pocheton J'ai rempli mes poches donc j'ai rempli ma mission Faut jamais ler-par à l'audition Cagoulés, gantés, on s'incruste dans ta maison Et j'avoue qu'les femelles me lassent J'fais d'la prévention, pas des menaces Y a qu'les vrais lauds-sa que j'dédicace On rentre, on prend tout et on s'casse 92140 sur le pocheton J'ai rempli mes poches donc j'ai rempli ma mission Faut jamais ler-par à l'audition Cagoulés, gantés, on s'incruste dans ta maison Et j'avoue qu'les femelles me lassent J'fais d'la prévention, pas des menaces Y a qu'les vrais lauds-sa que j'dédicace On rentre, on prend tout et on s'casse</t>
         </is>
       </c>
     </row>
@@ -956,7 +956,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Transaction rapide, comme d'habitude, y a personne qui m'a vu J'suis posé dans l'blocko avec tous mes rates-pi Tu poucaves des noms, normal qu'on te rate pas Bâtard, tu vas sauter l'dernier repas J'suis content, j'vois la BAC qui repart J'reprends ma part, cette sse-lia, elle m'appartient J'sors avec du détail et j'fais tout partir Binks Beatz On rabat les ients-cli dans ta guenda Et tous ceux qu'j'dois visser sont dans mon agenda Sale pute, t'étais pas là quand y avait drah Et si l'argent il part, il reviendra J'regrette ma vie si j'me fais pét' par les gendarmes Vas-y, viens, on parle en kilogrammes Askip, le savoir est une arme T'aimerais savoir quel jour on descend J'vais coffrer les sous, je redescends Avant d'la ken, j'enfume la bre-cham C'est pour criquette si tu m'vois sur les Champs On a fait trop de salasse et étant adolescents Quand l'bigo sonne, j'suis toujours à laffût Vi-sser, on fait les deux à la fois Et les condés, tu sais qu'on les fuck On t'encule ta mère, igo, même si t'es stock Dans ma cité, le pilon, il s'tord Si on descend chez vous, on augmentera le score Même s'il y a les forces de l'ordre, personne s'écarte Si tu parles en gros, il faut qu'tu parles en she-ca salope Et j'fais pas d'me-chro dans tous les cas Rien a changé, pour de l'or, ta vitre on la casse poh J'veux finir sur la plage en Lacoste Y a la sacoche, en décembre, tu sais bien qu'j'empoche J'allume le mortier sur les condés, c'est la base S'ils sont beaucoup, on mets les gaz J'rentre chez moi, histoire de changer mes sapes Mes négros, attirés par les mapessa J'allume un doré, t'es attiré par la frappe Tires trois taffes sur l'pilon, t'es dans les vapes Il a déjà pé-cho mais il m'renvoie un message T'es qu'un acteur, je crois pas à tes mensonges Parles moi d'plavon si tout est carré J'ai fait rentrer des sous et j'ai rien déclaré J'suis déjà parti quand les tes-schmi se sont garés wouh J'me fais courser, jamais j'm'arrête wouh J'pense à la mort, j'sais qu'elle m'aura wouh On t'encule si tu fais l'ancien, bon débarras T'es un te-traî, avant j'te considérais J'fais la guerre pour la paix un peu comme Madara Arrache, cours, fais les deux à la fois On en a rien à foutre, on respecte pas la loi Si t'es un négro che-lou, me sers pas la main Tu sais déjà, j'traîne pas avec faux renois Pourquoi ils font les Zé Pequeno En vérité, ils ont pas d'pognon Elle connaît ma bite mais elle connaît pas mon nom 92140 sur le pochton Quand t'écoutes mon son, tu sais la frappe elle vient d'où Les bacqueux aiment faire des 4-4-2 Quand j'tiens la bonbonne, j'ai des yeux derrière le dos J'suis impliqué, nan, j'calcule pas ces merdeux Ils m'rapportent pas un rond alors je m'éloigne d'eux J'peux découper la 'quette avec l'Opinel 12 Le te-shi est vert, c'est normal qu'il pue la beuh Le prochain qui parle de mon quartier on le baise Ça l'fait sans refrain, ça y est j'suis chaud comme la braise J'braque le rap à visage découvert J'suis dans les faits divers, des plavons en hiver En moins de dix minutes, toutes les portes elles sont ouvertes T'as poukie, fais tes adieux On a fait du sale, obligés d'quitter les lieux T'es une lope-sa, obligé d'couper les liens Si j'pète une somme, y en aura que pour les miens Bâtard, pourquoi tu m'tends la main ? Salope, pourquoi tu t'colles à moi ? Il m'faut la kichta à la fin du mois Faire la mala en boîte, ça sert a quoi ? Dis-moi J'préfères charbonner tous les jours, même le dimanche Et dans tous les cas, cherche pas, la vie elle est moche La vie elle est cheum, surtout quand t'as rien en poche Tu fais le malin, c'est normal qu'on te déclenche Les keufs vont passer, préviens moi quand j'dois lancer J'peux plus m'arrêter, sur l'instru', j'suis élancé J'peux plus la quitter, à la rue j'suis fiancé J'suis trop matrixé, personne peut m'influencer Le plavon il marche, donc on va recommencer T'écoutes le son, t'as capté le potentiel Comme toujours, y a des ients-cli sur mon tel Alors les épreuves, j'vais surmonter You might also like Pas mé-cra, ça v'-esqui la caméra Ramener les sous, gros t'as intérêt T'as trop parlé sur l'net, tu finis enterré À midi pile, tous les joueurs sont sur l'terrain La go-là, c'est p't-être une fille bien J'vais quand même lui casser les reins Sur la route du succès, je n'fais quaccélérer Mes gavas respectent rien, on a cassé les règles Brr, brr3</t>
+          <t>Transaction rapide, comme d'habitude, y a personne qui m'a vu J'suis posé dans l'blocko avec tous mes rates-pi Tu poucaves des noms, normal qu'on te rate pas Bâtard, tu vas sauter l'dernier repas J'suis content, j'vois la BAC qui repart J'reprends ma part, cette sse-lia, elle m'appartient J'sors avec du détail et j'fais tout partir Binks Beatz On rabat les ients-cli dans ta guenda Et tous ceux qu'j'dois visser sont dans mon agenda Sale pute, t'étais pas là quand y avait drah Et si l'argent il part, il reviendra J'regrette ma vie si j'me fais pét' par les gendarmes Vas-y, viens, on parle en kilogrammes Askip, le savoir est une arme T'aimerais savoir quel jour on descend J'vais coffrer les sous, je redescends Avant d'la ken, j'enfume la bre-cham C'est pour criquette si tu m'vois sur les Champs On a fait trop de salasse et étant adolescents Quand l'bigo sonne, j'suis toujours à laffût Vi-sser, on fait les deux à la fois Et les condés, tu sais qu'on les fuck On t'encule ta mère, igo, même si t'es stock Dans ma cité, le pilon, il s'tord Si on descend chez vous, on augmentera le score Même s'il y a les forces de l'ordre, personne s'écarte Si tu parles en gros, il faut qu'tu parles en she-ca salope Et j'fais pas d'me-chro dans tous les cas Rien a changé, pour de l'or, ta vitre on la casse poh J'veux finir sur la plage en Lacoste Y a la sacoche, en décembre, tu sais bien qu'j'empoche J'allume le mortier sur les condés, c'est la base S'ils sont beaucoup, on mets les gaz J'rentre chez moi, histoire de changer mes sapes Mes négros, attirés par les mapessa J'allume un doré, t'es attiré par la frappe Tires trois taffes sur l'pilon, t'es dans les vapes Il a déjà pé-cho mais il m'renvoie un message T'es qu'un acteur, je crois pas à tes mensonges Parles moi d'plavon si tout est carré J'ai fait rentrer des sous et j'ai rien déclaré J'suis déjà parti quand les tes-schmi se sont garés wouh J'me fais courser, jamais j'm'arrête wouh J'pense à la mort, j'sais qu'elle m'aura wouh On t'encule si tu fais l'ancien, bon débarras T'es un te-traî, avant j'te considérais J'fais la guerre pour la paix un peu comme Madara Arrache, cours, fais les deux à la fois On en a rien à foutre, on respecte pas la loi Si t'es un négro che-lou, me sers pas la main Tu sais déjà, j'traîne pas avec faux renois Pourquoi ils font les Zé Pequeno En vérité, ils ont pas d'pognon Elle connaît ma bite mais elle connaît pas mon nom 92140 sur le pochton Quand t'écoutes mon son, tu sais la frappe elle vient d'où Les bacqueux aiment faire des 4-4-2 Quand j'tiens la bonbonne, j'ai des yeux derrière le dos J'suis impliqué, nan, j'calcule pas ces merdeux Ils m'rapportent pas un rond alors je m'éloigne d'eux J'peux découper la 'quette avec l'Opinel 12 Le te-shi est vert, c'est normal qu'il pue la beuh Le prochain qui parle de mon quartier on le baise Ça l'fait sans refrain, ça y est j'suis chaud comme la braise J'braque le rap à visage découvert J'suis dans les faits divers, des plavons en hiver En moins de dix minutes, toutes les portes elles sont ouvertes T'as poukie, fais tes adieux On a fait du sale, obligés d'quitter les lieux T'es une lope-sa, obligé d'couper les liens Si j'pète une somme, y en aura que pour les miens Bâtard, pourquoi tu m'tends la main ? Salope, pourquoi tu t'colles à moi ? Il m'faut la kichta à la fin du mois Faire la mala en boîte, ça sert a quoi ? Dis-moi J'préfères charbonner tous les jours, même le dimanche Et dans tous les cas, cherche pas, la vie elle est moche La vie elle est cheum, surtout quand t'as rien en poche Tu fais le malin, c'est normal qu'on te déclenche Les keufs vont passer, préviens moi quand j'dois lancer J'peux plus m'arrêter, sur l'instru', j'suis élancé J'peux plus la quitter, à la rue j'suis fiancé J'suis trop matrixé, personne peut m'influencer Le plavon il marche, donc on va recommencer T'écoutes le son, t'as capté le potentiel Comme toujours, y a des ients-cli sur mon tel Alors les épreuves, j'vais surmonter Pas mé-cra, ça v'-esqui la caméra Ramener les sous, gros t'as intérêt T'as trop parlé sur l'net, tu finis enterré À midi pile, tous les joueurs sont sur l'terrain La go-là, c'est p't-être une fille bien J'vais quand même lui casser les reins Sur la route du succès, je n'fais quaccélérer Mes gavas respectent rien, on a cassé les règles Brr, brr3</t>
         </is>
       </c>
     </row>
@@ -973,7 +973,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>M1OnTheBeat M1OnTheBeat Pow, pow, eh, ehBeaucoup d'acteurs, de dormeurs, de poucaves dans ton tieks, négro, est-ce que tu savais ? Les keufs sur l'allée, mes négros jettent un pavé, l'instru' elle est sale, j'suis obligé d'la... Ients-cli qui défilent comme un gala, on t'envoie d'la peuf', kaméhaméha Les putes qui veulent s'ranger comme Khalifa Mia, tout ça, ça m'énerve, tout ça, ça m'zehef T's v'nu te péta, bison il t'as mis ien-b, j'vois ces rnois faire les mecs de gang, j'vois ces reubeus faire les mafieux italiens Pas pour la température qu'on met les gants J'ai toujours le bon shit pour calmer l'ancien, ils disent d'la merde, j'crois bien qu'ils écrivent en chiant Quand j'ai la dalle, salope, j'l'attrape par l'chignon, quand j'ai d'l'argent à faire, j'te laisse en chien Remonter le level, c'est pour ça qu'j'suis là, j'les entend dire il fait le malin c'lui là Ma sse-lia, elle est comme ces thiagas, dehors elle s'fait discrète, dans mon lit, elle se lâche Ça fait longtemps qu'j'ai lâché les temps pleins, faire des midi-minuit sur le R, j'ai passé l'âge J'ai fait beaucoup d'chemin, j'suis même passé chez la juge, et ma version, j'l'ai pas chée-lâ J'leur met la hchouma, eux, ils rappent archi mal, y a plus d'transports donc on rotte-ca le taximan J'casse ma Lebara et j'vais péter la Syma, j'enchaine les passes, on dirait que j'joue la finale, mmh J'lui met ma bite dans la boca sans lui donner l'signal, j'ai ché-cra le Signal, mmh J'connais ces mecs, c'est des tocards, ils parlent dans mon dos mais ils parlent pas quand j'suis à-l, eh On viens te pull-up en Quechua, j'ai un esprit d'vengeance comme Son Gohan J'crois qu'j'ai oublié les présentations, 1PLIKÉ 1-4-0 dans ton enceinte Même le haters succombe à la tentation, y a heja, on s'équipe en deux s'condes T'es prêt ou pas ? On déboule dans ta zone Eux, ils n'font pas que vendre de la C, ils s'la mettent aussi dans les nasaux, ils s'la mettent aussi dans les nasaux J'crois, j'crois, j'crois qu'j'ai oublié les présentations, 1PLIKÉ 1-4-0 dans ton enceinte Même le haters succombe à la tentation, y a heja, on s'équipe en deux s'condes T'es prêt ou pas ? On déboule dans ta zone Eux, ils n'font pas que vendre de la C, ils s'la mettent aussi dans les nasaux, ils s'la mettent aussi dans les nasaux You might also like Beaucoup d'menteurs qui bandent sur la rue, les tits-pe ont grandi, la hagra, ça paye plus La hasba ça paye mais les ients-cli appellent plus, j'ai déjà disparu, j'sais même pas qui a fait l'pu J'viens d'là où ça t'pull-up, ça t'arrache ton pull, c'est pour tout niquer si tu m'vois dans ta compil' Dans la te-stree, t'es qu'un floco, pourquoi tu fais l'malin d'vant ta copine ? L'inspiration vient des ténèbres, quand j'écris, y a des démons dans la cabine ! Y a trop d'transac' à faire dans la capi', pour doubler le bénef', j'ai pris le cro-mi Tellement d'liquide à faire avec des litres, le bosseur, le guetteur forment une équipe d'élite J'sors à peine du plavon, j'ai déjà embelli, les keufs s'infiltrent chez toi, armés comme dans Belly Le tarpé fait l'amour, le schlass fait les prélis, qu'est-ce que tu compte faire si on dépasse les limites ? J'crois qu'j'ai oublié les présentations, 1PLIKÉ 1-4-0 dans ton enceinte Même le haters succombe à la tentation, y a heja, on s'équipe en deux s'condes T'es prêt ou pas ? On déboule dans ta zone Eux, ils n'font pas que vendre de la C, ils s'la mettent aussi dans les nasaux, ils s'la mettent aussi dans les nasaux J'crois, j'crois, j'crois qu'j'ai oublié les présentations, 1PLIKÉ 1-4-0 dans ton enceinte Même le haters succombe à la tentation, y a heja, on s'équipe en deux s'condes T'es prêt ou pas ? On déboule dans ta zone Eux, ils n'font pas que vendre de la C, ils s'la mettent aussi dans les nasaux, ils s'la mettent aussi dans les nasaux 9-2-1-4-0 sur le pocheton, tu finis dans la ve-ca si tu cause trop Igo, bats les couilles si t'es claustro Longue vie à tous mes reuftons qui s'la tuent pour qu'les affaires tournent Longue vie à, longue vie à tous mes reuftons qui s'la tuent pour qu'les affaires tournent, pour qu'les affaires M1OnTheBeat M1OnTheBeat</t>
+          <t>M1OnTheBeat M1OnTheBeat Pow, pow, eh, ehBeaucoup d'acteurs, de dormeurs, de poucaves dans ton tieks, négro, est-ce que tu savais ? Les keufs sur l'allée, mes négros jettent un pavé, l'instru' elle est sale, j'suis obligé d'la... Ients-cli qui défilent comme un gala, on t'envoie d'la peuf', kaméhaméha Les putes qui veulent s'ranger comme Khalifa Mia, tout ça, ça m'énerve, tout ça, ça m'zehef T's v'nu te péta, bison il t'as mis ien-b, j'vois ces rnois faire les mecs de gang, j'vois ces reubeus faire les mafieux italiens Pas pour la température qu'on met les gants J'ai toujours le bon shit pour calmer l'ancien, ils disent d'la merde, j'crois bien qu'ils écrivent en chiant Quand j'ai la dalle, salope, j'l'attrape par l'chignon, quand j'ai d'l'argent à faire, j'te laisse en chien Remonter le level, c'est pour ça qu'j'suis là, j'les entend dire il fait le malin c'lui là Ma sse-lia, elle est comme ces thiagas, dehors elle s'fait discrète, dans mon lit, elle se lâche Ça fait longtemps qu'j'ai lâché les temps pleins, faire des midi-minuit sur le R, j'ai passé l'âge J'ai fait beaucoup d'chemin, j'suis même passé chez la juge, et ma version, j'l'ai pas chée-lâ J'leur met la hchouma, eux, ils rappent archi mal, y a plus d'transports donc on rotte-ca le taximan J'casse ma Lebara et j'vais péter la Syma, j'enchaine les passes, on dirait que j'joue la finale, mmh J'lui met ma bite dans la boca sans lui donner l'signal, j'ai ché-cra le Signal, mmh J'connais ces mecs, c'est des tocards, ils parlent dans mon dos mais ils parlent pas quand j'suis à-l, eh On viens te pull-up en Quechua, j'ai un esprit d'vengeance comme Son Gohan J'crois qu'j'ai oublié les présentations, 1PLIKÉ 1-4-0 dans ton enceinte Même le haters succombe à la tentation, y a heja, on s'équipe en deux s'condes T'es prêt ou pas ? On déboule dans ta zone Eux, ils n'font pas que vendre de la C, ils s'la mettent aussi dans les nasaux, ils s'la mettent aussi dans les nasaux J'crois, j'crois, j'crois qu'j'ai oublié les présentations, 1PLIKÉ 1-4-0 dans ton enceinte Même le haters succombe à la tentation, y a heja, on s'équipe en deux s'condes T'es prêt ou pas ? On déboule dans ta zone Eux, ils n'font pas que vendre de la C, ils s'la mettent aussi dans les nasaux, ils s'la mettent aussi dans les nasaux Beaucoup d'menteurs qui bandent sur la rue, les tits-pe ont grandi, la hagra, ça paye plus La hasba ça paye mais les ients-cli appellent plus, j'ai déjà disparu, j'sais même pas qui a fait l'pu J'viens d'là où ça t'pull-up, ça t'arrache ton pull, c'est pour tout niquer si tu m'vois dans ta compil' Dans la te-stree, t'es qu'un floco, pourquoi tu fais l'malin d'vant ta copine ? L'inspiration vient des ténèbres, quand j'écris, y a des démons dans la cabine ! Y a trop d'transac' à faire dans la capi', pour doubler le bénef', j'ai pris le cro-mi Tellement d'liquide à faire avec des litres, le bosseur, le guetteur forment une équipe d'élite J'sors à peine du plavon, j'ai déjà embelli, les keufs s'infiltrent chez toi, armés comme dans Belly Le tarpé fait l'amour, le schlass fait les prélis, qu'est-ce que tu compte faire si on dépasse les limites ? J'crois qu'j'ai oublié les présentations, 1PLIKÉ 1-4-0 dans ton enceinte Même le haters succombe à la tentation, y a heja, on s'équipe en deux s'condes T'es prêt ou pas ? On déboule dans ta zone Eux, ils n'font pas que vendre de la C, ils s'la mettent aussi dans les nasaux, ils s'la mettent aussi dans les nasaux J'crois, j'crois, j'crois qu'j'ai oublié les présentations, 1PLIKÉ 1-4-0 dans ton enceinte Même le haters succombe à la tentation, y a heja, on s'équipe en deux s'condes T'es prêt ou pas ? On déboule dans ta zone Eux, ils n'font pas que vendre de la C, ils s'la mettent aussi dans les nasaux, ils s'la mettent aussi dans les nasaux 9-2-1-4-0 sur le pocheton, tu finis dans la ve-ca si tu cause trop Igo, bats les couilles si t'es claustro Longue vie à tous mes reuftons qui s'la tuent pour qu'les affaires tournent Longue vie à, longue vie à tous mes reuftons qui s'la tuent pour qu'les affaires tournent, pour qu'les affaires M1OnTheBeat M1OnTheBeat</t>
         </is>
       </c>
     </row>
@@ -990,7 +990,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Freestyle 1 J'rigole quand je pense aux mecs que j'ai rasba Le criketeur, il danse quand il voit qu'le gérant s'barre C'est pas pour tractionner si on passe à la barre Il donne pas sa déposition, c'est une lance-ba Pas besoin d'te faire un schéma, il a chekem des blazes Alors avec lui j'peux pas che-mar J'la bloque une fois que j'lui ai mise Toi, tu portes tes couille quand tes sous tease poto Quand tes agin, t'arrêtes tes bêtises Comme d'hab' faut relever les potos qui bé-tom J'peux tenir le gun avec la main sur l'guidon C'est donc ça, la loi du ghetto T'as pété des kilos qu'on peut venir soulever Que des talbins à 9 heure, j'suis levé J'reconnais le vil-ci, il fait des va et viens J'veux finir dans une villa avec latina Le plan il est carré, j'pourrais jamais dire non J'allais charbonner j'étais pas là au dîner Décris pas ma tête, regarde bien c'que j't'ai donné Rentre à Chicago si ta du crant Y a des mecs qui font les gros Mais en embrouille ils appellent leurs grands Mais en embrouille ils appellent leurs grands Ramenez n'importe qui on s'deb' deb' Bande de suceurs de queue, vous venez quand y a le buzz Fuck les condés, la caméra qui nous pistent Et même si ils descendent j'vais pas quitter mon poste J'préfère aller au shtar que balancer mon pote Viens pas t'embrouiller à la fin tu portes plainte bâtard T'as laissé tes empreintes bâtard T'as laissé tes empreintes bâtard You might also likeFreestyle 2 Jai caler le doré entre les jambes Jfais que dtartiner pour avoir les couilles en or Jai fumé la beuh, et jai perdu le nord.hm hm Quand jétais ti-peu javais pas trop peur du noir Mais peur de la mort La rue ce nest pas un jeu.Ah bon Ne confond pas le bénéf et lamour.Ah bon Ils mettent largent de la drogue chez leur meuf Pourtant ya des négros qui la fourre Il manque des meu-gra Tu va pas la faire à noussalope Ne mfais pas croire que jsuis parano Jrentre dans sa schneck Jai pas besoin de lui passer lanneaubaw On tient la bonbonne toute lannée Tout ce quon veut cest billet entassé À trois sur un plavon à quatre chiffres Mon négro cest pas assez À midi lfacteur est djà passé Minuit vingt-deux le neiman est cassé Minuit vingt-trois la batman est passée Vingt-quatre ça cours, jfais Yamakasi Jme déshabille en bas Jme coffre à la casa.baw Et si thabite pas ici On prendra ta chaîne à loccasion.brrrt Jserais toujours en manque de billet Jserais jamais en manque daffection 9-2-1-4-0 sur le pocheton jentend la portière La bonbonne déjà jeté.Poh Sale pute sale putepoh Jdirais jamais je taime Tu me tend la main Igo moi jveux pas que tu maide.brrrt On fais de largent toutes les semaines. brrrt Du teu-shi sous la semelle. Wouh LOPJ de quoi il se mêle ? Freestyle 3 Faut casser toutes les caméras Rentre dans le bâtiment la cam est la On veut des beurettes et des Camélias Parfois jsuis égoïste negro jpense qu'à mes liasses Alors jfais tout pour un billet en plus Tu me dois des sous tu crois qu'jai oublier en plus Jveux pas finir les mains liés Jsuis un vrai lossa donc je ne fais que nier Pour brasser dans la Street negro faut pas s'noyer Si on t'carjack au feu rouge tu rentres à iep Si tu fais un trou igo t'auras pas ta paye Il fait que d'crier on la pas encore taper J'allais arracher j'étais pas intelligent Maintenant que j'ai grandi je ne pense qu'à rhasba les gens Et mes lossas ne pense qu'à la paye Ya des lopsa qui manquent à l'appel Jles entend parler de kalash y ont vu des me-ar qu'à la journée d'appel On te mêle casqués comme les daft punk Sa soit jperd la tête jme met à bédave la J'aime pas les salopes mais tu vas sucer ma queue J'aime pas trop parler j'aime pas me faire remarquer À minuit le terrain y ferme jsuis encore la gros j'ai pas fini de marquer Jmen balec de la meuf aux cheveux lisses jvoulais finir à Beverly Hills Parfois je me demande ce qu'elle préfère entre ma dégaine et ma liasse Mais l'argent sale ramène des malheurs et pour me consoler negro ya que ma liasse Parfois j'avoue que ce train de vie m'agace alors pour s'amuser on caillasse Fuck la police toute la journée Voilà la mentalité qu'on a</t>
+          <t>Freestyle 1 J'rigole quand je pense aux mecs que j'ai rasba Le criketeur, il danse quand il voit qu'le gérant s'barre C'est pas pour tractionner si on passe à la barre Il donne pas sa déposition, c'est une lance-ba Pas besoin d'te faire un schéma, il a chekem des blazes Alors avec lui j'peux pas che-mar J'la bloque une fois que j'lui ai mise Toi, tu portes tes couille quand tes sous tease poto Quand tes agin, t'arrêtes tes bêtises Comme d'hab' faut relever les potos qui bé-tom J'peux tenir le gun avec la main sur l'guidon C'est donc ça, la loi du ghetto T'as pété des kilos qu'on peut venir soulever Que des talbins à 9 heure, j'suis levé J'reconnais le vil-ci, il fait des va et viens J'veux finir dans une villa avec latina Le plan il est carré, j'pourrais jamais dire non J'allais charbonner j'étais pas là au dîner Décris pas ma tête, regarde bien c'que j't'ai donné Rentre à Chicago si ta du crant Y a des mecs qui font les gros Mais en embrouille ils appellent leurs grands Mais en embrouille ils appellent leurs grands Ramenez n'importe qui on s'deb' deb' Bande de suceurs de queue, vous venez quand y a le buzz Fuck les condés, la caméra qui nous pistent Et même si ils descendent j'vais pas quitter mon poste J'préfère aller au shtar que balancer mon pote Viens pas t'embrouiller à la fin tu portes plainte bâtard T'as laissé tes empreintes bâtard T'as laissé tes empreintes bâtard Freestyle 2 Jai caler le doré entre les jambes Jfais que dtartiner pour avoir les couilles en or Jai fumé la beuh, et jai perdu le nord.hm hm Quand jétais ti-peu javais pas trop peur du noir Mais peur de la mort La rue ce nest pas un jeu.Ah bon Ne confond pas le bénéf et lamour.Ah bon Ils mettent largent de la drogue chez leur meuf Pourtant ya des négros qui la fourre Il manque des meu-gra Tu va pas la faire à noussalope Ne mfais pas croire que jsuis parano Jrentre dans sa schneck Jai pas besoin de lui passer lanneaubaw On tient la bonbonne toute lannée Tout ce quon veut cest billet entassé À trois sur un plavon à quatre chiffres Mon négro cest pas assez À midi lfacteur est djà passé Minuit vingt-deux le neiman est cassé Minuit vingt-trois la batman est passée Vingt-quatre ça cours, jfais Yamakasi Jme déshabille en bas Jme coffre à la casa.baw Et si thabite pas ici On prendra ta chaîne à loccasion.brrrt Jserais toujours en manque de billet Jserais jamais en manque daffection 9-2-1-4-0 sur le pocheton jentend la portière La bonbonne déjà jeté.Poh Sale pute sale putepoh Jdirais jamais je taime Tu me tend la main Igo moi jveux pas que tu maide.brrrt On fais de largent toutes les semaines. brrrt Du teu-shi sous la semelle. Wouh LOPJ de quoi il se mêle ? Freestyle 3 Faut casser toutes les caméras Rentre dans le bâtiment la cam est la On veut des beurettes et des Camélias Parfois jsuis égoïste negro jpense qu'à mes liasses Alors jfais tout pour un billet en plus Tu me dois des sous tu crois qu'jai oublier en plus Jveux pas finir les mains liés Jsuis un vrai lossa donc je ne fais que nier Pour brasser dans la Street negro faut pas s'noyer Si on t'carjack au feu rouge tu rentres à iep Si tu fais un trou igo t'auras pas ta paye Il fait que d'crier on la pas encore taper J'allais arracher j'étais pas intelligent Maintenant que j'ai grandi je ne pense qu'à rhasba les gens Et mes lossas ne pense qu'à la paye Ya des lopsa qui manquent à l'appel Jles entend parler de kalash y ont vu des me-ar qu'à la journée d'appel On te mêle casqués comme les daft punk Sa soit jperd la tête jme met à bédave la J'aime pas les salopes mais tu vas sucer ma queue J'aime pas trop parler j'aime pas me faire remarquer À minuit le terrain y ferme jsuis encore la gros j'ai pas fini de marquer Jmen balec de la meuf aux cheveux lisses jvoulais finir à Beverly Hills Parfois je me demande ce qu'elle préfère entre ma dégaine et ma liasse Mais l'argent sale ramène des malheurs et pour me consoler negro ya que ma liasse Parfois j'avoue que ce train de vie m'agace alors pour s'amuser on caillasse Fuck la police toute la journée Voilà la mentalité qu'on a</t>
         </is>
       </c>
     </row>
@@ -1007,7 +1007,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>J'ai calé le doré entre les jambes J'fais que tartiner pour avoir les couilles en or J'ai fumé la beuh et j'ai perdu le nord Quand j'étais tipeu j'avais pas trop peur du noir mais peur de la mort La rue c'est pas un jeu Ne confonds pas le bénef et l'amour Ils mettent l'argent d'la drogue chez leurs meufs Pourtant y'a des négros qui la fourrent Ils manquent des me-gra tu vas pas la faire à nous Me fais pas croire que chui parano J'rentre dans sa schneck j'ai pas besoin de lui passer l'anneau On tiens la bonbonne toute l'année Tout ce qu'on veux c'est billets entassés A trois sur un plavon attractif Mon négro c'est pas assez A midi l'facteur est déjà passé Minuit 22 le Neiman est cassé Minuit 23 la batman est passée 24 sa cours J'fais Yamakazi J'me déshabille en bas J'me coffre à la casa You might also likeEt si t'habites pas ici On prendra ta chaîne à l'occassion J'serais toujours en manque de billets J'serais jamais en manque d'affection 92140 sur le pocheton J'entends la portière La bonbonne déjà jetée Sale pute Sale pute J'dirais jamais je t'aime Tu tends la main igo moi jveux pas que tu m'aides On fais de l'argent toutes les semaines Du teshi sous la semelle L'OPJ de quoi il se mêle</t>
+          <t>J'ai calé le doré entre les jambes J'fais que tartiner pour avoir les couilles en or J'ai fumé la beuh et j'ai perdu le nord Quand j'étais tipeu j'avais pas trop peur du noir mais peur de la mort La rue c'est pas un jeu Ne confonds pas le bénef et l'amour Ils mettent l'argent d'la drogue chez leurs meufs Pourtant y'a des négros qui la fourrent Ils manquent des me-gra tu vas pas la faire à nous Me fais pas croire que chui parano J'rentre dans sa schneck j'ai pas besoin de lui passer l'anneau On tiens la bonbonne toute l'année Tout ce qu'on veux c'est billets entassés A trois sur un plavon attractif Mon négro c'est pas assez A midi l'facteur est déjà passé Minuit 22 le Neiman est cassé Minuit 23 la batman est passée 24 sa cours J'fais Yamakazi J'me déshabille en bas J'me coffre à la casa Et si t'habites pas ici On prendra ta chaîne à l'occassion J'serais toujours en manque de billets J'serais jamais en manque d'affection 92140 sur le pocheton J'entends la portière La bonbonne déjà jetée Sale pute Sale pute J'dirais jamais je t'aime Tu tends la main igo moi jveux pas que tu m'aides On fais de l'argent toutes les semaines Du teshi sous la semelle L'OPJ de quoi il se mêle</t>
         </is>
       </c>
     </row>
@@ -1024,7 +1024,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Un-un truc à régler, on déboule en convoi, tu fais moins l'malin quand c'est nous, hein Quatre négros carbo' dans la ture-voi, si t'entends les sirènes, c'est pour nous, hein T'aimes-t'aimes pas quand elle veut t'tenir tête, tu préfères quand elle s'met à genoux, hein Pourquoi t'as pas couru quand les tchoys sont venus ? En vérité, c'est toi qu'es chelou, hein Tu veux bé-bar ? Tu peux finir les fesses à l'air, réveille-toi, y a que des somnambules dans ta cité, dans la street, ils ont pas d'salaires Poh Re-noi, belek, ta vie bascule au moment où l'opinel, il passe à travers Brr, parfois, l'destin fait zéro faveur Brr J'parle, j'parle pas, j'suis dans ma bulle Brr, brr, brr, les rageux veulent mon temps, t'inquiète, j'leur donne pas l'heure T'es pas en place, aux meufs, tu racontes des bara', la mienne, c'est Lebara À c'qui p', t'as le bras mais c'est toi qui débarrasse, les keufs font des barrages, gués-lar, bon débarras J'ai bicrave des CD, j'ai pochetonné ma rage Han, toi, tu veux nous chehell sur le prix du charras Ouh Y a la BAC, on s'arrache, on gère le démarrage Ouh, j'jette une kichta pendant la chasse Ah bon ? J'ai vu sourire la chance, les prières de maman m'font éviter la casse Ah bon ?, embrouille, on cogne dur, jamais on jacasse Au quartier, j'suis trop là, j'me dis faut qu'j'me casse, on m'accoste pour d'la beuh même quand j'suis en vacances Et si t'es le sang, j'pourrais pas répondre absent Uh, j'suis toujours OP, dis-moi juste on y va quand Uh ? J'ressors menotté, y a toujours des remplaçants, j'suis à l'hôtel pendant la perquis', ils m'attendent L'école, c'était casse-couilles Han, j'arrachais tout, j'sortais des cours, cache-cou, j'arrachais tout Han J'fume d'la frappe après m'être fait sé-cour, j'nique ma santé, j'sens qu'm'a durée d'vie s'écourte Poh, poh Idées malsaines dans la te-tê Poh, poh, si t'écoutes trop cette voix, tu finiras ché-tou Ouh T'as fini au trou, ta meuf, on la troue Ouh, salope, si ton mec tombe, c'est le mektoub Ouh, ouh Maman veut juste que son fils soit là, toutes mes ex veulent que j'finisse solo Solo Gardien d'la paix veut m'voir au sol Sol, sol, trop d'ennemis qui veulent me voir au ciel Ciel, ciel Autant marcher seul, igo, tu meurs seul Poh, poh, j'ai deux pénaves, j'réponds pas quand tu m'harcèles Poh, poh J'ai deux pénaves, j'réponds pas quand tu m'harcèles, j'sais qu'ils aimeraient m'voir dans un linceul Hum, hum Ils veulent m'enterrer mais c'est moi qu'a la pelle Hum, hum, t'es un floco, donc c'est moi qu'elle appelle Hum, hum T'as peur des représailles t'entretiens la paix, trop de haine dans le quartier d'la Plaine Y a, y a du sang sur ma paire à chaque fois qu'j'écris Han, du sang sur ma plume, j'ai perdu des frères, j'ai gardé ma puce Han J'suis pas un ient-cli, avant d'la mer-fu Poh, poh, j'ai vendu la pure, j'ai vendu la pure Dans l'four, y a des, dans l'four, y a des junkies en chaleur Ouh qui ne demandent qu'à inhaler Ouh Mais fais pas la meuf qui a des valeurs Han juste parce que, juste parce que t'as peur d'avaler Han Chez toi, ça dévalise, ils ont pas un los-ki, ils parlent de valises Ah bon ? Avant qu'tu ramasses le khaliss, faut qu'tu mettes un billet, le mal m'a habillé, normal que j'banalise Poh Le premier joint d'kamas quand j'livrais sur Beriz Poh, poh, quand j'étais solo, tout l'temps, c'était comme a-ç Hi-yih J'pensais à tout plaquer et r'mettre le kamis, dans la foulée, j'faisais mon client dans l'axe J'veux qu'on me sorte de là, j'aime pas qu'on m'idolâtre mais j'aime trop les dollars Dans ma chambre, j'culpabilise comme un taulard Brr, argent pêché j'comptabilise, y en a trop là Brr, brr You might also like J'aime pas quand ça fouille l'état des lieux, j'peux kill pour toi si dans mon sang, t'as des liens T'as des liens À c'qui p', tu rappes depuis longtemps mais on attend toujours que tu t'améliores T'améliores Prêt au pire pour avoir un monde meilleur, coffrer ou claquer, faut le juste milieu Travailler pour un SMIC, c'est insultant, à la fin du mois, t'as même pas fait mille-deux Eh-eh Y a du, y a du marron, du doré, j'pense qu'à mes liasses Ouh, ça bicrave la Fatou, la Camélia Ouh On est partout, on baise tout, en cache-cou Brr, on casse tout Brr, un keuf au sol Brr, ça crie Alléluia Brr Jamais d'la vie j'me tatoue comme ces renois Eh, même si elle a des atouts, j'la baise qu'une fois Eh On passe partout, on s'incruste dans ta rée-soi Poh, la frappe, ambiance des babtous, est-ce que tu m'reçois Ouh, ouh, ouh ? Y a du, y a du marron, du doré, j'pense qu'à mes liasses Hein ?, ça bicrave la Fatou, la Camélia Han On est partout, on baise tout, en cache-cou Brr, on casse tout Brr, un keuf au sol Brr, ça crie Alléluia Brr Jamais d'la vie j'me tatoue comme ces renois Eh, même si elle a des atouts, j'la baise qu'une fois Eh On passe partout, on s'incruste dans ta rée-soi Poh, la frappe, ambiance des babtous, est-ce que tu m'reçois Poh, poh ?</t>
+          <t>Un-un truc à régler, on déboule en convoi, tu fais moins l'malin quand c'est nous, hein Quatre négros carbo' dans la ture-voi, si t'entends les sirènes, c'est pour nous, hein T'aimes-t'aimes pas quand elle veut t'tenir tête, tu préfères quand elle s'met à genoux, hein Pourquoi t'as pas couru quand les tchoys sont venus ? En vérité, c'est toi qu'es chelou, hein Tu veux bé-bar ? Tu peux finir les fesses à l'air, réveille-toi, y a que des somnambules dans ta cité, dans la street, ils ont pas d'salaires Poh Re-noi, belek, ta vie bascule au moment où l'opinel, il passe à travers Brr, parfois, l'destin fait zéro faveur Brr J'parle, j'parle pas, j'suis dans ma bulle Brr, brr, brr, les rageux veulent mon temps, t'inquiète, j'leur donne pas l'heure T'es pas en place, aux meufs, tu racontes des bara', la mienne, c'est Lebara À c'qui p', t'as le bras mais c'est toi qui débarrasse, les keufs font des barrages, gués-lar, bon débarras J'ai bicrave des CD, j'ai pochetonné ma rage Han, toi, tu veux nous chehell sur le prix du charras Ouh Y a la BAC, on s'arrache, on gère le démarrage Ouh, j'jette une kichta pendant la chasse Ah bon ? J'ai vu sourire la chance, les prières de maman m'font éviter la casse Ah bon ?, embrouille, on cogne dur, jamais on jacasse Au quartier, j'suis trop là, j'me dis faut qu'j'me casse, on m'accoste pour d'la beuh même quand j'suis en vacances Et si t'es le sang, j'pourrais pas répondre absent Uh, j'suis toujours OP, dis-moi juste on y va quand Uh ? J'ressors menotté, y a toujours des remplaçants, j'suis à l'hôtel pendant la perquis', ils m'attendent L'école, c'était casse-couilles Han, j'arrachais tout, j'sortais des cours, cache-cou, j'arrachais tout Han J'fume d'la frappe après m'être fait sé-cour, j'nique ma santé, j'sens qu'm'a durée d'vie s'écourte Poh, poh Idées malsaines dans la te-tê Poh, poh, si t'écoutes trop cette voix, tu finiras ché-tou Ouh T'as fini au trou, ta meuf, on la troue Ouh, salope, si ton mec tombe, c'est le mektoub Ouh, ouh Maman veut juste que son fils soit là, toutes mes ex veulent que j'finisse solo Solo Gardien d'la paix veut m'voir au sol Sol, sol, trop d'ennemis qui veulent me voir au ciel Ciel, ciel Autant marcher seul, igo, tu meurs seul Poh, poh, j'ai deux pénaves, j'réponds pas quand tu m'harcèles Poh, poh J'ai deux pénaves, j'réponds pas quand tu m'harcèles, j'sais qu'ils aimeraient m'voir dans un linceul Hum, hum Ils veulent m'enterrer mais c'est moi qu'a la pelle Hum, hum, t'es un floco, donc c'est moi qu'elle appelle Hum, hum T'as peur des représailles t'entretiens la paix, trop de haine dans le quartier d'la Plaine Y a, y a du sang sur ma paire à chaque fois qu'j'écris Han, du sang sur ma plume, j'ai perdu des frères, j'ai gardé ma puce Han J'suis pas un ient-cli, avant d'la mer-fu Poh, poh, j'ai vendu la pure, j'ai vendu la pure Dans l'four, y a des, dans l'four, y a des junkies en chaleur Ouh qui ne demandent qu'à inhaler Ouh Mais fais pas la meuf qui a des valeurs Han juste parce que, juste parce que t'as peur d'avaler Han Chez toi, ça dévalise, ils ont pas un los-ki, ils parlent de valises Ah bon ? Avant qu'tu ramasses le khaliss, faut qu'tu mettes un billet, le mal m'a habillé, normal que j'banalise Poh Le premier joint d'kamas quand j'livrais sur Beriz Poh, poh, quand j'étais solo, tout l'temps, c'était comme a-ç Hi-yih J'pensais à tout plaquer et r'mettre le kamis, dans la foulée, j'faisais mon client dans l'axe J'veux qu'on me sorte de là, j'aime pas qu'on m'idolâtre mais j'aime trop les dollars Dans ma chambre, j'culpabilise comme un taulard Brr, argent pêché j'comptabilise, y en a trop là Brr, brr J'aime pas quand ça fouille l'état des lieux, j'peux kill pour toi si dans mon sang, t'as des liens T'as des liens À c'qui p', tu rappes depuis longtemps mais on attend toujours que tu t'améliores T'améliores Prêt au pire pour avoir un monde meilleur, coffrer ou claquer, faut le juste milieu Travailler pour un SMIC, c'est insultant, à la fin du mois, t'as même pas fait mille-deux Eh-eh Y a du, y a du marron, du doré, j'pense qu'à mes liasses Ouh, ça bicrave la Fatou, la Camélia Ouh On est partout, on baise tout, en cache-cou Brr, on casse tout Brr, un keuf au sol Brr, ça crie Alléluia Brr Jamais d'la vie j'me tatoue comme ces renois Eh, même si elle a des atouts, j'la baise qu'une fois Eh On passe partout, on s'incruste dans ta rée-soi Poh, la frappe, ambiance des babtous, est-ce que tu m'reçois Ouh, ouh, ouh ? Y a du, y a du marron, du doré, j'pense qu'à mes liasses Hein ?, ça bicrave la Fatou, la Camélia Han On est partout, on baise tout, en cache-cou Brr, on casse tout Brr, un keuf au sol Brr, ça crie Alléluia Brr Jamais d'la vie j'me tatoue comme ces renois Eh, même si elle a des atouts, j'la baise qu'une fois Eh On passe partout, on s'incruste dans ta rée-soi Poh, la frappe, ambiance des babtous, est-ce que tu m'reçois Poh, poh ?</t>
         </is>
       </c>
     </row>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Yeh, yeh, yeh, yeh, yeh, yeh, yeh Yeh, yeh, yeh, yeh, yeh, yeh, yeh Boo? Vous ne vous sentez pas bien? Va t'en vite loin d'ici, très loin Kss, va-t'en Y a pas qu'le buteur qui compte les secondes, y a des darons d'famille qui se cassent les os uh J'entends deux fois ma voix, j'ai du mal à capter l'réseau uh, y a hamar de kush sous mes ongles J'ai rien divulgué chaque fois, qu'j'prenais dollars poh, non, j'ai pas pris exemple sur les autres poh Zahma, tu connais du monde poh, pourtant, t'sais pas qui est prêt à ter-sau poh Le gérant be-tom, j'sais qu'ça fait sourire les tits-pe han, méfie-toi de celui qui t'en dit peu han J'ai ramassé plus, j'ai pas fait c'que j'ai pu brr, brr, pourquoi j'oublie c'que j'ai ? J'repense à c'que j'ai plus Si l'monde est à nous, il est surtout à moi, même si la terre est si nombreux, tu m'as pas vu cher-lâ Mais prendre mon avenir à deux mains uh, uh, uh, j'ai mis une boulette aux baceux qui tenaient mes bras Chleh, les qué-ple ont vidé ma cachette, ça fait deux jours qu'j'réalise pas Ils savent rien du rrain-te à part celui qu'achète, pourtant, celui qui pousse se déguise pas J'ai des vis que ton tournevis ne te dévisse pas On réinvestit l'bénéfice, on l'divise pas Tout l'monde t'entoure quand c'est fleurissant han, han mais quand c'est la merda, tes potos, ils disent quoi han, let's go ? You might also like J'm'enfume le veau-cer comme Bou comme Bou Pas d'boucan quand ça cambute cambute J'fuck le bout-mara comme Bou comme Bou J'fais c'que j'veux, nan, j'aime pas faire comme vous comme vous J'm'enfume le veau-cer comme Bou comme BouPas d'boucan quand ça cambute cambute J'fuck le bout-mara comme Bou comme Bou J'fais c'que j'veux, nan, j'aime pas faire comme vous comme vous Comme Bou, j'ai pas besoin du marabout Comme Bou, j'ai pas besoin du marabout drr M'éloigner des vices et des tes-traî drr, drr, c'est pas ça qui m'a attristé drr Comme Bou, j'ai pas besoin du marabout Comme Bou, j'ai pas besoin du marabout po-poh La monnaie nous a fait perdre la te-tê po-poh, eux, c'est l'rap qui les a matrixé po-poh C'est l'heure de se mettre à table, t'es pas invité, ne viens pas gratter un bout T'as connu l'époque des freestyles, t'es un bon, si t'as saigné le volume 1, t'es un bon J'mets un pied hors du tieks, j'ai d'jà raté un bail, j'ai entendu qu'tu m'graille, ah bon ? La flicaille, le 14, on va en prison, la boule, d'mande à Ibé, on laisse pas rentrer ces mabouls Ça t'allume sur des quettes-pla d'semi, t'es trop naïf, gros, arrête tes manies Est-ce que Sosa aurait arrêté Manny ? C'est mes semblables qui viennent gâcher ton anniv' Quand ils sont chés-tout par la cleptomanie, c'est la tess qui m'épaule, c'est l'ghetto qui m'anime C'que j'raconte dans mes textes, c'est ma ie-v, j'voulais pas feater, j'voulais garder ma ligne J'fais des passes dé', j'm'en fous d'regarder la ligne Chleh, les qué-ple ont vidé ma cachette, ça fait deux jours qu'j'réalise pas Ils savent rien du rrain-te à part celui qu'achète, pourtant, celui qui pousse se déguise pas J'ai des vices que ton tournevis ne dévisse pas On réinvestit l'bénéfice, on l'divise pas Tout l'monde t'entoure quand c'est fleurissant han, han mais quand c'est la merda, tes potos, ils disent quoi han, let's go ? J'm'enfume le veau-cer comme Bou comme Bou Pas d'boucan quand ça cambute cambute J'fuck le bout-mara comme Bou comme Bou J'fais c'que j'veux, nan, j'aime pas faire comme vous comme vous J'm'enfume le veau-cer comme Bou comme BouPas d'boucan quand ça cambute cambute J'fuck le bout-mara comme Bou comme Bou J'fais c'que j'veux, nan, j'aime pas faire comme vous comme vous Comme Bou, j'ai pas besoin du marabout Comme Bou, j'ai pas besoin du marabout drr M'éloigner des vices et des tes-traî drr, drr, c'est pas ça qui m'a attristé drr Comme Bou, j'ai pas besoin du marabout Comme Bou, j'ai pas besoin du marabout po-poh La monnaie nous a fait perdre la te-tê po-poh, eux, c'est l'rap qui les a matrixé po-poh J'm'enfume le veau-cer comme Bou comme Bou Pas d'boucan quand ça cambute cambute J'fuck le bout-mara comme Bou comme Bou J'fais c'que j'veux, nan, j'aime pas faire comme vous comme vous J'm'enfume le veau-cer comme Bou comme BouPas d'boucan quand ça cambute cambute J'fuck le bout-mara comme Bou comme Bou J'fais c'que j'veux, nan, j'aime pas faire comme vous comme vous Comme Bou, j'ai pas besoin du marabout Comme Bou, j'ai pas besoin du marabout drr M'éloigner des vices et des tes-traî drr, drr, c'est pas ça qui m'a attristé drr Comme Bou, j'ai pas besoin du marabout Comme Bou, j'ai pas besoin du marabout po-poh La monnaie nous a fait perdre la te-tê po-poh, eux, c'est l'rap qui les a matrixé po-poh Wou-ouh</t>
+          <t>Yeh, yeh, yeh, yeh, yeh, yeh, yeh Yeh, yeh, yeh, yeh, yeh, yeh, yeh Boo? Vous ne vous sentez pas bien? Va t'en vite loin d'ici, très loin Kss, va-t'en Y a pas qu'le buteur qui compte les secondes, y a des darons d'famille qui se cassent les os uh J'entends deux fois ma voix, j'ai du mal à capter l'réseau uh, y a hamar de kush sous mes ongles J'ai rien divulgué chaque fois, qu'j'prenais dollars poh, non, j'ai pas pris exemple sur les autres poh Zahma, tu connais du monde poh, pourtant, t'sais pas qui est prêt à ter-sau poh Le gérant be-tom, j'sais qu'ça fait sourire les tits-pe han, méfie-toi de celui qui t'en dit peu han J'ai ramassé plus, j'ai pas fait c'que j'ai pu brr, brr, pourquoi j'oublie c'que j'ai ? J'repense à c'que j'ai plus Si l'monde est à nous, il est surtout à moi, même si la terre est si nombreux, tu m'as pas vu cher-lâ Mais prendre mon avenir à deux mains uh, uh, uh, j'ai mis une boulette aux baceux qui tenaient mes bras Chleh, les qué-ple ont vidé ma cachette, ça fait deux jours qu'j'réalise pas Ils savent rien du rrain-te à part celui qu'achète, pourtant, celui qui pousse se déguise pas J'ai des vis que ton tournevis ne te dévisse pas On réinvestit l'bénéfice, on l'divise pas Tout l'monde t'entoure quand c'est fleurissant han, han mais quand c'est la merda, tes potos, ils disent quoi han, let's go ? J'm'enfume le veau-cer comme Bou comme Bou Pas d'boucan quand ça cambute cambute J'fuck le bout-mara comme Bou comme Bou J'fais c'que j'veux, nan, j'aime pas faire comme vous comme vous J'm'enfume le veau-cer comme Bou comme BouPas d'boucan quand ça cambute cambute J'fuck le bout-mara comme Bou comme Bou J'fais c'que j'veux, nan, j'aime pas faire comme vous comme vous Comme Bou, j'ai pas besoin du marabout Comme Bou, j'ai pas besoin du marabout drr M'éloigner des vices et des tes-traî drr, drr, c'est pas ça qui m'a attristé drr Comme Bou, j'ai pas besoin du marabout Comme Bou, j'ai pas besoin du marabout po-poh La monnaie nous a fait perdre la te-tê po-poh, eux, c'est l'rap qui les a matrixé po-poh C'est l'heure de se mettre à table, t'es pas invité, ne viens pas gratter un bout T'as connu l'époque des freestyles, t'es un bon, si t'as saigné le volume 1, t'es un bon J'mets un pied hors du tieks, j'ai d'jà raté un bail, j'ai entendu qu'tu m'graille, ah bon ? La flicaille, le 14, on va en prison, la boule, d'mande à Ibé, on laisse pas rentrer ces mabouls Ça t'allume sur des quettes-pla d'semi, t'es trop naïf, gros, arrête tes manies Est-ce que Sosa aurait arrêté Manny ? C'est mes semblables qui viennent gâcher ton anniv' Quand ils sont chés-tout par la cleptomanie, c'est la tess qui m'épaule, c'est l'ghetto qui m'anime C'que j'raconte dans mes textes, c'est ma ie-v, j'voulais pas feater, j'voulais garder ma ligne J'fais des passes dé', j'm'en fous d'regarder la ligne Chleh, les qué-ple ont vidé ma cachette, ça fait deux jours qu'j'réalise pas Ils savent rien du rrain-te à part celui qu'achète, pourtant, celui qui pousse se déguise pas J'ai des vices que ton tournevis ne dévisse pas On réinvestit l'bénéfice, on l'divise pas Tout l'monde t'entoure quand c'est fleurissant han, han mais quand c'est la merda, tes potos, ils disent quoi han, let's go ? J'm'enfume le veau-cer comme Bou comme Bou Pas d'boucan quand ça cambute cambute J'fuck le bout-mara comme Bou comme Bou J'fais c'que j'veux, nan, j'aime pas faire comme vous comme vous J'm'enfume le veau-cer comme Bou comme BouPas d'boucan quand ça cambute cambute J'fuck le bout-mara comme Bou comme Bou J'fais c'que j'veux, nan, j'aime pas faire comme vous comme vous Comme Bou, j'ai pas besoin du marabout Comme Bou, j'ai pas besoin du marabout drr M'éloigner des vices et des tes-traî drr, drr, c'est pas ça qui m'a attristé drr Comme Bou, j'ai pas besoin du marabout Comme Bou, j'ai pas besoin du marabout po-poh La monnaie nous a fait perdre la te-tê po-poh, eux, c'est l'rap qui les a matrixé po-poh J'm'enfume le veau-cer comme Bou comme Bou Pas d'boucan quand ça cambute cambute J'fuck le bout-mara comme Bou comme Bou J'fais c'que j'veux, nan, j'aime pas faire comme vous comme vous J'm'enfume le veau-cer comme Bou comme BouPas d'boucan quand ça cambute cambute J'fuck le bout-mara comme Bou comme Bou J'fais c'que j'veux, nan, j'aime pas faire comme vous comme vous Comme Bou, j'ai pas besoin du marabout Comme Bou, j'ai pas besoin du marabout drr M'éloigner des vices et des tes-traî drr, drr, c'est pas ça qui m'a attristé drr Comme Bou, j'ai pas besoin du marabout Comme Bou, j'ai pas besoin du marabout po-poh La monnaie nous a fait perdre la te-tê po-poh, eux, c'est l'rap qui les a matrixé po-poh Wou-ouh</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Binks Beatz Mmh, mmh Mmh, mmh Crois pas qu'on est des racailles, crois pas qu'on est des racailles Contre le système, on pense qu'à lutter S'ils aiment pas ta mentalité, tu peux t'faire canner comme Martin Luther J'ai mis des gants et un masque pour un plan sous, nan, c'est pas pour des histoires sanitaires J'suis à deux doigts d'lâcher des insanités au micro, mais les médias vont s'agiter J'gué-lar la concu', j'ai grave du nitro, ils ont rien vendu mais ils parlent grave de litron Ils font genre qu'ils m'ché-cher, si ils veulnt, ils me trouvent, j'ai jamais changé d'position J'voulais baiser la c-Fran, j'me suis trompé d'trou, et c'est sur ce son qu't'allumes ton pétou Tu veux t'la donner ? Dis-moi on s'pète où, tu passe du rire aux larmes sans transition J'terrorise le game, j'suis à deux doigts d'tout péter, un schmitt en vélo, trois pédales sur l'VTT Le 14 juillet, ils finissent en ITT, on faisait des sous pendant qu'les seins, ils tétaient Le cur noirci, j'écris les lumières éteintes, faut venir m'allumer, gros, si tu veux m'éteindre T'as deux bras, deux jambes, donc comment peux-tu te plaindre ? Regarde autour de toi s'il te plaît Il aime trop la rue, répond à ses désirs Trainer en groupe lui fait pousser des ailes Il a trop rêvé des îles, donc sur le plavon, il est cruel Tous ses sentiments sont cadenassés Cruel comme l'euthanasie, tous les fous n'sont pas dans un asile Il peut ber-tom pour vol aggravé Il aime trop la rue, répond à ses désirs Trainer en groupe lui fait pousser des ailes Il a trop rêvé des îles, donc sur le plavon, il est cruel Tous ses sentiments sont cadenassés Cruel comme l'euthanasie, tous les fous n'sont pas dans un asile Il peut ber-tom pour vol aggravé You might also like Nan, nan, nan, nan, nan, nan Nan, nan, nan, nan, nan, nan J'entends cette voix qui m'chuchote à l'oreille, le million est loin mais je l'aurais Le million est loin mais je l'aurais, le million est loin mais je l'aurais J'entends cette voix qui m'chuchote à l'oreille, le million est loin mais je l'aurais Le million est loin mais je l'aurais, le million est loin mais je l'aurais La dalle des sous s'cultive depuis petit, à la fin du plavon, j'entends bon appétit Faut coffrer un pétard, c'est fini les bêtises, beaucoup qui parlent, très peu qui concrétisent Remercie Dieu si on te rate de justesse, chez nous, la vengeance est une forme de justice On respecte aucune limitation d'vitesse, donc, impossible qu'ils nous ralentissent Dans la te-stree, ils restent actifs, pour qu'tu lâches des thunes, ils parlent qu'à l'impératif Ils parlent qu'aux ients-cli, ils tchatchent pas trop aux raclis Si tu fais l'baraqué, ça dégaine un truc, là tu fais peur à qui ? Le bonheur, il est prêt à l'braquer, comme si elle appartient, il s'attache à cette vie Il reste conscient que pour s'en sortir, faut qu'il s'détache de ces vices Il aime trop la rue, répond à ses désirs Trainer en groupe lui fait pousser des ailes Il a trop rêvé des îles, donc sur le plavon, il est cruel Tous ses sentiments sont cadenassés Cruel comme l'euthanasie, tous les fous n'sont pas dans un asile Il peut ber-tom pour vol aggravé Il aime trop la rue, répond à ses désirs Trainer en groupe lui fait pousser des ailes Il a trop rêvé des îles, donc sur le plavon, il est cruel Tous ses sentiments sont cadenassés Cruel comme l'euthanasie, tous les fous n'sont pas dans un asile Il peut ber-tom pour vol aggravé Cette voix qui m'chuchote à l'oreille, le million est loin mais je l'aurais Le million est loin mais je l'aurais nan, nan, nan, nan, nan, nan Le million est loin mais je l'aurais</t>
+          <t>Binks Beatz Mmh, mmh Mmh, mmh Crois pas qu'on est des racailles, crois pas qu'on est des racailles Contre le système, on pense qu'à lutter S'ils aiment pas ta mentalité, tu peux t'faire canner comme Martin Luther J'ai mis des gants et un masque pour un plan sous, nan, c'est pas pour des histoires sanitaires J'suis à deux doigts d'lâcher des insanités au micro, mais les médias vont s'agiter J'gué-lar la concu', j'ai grave du nitro, ils ont rien vendu mais ils parlent grave de litron Ils font genre qu'ils m'ché-cher, si ils veulnt, ils me trouvent, j'ai jamais changé d'position J'voulais baiser la c-Fran, j'me suis trompé d'trou, et c'est sur ce son qu't'allumes ton pétou Tu veux t'la donner ? Dis-moi on s'pète où, tu passe du rire aux larmes sans transition J'terrorise le game, j'suis à deux doigts d'tout péter, un schmitt en vélo, trois pédales sur l'VTT Le 14 juillet, ils finissent en ITT, on faisait des sous pendant qu'les seins, ils tétaient Le cur noirci, j'écris les lumières éteintes, faut venir m'allumer, gros, si tu veux m'éteindre T'as deux bras, deux jambes, donc comment peux-tu te plaindre ? Regarde autour de toi s'il te plaît Il aime trop la rue, répond à ses désirs Trainer en groupe lui fait pousser des ailes Il a trop rêvé des îles, donc sur le plavon, il est cruel Tous ses sentiments sont cadenassés Cruel comme l'euthanasie, tous les fous n'sont pas dans un asile Il peut ber-tom pour vol aggravé Il aime trop la rue, répond à ses désirs Trainer en groupe lui fait pousser des ailes Il a trop rêvé des îles, donc sur le plavon, il est cruel Tous ses sentiments sont cadenassés Cruel comme l'euthanasie, tous les fous n'sont pas dans un asile Il peut ber-tom pour vol aggravé Nan, nan, nan, nan, nan, nan Nan, nan, nan, nan, nan, nan J'entends cette voix qui m'chuchote à l'oreille, le million est loin mais je l'aurais Le million est loin mais je l'aurais, le million est loin mais je l'aurais J'entends cette voix qui m'chuchote à l'oreille, le million est loin mais je l'aurais Le million est loin mais je l'aurais, le million est loin mais je l'aurais La dalle des sous s'cultive depuis petit, à la fin du plavon, j'entends bon appétit Faut coffrer un pétard, c'est fini les bêtises, beaucoup qui parlent, très peu qui concrétisent Remercie Dieu si on te rate de justesse, chez nous, la vengeance est une forme de justice On respecte aucune limitation d'vitesse, donc, impossible qu'ils nous ralentissent Dans la te-stree, ils restent actifs, pour qu'tu lâches des thunes, ils parlent qu'à l'impératif Ils parlent qu'aux ients-cli, ils tchatchent pas trop aux raclis Si tu fais l'baraqué, ça dégaine un truc, là tu fais peur à qui ? Le bonheur, il est prêt à l'braquer, comme si elle appartient, il s'attache à cette vie Il reste conscient que pour s'en sortir, faut qu'il s'détache de ces vices Il aime trop la rue, répond à ses désirs Trainer en groupe lui fait pousser des ailes Il a trop rêvé des îles, donc sur le plavon, il est cruel Tous ses sentiments sont cadenassés Cruel comme l'euthanasie, tous les fous n'sont pas dans un asile Il peut ber-tom pour vol aggravé Il aime trop la rue, répond à ses désirs Trainer en groupe lui fait pousser des ailes Il a trop rêvé des îles, donc sur le plavon, il est cruel Tous ses sentiments sont cadenassés Cruel comme l'euthanasie, tous les fous n'sont pas dans un asile Il peut ber-tom pour vol aggravé Cette voix qui m'chuchote à l'oreille, le million est loin mais je l'aurais Le million est loin mais je l'aurais nan, nan, nan, nan, nan, nan Le million est loin mais je l'aurais</t>
         </is>
       </c>
     </row>
@@ -1075,7 +1075,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Y a l'chant des guetteurs qui forme une chorale Tu peux déménager si t'es pas d'accord J'm'en bats les c' d'la couronne tant que j'porte mes cojo' Salope, personne veut t'cher-chou comme si t'as l'coro' J'connais pas l'effet d'groupe, j'suis l'même quand j'suis solo Tous les jours, j'te vois dans l'tier-quar, c'est quoi ton rôle ? Tous les jours, j'te vois dans l'tieks mais c'est quoi ton rôle ? Tu cherches un plan sous, j'ai le bras à Piccolo Y a l'chant des guetteurs qui forme une chorale Tu peux déménager si t'es pas d'accord J'm'en bats les c' d'la couronne tant que j'porte mes cojo' Salope, personne veut t'cher-chou comme si t'as l'coro' J'connais pas l'effet d'groupe, j'suis l'même quand j'suis solo Tous les jours, j'te vois dans l'tier-quar, c'est quoi ton rôle ? Tous les jours, j'te vois dans l'tieks mais c'est quoi ton rôle ? Tu cherches un plan sous, j'ai le bras à Piccolo C'est pas la rue, c'est maman qui m'éduque brr Dis-moi, ici, les règles, c'est qui qui les dicte ? brr 1PLIKÉ revient, balance des inédits brr, brr Quitte le R sur un coup de tête comme Zinédine brr J'pars en cances-va avec l'argent d'la résine han Plus d'réseau sur la ligne, ça résonne han C'est bientôt la fin, t'as vu les signes han, han C'est bientôt la fin, t'as vu les signes han Askip t'as volé ça ? T'as volé ci uh Ça t'lave à l'extinct', ça te lessive uh Sale pute, on veut pas d'tafiole ici J'ai pas l'trac, j'ai vidé tout l'Hennessy Nan, mon négro, j'ai pas quitté l'illicite brr Nan, mon négro, j'suis toujours dans l'illicite brr J'monte au charbon, j'reviens avec le butin brr, brr Tous mes négros et mes démons m'félicitent brr You might also like J'suis très loin du recel, protège ta re-s' comme tu protèges ta recette poh J'vois qu'les tits-pe ramassent plus que les grands poh Et qu'les anciens ne veulent pas prendre leur retraite mais nan Faut l'faire, j'y vais à fond, jamais je regrette J'fume, j'oublie les souvenirs de la récrée Les tales m'ont rendu fou, encaisser, c'est l'remède Que la puce elle débite, c'était écrit Tu sais pas rapper, négro, rien qu'tu m'imites ah bon ?, 9.2.1.4.0, aucun timinik ah bon ? Charbon, catimini pow, pow, pow, en aucun cas faut qu'ma liasse diminue Que des contrats à durées indéfinies Qui prennent fin une fois qu'la gàv est finie Même si j'suis plein, j'm'habillerai pas en Philipp T'embrouilles pas avec nous, c'est jamais fini J'baise ta fimbi même si y a zéro feeling Mon chemin est droit, tous mes pas sont alignés L'argent m'réchauffe quand j'passe un sale hiver Obligé d'mettre le feu, j'me suis fait à l'idée Ton pote doit grave des sous, t'as du mal à l'aider Parfois, histoires de sous laissent des familles en deuil brr Ça t'pose un lapin pour te rotte-ca brr, brr Trop méchants, on fait fuir la clientèle brr C'est pas la rue, c'est maman qui m'éduque brr Dis-moi, ici, les règles, c'est qui qui les dicte ? brr 1PLIKÉ revient, balance des inédits brr, brr Quitte le R sur un coup de tête comme Zinédine brr J'pars en cances-va avec l'argent d'la résine han Plus d'réseau sur la ligne, ça résonne han C'est bientôt la fin, t'as vu les signes han, han C'est bientôt la fin, t'as vu les signes han Askip t'as volé ça ? T'as volé ci uh Ça t'lave à l'extinct', ça te lessive uh Sale pute, on veut pas d'tafiole ici J'ai pas l'trac, j'ai vidé tout l'Hennessy Nan, mon négro, j'ai pas quitté l'illicite brr Nan, mon négro, j'suis toujours dans l'illicite brr J'monte au charbon, j'reviens avec le butin brr, brr Tous mes négros et mes démons m'félicitent brr Que des buts sur l'terrain, pas l'temps d'les célébrer Ça t'vend la frappe qui t'laisse des lésions cérébrales t'inquiète pas On sait comment chiffrer Même en période de crise, faut pas baisser les bras des rrettes-ba Un tit-pe vient te livrer, si tu veux plus d'100 balles, n'essaie pas d'le mer-cra Illicite est l'contrat, même sous CR, le trafic ne s'arrête pas s'arrête pas Pour la street, j'ai trop donné, ces flocos, j'les connais Ils font du bruit pour faire mouiller les gadjis ah bon ? Que des réponses négatives, nous, c'est en silence quand on sort les gadgets ah bon ? On s'éloigne du paradis, pour ça qu'les keufs font les paparazzis salope Illicite comme la frappe dans mon jeans, mon ami La moitié d'leurs ses-phra, j'les ai déjà dites J'ai trop les crocs, j'veux pas t'attendre pour damer Tu peux venir à 1000, poto, si t'as tant d'amis Pourquoi, pour payer, du temps, t'en as mis ? t'en as mis On a fait des dégâts pendant tant d'années Que des mecs gantés qui sèment la zizanie Seul le crime paie, illicite la mentalité Laisse tous les passants en panique passants en panique C'est pas la rue, c'est maman qui m'éduque brr Dis-moi, ici, les règles, c'est qui qui les dicte ? brr 1PLIKÉ revient, balance des inédits brr, brr Quitte le R sur un coup de tête comme Zinédine brr J'pars en cances-va avec l'argent d'la résine han Plus d'réseau sur la ligne, ça résonne han C'est bientôt la fin, t'as vu les signes han, han C'est bientôt la fin, t'as vu les signes han Askip t'as volé ça ? T'as volé ci uh Ça t'lave à l'extinct', ça te lessive uh Sale pute, on veut pas d'tafiole J'ai pas l'trac, j'ai vidé tout l'Hennessy Nan, mon négro, j'ai pas quitté l'illicite brr Nan, mon négro, j'suis toujours dans l'illicite brr J'monte au charbon, j'reviens avec le butin brr, brr Tous mes négros et mes démons m'félicitent brr 9.2.1.4.0 sur le pocheton, comme d'habitude, les blases, ils faut pas qu'tu les cites ah bon ? J'connais bien les tiagas d'la ville mais elles veulent pas faire les putes ici ah bon ? On sait très bien qu'tu bicraves ton cavu, salope, j't'ai reconnu sur le site ah bon ? Igo, j'suis tellement dans l'illicite que j'sais même plus c'qu'il est illicite uh</t>
+          <t>Y a l'chant des guetteurs qui forme une chorale Tu peux déménager si t'es pas d'accord J'm'en bats les c' d'la couronne tant que j'porte mes cojo' Salope, personne veut t'cher-chou comme si t'as l'coro' J'connais pas l'effet d'groupe, j'suis l'même quand j'suis solo Tous les jours, j'te vois dans l'tier-quar, c'est quoi ton rôle ? Tous les jours, j'te vois dans l'tieks mais c'est quoi ton rôle ? Tu cherches un plan sous, j'ai le bras à Piccolo Y a l'chant des guetteurs qui forme une chorale Tu peux déménager si t'es pas d'accord J'm'en bats les c' d'la couronne tant que j'porte mes cojo' Salope, personne veut t'cher-chou comme si t'as l'coro' J'connais pas l'effet d'groupe, j'suis l'même quand j'suis solo Tous les jours, j'te vois dans l'tier-quar, c'est quoi ton rôle ? Tous les jours, j'te vois dans l'tieks mais c'est quoi ton rôle ? Tu cherches un plan sous, j'ai le bras à Piccolo C'est pas la rue, c'est maman qui m'éduque brr Dis-moi, ici, les règles, c'est qui qui les dicte ? brr 1PLIKÉ revient, balance des inédits brr, brr Quitte le R sur un coup de tête comme Zinédine brr J'pars en cances-va avec l'argent d'la résine han Plus d'réseau sur la ligne, ça résonne han C'est bientôt la fin, t'as vu les signes han, han C'est bientôt la fin, t'as vu les signes han Askip t'as volé ça ? T'as volé ci uh Ça t'lave à l'extinct', ça te lessive uh Sale pute, on veut pas d'tafiole ici J'ai pas l'trac, j'ai vidé tout l'Hennessy Nan, mon négro, j'ai pas quitté l'illicite brr Nan, mon négro, j'suis toujours dans l'illicite brr J'monte au charbon, j'reviens avec le butin brr, brr Tous mes négros et mes démons m'félicitent brr J'suis très loin du recel, protège ta re-s' comme tu protèges ta recette poh J'vois qu'les tits-pe ramassent plus que les grands poh Et qu'les anciens ne veulent pas prendre leur retraite mais nan Faut l'faire, j'y vais à fond, jamais je regrette J'fume, j'oublie les souvenirs de la récrée Les tales m'ont rendu fou, encaisser, c'est l'remède Que la puce elle débite, c'était écrit Tu sais pas rapper, négro, rien qu'tu m'imites ah bon ?, 9.2.1.4.0, aucun timinik ah bon ? Charbon, catimini pow, pow, pow, en aucun cas faut qu'ma liasse diminue Que des contrats à durées indéfinies Qui prennent fin une fois qu'la gàv est finie Même si j'suis plein, j'm'habillerai pas en Philipp T'embrouilles pas avec nous, c'est jamais fini J'baise ta fimbi même si y a zéro feeling Mon chemin est droit, tous mes pas sont alignés L'argent m'réchauffe quand j'passe un sale hiver Obligé d'mettre le feu, j'me suis fait à l'idée Ton pote doit grave des sous, t'as du mal à l'aider Parfois, histoires de sous laissent des familles en deuil brr Ça t'pose un lapin pour te rotte-ca brr, brr Trop méchants, on fait fuir la clientèle brr C'est pas la rue, c'est maman qui m'éduque brr Dis-moi, ici, les règles, c'est qui qui les dicte ? brr 1PLIKÉ revient, balance des inédits brr, brr Quitte le R sur un coup de tête comme Zinédine brr J'pars en cances-va avec l'argent d'la résine han Plus d'réseau sur la ligne, ça résonne han C'est bientôt la fin, t'as vu les signes han, han C'est bientôt la fin, t'as vu les signes han Askip t'as volé ça ? T'as volé ci uh Ça t'lave à l'extinct', ça te lessive uh Sale pute, on veut pas d'tafiole ici J'ai pas l'trac, j'ai vidé tout l'Hennessy Nan, mon négro, j'ai pas quitté l'illicite brr Nan, mon négro, j'suis toujours dans l'illicite brr J'monte au charbon, j'reviens avec le butin brr, brr Tous mes négros et mes démons m'félicitent brr Que des buts sur l'terrain, pas l'temps d'les célébrer Ça t'vend la frappe qui t'laisse des lésions cérébrales t'inquiète pas On sait comment chiffrer Même en période de crise, faut pas baisser les bras des rrettes-ba Un tit-pe vient te livrer, si tu veux plus d'100 balles, n'essaie pas d'le mer-cra Illicite est l'contrat, même sous CR, le trafic ne s'arrête pas s'arrête pas Pour la street, j'ai trop donné, ces flocos, j'les connais Ils font du bruit pour faire mouiller les gadjis ah bon ? Que des réponses négatives, nous, c'est en silence quand on sort les gadgets ah bon ? On s'éloigne du paradis, pour ça qu'les keufs font les paparazzis salope Illicite comme la frappe dans mon jeans, mon ami La moitié d'leurs ses-phra, j'les ai déjà dites J'ai trop les crocs, j'veux pas t'attendre pour damer Tu peux venir à 1000, poto, si t'as tant d'amis Pourquoi, pour payer, du temps, t'en as mis ? t'en as mis On a fait des dégâts pendant tant d'années Que des mecs gantés qui sèment la zizanie Seul le crime paie, illicite la mentalité Laisse tous les passants en panique passants en panique C'est pas la rue, c'est maman qui m'éduque brr Dis-moi, ici, les règles, c'est qui qui les dicte ? brr 1PLIKÉ revient, balance des inédits brr, brr Quitte le R sur un coup de tête comme Zinédine brr J'pars en cances-va avec l'argent d'la résine han Plus d'réseau sur la ligne, ça résonne han C'est bientôt la fin, t'as vu les signes han, han C'est bientôt la fin, t'as vu les signes han Askip t'as volé ça ? T'as volé ci uh Ça t'lave à l'extinct', ça te lessive uh Sale pute, on veut pas d'tafiole J'ai pas l'trac, j'ai vidé tout l'Hennessy Nan, mon négro, j'ai pas quitté l'illicite brr Nan, mon négro, j'suis toujours dans l'illicite brr J'monte au charbon, j'reviens avec le butin brr, brr Tous mes négros et mes démons m'félicitent brr 9.2.1.4.0 sur le pocheton, comme d'habitude, les blases, ils faut pas qu'tu les cites ah bon ? J'connais bien les tiagas d'la ville mais elles veulent pas faire les putes ici ah bon ? On sait très bien qu'tu bicraves ton cavu, salope, j't'ai reconnu sur le site ah bon ? Igo, j'suis tellement dans l'illicite que j'sais même plus c'qu'il est illicite uh</t>
         </is>
       </c>
     </row>
@@ -1092,7 +1092,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Les condés tournent trop dans mon tieks, normal si j'en parle souvent dans mes textes Faire du pe-ra, jy avais pensé depuis, mais j'étais freiné par ces fils de putes Mon parcours est vrai depuis l'début brr, jamais tu mverras sucer des bites brr Les embrouilles se règlent souvent dans l'bus brr, brr mais belek si on sait où t'habites brr J'me rappelle plus des meufs que j'ai qué-ni han, j'me rappelle des transac' à Hnri Barbusse han Jusqu'à Marcadet-Poissonniers ah bon ?, la hain quand lbigo veut pas sonner ah bon ? Il tharcèle quand il veut un me-chro, quand faut payer, il veut pas pointer son nez Ça l'a fumé, ça la raté, il a eu d'la chance que c'était pas son heure En si peu d'temps elle ma donné son corps, normal si je joue avec son cur Han J'viens d'là où le tartineur fait son beurre pow, j'viens d'là où le tartineur fait son blé pow Mais si il est pas vigilant deux-trois photos pourront le faire tomber po-pow Au début il était sage, y a deux trois potos qui l'ont fait sombrer wouh Askip, t'es mon re-frè, mais bon, j'sens qu'tu m'manques d'honnêteté han J'ai répondu présent au charbon en hiver mais j'ai fait plus de cash en été han Bâtard, j'sais bien qu'tu connais tchi, t'as zéro connexion Dans le tier-quar, tu peux cher-bran que les p'tits T'as zéro connexion, dans le tier-quar, tu peux cher-bran que les p'tits Sur Insta', elle est gée-char, en vrai, elle est squelettique J'gaze, j'piétine, j'gaze, j'piétine, putain, on dirait qu'j'ai des tics Faut pas claquer, faut investir sur un 9 milli' ou une arme soviétique You might also like Enculé, tu peux appeler le 17 dans l'tier-quar, tu crois qu'ils vont sauver qui ? Enculé, une fois qu'ça le-par en quali, normal tes gars, ils veulent se v'-esqui Et si le plan sous est trop risqué, tu peux noyer ta peur avec le whisky J'connais des mecs qui revendent la neige, cagoulés, pas de lunettes de ski J'suis pas dans la mala, j'suis dans l'discret, ils snappent les blocs mais ne sont pas d'ici Par les sirènes, le charbonneur est distrait comme si c'était déjà la fin du film déjà la fin du film Toujours agir en silence comme le J, en silence comme le J Depuis BÂTARD 2, ces salopes collent mon chibre pow, ces salopes collent mon chibre salope Askip, t'es mon re-frè, mais bon, j'sens qu'tu m'manques d'honnêteté han J'ai répondu présent au charbon en hiver mais j'ai fait plus de cash en été han Bâtard, j'sais bien qu'tu connais tchi, t'as zéro connexion Dans le tier-quar, tu peux cher-bran que les p'tits T'as zéro connexion, dans le tier-quar, tu peux cher-bran que les p'tits Sur Insta', elle est gée-char, en vrai, elle est squelettique J'gaze, j'piétine, j'gaze, j'piétine, putain, on dirait qu'j'ai des tics Faut pas claquer, faut investir sur un 9 milli' ou une arme soviétique On sème le désordre, on sème la panique, du quartier, les poucaves seront toujours bannis Y a plus trop d'amis, des amitiés s'déchirent comme Tony et Many, c'est les descentes qui font monter l'adrénaline Tous mes couplets font l'effet d'un tsunami, la vie elle est cheum comme la grosse chatte à Marine salope Ou comme son daron Jean-Marie salope, si c'est une lope-sa, impossible que j'la marie Parfois, j'suis en perte, j'ai le mort quand ça m'arrive, après la perquis', j'en ai fait des cauchemars Tu ressors du shtar mais tu be-tom aussi vite que Schumacher ah bon ? Ils font les gros, ils sont trop marrants, comme le J, on agit en sous-marin Comme le J, on agit en sous-marin T'as zéro connexion dans le tier-quar, tu peux cher-bran que les p'tits T'as zéro connexion dans le tier-quar, tu peux cher-bran que les p'tits Sur Insta', elle est gée-char, en vrai, elle est squelettique eh, eh !</t>
+          <t>Les condés tournent trop dans mon tieks, normal si j'en parle souvent dans mes textes Faire du pe-ra, jy avais pensé depuis, mais j'étais freiné par ces fils de putes Mon parcours est vrai depuis l'début brr, jamais tu mverras sucer des bites brr Les embrouilles se règlent souvent dans l'bus brr, brr mais belek si on sait où t'habites brr J'me rappelle plus des meufs que j'ai qué-ni han, j'me rappelle des transac' à Hnri Barbusse han Jusqu'à Marcadet-Poissonniers ah bon ?, la hain quand lbigo veut pas sonner ah bon ? Il tharcèle quand il veut un me-chro, quand faut payer, il veut pas pointer son nez Ça l'a fumé, ça la raté, il a eu d'la chance que c'était pas son heure En si peu d'temps elle ma donné son corps, normal si je joue avec son cur Han J'viens d'là où le tartineur fait son beurre pow, j'viens d'là où le tartineur fait son blé pow Mais si il est pas vigilant deux-trois photos pourront le faire tomber po-pow Au début il était sage, y a deux trois potos qui l'ont fait sombrer wouh Askip, t'es mon re-frè, mais bon, j'sens qu'tu m'manques d'honnêteté han J'ai répondu présent au charbon en hiver mais j'ai fait plus de cash en été han Bâtard, j'sais bien qu'tu connais tchi, t'as zéro connexion Dans le tier-quar, tu peux cher-bran que les p'tits T'as zéro connexion, dans le tier-quar, tu peux cher-bran que les p'tits Sur Insta', elle est gée-char, en vrai, elle est squelettique J'gaze, j'piétine, j'gaze, j'piétine, putain, on dirait qu'j'ai des tics Faut pas claquer, faut investir sur un 9 milli' ou une arme soviétique Enculé, tu peux appeler le 17 dans l'tier-quar, tu crois qu'ils vont sauver qui ? Enculé, une fois qu'ça le-par en quali, normal tes gars, ils veulent se v'-esqui Et si le plan sous est trop risqué, tu peux noyer ta peur avec le whisky J'connais des mecs qui revendent la neige, cagoulés, pas de lunettes de ski J'suis pas dans la mala, j'suis dans l'discret, ils snappent les blocs mais ne sont pas d'ici Par les sirènes, le charbonneur est distrait comme si c'était déjà la fin du film déjà la fin du film Toujours agir en silence comme le J, en silence comme le J Depuis BÂTARD 2, ces salopes collent mon chibre pow, ces salopes collent mon chibre salope Askip, t'es mon re-frè, mais bon, j'sens qu'tu m'manques d'honnêteté han J'ai répondu présent au charbon en hiver mais j'ai fait plus de cash en été han Bâtard, j'sais bien qu'tu connais tchi, t'as zéro connexion Dans le tier-quar, tu peux cher-bran que les p'tits T'as zéro connexion, dans le tier-quar, tu peux cher-bran que les p'tits Sur Insta', elle est gée-char, en vrai, elle est squelettique J'gaze, j'piétine, j'gaze, j'piétine, putain, on dirait qu'j'ai des tics Faut pas claquer, faut investir sur un 9 milli' ou une arme soviétique On sème le désordre, on sème la panique, du quartier, les poucaves seront toujours bannis Y a plus trop d'amis, des amitiés s'déchirent comme Tony et Many, c'est les descentes qui font monter l'adrénaline Tous mes couplets font l'effet d'un tsunami, la vie elle est cheum comme la grosse chatte à Marine salope Ou comme son daron Jean-Marie salope, si c'est une lope-sa, impossible que j'la marie Parfois, j'suis en perte, j'ai le mort quand ça m'arrive, après la perquis', j'en ai fait des cauchemars Tu ressors du shtar mais tu be-tom aussi vite que Schumacher ah bon ? Ils font les gros, ils sont trop marrants, comme le J, on agit en sous-marin Comme le J, on agit en sous-marin T'as zéro connexion dans le tier-quar, tu peux cher-bran que les p'tits T'as zéro connexion dans le tier-quar, tu peux cher-bran que les p'tits Sur Insta', elle est gée-char, en vrai, elle est squelettique eh, eh !</t>
         </is>
       </c>
     </row>
@@ -1109,7 +1109,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>J'souris quand le produit, j'le déballe Poh, poh, poh, poh J'souris quand le produit, j'le déballe faut du liquide, j'aime quand ça déborde J'aime quand ça les piétine en cassant des barres brr, le jackpot en cassant des portes Ce-pu d'gue-shla, dessus, y a pas d'amis tant qu'on n'a pas d'amis, la cagoule sera mise Pochton, pesette, couteau en céramique, pour taille-dé ou finir sur un mec uh 140 BPM, 140 au compteur, pas d'adrénaline Belek, y a les mes-ar à Staline uh, s'ils font les Sylvestr Stallon poh, poh, poh, poh C'est le cash pas la gloire qu'on voulait donc on s'n bats les c' si on reste à l'ombre han Dans la distribution, j'ai du talent, j'fais ma sse-pa, j'disparais d'une minute à l'autre oh On vient t'pull-up ton tieks mais y a aucun gars brr, devant l'brr, y'a plus aucun gab Ça t'doro, tu vas péter aucun câble, on rendra les ffaires-a dans aucun cas han Ces cons t'cala quand y a d'la skalape, quand y a d'la salope et d'la cons' calée eh Y a qu'avec des millions qu'on sera libres eh, on s'met sous calibre, crois pas qu'on s'est calmés C'est pour la mauvaise cause qu'on se rallie, si y avait pas des billets, on n'y serait pas allés J'monte sur Paris, j'suis en déplacement, dans les couilles, j'ai les pochons d'frappe qui t'paralyse wouh Combien d'sses-pa j'ai dû faire dans l'année pendant qu'j'te voyais t'faire ralentir par ta miss poh ? Y a ceux qui partent au niouf, d'autres qui partent à Nice Tu peux m'voir avec les négros qui parlent khaliss ah bon ? Il m'faut du putain d'cash à mort, il m'faut du putain d'she-ca à mort ah bon ? Tes gars au charbon, on les voit rarement, sous la North Face, j'ai d'quoi donner la mort brr Le tard-pé nehess pas dans l'armoire, , tu fais que d'penser à moi Pour qu'on vienne à dix, il suffit d'un mot, pour stopper l'ennemi, il suffit d'un mort On évite le zgah, on est tous gores, fais pas l'Hokage, y a des touches-car oui J'veux des lash'-Ka, elle veut que j'lâche cool, elle m'parle du pe-ra, j'm'en bats les couilles, gars oui Quand y a brouille-em, on est chiants, chaud bouillant sors le que-tru à mauvais escient Casse ta mère si pour ta ce-pla, t'as léché, quatre salaires, quatre tits-pe déter' te déchirent C'est elle ta meuf, elle est plate, elle est chime salope, elle consomme des plaquettes de shit salope Ça t'fait le coup d'la 10 à 20 ou du faux savon même si t'as grandi ici Cest la ue-r dans le fond et la forme, le tit-pe qui t'che-'rra, il a faim d'illicite poh J'lâche des flows tah l'époque des missions à Versailles quand j'étais pisté par les vils-ci poh Avant d'bicrave la douce, on a volé dur mmh, j'rentre défoncé dans ma bre-ch', j'ai vu les djinns mmh Tu khleh de l'équipe qui descend cagoulée mmh, t'as d'jà oublié tout c'que tu voulais dire mmh You might also like L'école, c'était casse-couilles, j'arrachais tout uh, j'sortais des cours Cache-cou, j'arrachais tout uh Mentalité vole tout et revend tout uh, uh, dégaine si ça veut hausser l'ton uh 9-2-1-4 sur l'pochton, 1-4 sur l'pochton Rentrer avec un billet, on l'fait tout l'temps poh, sinon, on pète les plombs poh L'école, c'était casse-couilles, j'arrachais tout, j'sortais des cours, Cache-cou, j'arrachais tout Mentalité vole tout et revend tout, dégaine si ça veut hausser l'ton uh 9-2-1-4 sur l'pochton poh, 1-4 sur l'pochton poh Rentrer avec un billet, on l'fait tout l'temps poh, poh, sinon, on pète les plombs poh On était jeunes et déter' dans la , on en a fait sauter des têtes Même si le plan est chaud, jai pas peur de monter Elle est trop cheum, normal, jai pas tendu mon teh Jcrois qu'cest la fin, té-ma les signes Belek téma la , bientôt ltremblement de terre Jlâche des flows, jfais kiffer l'monteur J'men sors de Nanterre comme un sacré menteur Jvais kiffé mon pers' poh, pourtant, on sort le truc qui fait moins peur poh Pourtant, on sort le truc qui fait moins d'pertes brr, brr, avant de tfaire, on tlaisse kiffer un peu brr Dans mon clan, que des gars qui font couler lsang Dans ltien, des putes qui prennent dans tous les sens Putain, jvoulais pas être blessant On a coffré des 9 millimètres mais pour ces putes, on va débouler sans L'école, c'était casse-couilles, j'arrachais tout, j'sortais des cours Cache-cou, j'arrachais tout2</t>
+          <t>J'souris quand le produit, j'le déballe Poh, poh, poh, poh J'souris quand le produit, j'le déballe faut du liquide, j'aime quand ça déborde J'aime quand ça les piétine en cassant des barres brr, le jackpot en cassant des portes Ce-pu d'gue-shla, dessus, y a pas d'amis tant qu'on n'a pas d'amis, la cagoule sera mise Pochton, pesette, couteau en céramique, pour taille-dé ou finir sur un mec uh 140 BPM, 140 au compteur, pas d'adrénaline Belek, y a les mes-ar à Staline uh, s'ils font les Sylvestr Stallon poh, poh, poh, poh C'est le cash pas la gloire qu'on voulait donc on s'n bats les c' si on reste à l'ombre han Dans la distribution, j'ai du talent, j'fais ma sse-pa, j'disparais d'une minute à l'autre oh On vient t'pull-up ton tieks mais y a aucun gars brr, devant l'brr, y'a plus aucun gab Ça t'doro, tu vas péter aucun câble, on rendra les ffaires-a dans aucun cas han Ces cons t'cala quand y a d'la skalape, quand y a d'la salope et d'la cons' calée eh Y a qu'avec des millions qu'on sera libres eh, on s'met sous calibre, crois pas qu'on s'est calmés C'est pour la mauvaise cause qu'on se rallie, si y avait pas des billets, on n'y serait pas allés J'monte sur Paris, j'suis en déplacement, dans les couilles, j'ai les pochons d'frappe qui t'paralyse wouh Combien d'sses-pa j'ai dû faire dans l'année pendant qu'j'te voyais t'faire ralentir par ta miss poh ? Y a ceux qui partent au niouf, d'autres qui partent à Nice Tu peux m'voir avec les négros qui parlent khaliss ah bon ? Il m'faut du putain d'cash à mort, il m'faut du putain d'she-ca à mort ah bon ? Tes gars au charbon, on les voit rarement, sous la North Face, j'ai d'quoi donner la mort brr Le tard-pé nehess pas dans l'armoire, , tu fais que d'penser à moi Pour qu'on vienne à dix, il suffit d'un mot, pour stopper l'ennemi, il suffit d'un mort On évite le zgah, on est tous gores, fais pas l'Hokage, y a des touches-car oui J'veux des lash'-Ka, elle veut que j'lâche cool, elle m'parle du pe-ra, j'm'en bats les couilles, gars oui Quand y a brouille-em, on est chiants, chaud bouillant sors le que-tru à mauvais escient Casse ta mère si pour ta ce-pla, t'as léché, quatre salaires, quatre tits-pe déter' te déchirent C'est elle ta meuf, elle est plate, elle est chime salope, elle consomme des plaquettes de shit salope Ça t'fait le coup d'la 10 à 20 ou du faux savon même si t'as grandi ici Cest la ue-r dans le fond et la forme, le tit-pe qui t'che-'rra, il a faim d'illicite poh J'lâche des flows tah l'époque des missions à Versailles quand j'étais pisté par les vils-ci poh Avant d'bicrave la douce, on a volé dur mmh, j'rentre défoncé dans ma bre-ch', j'ai vu les djinns mmh Tu khleh de l'équipe qui descend cagoulée mmh, t'as d'jà oublié tout c'que tu voulais dire mmh L'école, c'était casse-couilles, j'arrachais tout uh, j'sortais des cours Cache-cou, j'arrachais tout uh Mentalité vole tout et revend tout uh, uh, dégaine si ça veut hausser l'ton uh 9-2-1-4 sur l'pochton, 1-4 sur l'pochton Rentrer avec un billet, on l'fait tout l'temps poh, sinon, on pète les plombs poh L'école, c'était casse-couilles, j'arrachais tout, j'sortais des cours, Cache-cou, j'arrachais tout Mentalité vole tout et revend tout, dégaine si ça veut hausser l'ton uh 9-2-1-4 sur l'pochton poh, 1-4 sur l'pochton poh Rentrer avec un billet, on l'fait tout l'temps poh, poh, sinon, on pète les plombs poh On était jeunes et déter' dans la , on en a fait sauter des têtes Même si le plan est chaud, jai pas peur de monter Elle est trop cheum, normal, jai pas tendu mon teh Jcrois qu'cest la fin, té-ma les signes Belek téma la , bientôt ltremblement de terre Jlâche des flows, jfais kiffer l'monteur J'men sors de Nanterre comme un sacré menteur Jvais kiffé mon pers' poh, pourtant, on sort le truc qui fait moins peur poh Pourtant, on sort le truc qui fait moins d'pertes brr, brr, avant de tfaire, on tlaisse kiffer un peu brr Dans mon clan, que des gars qui font couler lsang Dans ltien, des putes qui prennent dans tous les sens Putain, jvoulais pas être blessant On a coffré des 9 millimètres mais pour ces putes, on va débouler sans L'école, c'était casse-couilles, j'arrachais tout, j'sortais des cours Cache-cou, j'arrachais tout2</t>
         </is>
       </c>
     </row>
@@ -1126,7 +1126,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Ils sauront jamais c'qu'il y a dans ma tête, ils sauront jamais c'qu'il y a dans mon cur Au volant du rap game, j'suis à deux doigts d'ton-car Toutes mes idées claires ont été noircies par l'bon-char Toutes mes idées claires ont été noircies par l'bon-char La rue m'fait du pied, j'crois bien qu'j'ai l'bon charme J'peux pas quitter un re-frè, qui s'ra toujours la pour moi J'dévoilerai pas toute ma vie même si j'suis bercé par l'instrument Course poursuite, j'm'arrêtais pas, j'avais grave du shit dans les poumons Guette le prix du litron, tout l'monde allume tout l'monde J'avance même si le chemin est tout noir, transformer mes billets bleus en billets saumon Le ient-cli vient pécho pour oublier ce monde, posté sur l'bitume, j'attends qu'le bonheur se montre Y a ceux qui font les trucs et puis y a ceux qui commentent Faire des thunes, t'inquiètes, on sait faire comment On perd tout, on s'refait, et puis on recommence Ce son c'est pour tous les vrais charos comme moi Tu captes ma mentalité dans mes ceaux-mor Toujours la tête dans les sommes, plavon, évite d'aller sans moi La bonbonne est vide alors si tu veux ton shit, attends Crois pas qu'on peut pas t'retrouver si t'es chez ta tante Eteindre la concu', parfois j'y réfléchit, ça m'tente Pour faire une bonne cepu, minimum que des barrettes de 50 La bonbonne est vide alors si tu veux ton shit, attends Crois pas qu'on peut pas t'retrouver si t'es chez ta tante Eteindre la concu', parfois j'y réfléchit, ça m'tente Pour faire une bonne cepu, minimum que des barrettes de 50 You might also like Pas besoin d'alliance pour mener nos batailles J'm'éloigne des faux semblants, j'm'éloigne des batards J'viens représenter l'tier-quar, est-ce que tu m'entends ? Ça sent la perquis', j'reste éveillé à 6h du matin Le temps c'est d'l'argent, j'prends mon temps, j'm'en fout d'c'qu'il m'attend, la moitié des anciens, ils sont tous atteints C'est pour les re-frè toujours là au bon moment, y en a qu'esquivent les salades, t'inquiète, on connait ces charlatans Y en a qu'esquivent les salam, ça j'lai appris en rabbatant Faut s'rapprocher d'la salat et pas écouter la voix d'satan Si ça parle seulement monnaie, c'est normal qu'on s'entend Beaucoup d'entre eux se prétendent rappeurs en chantant Y a du doré et d'la verte, mon négro, ça dépend Vrai laud-sa, pas pour les meufs qu'il dépense Encore un mec che-lou qui vient pécho sa défonce On reconnait l'vil-ci, y a l'talkie qui dépasse La bonbonne est vide alors si tu veux ton shit, attends Crois pas qu'on peut pas t'retrouver si t'es chez ta tante Eteindre la concu', parfois j'y réfléchit, ça m'tente Pour faire une bonne cepu, minimum que des barrettes de 50 La bonbonne est vide alors si tu veux ton shit, attends Crois pas qu'on peut pas t'retrouver si t'es chez ta tante Eteindre la concu', parfois j'y réfléchit, ça m'tente Pour faire une bonne cepu, minimum que des barrettes de 50 Si tu veux ton shit, attends Si t'es chez ta tante Parfois j'y réfléchit, ça m'tente Que des barrettes de 50 Eh, eh !1</t>
+          <t>Ils sauront jamais c'qu'il y a dans ma tête, ils sauront jamais c'qu'il y a dans mon cur Au volant du rap game, j'suis à deux doigts d'ton-car Toutes mes idées claires ont été noircies par l'bon-char Toutes mes idées claires ont été noircies par l'bon-char La rue m'fait du pied, j'crois bien qu'j'ai l'bon charme J'peux pas quitter un re-frè, qui s'ra toujours la pour moi J'dévoilerai pas toute ma vie même si j'suis bercé par l'instrument Course poursuite, j'm'arrêtais pas, j'avais grave du shit dans les poumons Guette le prix du litron, tout l'monde allume tout l'monde J'avance même si le chemin est tout noir, transformer mes billets bleus en billets saumon Le ient-cli vient pécho pour oublier ce monde, posté sur l'bitume, j'attends qu'le bonheur se montre Y a ceux qui font les trucs et puis y a ceux qui commentent Faire des thunes, t'inquiètes, on sait faire comment On perd tout, on s'refait, et puis on recommence Ce son c'est pour tous les vrais charos comme moi Tu captes ma mentalité dans mes ceaux-mor Toujours la tête dans les sommes, plavon, évite d'aller sans moi La bonbonne est vide alors si tu veux ton shit, attends Crois pas qu'on peut pas t'retrouver si t'es chez ta tante Eteindre la concu', parfois j'y réfléchit, ça m'tente Pour faire une bonne cepu, minimum que des barrettes de 50 La bonbonne est vide alors si tu veux ton shit, attends Crois pas qu'on peut pas t'retrouver si t'es chez ta tante Eteindre la concu', parfois j'y réfléchit, ça m'tente Pour faire une bonne cepu, minimum que des barrettes de 50 Pas besoin d'alliance pour mener nos batailles J'm'éloigne des faux semblants, j'm'éloigne des batards J'viens représenter l'tier-quar, est-ce que tu m'entends ? Ça sent la perquis', j'reste éveillé à 6h du matin Le temps c'est d'l'argent, j'prends mon temps, j'm'en fout d'c'qu'il m'attend, la moitié des anciens, ils sont tous atteints C'est pour les re-frè toujours là au bon moment, y en a qu'esquivent les salades, t'inquiète, on connait ces charlatans Y en a qu'esquivent les salam, ça j'lai appris en rabbatant Faut s'rapprocher d'la salat et pas écouter la voix d'satan Si ça parle seulement monnaie, c'est normal qu'on s'entend Beaucoup d'entre eux se prétendent rappeurs en chantant Y a du doré et d'la verte, mon négro, ça dépend Vrai laud-sa, pas pour les meufs qu'il dépense Encore un mec che-lou qui vient pécho sa défonce On reconnait l'vil-ci, y a l'talkie qui dépasse La bonbonne est vide alors si tu veux ton shit, attends Crois pas qu'on peut pas t'retrouver si t'es chez ta tante Eteindre la concu', parfois j'y réfléchit, ça m'tente Pour faire une bonne cepu, minimum que des barrettes de 50 La bonbonne est vide alors si tu veux ton shit, attends Crois pas qu'on peut pas t'retrouver si t'es chez ta tante Eteindre la concu', parfois j'y réfléchit, ça m'tente Pour faire une bonne cepu, minimum que des barrettes de 50 Si tu veux ton shit, attends Si t'es chez ta tante Parfois j'y réfléchit, ça m'tente Que des barrettes de 50 Eh, eh !1</t>
         </is>
       </c>
     </row>
@@ -1143,7 +1143,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Ouais, mon gars Ouais, allô, allo, allô, allô, allô ? Eh, mais thabites où, toi ? Hein ? Eh, mais thabites où, toi ? Zéro Manu le Coq, y a que des dindins poh, on tallume sur la frappe qui téteint-guin poh Lope-sa est prête à quitter son gars, pour moi, lancien peut pousser des pains-guin Jamais rester en repli quand ça sbagarre brr, jretire pas mes bagues et tu peux mparler battle brr, brr Pcht, pcht, tiens, prends celle-là bâtard salope, ça ta lavé pour ton baptême salope, salope Jcrois que cest fini genre jbicrave des albums uh, tu peux mbiper, jte fais bosser la came uh Ça parle en filtré mais ils ont que dla com, uh connard, tes passé trois fois devant la cam uh, uh, uh 35, pas d'gomme-cogne sale con oui, côté Chicago pas Compton oui Comme dhab', mon son ne-tour dans les DOM-TOM oui, tes mort si tu perds la clé du Teum-Teum oui Tape une gestu en mode jfais du tam-tam hein, tu vends la C, en vrai, tu tapes-tapes hein On fait la guerre, cest pas équitable-table, on fait la guerre cest pas équitable-table poh, poh Jai enchaîné les plans même quand jétais keleh, tu m'appelais, j'te répondais à n'importe quelle heure viens là Ça fait des ous-s, t'es con si tu crois que ça galère, on marche sur ton terrain, y a même pas de goal Y a rien à faire ? Arrache un sac alors j'suis dans la bine-ca, hace mucho calor Dites bien à la proc' de fermer sa gueule, dans la rue elle mangerait des calottes Au studio j'fais l'taff sans Poliakov, y a garre-ba, on parle pas, on remplit la gov' Cette pute elle donne tout pour que j'la coffre, pour pas un rond certaines peuvent donner l'go J'ai des reufs qui peuvent plaider ma cause, équipe soudée comme les Dalton Quand j'rappe, té-ma les dégâts qu'j'cause té-ma les dégâts qu'j'cause J'pochtonne tout, j'monte faire des passes dé', quand j'ai brr, j'donne même quand j'ai pas, j'donne brr Même pour le pactole, j'vais pas pacter brr, fuck le tan-Shei, tant mieux Dieu nous pardonne brr Faut mailler c'est les p'tits qui t'le rappellent uh, que d'la peuf', les junkies me courent après uh Tu bombes mais tu cries Au secours après uh, si ça payait pas, ne crois pas qu'on rapperait Poto, la haine endurcit mes rates-pi poh, après la hassbah, ça sert à rien d'rappeler poh Dale-pé, j'espère que t'es sur tes appuis, ça sort un truc juste pour voir si t'es rapide ah bon ? Tu dis qu't'as pas peur mais ton cur palpite, palpite, j'm'en fous d'ses formes, c'est les billets qu'j'veux palper ah bon ? C'est pas pour les niara si on part au casse-pipe, ganté, cagoulé, casqué comme les Daft P' 1.4. on choque le quartier d'à côté, les porcs me sucent la queue, j'ai la côte hum On fait des affaires on n'est pas potes hum Poto si t'es pas réglo tu sautes hum Pourquoi quand on arrive tu chuchotes ? Ils veulent pas que j'kicke ils préfèrent que j'chante hum C'est ta meuf qui ramène les capotes hum, c'est ta meuf qui ramène les capotes hum J'ai connu l'gator pour faire mes premiers sous et mes premiers sons Dites à la miss que j'tiens pas mes promesses et que j'offre des cadeaux que pour mes surs Dites à la miss que j'tiens pas mes promesses et que j'offre des cadeaux que pour mes surs V'-esqui le 3-8 et les 3-6 han, j'ai pas l'temps d'rester assis han J'sais qu'on m'attend comme GTA VI, m'attend comme GTA VI C'est mon pilon qui tape ton cochi, pour que la kichta grossisse uh On rentre le plus tard possible uh, on rentre le plus tard possible uh, uh Maman m'a bercé, j'suis devenu bre-som oui, tu veux porter plainte, ça t'met un coup d'pression oui Est-ce-que les mecs que j'ai fait écoutent mes sons ? oui Est-ce-que les mecs que j'ai fait écoutent mes sons ? oui, oui Maman m'a bercé, j'suis devenu bre-som oui, tu veux porter plainte, ça t'met un coup d'pression oui Est-ce-que les mecs que j'ai fait écoutent mes sons ? oui Est-ce-que les mecs que j'ai fait écoutent mes sons ? Oui, oui, oui Est-ce-que les mecs que j'ai fait écoutent mes sons ? Aah, aah You might also like 35, pas d'gomme-cogne sale con, côté Chicago pas Compton Comme dhab' aah, aah, mon son ne-tour dans les DOM-TOM, tes mort si tu perds la clé du Teum-Teum Tape une gestu en mode jfais du tam-tam, tu vends la C, en vrai, tu tapes-tapes On fait la guerre, cest pas équitable-table, Cest pas équitable-table Eh, eh, eh, eh1</t>
+          <t>Ouais, mon gars Ouais, allô, allo, allô, allô, allô ? Eh, mais thabites où, toi ? Hein ? Eh, mais thabites où, toi ? Zéro Manu le Coq, y a que des dindins poh, on tallume sur la frappe qui téteint-guin poh Lope-sa est prête à quitter son gars, pour moi, lancien peut pousser des pains-guin Jamais rester en repli quand ça sbagarre brr, jretire pas mes bagues et tu peux mparler battle brr, brr Pcht, pcht, tiens, prends celle-là bâtard salope, ça ta lavé pour ton baptême salope, salope Jcrois que cest fini genre jbicrave des albums uh, tu peux mbiper, jte fais bosser la came uh Ça parle en filtré mais ils ont que dla com, uh connard, tes passé trois fois devant la cam uh, uh, uh 35, pas d'gomme-cogne sale con oui, côté Chicago pas Compton oui Comme dhab', mon son ne-tour dans les DOM-TOM oui, tes mort si tu perds la clé du Teum-Teum oui Tape une gestu en mode jfais du tam-tam hein, tu vends la C, en vrai, tu tapes-tapes hein On fait la guerre, cest pas équitable-table, on fait la guerre cest pas équitable-table poh, poh Jai enchaîné les plans même quand jétais keleh, tu m'appelais, j'te répondais à n'importe quelle heure viens là Ça fait des ous-s, t'es con si tu crois que ça galère, on marche sur ton terrain, y a même pas de goal Y a rien à faire ? Arrache un sac alors j'suis dans la bine-ca, hace mucho calor Dites bien à la proc' de fermer sa gueule, dans la rue elle mangerait des calottes Au studio j'fais l'taff sans Poliakov, y a garre-ba, on parle pas, on remplit la gov' Cette pute elle donne tout pour que j'la coffre, pour pas un rond certaines peuvent donner l'go J'ai des reufs qui peuvent plaider ma cause, équipe soudée comme les Dalton Quand j'rappe, té-ma les dégâts qu'j'cause té-ma les dégâts qu'j'cause J'pochtonne tout, j'monte faire des passes dé', quand j'ai brr, j'donne même quand j'ai pas, j'donne brr Même pour le pactole, j'vais pas pacter brr, fuck le tan-Shei, tant mieux Dieu nous pardonne brr Faut mailler c'est les p'tits qui t'le rappellent uh, que d'la peuf', les junkies me courent après uh Tu bombes mais tu cries Au secours après uh, si ça payait pas, ne crois pas qu'on rapperait Poto, la haine endurcit mes rates-pi poh, après la hassbah, ça sert à rien d'rappeler poh Dale-pé, j'espère que t'es sur tes appuis, ça sort un truc juste pour voir si t'es rapide ah bon ? Tu dis qu't'as pas peur mais ton cur palpite, palpite, j'm'en fous d'ses formes, c'est les billets qu'j'veux palper ah bon ? C'est pas pour les niara si on part au casse-pipe, ganté, cagoulé, casqué comme les Daft P' 1.4. on choque le quartier d'à côté, les porcs me sucent la queue, j'ai la côte hum On fait des affaires on n'est pas potes hum Poto si t'es pas réglo tu sautes hum Pourquoi quand on arrive tu chuchotes ? Ils veulent pas que j'kicke ils préfèrent que j'chante hum C'est ta meuf qui ramène les capotes hum, c'est ta meuf qui ramène les capotes hum J'ai connu l'gator pour faire mes premiers sous et mes premiers sons Dites à la miss que j'tiens pas mes promesses et que j'offre des cadeaux que pour mes surs Dites à la miss que j'tiens pas mes promesses et que j'offre des cadeaux que pour mes surs V'-esqui le 3-8 et les 3-6 han, j'ai pas l'temps d'rester assis han J'sais qu'on m'attend comme GTA VI, m'attend comme GTA VI C'est mon pilon qui tape ton cochi, pour que la kichta grossisse uh On rentre le plus tard possible uh, on rentre le plus tard possible uh, uh Maman m'a bercé, j'suis devenu bre-som oui, tu veux porter plainte, ça t'met un coup d'pression oui Est-ce-que les mecs que j'ai fait écoutent mes sons ? oui Est-ce-que les mecs que j'ai fait écoutent mes sons ? oui, oui Maman m'a bercé, j'suis devenu bre-som oui, tu veux porter plainte, ça t'met un coup d'pression oui Est-ce-que les mecs que j'ai fait écoutent mes sons ? oui Est-ce-que les mecs que j'ai fait écoutent mes sons ? Oui, oui, oui Est-ce-que les mecs que j'ai fait écoutent mes sons ? Aah, aah 35, pas d'gomme-cogne sale con, côté Chicago pas Compton Comme dhab' aah, aah, mon son ne-tour dans les DOM-TOM, tes mort si tu perds la clé du Teum-Teum Tape une gestu en mode jfais du tam-tam, tu vends la C, en vrai, tu tapes-tapes On fait la guerre, cest pas équitable-table, Cest pas équitable-table Eh, eh, eh, eh1</t>
         </is>
       </c>
     </row>
@@ -1160,7 +1160,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Paw Paw Y'a les 22, j'suis sur mes gardes, j'ai confiance en ma force et la force de mes gars Sur la balance, y'a les mmes-gra, si t'as balance, sur ta tête y'a un contrat Le terrain est mé-cra, j'canalise mon chakra, j'viens baiser l'pe-ra, j'me demande si j'dois cher-cra Qu'est-c'tu vas faire si des négros déboulent chez toi ? Le guetteur a crié, j'ai entendu sa voix Les keufs cherchent la bonbonne, ils vont jamais savoir et quand ils repartent, ça vend Le ient-cli vient per-cho, il éclate son cerveau, la miss elle dit qu'j'suis un salaud À force de croiser les chickens dans le tier-quar, j'crois qu'j'suis devenu parano Avant d'dormir, j'pense à la mort, si y'a embrouille, obligé d'vous mettre à l'amende T'as du mal à payer tes dettes, belek y'a une prime sur ta tête Jves-qui ldépôt, j'mets la tempête, si l'bosseur se fait pet', il met l'terrain en perte J'allume un royal, y a du doré et d'la verte, des renois cagoulés dans ton salon Fallait pas laisser ta fenêtre ouverte, tu t'fais pister en pleine transaction Les condés, ils t'ont retrouvé, j'rode, cagoulé, j'suis dans l'action Dans l'tier-quar, j'ai rien à prouver, y a embrouille, tu sais où nous trouver Tu peux repartir avec les sapes trouées, j'suis content quand je vois le sang couler J'suis content quand l'cent meujs de beuh j'l'ai écoulé, j'veux une sse-lia de toutes les couleurs Pendant ltemps plein, t'as mon son dans tes écouteurs, si t'as poucave, t'es plus un des nôtres bow Fils de pute, t'es un des leurs, bâtard, t'as vingt-quatre heures pour payer batard J'suis gentil, j't'ai laissé un délai, y'a un losse-bo à faire, j'viens de me réveiller Y'a un plavon à faire, j'pourrais pas bégayer, avant d'dormir, je cache une liasse sous l'oreiller You might also like J'me fais pister par les méchants, si tu dois des tals, on te fume, on t'fait du sale Les armes on connaît ça, t'inquiète on collectionne, j'visser dans l'bat, tous les jours, il faut qu'j'additionne Le rrain-té sous CR, les keufs, ils m'ont dit ça, tu vas donner tes mapessa J'enfile les gants pour faire des sous, le temps c'est d'l'argent, obligé d'me dépêcher J'me fais pister par les méchants, si tu dois des tals, on te fume, on t'fait du sale Les armes on connaît ça, t'inquiète on collectionne, j'visser dans l'bat, tous les jours, il faut qu'j'additionne Le rrain-té sous CR, les keufs, ils m'ont dit ça, tu vas donner tes mapessa J'enfile les gants pour faire des sous, le temps c'est d'l'argent, obligé d'me dépêcher 9-2-1-4-0 sur le poch'ton, je visser ces geushs mais la BAC veut m'empêcher Tu peux perdre tes affaires pendant la baston, igo, fais belek à ta chaîne Fuck les teus-shmi qui toquent à ma porte, j'ai la haine, maman m'a vu les mains attachées J'té-cla un kamas, j'ai les yeux rouges d'Itachi, le bosseur fait des tours, il surveille ta cachette 9-2-1-4-0 sur le poch'ton, je visser ces geushs mais la BAC veut m'empêcher Tu peux perdre tes affaires pendant la baston, igo, fais belek à ta chaîne Fuck les teus-shmi qui toquent à ma porte, j'ai la haine, maman m'a vu les mains attachées J'té-cla un kamas, j'ai les yeux rouges d'Itachi, le bosseur fait des tours, il surveille ta cachette Hein, 9-2-1-4-0 sur le poch'ton 9-2-1-4-0 sur le poch'ton, j'entends la portière, la bonbonne déjà jetée Salope, salope, brr, brr J'me fais pister par les méchants, si tu dois des tals, on te fume, on t'fait du sale Les armes on connaît ça, t'inquiète on collectionne, j'visser dans l'bat, tous les jours, il faut qu'j'additionne Le rrain-té sous CR, les keufs, ils m'ont dit ça, tu vas donner tes mapessa J'enfile les gants pour faire des sous, le temps c'est d'l'argent, obligé d'me dépêcher J'me fais pister par les méchants, si tu dois des tals, on te fume, on t'fait du sale Les armes on connaît ça, t'inquiète on collectionne, j'visser dans l'bat, tous les jours, il faut qu'j'additionne Le rrain-té sous CR, les keufs, ils m'ont dit ça, tu vas donner tes mapessa J'enfile les gants pour faire des sous, le temps c'est d'l'argent, obligé d'me dépêcher</t>
+          <t>Paw Paw Y'a les 22, j'suis sur mes gardes, j'ai confiance en ma force et la force de mes gars Sur la balance, y'a les mmes-gra, si t'as balance, sur ta tête y'a un contrat Le terrain est mé-cra, j'canalise mon chakra, j'viens baiser l'pe-ra, j'me demande si j'dois cher-cra Qu'est-c'tu vas faire si des négros déboulent chez toi ? Le guetteur a crié, j'ai entendu sa voix Les keufs cherchent la bonbonne, ils vont jamais savoir et quand ils repartent, ça vend Le ient-cli vient per-cho, il éclate son cerveau, la miss elle dit qu'j'suis un salaud À force de croiser les chickens dans le tier-quar, j'crois qu'j'suis devenu parano Avant d'dormir, j'pense à la mort, si y'a embrouille, obligé d'vous mettre à l'amende T'as du mal à payer tes dettes, belek y'a une prime sur ta tête Jves-qui ldépôt, j'mets la tempête, si l'bosseur se fait pet', il met l'terrain en perte J'allume un royal, y a du doré et d'la verte, des renois cagoulés dans ton salon Fallait pas laisser ta fenêtre ouverte, tu t'fais pister en pleine transaction Les condés, ils t'ont retrouvé, j'rode, cagoulé, j'suis dans l'action Dans l'tier-quar, j'ai rien à prouver, y a embrouille, tu sais où nous trouver Tu peux repartir avec les sapes trouées, j'suis content quand je vois le sang couler J'suis content quand l'cent meujs de beuh j'l'ai écoulé, j'veux une sse-lia de toutes les couleurs Pendant ltemps plein, t'as mon son dans tes écouteurs, si t'as poucave, t'es plus un des nôtres bow Fils de pute, t'es un des leurs, bâtard, t'as vingt-quatre heures pour payer batard J'suis gentil, j't'ai laissé un délai, y'a un losse-bo à faire, j'viens de me réveiller Y'a un plavon à faire, j'pourrais pas bégayer, avant d'dormir, je cache une liasse sous l'oreiller J'me fais pister par les méchants, si tu dois des tals, on te fume, on t'fait du sale Les armes on connaît ça, t'inquiète on collectionne, j'visser dans l'bat, tous les jours, il faut qu'j'additionne Le rrain-té sous CR, les keufs, ils m'ont dit ça, tu vas donner tes mapessa J'enfile les gants pour faire des sous, le temps c'est d'l'argent, obligé d'me dépêcher J'me fais pister par les méchants, si tu dois des tals, on te fume, on t'fait du sale Les armes on connaît ça, t'inquiète on collectionne, j'visser dans l'bat, tous les jours, il faut qu'j'additionne Le rrain-té sous CR, les keufs, ils m'ont dit ça, tu vas donner tes mapessa J'enfile les gants pour faire des sous, le temps c'est d'l'argent, obligé d'me dépêcher 9-2-1-4-0 sur le poch'ton, je visser ces geushs mais la BAC veut m'empêcher Tu peux perdre tes affaires pendant la baston, igo, fais belek à ta chaîne Fuck les teus-shmi qui toquent à ma porte, j'ai la haine, maman m'a vu les mains attachées J'té-cla un kamas, j'ai les yeux rouges d'Itachi, le bosseur fait des tours, il surveille ta cachette 9-2-1-4-0 sur le poch'ton, je visser ces geushs mais la BAC veut m'empêcher Tu peux perdre tes affaires pendant la baston, igo, fais belek à ta chaîne Fuck les teus-shmi qui toquent à ma porte, j'ai la haine, maman m'a vu les mains attachées J'té-cla un kamas, j'ai les yeux rouges d'Itachi, le bosseur fait des tours, il surveille ta cachette Hein, 9-2-1-4-0 sur le poch'ton 9-2-1-4-0 sur le poch'ton, j'entends la portière, la bonbonne déjà jetée Salope, salope, brr, brr J'me fais pister par les méchants, si tu dois des tals, on te fume, on t'fait du sale Les armes on connaît ça, t'inquiète on collectionne, j'visser dans l'bat, tous les jours, il faut qu'j'additionne Le rrain-té sous CR, les keufs, ils m'ont dit ça, tu vas donner tes mapessa J'enfile les gants pour faire des sous, le temps c'est d'l'argent, obligé d'me dépêcher J'me fais pister par les méchants, si tu dois des tals, on te fume, on t'fait du sale Les armes on connaît ça, t'inquiète on collectionne, j'visser dans l'bat, tous les jours, il faut qu'j'additionne Le rrain-té sous CR, les keufs, ils m'ont dit ça, tu vas donner tes mapessa J'enfile les gants pour faire des sous, le temps c'est d'l'argent, obligé d'me dépêcher</t>
         </is>
       </c>
     </row>
@@ -1177,7 +1177,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Fais belleck aux folles qui te veulent parce que tes célèbre Ceux qui rentrent au chtar en couple ressortent très souvent célib' Ils veulent pas que jmassois sur le rap même si la place est libre Tire sur la frappe qui tenvoie sur les satellites Quand tout va bien tout le monde tentoure quand tout va mal ça tévite Mauvaise cachette toi tu reviens le sac est vide Sur le rrain-té sous CR le charbonneur se sacrifie Avec la voix dans ma tête jpourrais faire de sacrés feat' J'me fais pister par les D qui sont à droite jvais vers la gauche, jvesqui deux fois lberlingot Jai l'mort quand jperd un billet, jmen ballec quand je perd la gow Dans sa tête cest un enfant donc pourquoi elle me parle de gosses Les ptits ont lâchés les vélos, sont dans le vol de motos Les grands ils ont trop matter ils veulent sacheter des gros matos Tas une meuf tas piqué tu réponds plus à tes vatos Tes quune pédale on veut plus de toi va ten Cest quand tu meurs quta vie commence réellement Zéro arme factice, jsuis dans lréel moi Parfois ya du doré qui peut tfaire tomber raide mort Comment trouver lsommeil sans ces billets auprès dmoi Auprès dmoi on traffic illégalement pour ceux qui sréveillent a 6 heures pour aller au khedma Pour ceux qui charbonnent à la puce cramée sur un vespa Pas ceux qui font genre quon est pote alors quils mconnaissent pas You might also like 1PLIKÉ il veut pas changer il parle toujours des mêmes thèmes Tant quma vie na pas changé comment veux-tu que je fasse ? Jvois le mal et le bien dans ma tête en train dfaire un bras dfer mec Sans smouiller comment veux-tu que je brasse Largent jai pas peur den faire mais, sur un mauvais plan je peux finir enfermé Largent jai pas peur den faire mais, sur un mauvais plan je peux finir enfermé 1PLIKÉ il veut pas changer il parle toujours des mêmes thèmes Tant quma vie na pas changé comment veux-tu que je fasse ? Jvois le mal et le bien dans ma tête en train dfaire un bras dfer mec Sans smouiller comment veux-tu que je brasse Largent jai pas peur den faire mais, sur un mauvais plan je peux finir enfermé Largent jai pas peur den faire mais, sur un mauvais plan je peux finir enfermé Ça commence en low kick, ça finit en coup dcoude Certains dmes gars dégainent direct ne pratiquent pas le kung fu Ya des mecs sans sentiment qui ne connaissent pas le coup dfoudre Ya des lames de 30 centimètres non on met pas des coups dfouets Langage codé au téléphone les keufs ils nous écoutent frère Largent fait pas lbonheur mais lbonheur ça coûte cher Dans tous les cas on repartira poussière, jpourrais tirer pour le premier qui ma pousser Trop dconneries on a fait étant mineur On se sacrifie même si lterrain est miné Tu tes fais péter jespère tas pas dis mon name Jaime quand lyencli a la dégaine dEminem Ils jouent les bandits, mais ils savent que jouer des rôles Pourquoi être riche sans être généreux a quoi bon être riche sans être généreux Chaque coups quon met te fais perdre tes neurones Cest quand tu meurs quta vie commence réellement Zéro arme factice, jsuis dans lréel moi Parfois ya du doré qui peut tfaire tomber raide mort Comment trouver lsommeil sans ces billets auprès dmoi Auprès dmoi on traffic illégalement pour ceux qui sréveillent a 6 heures pour aller au khedma Pour ceux qui charbonnent à la puce cramée sur un vespa Pas ceux qui font genre quon est pote alors quils mconnaissent pas 1pliké veut pas changer il parle toujours des mêmes thèmes, tant quma vie na pas changé comment veux-tu que je fasse Jvois le mal et le bien dans ma tête en train dfaire un bras dfer mec Sans smouiller comment veux-tu que je brasse Largent jai pas peur den faire mais, sur un mauvais plan je peux finir enfermé Largent jai pas peur den faire mais, sur un mauvais plan je peux finir enfermé 1pliké veut pas changer il parle toujours des mêmes thèmes tant quma vie na pas changé comment veux-tu que je fasse Jvois le mal et le bien dans ma tête en train dfaire un bras dfer mec Sans smouiller comment veux-tu que je brasse Largent jai pas peur den faire mais, sur un mauvais plan je peux finir enfermé Largent jai pas peur den faire mais, sur un mauvais plan je peux finir enfermé</t>
+          <t>Fais belleck aux folles qui te veulent parce que tes célèbre Ceux qui rentrent au chtar en couple ressortent très souvent célib' Ils veulent pas que jmassois sur le rap même si la place est libre Tire sur la frappe qui tenvoie sur les satellites Quand tout va bien tout le monde tentoure quand tout va mal ça tévite Mauvaise cachette toi tu reviens le sac est vide Sur le rrain-té sous CR le charbonneur se sacrifie Avec la voix dans ma tête jpourrais faire de sacrés feat' J'me fais pister par les D qui sont à droite jvais vers la gauche, jvesqui deux fois lberlingot Jai l'mort quand jperd un billet, jmen ballec quand je perd la gow Dans sa tête cest un enfant donc pourquoi elle me parle de gosses Les ptits ont lâchés les vélos, sont dans le vol de motos Les grands ils ont trop matter ils veulent sacheter des gros matos Tas une meuf tas piqué tu réponds plus à tes vatos Tes quune pédale on veut plus de toi va ten Cest quand tu meurs quta vie commence réellement Zéro arme factice, jsuis dans lréel moi Parfois ya du doré qui peut tfaire tomber raide mort Comment trouver lsommeil sans ces billets auprès dmoi Auprès dmoi on traffic illégalement pour ceux qui sréveillent a 6 heures pour aller au khedma Pour ceux qui charbonnent à la puce cramée sur un vespa Pas ceux qui font genre quon est pote alors quils mconnaissent pas 1PLIKÉ il veut pas changer il parle toujours des mêmes thèmes Tant quma vie na pas changé comment veux-tu que je fasse ? Jvois le mal et le bien dans ma tête en train dfaire un bras dfer mec Sans smouiller comment veux-tu que je brasse Largent jai pas peur den faire mais, sur un mauvais plan je peux finir enfermé Largent jai pas peur den faire mais, sur un mauvais plan je peux finir enfermé 1PLIKÉ il veut pas changer il parle toujours des mêmes thèmes Tant quma vie na pas changé comment veux-tu que je fasse ? Jvois le mal et le bien dans ma tête en train dfaire un bras dfer mec Sans smouiller comment veux-tu que je brasse Largent jai pas peur den faire mais, sur un mauvais plan je peux finir enfermé Largent jai pas peur den faire mais, sur un mauvais plan je peux finir enfermé Ça commence en low kick, ça finit en coup dcoude Certains dmes gars dégainent direct ne pratiquent pas le kung fu Ya des mecs sans sentiment qui ne connaissent pas le coup dfoudre Ya des lames de 30 centimètres non on met pas des coups dfouets Langage codé au téléphone les keufs ils nous écoutent frère Largent fait pas lbonheur mais lbonheur ça coûte cher Dans tous les cas on repartira poussière, jpourrais tirer pour le premier qui ma pousser Trop dconneries on a fait étant mineur On se sacrifie même si lterrain est miné Tu tes fais péter jespère tas pas dis mon name Jaime quand lyencli a la dégaine dEminem Ils jouent les bandits, mais ils savent que jouer des rôles Pourquoi être riche sans être généreux a quoi bon être riche sans être généreux Chaque coups quon met te fais perdre tes neurones Cest quand tu meurs quta vie commence réellement Zéro arme factice, jsuis dans lréel moi Parfois ya du doré qui peut tfaire tomber raide mort Comment trouver lsommeil sans ces billets auprès dmoi Auprès dmoi on traffic illégalement pour ceux qui sréveillent a 6 heures pour aller au khedma Pour ceux qui charbonnent à la puce cramée sur un vespa Pas ceux qui font genre quon est pote alors quils mconnaissent pas 1pliké veut pas changer il parle toujours des mêmes thèmes, tant quma vie na pas changé comment veux-tu que je fasse Jvois le mal et le bien dans ma tête en train dfaire un bras dfer mec Sans smouiller comment veux-tu que je brasse Largent jai pas peur den faire mais, sur un mauvais plan je peux finir enfermé Largent jai pas peur den faire mais, sur un mauvais plan je peux finir enfermé 1pliké veut pas changer il parle toujours des mêmes thèmes tant quma vie na pas changé comment veux-tu que je fasse Jvois le mal et le bien dans ma tête en train dfaire un bras dfer mec Sans smouiller comment veux-tu que je brasse Largent jai pas peur den faire mais, sur un mauvais plan je peux finir enfermé Largent jai pas peur den faire mais, sur un mauvais plan je peux finir enfermé</t>
         </is>
       </c>
     </row>
@@ -1194,7 +1194,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Batman, Batman Batman Batman, Batman Batman S Beat It Up Ayo, Ludo Quatre patrouilles, j'm'évapore comme Joséphine T'as des trucs sur toi, renoi t'aurais dû filer Trop d'histoires de salades qui nent-tour au vinaigre Elle voulait ton cash quand tu voulais la piner Ennemis dans l'kamas même si c'est d'la caille Une fois qu'j'ai roulé ça, obligé d'calciner J'en veux pas mais elle m'envoie son tinié J'veux ma villa, j'en ai marre de l'imaginer J'ai quitté l'rrain-te sur un coup d'tête comme Ziné' han J'ai quitté l'rrain-te sur un coup d'tête comme Ziné' han En cas d'pépin, j'appelle aucun grand T'inquiète pas, gros, j'ramèn que ma géné' han Pour skalape, ça peut t'massr comme le kiné J'suis zehef, mes démons n'veulent pas s'confiner Rentre à Chicago si t'as du cran ou si tu viens pour butiner Ça t'pull up devant ta nana, y a d'quoi faire courir la BAC et la Nat'' Jsuis plutôt Menace, fuck Tony Montana, na J'gue-lar la batman même s'ils sont tenaces, bande de putes L'amour des sommes, dans le tier-quar, c'est devenu une maladie L'argent comble le bonheur des hommes, mon négro Pourquoi t'as du mal à l'dire ? Bande de putes ah bon ? You might also like Et on veut tous le paradis, billets bleus, oranges, verts Kichta arc-en-ciel pour faire la diff', bande de putes ah bon ? Et on veut tous le paradis, billets bleus, oranges, verts Kichta arc-en-ciel pour faire la diff', bande de putes poh Il était pas dans l'embrouille, il s'est fait mêler, on reste bre-som même en journée ensoleillée J'tire un trait sur les mecs chelous, on se retrouvera si nos destins sont liés Tas déjà chaud mais on t'a pas ché-tou, bâtard, si j'sors le truc, c'est pour t'humilier Si j're-ti, gros, j'vais viser au milieu, si j're-ti, gros, j'vais viser au milieu Les ients-cli aiment la frappe du Rif, dans mon pocheton, la frappe vient du Maroc J'connais des mecs bien déter' qui visser pendant les concerts de rock Pourquoi l'argent nous fascine autant uh ? Pourquoi l'argent nous fascine autant uh ? Sur l'chemin du succès, j'prends le virage sans le clignotant Bientôt le feat' histoire de grignoter ici, les keufs, on les fait pivoter Quand j'prend l'micro, on dirait qu'j'suis dopé, c'est la pénurie mais j'suis encore OP On s'fait contrôler sur le bas-côté ouh, tous mes négros sont pas contents ouh Tu sais très bien qu'le temps, c'est du seille-o, ici, on déteste les pertes de temps brr Sourire du Joker quand j'suis devant la Batman Batman Ya ltata si tu sais pas t'battre, man brr Bâtard, y a du pilon tout jaune comme Pacman Pacman J'sers tout l'monde comme si j'suis barman Regarde dans les yeux quand tu m'serres la main En une journée, j'peux faire ton salaire, man J'niquais des neiman, j'étais encore gamin Peu d'temps après, j'ai revendu la lemon Les ients-cli ont faim, le bosseur les alimente Le terrain est fermé, il reste des aliments À la base, la racli, c'était une meuf clean Aujourd'hui, elle me déshabille moi Tu sais bien qu'on gère la mélo' J'en veux au condé qui en veut à mes loves J'peux te faire la guerre si tu veux prendre mes 'loss On peut s'faire la guerre si tu veux prendre mes 'loss Sourire du Joker quand j'suis devant la Batman Batman Ya ltata si tu sais pas t'battre, man brr Bâtard, y a du pilon tout jaune comme Pacman Pacman J'sers tout l'monde comme si j'suis barman Sourire du Joker quand j'suis devant la Batman Batman Ya ltata si tu sais pas t'battre, man brr Bâtard, y a du pilon tout jaune comme Pacman Pacman J'sers tout l'monde comme si j'suis barman</t>
+          <t>Batman, Batman Batman Batman, Batman Batman S Beat It Up Ayo, Ludo Quatre patrouilles, j'm'évapore comme Joséphine T'as des trucs sur toi, renoi t'aurais dû filer Trop d'histoires de salades qui nent-tour au vinaigre Elle voulait ton cash quand tu voulais la piner Ennemis dans l'kamas même si c'est d'la caille Une fois qu'j'ai roulé ça, obligé d'calciner J'en veux pas mais elle m'envoie son tinié J'veux ma villa, j'en ai marre de l'imaginer J'ai quitté l'rrain-te sur un coup d'tête comme Ziné' han J'ai quitté l'rrain-te sur un coup d'tête comme Ziné' han En cas d'pépin, j'appelle aucun grand T'inquiète pas, gros, j'ramèn que ma géné' han Pour skalape, ça peut t'massr comme le kiné J'suis zehef, mes démons n'veulent pas s'confiner Rentre à Chicago si t'as du cran ou si tu viens pour butiner Ça t'pull up devant ta nana, y a d'quoi faire courir la BAC et la Nat'' Jsuis plutôt Menace, fuck Tony Montana, na J'gue-lar la batman même s'ils sont tenaces, bande de putes L'amour des sommes, dans le tier-quar, c'est devenu une maladie L'argent comble le bonheur des hommes, mon négro Pourquoi t'as du mal à l'dire ? Bande de putes ah bon ? Et on veut tous le paradis, billets bleus, oranges, verts Kichta arc-en-ciel pour faire la diff', bande de putes ah bon ? Et on veut tous le paradis, billets bleus, oranges, verts Kichta arc-en-ciel pour faire la diff', bande de putes poh Il était pas dans l'embrouille, il s'est fait mêler, on reste bre-som même en journée ensoleillée J'tire un trait sur les mecs chelous, on se retrouvera si nos destins sont liés Tas déjà chaud mais on t'a pas ché-tou, bâtard, si j'sors le truc, c'est pour t'humilier Si j're-ti, gros, j'vais viser au milieu, si j're-ti, gros, j'vais viser au milieu Les ients-cli aiment la frappe du Rif, dans mon pocheton, la frappe vient du Maroc J'connais des mecs bien déter' qui visser pendant les concerts de rock Pourquoi l'argent nous fascine autant uh ? Pourquoi l'argent nous fascine autant uh ? Sur l'chemin du succès, j'prends le virage sans le clignotant Bientôt le feat' histoire de grignoter ici, les keufs, on les fait pivoter Quand j'prend l'micro, on dirait qu'j'suis dopé, c'est la pénurie mais j'suis encore OP On s'fait contrôler sur le bas-côté ouh, tous mes négros sont pas contents ouh Tu sais très bien qu'le temps, c'est du seille-o, ici, on déteste les pertes de temps brr Sourire du Joker quand j'suis devant la Batman Batman Ya ltata si tu sais pas t'battre, man brr Bâtard, y a du pilon tout jaune comme Pacman Pacman J'sers tout l'monde comme si j'suis barman Regarde dans les yeux quand tu m'serres la main En une journée, j'peux faire ton salaire, man J'niquais des neiman, j'étais encore gamin Peu d'temps après, j'ai revendu la lemon Les ients-cli ont faim, le bosseur les alimente Le terrain est fermé, il reste des aliments À la base, la racli, c'était une meuf clean Aujourd'hui, elle me déshabille moi Tu sais bien qu'on gère la mélo' J'en veux au condé qui en veut à mes loves J'peux te faire la guerre si tu veux prendre mes 'loss On peut s'faire la guerre si tu veux prendre mes 'loss Sourire du Joker quand j'suis devant la Batman Batman Ya ltata si tu sais pas t'battre, man brr Bâtard, y a du pilon tout jaune comme Pacman Pacman J'sers tout l'monde comme si j'suis barman Sourire du Joker quand j'suis devant la Batman Batman Ya ltata si tu sais pas t'battre, man brr Bâtard, y a du pilon tout jaune comme Pacman Pacman J'sers tout l'monde comme si j'suis barman</t>
         </is>
       </c>
     </row>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Ça fait trop longtemps qu'c'est mon tour, c'est les blocs qui m'entourent J'connais quasiment tout poh, poh, j'vois son gros cul passer, j'ai pas cassé mon cou poh, poh T'as pas craché mon dû, j'vais pas cacher mon douze J'big up les mecs du hall, les p'tits qui font des ousses', qui fuck la météo T'es en mala mais t'as rien d'plus qu'un autre, fin du jugement, zéro dommages collatéraux brr J'sais qu'ça s'ra pas le même drr quand on va tous canner brr J'montre une partie d'moi, j'sais même pas combien j'en ai J'dissimule ma joie, en vrai, j'sais pas si j'en ai han La vie d'vant moi mais j'me dis qu'j'suis pas si jeune han Imagine demain si je meurs, j'ramasse des cachets mais j'ai pas crié victoire J'ai d'autres projets que rester sous les projecteurs Même si t'es pas si cheum', j'veux pas ken avec toi Le Diable, ton possesseur, dans tes yeux, j'l'aperçois J'suis à 40 , j'le fais pour l'140, pour ma cité, j'me suis porté garant Tu fais péter l'tron-li, tu mets cent fois quarante Trahis pas ma confiance comme celle de Sankhara Grosses sses-lia sous scellés, j'y pense encore Grosses sses-lia sous scellés, j'y pense encore J'voulais rouler sur l'or en volant tes carats T'as voulu décale, t'as fait le grand écart pow J'attends une phase pour les baiser, suffit d'un mauvais coup, j'finis dans les faits div' Laisse-les venir à mille, dans la cave, y'a de quoi réduire leur effectif effectif Est-ce que t'auras le temps de chénef ? On sort le Dere', Dere', Dere', Deref' po-pow You might also like Bénéf', bénéf', bénéf', bénéf' On veut s'mettre en bénéf', bénéf', bénéf', bénéf' Comme Béné, Béné, Béné, Béné On veut s'mettre en bénéf', bénéf', bénéf', bénéf' Donc on sort le Dere', Dere', Dere', Deref' On sort le Dere', Dere', Dere', Deref' On veut s'mettre en bénéf', bénéf', bénéf', bénéfice J'ai changé la méthode mais j'ai pas changé d'objectif J'ai vendu pour ma pomme, le point d'vente, c'est moi qui l'ouvrait Pour vider mon sac, j'me postais à l'heure qu'j'voulais Demande à mes gars si j'dis vrai, tu fais l'mec, bâtard, on t'a vu bafouiller Fuck les tte-schmi', ils savent même pas fouiller Même s'ils sont full up, gros, on va même pas filer han, han Trop d'junkies, on les met tous à l'affilée han, han Tu cours, tu bétom, par terre, ça t'finit, par terre, ça t'finit J'big up les profs qui croyaient en moi, même même quand je n'croyais plus en moi-même J'cartonne pas la que-lo, gros, même si tu 3ein Dans l'tier-quar, tu sers à rien à rien J'ai baisé l'rap combien d'fois pour laisser tant d'enfants ? Il est encore sous césarienne 9.2.1.4.0 sur le pochton, c'est le 9 milli' qui vient couvrir mes arrières mes arrières J'attends une phase pour les baiser, suffit d'un mauvais coup, j'finis dans les faits div' Laisse-les venir à mille, dans la cave, y'a de quoi réduire leur effectif effectif Est-ce que t'auras le temps de chénef ? On sort le Dere', Dere', Dere', Deref' po-pow Bénéf', bénéf', bénéf', bénéf' On veut s'mettre en bénéf', bénéf', bénéf', bénéf' Comme Béné, Béné, Béné, Béné On veut s'mettre en bénéf', bénéf', bénéf', bénéf' Donc on sort le Dere', Dere', Dere', Deref' On sort le Dere', Dere', Dere', Deref' On veut s'mettre en bénéf', bénéf', bénéf', bénéfice J'ai changé la méthode mais j'ai pas changé d'objectif Eh moinamché, eh moinamché, eh moinamché Eh moinamché mnouka koumba, eh moinamché, eh moinamché mnouka koumba Eh moinamché bénéf,bénef, eh moinamché hougni houli, eh moinamché hougni houli</t>
+          <t>Ça fait trop longtemps qu'c'est mon tour, c'est les blocs qui m'entourent J'connais quasiment tout poh, poh, j'vois son gros cul passer, j'ai pas cassé mon cou poh, poh T'as pas craché mon dû, j'vais pas cacher mon douze J'big up les mecs du hall, les p'tits qui font des ousses', qui fuck la météo T'es en mala mais t'as rien d'plus qu'un autre, fin du jugement, zéro dommages collatéraux brr J'sais qu'ça s'ra pas le même drr quand on va tous canner brr J'montre une partie d'moi, j'sais même pas combien j'en ai J'dissimule ma joie, en vrai, j'sais pas si j'en ai han La vie d'vant moi mais j'me dis qu'j'suis pas si jeune han Imagine demain si je meurs, j'ramasse des cachets mais j'ai pas crié victoire J'ai d'autres projets que rester sous les projecteurs Même si t'es pas si cheum', j'veux pas ken avec toi Le Diable, ton possesseur, dans tes yeux, j'l'aperçois J'suis à 40 , j'le fais pour l'140, pour ma cité, j'me suis porté garant Tu fais péter l'tron-li, tu mets cent fois quarante Trahis pas ma confiance comme celle de Sankhara Grosses sses-lia sous scellés, j'y pense encore Grosses sses-lia sous scellés, j'y pense encore J'voulais rouler sur l'or en volant tes carats T'as voulu décale, t'as fait le grand écart pow J'attends une phase pour les baiser, suffit d'un mauvais coup, j'finis dans les faits div' Laisse-les venir à mille, dans la cave, y'a de quoi réduire leur effectif effectif Est-ce que t'auras le temps de chénef ? On sort le Dere', Dere', Dere', Deref' po-pow Bénéf', bénéf', bénéf', bénéf' On veut s'mettre en bénéf', bénéf', bénéf', bénéf' Comme Béné, Béné, Béné, Béné On veut s'mettre en bénéf', bénéf', bénéf', bénéf' Donc on sort le Dere', Dere', Dere', Deref' On sort le Dere', Dere', Dere', Deref' On veut s'mettre en bénéf', bénéf', bénéf', bénéfice J'ai changé la méthode mais j'ai pas changé d'objectif J'ai vendu pour ma pomme, le point d'vente, c'est moi qui l'ouvrait Pour vider mon sac, j'me postais à l'heure qu'j'voulais Demande à mes gars si j'dis vrai, tu fais l'mec, bâtard, on t'a vu bafouiller Fuck les tte-schmi', ils savent même pas fouiller Même s'ils sont full up, gros, on va même pas filer han, han Trop d'junkies, on les met tous à l'affilée han, han Tu cours, tu bétom, par terre, ça t'finit, par terre, ça t'finit J'big up les profs qui croyaient en moi, même même quand je n'croyais plus en moi-même J'cartonne pas la que-lo, gros, même si tu 3ein Dans l'tier-quar, tu sers à rien à rien J'ai baisé l'rap combien d'fois pour laisser tant d'enfants ? Il est encore sous césarienne 9.2.1.4.0 sur le pochton, c'est le 9 milli' qui vient couvrir mes arrières mes arrières J'attends une phase pour les baiser, suffit d'un mauvais coup, j'finis dans les faits div' Laisse-les venir à mille, dans la cave, y'a de quoi réduire leur effectif effectif Est-ce que t'auras le temps de chénef ? On sort le Dere', Dere', Dere', Deref' po-pow Bénéf', bénéf', bénéf', bénéf' On veut s'mettre en bénéf', bénéf', bénéf', bénéf' Comme Béné, Béné, Béné, Béné On veut s'mettre en bénéf', bénéf', bénéf', bénéf' Donc on sort le Dere', Dere', Dere', Deref' On sort le Dere', Dere', Dere', Deref' On veut s'mettre en bénéf', bénéf', bénéf', bénéfice J'ai changé la méthode mais j'ai pas changé d'objectif Eh moinamché, eh moinamché, eh moinamché Eh moinamché mnouka koumba, eh moinamché, eh moinamché mnouka koumba Eh moinamché bénéf,bénef, eh moinamché hougni houli, eh moinamché hougni houli</t>
         </is>
       </c>
     </row>
@@ -1228,7 +1228,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Yugo Daddy Jo Un billet et j'revis grâce aux zombies Buteur lacosté, tu connais la combi' Un billet et j'revis grâce aux zombies Buteur lacosté, tu connais la combi' J'en ai vu tomber, s'relever et courir, tomber, recourir Ford Focus, j'leur lâche pas d'sourire, insolent, j'dis pas Sorry Le CV est clean, le train d'vie est pourri, toi, t'as rien fait sinon, ça s'saurait Ça tient les manettes comme Sasori, envoie une équipe en mode Sosa, oui Que d'la haine à semer, le respect a sommeil, pour l'butin, la victime, j'suis prêt à l'assommer Déboule pétardé depuis qu't'as plus Uh, ça péta plus, une vie stable Uh Une vie sans bleu, près du sable Uh, uh, uh, combien d'fois j'ai dû rêver d'ça ? Combien d'fois j'ai dû changer mon vêt'-sur Poh ? Combien d'folles j'ai dû vexer Poh ? Combien d'fois ça les a coursé Poh ? Combien d'fois Poh, poh ? Nouvelle journée, y'a trop d'fourmis , là, j'suis pas en détente Uh, j'attends l'soir Un pied dehors, j'suis déjà en tort Han, un pied dehors, j'suis déjà en renta' han, han J'attends qu'ça pète, ça pète et j'me tard J'fume devant les tards', j'ai un esprit d'Meda, plus d'bonbonnes de pilon, j'oublie pas une dar Pour faire son empire, faut des bons soldats, fais pas genre t'as les drahems, c'est pas un drame Tant qu't'as la santé, prends soin d'toi Brr, toujours la même histoire L'État nous met l'suppositoire Brr, ils nous endorment, ressaisis-toi You might also like 1PLIKÉ, leur cauchemar, encore un accouchement, okay Sous soké, j'vais pas aller doucement, okay J'vais pas t'arranger, j'sais qu'tu vas tout smoker Elle veut cer-us, sa mâchoire s'est disloquée Sur la Lyca', pas d'appel manqué Sur la Lyca', pas d'appel manqué J'connais la vérité mais tu mens encore, la vérité mais tu mens encore Chez nous, c'qui rapporte le plus, gros, c'est la gratte J'connais les faux d'puis l'époque du dégradé Il faut jamais nous gratter, nan, jamais nous gratter Les tits-pe sont partout, les anciens sont par terre J'rentre dans un thème où j'm'en bats les couilles si t'aimes Uh Bats les c' du système Uh, uh, uh, cojo' consistantes Ouh, ouh Ouh, ouh Ouh, ouh Depuis midi, ça transforme la matière en cash, je viens d'là où ça monte tout c'que les porcs en cachent À l'étage, ça s'tue à la tâche, j'descends marquer , mon but, j'me tue à l'atteindre J'coupe les réseaux, mes soucis j'résous, un cavu à té-cô, pas envie d'en découdre Un ne-jeu, un bigo, trop la flemme de ger-bou Paw, ça pue, escampette, j'mets la poudre La bibi, j'l'approche à Apu, la copine est à fond, j'la branche un peu Deux bras, deux bes-j', ça fait quatre cent coups, tu m'connais, gros, ça fait plus d'quatre ans que J'ai compris qu't'es solo quand ça coule, Biggie, Marley, Tupac Shakur Prêt à le faire, on s'en fout d'c'que ça coûte Brr, prêt à l'faire, on s'en fout d'c'que ça coûte Brr, brr Parsème le seum vu que la vie est cheum, toi, tu brises pas les chaînes Casse, casse, casse, casser des tes-por, balayer devant la sienne J'encaisse, j'enchaîne, v'là les follasses devant la scène et me parle pas de corazón Tous les jours, la mort rien qu'on la sert Sert 1PLIKÉ, leur cauchemar, encore un accouchement, okay Sous soké, j'vais pas aller doucement, okay J'vais pas t'arranger, j'sais qu'tu vas tout smoker Elle veut cer-us, sa mâchoire s'est disloquée Sur la Lyca', pas d'appel manqué Sur la Lyca', pas d'appel manqué J'connais la vérité mais tu mens encore, la vérité mais tu mens encore Chez nous, c'qui rapporte le plus, gros, c'est la gratte J'connais les faux d'puis l'époque du dégradé Il faut jamais nous gratter, nan, jamais nous gratter Les tits-pe sont partout, les anciens sont par terre J'rentre dans un thème où j'm'en bats les couilles si t'aimes Uh Bats les c' du système Uh, uh, uh, cojo' consistantes Ouh, ouh Pa-pa-pa-pa-pa-pa-pah Ouh, ouh Ouh, ouh</t>
+          <t>Yugo Daddy Jo Un billet et j'revis grâce aux zombies Buteur lacosté, tu connais la combi' Un billet et j'revis grâce aux zombies Buteur lacosté, tu connais la combi' J'en ai vu tomber, s'relever et courir, tomber, recourir Ford Focus, j'leur lâche pas d'sourire, insolent, j'dis pas Sorry Le CV est clean, le train d'vie est pourri, toi, t'as rien fait sinon, ça s'saurait Ça tient les manettes comme Sasori, envoie une équipe en mode Sosa, oui Que d'la haine à semer, le respect a sommeil, pour l'butin, la victime, j'suis prêt à l'assommer Déboule pétardé depuis qu't'as plus Uh, ça péta plus, une vie stable Uh Une vie sans bleu, près du sable Uh, uh, uh, combien d'fois j'ai dû rêver d'ça ? Combien d'fois j'ai dû changer mon vêt'-sur Poh ? Combien d'folles j'ai dû vexer Poh ? Combien d'fois ça les a coursé Poh ? Combien d'fois Poh, poh ? Nouvelle journée, y'a trop d'fourmis , là, j'suis pas en détente Uh, j'attends l'soir Un pied dehors, j'suis déjà en tort Han, un pied dehors, j'suis déjà en renta' han, han J'attends qu'ça pète, ça pète et j'me tard J'fume devant les tards', j'ai un esprit d'Meda, plus d'bonbonnes de pilon, j'oublie pas une dar Pour faire son empire, faut des bons soldats, fais pas genre t'as les drahems, c'est pas un drame Tant qu't'as la santé, prends soin d'toi Brr, toujours la même histoire L'État nous met l'suppositoire Brr, ils nous endorment, ressaisis-toi 1PLIKÉ, leur cauchemar, encore un accouchement, okay Sous soké, j'vais pas aller doucement, okay J'vais pas t'arranger, j'sais qu'tu vas tout smoker Elle veut cer-us, sa mâchoire s'est disloquée Sur la Lyca', pas d'appel manqué Sur la Lyca', pas d'appel manqué J'connais la vérité mais tu mens encore, la vérité mais tu mens encore Chez nous, c'qui rapporte le plus, gros, c'est la gratte J'connais les faux d'puis l'époque du dégradé Il faut jamais nous gratter, nan, jamais nous gratter Les tits-pe sont partout, les anciens sont par terre J'rentre dans un thème où j'm'en bats les couilles si t'aimes Uh Bats les c' du système Uh, uh, uh, cojo' consistantes Ouh, ouh Ouh, ouh Ouh, ouh Depuis midi, ça transforme la matière en cash, je viens d'là où ça monte tout c'que les porcs en cachent À l'étage, ça s'tue à la tâche, j'descends marquer , mon but, j'me tue à l'atteindre J'coupe les réseaux, mes soucis j'résous, un cavu à té-cô, pas envie d'en découdre Un ne-jeu, un bigo, trop la flemme de ger-bou Paw, ça pue, escampette, j'mets la poudre La bibi, j'l'approche à Apu, la copine est à fond, j'la branche un peu Deux bras, deux bes-j', ça fait quatre cent coups, tu m'connais, gros, ça fait plus d'quatre ans que J'ai compris qu't'es solo quand ça coule, Biggie, Marley, Tupac Shakur Prêt à le faire, on s'en fout d'c'que ça coûte Brr, prêt à l'faire, on s'en fout d'c'que ça coûte Brr, brr Parsème le seum vu que la vie est cheum, toi, tu brises pas les chaînes Casse, casse, casse, casser des tes-por, balayer devant la sienne J'encaisse, j'enchaîne, v'là les follasses devant la scène et me parle pas de corazón Tous les jours, la mort rien qu'on la sert Sert 1PLIKÉ, leur cauchemar, encore un accouchement, okay Sous soké, j'vais pas aller doucement, okay J'vais pas t'arranger, j'sais qu'tu vas tout smoker Elle veut cer-us, sa mâchoire s'est disloquée Sur la Lyca', pas d'appel manqué Sur la Lyca', pas d'appel manqué J'connais la vérité mais tu mens encore, la vérité mais tu mens encore Chez nous, c'qui rapporte le plus, gros, c'est la gratte J'connais les faux d'puis l'époque du dégradé Il faut jamais nous gratter, nan, jamais nous gratter Les tits-pe sont partout, les anciens sont par terre J'rentre dans un thème où j'm'en bats les couilles si t'aimes Uh Bats les c' du système Uh, uh, uh, cojo' consistantes Ouh, ouh Pa-pa-pa-pa-pa-pa-pah Ouh, ouh Ouh, ouh</t>
         </is>
       </c>
     </row>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Shoot out Yamaica Wouh, wouh, wouh Be-be-be-beat by Yamaica Productions, baby Wouh, wouh J'dors pas, j'suis sous teu-teu Han, au charbon donc j'pars pas cet été Han Gros sac de beuh près d'la be-teu, t'as fumé, t'es tombé, pourtant, j'pensais t'aider Han, han L'implication à vie on s'était dit, ces cons descendent pour courir dans la cité Gros, dis-moi, c'est quelle vie ? Elle tapine pour la vie d'Elvi' Ah bon ? Sa chatte, elle pue mais elle a un sac LV Ah bon ? Bah bravo Bravo, brr, trop d'interdits, on a bravé Brr J'commence par des vols aggravés Brr, j'fini par voler les gravons Oui T'as bavé, bâtard, tu vas en baver Poh, on t'attrape, t'es n mode avion Poh L'appart', il est sale, il st rempli d'savons, c'est comme avant, y a toujours pas d'S.A.V Poh, poh Paro', j'm'endors sur mes affaires, ça envoie fort Oui, tu bandes sur les offres quand y a cagoule, gants Oui Faites rentrer les enfants, il veut pas cher-lâ, ça l'piétine en force Oui L'enquête est méchante, le buteur, il passe Salope, tranquille, c'est en faisant les sommes qu'on riposte Salope, salope Les filles bien d'aujourd'hui sont les futures 'tasses Poh, poh, les gosses de riches sont les futurs tox' Poh Eh, eh, calmez-vous Brr, j'suis revenu, maintenant, calmez-vous Brr J'ai pas la cote mais la proc', elle me veut, on t'éteint même si t'as un passé fou Uh La R, elle est vide, quand j'passe, elle est full, tu veux aller vite, gros, tu vas aller où Uh ? Finir à Miami comme Léo, charbonne, calcule pas les bas et les hauts You might also like Bouge ton tarma, des sous, y en a tellement Allô Vers chez nous, ça vit, mon gars, bat les couilles qu't'as l'mort Salope Zehef comme Sefyu qui allume un cocktail mo' Poh, poh, le produit emballé Toutankhamon Poh Tu veux la quer-ni, tu khalass les ballons, une mission en balle, pour nous, c'est balourd J'les vois, ils sont pâles quand ça parle en palots Poh, poh, j'voulais v'-esqui la street, j'l'ai croisée au tel-hô Poh Hmm, celle-là j'la sens pas Ok, j't'envoie la beugueuh comme Sativa Ok Dors pas, la puce est activée, j'l'ai ken, j'l'ai bloquée, elle faisait trop la diva Parfois, j'peux être relou comme un billet d'vingt, parfois, j'donne le sourire comme nouvel arrivage J'ai trois trous aux visages, ça fait peur aux riverains, tranquille, j'les gué-lar au prochain virage Bâtard J'ai fumé la Costa, la French Riviera, mes peines sont enfermées, ma haine est libérable Brr, brr, pah La concu' dans l'trafic, zéro dans le rap, faut investir en Afrique, non pas en Europe Eux, c'est des faux, ils sont pas honorables, ils veulent négocier, on envoie rien au rabais Ils sont bons qu'à ser-uc, je l'leur envoie Oral B, compte le bénéf quand la pute se r'habille Si ça payerait pas, on n'aurait pas rappé, avant d'voir la vida, j'pillais comme un rate-pi Mon pote agrippe son cou, il lui fait une khabib, jamais j'reconnais mes torts, toujours j'mets tapis Brr Le trajet est long mais bon, j'vais l'taper à pied, t'investis pas, t'as peur de finir à perte Loin d'moi les tapeurs, on préfère la verte, on sait qu't'es avec des bons mais j'suis loin d'la vérité Poh Baise la drill comme dans Everyday Bang, bang, elle sait que j'suis busy mais elle veut un date Bang, bang Tu veux douiller ? Ah bon ? J'vais t'enlever l'idée, à croire qu'ce con il veut dead Bang, bang Mmh Mmh, mmh, un pied dans leur tieks, que des changements d'tête Poh On est venu tout en black Poh, y aura pas d'changement d'thème Poh Ça pue la volaille, faut changer le teum, tu m'appelles Le sang, il a changé le deum Ça a levé ma cachette ça m'a mis le demon, posé sur le hazi, haze et la lemon Tu l'vois comme un dormeur, hassoul, il alimente, le calibre est p'tit, les dégâts sont immenses Eux, c'est pas des hommes, eux, c'est des garçons, ils mentent La Batman descend, y a même plus d'adré' qui monte Ils m'collent à la peau, j'crois qu'on a décrit mon teint, prêt à gravir les montagnes Décrit mon teint Des montagnes</t>
+          <t>Shoot out Yamaica Wouh, wouh, wouh Be-be-be-beat by Yamaica Productions, baby Wouh, wouh J'dors pas, j'suis sous teu-teu Han, au charbon donc j'pars pas cet été Han Gros sac de beuh près d'la be-teu, t'as fumé, t'es tombé, pourtant, j'pensais t'aider Han, han L'implication à vie on s'était dit, ces cons descendent pour courir dans la cité Gros, dis-moi, c'est quelle vie ? Elle tapine pour la vie d'Elvi' Ah bon ? Sa chatte, elle pue mais elle a un sac LV Ah bon ? Bah bravo Bravo, brr, trop d'interdits, on a bravé Brr J'commence par des vols aggravés Brr, j'fini par voler les gravons Oui T'as bavé, bâtard, tu vas en baver Poh, on t'attrape, t'es n mode avion Poh L'appart', il est sale, il st rempli d'savons, c'est comme avant, y a toujours pas d'S.A.V Poh, poh Paro', j'm'endors sur mes affaires, ça envoie fort Oui, tu bandes sur les offres quand y a cagoule, gants Oui Faites rentrer les enfants, il veut pas cher-lâ, ça l'piétine en force Oui L'enquête est méchante, le buteur, il passe Salope, tranquille, c'est en faisant les sommes qu'on riposte Salope, salope Les filles bien d'aujourd'hui sont les futures 'tasses Poh, poh, les gosses de riches sont les futurs tox' Poh Eh, eh, calmez-vous Brr, j'suis revenu, maintenant, calmez-vous Brr J'ai pas la cote mais la proc', elle me veut, on t'éteint même si t'as un passé fou Uh La R, elle est vide, quand j'passe, elle est full, tu veux aller vite, gros, tu vas aller où Uh ? Finir à Miami comme Léo, charbonne, calcule pas les bas et les hauts Bouge ton tarma, des sous, y en a tellement Allô Vers chez nous, ça vit, mon gars, bat les couilles qu't'as l'mort Salope Zehef comme Sefyu qui allume un cocktail mo' Poh, poh, le produit emballé Toutankhamon Poh Tu veux la quer-ni, tu khalass les ballons, une mission en balle, pour nous, c'est balourd J'les vois, ils sont pâles quand ça parle en palots Poh, poh, j'voulais v'-esqui la street, j'l'ai croisée au tel-hô Poh Hmm, celle-là j'la sens pas Ok, j't'envoie la beugueuh comme Sativa Ok Dors pas, la puce est activée, j'l'ai ken, j'l'ai bloquée, elle faisait trop la diva Parfois, j'peux être relou comme un billet d'vingt, parfois, j'donne le sourire comme nouvel arrivage J'ai trois trous aux visages, ça fait peur aux riverains, tranquille, j'les gué-lar au prochain virage Bâtard J'ai fumé la Costa, la French Riviera, mes peines sont enfermées, ma haine est libérable Brr, brr, pah La concu' dans l'trafic, zéro dans le rap, faut investir en Afrique, non pas en Europe Eux, c'est des faux, ils sont pas honorables, ils veulent négocier, on envoie rien au rabais Ils sont bons qu'à ser-uc, je l'leur envoie Oral B, compte le bénéf quand la pute se r'habille Si ça payerait pas, on n'aurait pas rappé, avant d'voir la vida, j'pillais comme un rate-pi Mon pote agrippe son cou, il lui fait une khabib, jamais j'reconnais mes torts, toujours j'mets tapis Brr Le trajet est long mais bon, j'vais l'taper à pied, t'investis pas, t'as peur de finir à perte Loin d'moi les tapeurs, on préfère la verte, on sait qu't'es avec des bons mais j'suis loin d'la vérité Poh Baise la drill comme dans Everyday Bang, bang, elle sait que j'suis busy mais elle veut un date Bang, bang Tu veux douiller ? Ah bon ? J'vais t'enlever l'idée, à croire qu'ce con il veut dead Bang, bang Mmh Mmh, mmh, un pied dans leur tieks, que des changements d'tête Poh On est venu tout en black Poh, y aura pas d'changement d'thème Poh Ça pue la volaille, faut changer le teum, tu m'appelles Le sang, il a changé le deum Ça a levé ma cachette ça m'a mis le demon, posé sur le hazi, haze et la lemon Tu l'vois comme un dormeur, hassoul, il alimente, le calibre est p'tit, les dégâts sont immenses Eux, c'est pas des hommes, eux, c'est des garçons, ils mentent La Batman descend, y a même plus d'adré' qui monte Ils m'collent à la peau, j'crois qu'on a décrit mon teint, prêt à gravir les montagnes Décrit mon teint Des montagnes</t>
         </is>
       </c>
     </row>
@@ -1262,7 +1262,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Y a pas qu'le buteur qui compte les secondes, y a des darons d'famille qui se cassent les os uh J'entends deux fois ma voix, du mal à capter l'réseau uh Jsais quya les r-shta sur les ondes J'ai rien divulguer chaque fois qu'j'prenais des llars nan, j'ai pas pris exemple sur les autres Zarma tu connais du monde, pourtant, t'sais pas qui est prêt à ter-sau poh Le gérant bé-tom, ça fait sourire les tits-pe Méfie-toi de celui qui t'en dis peu han J'ai ramassé plus, j'ai pas fait c'que j'ai pu Pourquoi j'oublie c'que j'ai ? J'repense à c'que j'ai plus Si l'monde est à nous, il est surtout à moi Même si la terre elle sinnondera tu m'as pas vu cher-lâ et prendre mon avenir à deux mains J'ai mis boulette aux bacqueux qui tenaient mon bras Jsuis en train drleh les kepis ont vidé ma cachette, ça fait deux jours qu'j'réalise pas Ils savent rien du rrain-té à part celui qu'achète Pourtant, celui qui push se déguise pas J'ai des vices que ton tournevis ne dévisse pas On réinvestit l'bénéfice, on l'divise pas Tout l'monde t'entoure quand c'est fleurissant mais quand c'est la merda, tes potos, ils disent quoi ? J'm'enfume le veau-cer comme Boo comme Boo Pas d'boucan quand ça cambute cambute J'fucke le bout-mara comme Boo comme Boo J'fais a ma manière nan, j'aime pas faire comme vous comme vous J'm'enfume le veau-cer comme Boo comme Boo Pas d'boucan quand ça cambute cambute J'fucke le bout-mara comme Boo comme Boo J'fais a ma manière, nan, j'aime pas faire comme vous comme vous You might also like Comme Boo, j'ai pas besoin du marabout Comme Boo, j'ai pas besoin du marabout drr M'éloigner des vices et des tes-traî drr, drr, c'est pas ça qui m'a attristé drr Comme Boo, j'ai pas besoin du marabout Comme Boo, j'ai pas besoin du marabout po-poh La monnaie nous a fait perdre la te-tê po-poh, eux, c'est l'rap qui les a matrixé po-poh C'est l'heure de se mettre à table, t'es pas invité, ne viens pas gratter un bout Si t'as connu l'époque des freestyles, t'es un bon Si t'as saigné le volume 1, t'es un bon J'mets un pied hors du tieks, j'ai d'jà raté un bail, j'ai entendu ? tu me graille Ah bon, la flicaille, le 14, on va en prison , d'mande à , on laisse pas rentrer ces mabouls Ça t'allume sur des quettes-pla d'semi, t'es trop naïf, gros, arrête tes manies Est-ce que Sossa aurait arrêté Many ? C'est mes semblables qui viennent gâcher ton anniv' Quand ils sont chés-tout par la cleptomanie, c'est la tess qui m'épaule, c'est l'ghetto qui m'anime C'que j'raconte dans mes textes, c'est ma ie-v , j'voulais pas feater, j'voulais garder ma ligne J'fais des passes dé', j'm'en fous d'regarder la ligne Jsuis en train drleh les képis ont vidé ma cachette, ça fait deux jours qu'j'réalise pas Ils savent rien du rrain-té à part celui qu'achète Pourtant, celui qui push se déguise pas J'ai des vices que ton tournevis ne dévisse pas On réinvestit l'bénéfice, on l'divise pas Tout l'monde t'entoure quand c'est fleurissant han, han mais quand c'est la merda, tes potos, ils disent quoi han, let's go ? J'm'enfume le veau-cer comme Boo comme Boo Pas d'boucan quand ça cambute cambute J'fucke le bout-mara comme Boo comme Boo J'fais a ma manière, nan, j'aime pas faire comme vous comme vous J'm'enfume le veau-cer comme Boo comme Boo Pas d'boucan quand ça cambute cambute J'fucke le bout-mara comme Boo comme Boo J'fais a ma manière, nan, j'aime pas faire comme vous comme vous Comme Boo, j'ai pas besoin du marabout Comme Boo, j'ai pas besoin du marabout drr M'éloigner des vices et des te-traî, c'est pas ça qui m'a attristé drr Comme Boo, j'ai pas besoin du marabout Comme Boo, j'ai pas besoin du marabout po-poh La monnaie nous a fait perdre la te-tê po-poh, eux, c'est l'rap qui les a matrixé po-poh J'm'enfume le veau-cer comme Boo comme Boo Pas d'boucan quand ça cambute cambute J'fucke le bout-mara comme comme J'fais a ma manière ,nan, j'aime pas faire comme vous comme vous J'm'enfume le veau-cer comme Boo comme Boo Pas d'boucan quand ça cambute cambute J'fucke le bout-mara comme comme J'fais c'que j'veux, nan, j'aime pas faire comme vous comme vous Comme Boo, j'ai pas besoin du marabout Comme Boo, j'ai pas besoin du marabout drr M'éloigner des vices et des te-traî, c'est pas ça qui m'a attristé drr Comme Boo, j'ai pas besoin du marabout Comme Boo, j'ai pas besoin du marabout po-poh La monnaie nous a fait perdre la te-tê po-poh, eux, c'est l'rap qui les a matrixé po-poh Wou-ouh</t>
+          <t>Y a pas qu'le buteur qui compte les secondes, y a des darons d'famille qui se cassent les os uh J'entends deux fois ma voix, du mal à capter l'réseau uh Jsais quya les r-shta sur les ondes J'ai rien divulguer chaque fois qu'j'prenais des llars nan, j'ai pas pris exemple sur les autres Zarma tu connais du monde, pourtant, t'sais pas qui est prêt à ter-sau poh Le gérant bé-tom, ça fait sourire les tits-pe Méfie-toi de celui qui t'en dis peu han J'ai ramassé plus, j'ai pas fait c'que j'ai pu Pourquoi j'oublie c'que j'ai ? J'repense à c'que j'ai plus Si l'monde est à nous, il est surtout à moi Même si la terre elle sinnondera tu m'as pas vu cher-lâ et prendre mon avenir à deux mains J'ai mis boulette aux bacqueux qui tenaient mon bras Jsuis en train drleh les kepis ont vidé ma cachette, ça fait deux jours qu'j'réalise pas Ils savent rien du rrain-té à part celui qu'achète Pourtant, celui qui push se déguise pas J'ai des vices que ton tournevis ne dévisse pas On réinvestit l'bénéfice, on l'divise pas Tout l'monde t'entoure quand c'est fleurissant mais quand c'est la merda, tes potos, ils disent quoi ? J'm'enfume le veau-cer comme Boo comme Boo Pas d'boucan quand ça cambute cambute J'fucke le bout-mara comme Boo comme Boo J'fais a ma manière nan, j'aime pas faire comme vous comme vous J'm'enfume le veau-cer comme Boo comme Boo Pas d'boucan quand ça cambute cambute J'fucke le bout-mara comme Boo comme Boo J'fais a ma manière, nan, j'aime pas faire comme vous comme vous Comme Boo, j'ai pas besoin du marabout Comme Boo, j'ai pas besoin du marabout drr M'éloigner des vices et des tes-traî drr, drr, c'est pas ça qui m'a attristé drr Comme Boo, j'ai pas besoin du marabout Comme Boo, j'ai pas besoin du marabout po-poh La monnaie nous a fait perdre la te-tê po-poh, eux, c'est l'rap qui les a matrixé po-poh C'est l'heure de se mettre à table, t'es pas invité, ne viens pas gratter un bout Si t'as connu l'époque des freestyles, t'es un bon Si t'as saigné le volume 1, t'es un bon J'mets un pied hors du tieks, j'ai d'jà raté un bail, j'ai entendu ? tu me graille Ah bon, la flicaille, le 14, on va en prison , d'mande à , on laisse pas rentrer ces mabouls Ça t'allume sur des quettes-pla d'semi, t'es trop naïf, gros, arrête tes manies Est-ce que Sossa aurait arrêté Many ? C'est mes semblables qui viennent gâcher ton anniv' Quand ils sont chés-tout par la cleptomanie, c'est la tess qui m'épaule, c'est l'ghetto qui m'anime C'que j'raconte dans mes textes, c'est ma ie-v , j'voulais pas feater, j'voulais garder ma ligne J'fais des passes dé', j'm'en fous d'regarder la ligne Jsuis en train drleh les képis ont vidé ma cachette, ça fait deux jours qu'j'réalise pas Ils savent rien du rrain-té à part celui qu'achète Pourtant, celui qui push se déguise pas J'ai des vices que ton tournevis ne dévisse pas On réinvestit l'bénéfice, on l'divise pas Tout l'monde t'entoure quand c'est fleurissant han, han mais quand c'est la merda, tes potos, ils disent quoi han, let's go ? J'm'enfume le veau-cer comme Boo comme Boo Pas d'boucan quand ça cambute cambute J'fucke le bout-mara comme Boo comme Boo J'fais a ma manière, nan, j'aime pas faire comme vous comme vous J'm'enfume le veau-cer comme Boo comme Boo Pas d'boucan quand ça cambute cambute J'fucke le bout-mara comme Boo comme Boo J'fais a ma manière, nan, j'aime pas faire comme vous comme vous Comme Boo, j'ai pas besoin du marabout Comme Boo, j'ai pas besoin du marabout drr M'éloigner des vices et des te-traî, c'est pas ça qui m'a attristé drr Comme Boo, j'ai pas besoin du marabout Comme Boo, j'ai pas besoin du marabout po-poh La monnaie nous a fait perdre la te-tê po-poh, eux, c'est l'rap qui les a matrixé po-poh J'm'enfume le veau-cer comme Boo comme Boo Pas d'boucan quand ça cambute cambute J'fucke le bout-mara comme comme J'fais a ma manière ,nan, j'aime pas faire comme vous comme vous J'm'enfume le veau-cer comme Boo comme Boo Pas d'boucan quand ça cambute cambute J'fucke le bout-mara comme comme J'fais c'que j'veux, nan, j'aime pas faire comme vous comme vous Comme Boo, j'ai pas besoin du marabout Comme Boo, j'ai pas besoin du marabout drr M'éloigner des vices et des te-traî, c'est pas ça qui m'a attristé drr Comme Boo, j'ai pas besoin du marabout Comme Boo, j'ai pas besoin du marabout po-poh La monnaie nous a fait perdre la te-tê po-poh, eux, c'est l'rap qui les a matrixé po-poh Wou-ouh</t>
         </is>
       </c>
     </row>
@@ -1279,7 +1279,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Nan, nan, nan, nan, nan, nan Nan, nan, nan, nan, nan, nan, nan, nan Nan, nan, nan, nan, nan, nan, nan, nan Nan, nan, nan, nan, nan, nan, nan, nan Que des missions en tête chaque fois qu'j'ouvre les paupières Prêt à toutes les faires, j'me suis levé du bon pied On double la mise, on bande pas sur la recette d'hier C'est nous, on met l'fuego, c'est nous, on appelle les pompiers drr, drr, drr Chez nous, on commence la journée souvent en allant couper D'une peine, on peut écoper, donc on ramasse autant qu'on put pendant qu'ils cherchent à s'accouplr han Rencard sur Paname han, c'est pas pour s'mettre en couple han Laisse-moi t'raconter l'quotidien l'temps d'un couplet poh Sans la foi comment éviter d'être triste, sans risque, comment veux-tu être riche ? J'écris pas en fonction des rimes, j'prends l'cro-mi, j'crache la té-véri Ça pue la tess entre mes lignes, dans story bre-som, j'suis mêlé Titulaire, y a pas d'intérim, j'cause pas si y a pas d'intêret Parle moi d'la baraka, j'vesqui' l'malheur mais j'connais pas la chance uh Éclairé par le livre, j'écoute pas ceux qu'ont raconté leur chance uh Ça baraude tard la nuit, avec grave des tentations T'sais qu'il y a zéro compassion une fois qu'il y a d'moins en moins d'passants Maman s'inquiète pour mon avenir, elle s'demande c'que j'fais sur l'avenue ah bon ? J'ai aucun but dans la vie à part multiplier les revenus poh Protège tes proches, tes projets poh, dans l'peura, j'crois qu'j'les ai trop cheb poh Y'a que ton adresse qu'on recherche poh, poh, pour te faire, c'est jamais trop cher poh You might also like Batman sur le R mais bon, j'suis resté serein toujours serein Ils ont rien trouvé, j'crois qu'ils vont bientôt serrer ils vont serrer Elle veut un mec en place mais elle a pas d'oseille han Quand ça parle de seille-o han J'dois rentrer avec l'or dans les mains poh, poh, il m'en faut énormément poh, poh On s'est forgé en s'mêlant, y a qu'pour le cash qu'on se mélange drr J'mène double-vie, j'arrive pas à lâcher l'autre drr J'dois rentrer avec l'or dans les mains poh, poh, il m'en faut énormément poh, poh On s'est forgé en s'mêlant, y a qu'pour le cash qu'on se mélange drr J'mène double-vie, j'arrive pas à lâcher l'autre drr Comment veux-tu qu'on reste calmes ? Le coup d'extinct' nous fait plus d'mal Trop d'bavures comme si c'était légal, à quoi bon faire les diplomates ? Pas b'soin d'insister, les gars, remplit l'taille-dé, j'te parle pas des détails J'coupe, j'emballe, tu plies des sky', y'a des clics qui m'attendent dans l'bât' Problèmes, on assume, y'a des armes, t'inquiète, on assure Belek, ça exécute, poto, ça fait plus d'menaces On sourit quand c'est florissant, un reuf bé-tom, tout l'monde a l'seum Mon droit ch'min, un terrain glissant, j'combats l'mal, j'combats seul J'ai pas connu la misère, poto, ça s'rait mentir d'le dire J'l'ai fait pour acheter c'que j'voulais, tout d'suite sans demandé Mais j'sais qu'on devra des comptes , et q'j'suis pas là pour décorer Ils ont tremblé en tenant l'talkie, pas la peine de courir brr Batman sur le R mais bon, j'suis resté serein toujours serein Ils ont rien trouvé, j'crois qu'ils vont bientôt serrer ils vont serrer Elle veut un mec en place mais elle a pas d'oseille han Quand ça parle de seille-o han J'dois rentrer avec l'or dans les mains poh, poh, il m'en faut énormément poh, poh On s'est forgé en s'mêlant, y a qu'pour le cash qu'on se mélange drr J'mène double-vie, j'arrive pas à lâcher l'autre drr J'dois rentrer avec l'or dans les mains poh, poh, il m'en faut énormément poh, poh On s'est forgé en s'mêlant, y a qu'pour le cash qu'on se mélange drr J'mène double-vie, j'arrive pas à lâcher l'autre drr Nan, nan, nan, nan, nan, nan, nan, nan Nan, nan, nan, nan, nan, nan, nan, nan Nan, nan, nan, nan, nan, nan, nan, nan Nan, nan, nan, nan, nan, nan, nan, nan1</t>
+          <t>Nan, nan, nan, nan, nan, nan Nan, nan, nan, nan, nan, nan, nan, nan Nan, nan, nan, nan, nan, nan, nan, nan Nan, nan, nan, nan, nan, nan, nan, nan Que des missions en tête chaque fois qu'j'ouvre les paupières Prêt à toutes les faires, j'me suis levé du bon pied On double la mise, on bande pas sur la recette d'hier C'est nous, on met l'fuego, c'est nous, on appelle les pompiers drr, drr, drr Chez nous, on commence la journée souvent en allant couper D'une peine, on peut écoper, donc on ramasse autant qu'on put pendant qu'ils cherchent à s'accouplr han Rencard sur Paname han, c'est pas pour s'mettre en couple han Laisse-moi t'raconter l'quotidien l'temps d'un couplet poh Sans la foi comment éviter d'être triste, sans risque, comment veux-tu être riche ? J'écris pas en fonction des rimes, j'prends l'cro-mi, j'crache la té-véri Ça pue la tess entre mes lignes, dans story bre-som, j'suis mêlé Titulaire, y a pas d'intérim, j'cause pas si y a pas d'intêret Parle moi d'la baraka, j'vesqui' l'malheur mais j'connais pas la chance uh Éclairé par le livre, j'écoute pas ceux qu'ont raconté leur chance uh Ça baraude tard la nuit, avec grave des tentations T'sais qu'il y a zéro compassion une fois qu'il y a d'moins en moins d'passants Maman s'inquiète pour mon avenir, elle s'demande c'que j'fais sur l'avenue ah bon ? J'ai aucun but dans la vie à part multiplier les revenus poh Protège tes proches, tes projets poh, dans l'peura, j'crois qu'j'les ai trop cheb poh Y'a que ton adresse qu'on recherche poh, poh, pour te faire, c'est jamais trop cher poh Batman sur le R mais bon, j'suis resté serein toujours serein Ils ont rien trouvé, j'crois qu'ils vont bientôt serrer ils vont serrer Elle veut un mec en place mais elle a pas d'oseille han Quand ça parle de seille-o han J'dois rentrer avec l'or dans les mains poh, poh, il m'en faut énormément poh, poh On s'est forgé en s'mêlant, y a qu'pour le cash qu'on se mélange drr J'mène double-vie, j'arrive pas à lâcher l'autre drr J'dois rentrer avec l'or dans les mains poh, poh, il m'en faut énormément poh, poh On s'est forgé en s'mêlant, y a qu'pour le cash qu'on se mélange drr J'mène double-vie, j'arrive pas à lâcher l'autre drr Comment veux-tu qu'on reste calmes ? Le coup d'extinct' nous fait plus d'mal Trop d'bavures comme si c'était légal, à quoi bon faire les diplomates ? Pas b'soin d'insister, les gars, remplit l'taille-dé, j'te parle pas des détails J'coupe, j'emballe, tu plies des sky', y'a des clics qui m'attendent dans l'bât' Problèmes, on assume, y'a des armes, t'inquiète, on assure Belek, ça exécute, poto, ça fait plus d'menaces On sourit quand c'est florissant, un reuf bé-tom, tout l'monde a l'seum Mon droit ch'min, un terrain glissant, j'combats l'mal, j'combats seul J'ai pas connu la misère, poto, ça s'rait mentir d'le dire J'l'ai fait pour acheter c'que j'voulais, tout d'suite sans demandé Mais j'sais qu'on devra des comptes , et q'j'suis pas là pour décorer Ils ont tremblé en tenant l'talkie, pas la peine de courir brr Batman sur le R mais bon, j'suis resté serein toujours serein Ils ont rien trouvé, j'crois qu'ils vont bientôt serrer ils vont serrer Elle veut un mec en place mais elle a pas d'oseille han Quand ça parle de seille-o han J'dois rentrer avec l'or dans les mains poh, poh, il m'en faut énormément poh, poh On s'est forgé en s'mêlant, y a qu'pour le cash qu'on se mélange drr J'mène double-vie, j'arrive pas à lâcher l'autre drr J'dois rentrer avec l'or dans les mains poh, poh, il m'en faut énormément poh, poh On s'est forgé en s'mêlant, y a qu'pour le cash qu'on se mélange drr J'mène double-vie, j'arrive pas à lâcher l'autre drr Nan, nan, nan, nan, nan, nan, nan, nan Nan, nan, nan, nan, nan, nan, nan, nan Nan, nan, nan, nan, nan, nan, nan, nan Nan, nan, nan, nan, nan, nan, nan, nan1</t>
         </is>
       </c>
     </row>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>J'ai des reufs qui veulent me guider même si, ensemble, les interdits, on a bravé mais nan Nos liens, on a consolidé dans des vols aggravés, on n'a pas eu d'gravons mais nan J'fais semblant d'écouter quand cette pute, elle raconte sa vie, j'sais qu'j'vais rien mémoriser C'est pour péter l'salaire qu'on a dû salir, qu'est-ce que l'destin m'réserve après l'plavon ? On visser ta défonce on côtoie les camés On sait qu'on s'enfonce mais on continue quand même Les imite pas si tu veux pas finir comme eux J'mets tempête aux bacqueux, j'vais où le vent memmène Ça m'démange quand y a du papier à gratter, si t'es mon reuf, j'suis prêt à t'aider à grimper Dites à ces lopes-sa d'me lâcher la grappe uh, uh, j'peux pas acheter le temps à rattraper uh Tu peux pas vesqui' l'paiement, si tu fais l'mort, ça te réveille à la pelle On fait la guerre, on fait pas d'appel à la paix, est-ce que tu la veux vraiment ? Faut qu'ça défile tous les jours, mon frère, faut pas qu'ça soit un évènement wouh Faut qu'ça défile tous les jours, mon frère, faut pas qu'ça soit un évènement wouh Tu peux pas vesqui' l'paiement, si tu fais l'mort, ça te réveille à la pelle On fait la guerre, on fait pas d'appel à la paix, est-ce que tu la veux vraiment ? Faut qu'ça défile tous les jours, mon frère, faut pas qu'ça soit un évènement brr Faut qu'ça défile tous les jours, mon frère, faut pas qu'ça soit un évènement brr 9.2.1.4.0, 140-BRICKS, chez nous, la drill, c'est la mélodie du tieks ah bon J'vois les gyro' dans l'cavu, j'ai coffré un diez, nique la mère aux poucaves en diez-31-diez ah bon Tu t'rappelles à l'ancienne quand j'ai ouvert mon diez devant le pakat, j'les mettais tous en file indienne Ça défile tous les jours, mon frère, faire gonfler la paie quotidienne Elle a mouillé même si c'est une loc', ton son il est guez j'bouge même pas une locks Même pas une locks, t'as bossé deux semaines, t'as même pas eu d'loves han Bâtard, faut coffrer un billet et rebondir dessus, on tient le R, pas le mur, téma la posture Laisse pas traîner ton fils, sinon, il postule tes con si tu vois l'avenir dans la pe-stu You might also like Tu peux pas vesqui' l'paiement, si tu fais l'mort, ça te réveille à la pelle On fait la guerre, on fait pas d'appel à la paix, est-ce que tu la veux vraiment ? Faut qu'ça défile tous les jours, mon frère, faut pas qu'ça soit un évènement wouh Faut qu'ça défile tous les jours, mon frère, faut pas qu'ça soit un évènement wouh Tu peux pas vesqui' l'paiement, si tu fais l'mort, ça te réveille à la pelle On fait la guerre, on fait pas d'appel à la paix, est-ce que tu la veux vraiment ? Faut qu'ça défile tous les jours, mon frère, faut pas qu'ça soit un évènement brr Faut qu'ça défile tous les jours, mon frère, faut pas qu'ça soit un évènement brr On pense avoir gagné mais, quand on les tabasse, c'est des daronnes qui ré-pleu Quand j'y pense, je souris plus, enculé, tu l'as pas fermé poh quand t'aurais pu J'reçois d'l'amour mais j'ai plus d'attache poh, j'ressens plus rien pour ces pétasses poh T'as voulu brasser mais t'as bu la tasse brr, la tasse brr, miskine les victimes quon entasse brr 2-3 coups d'couteau, il est déjà coffré celui qu'a fait son taff emeuh On s'est servi quand on avait soif emeuh, bat les couilles de l'ancien qu'a fait son temps poh Tout ce temps, on a perdu à braver les interdits, chouara, on allait au moment tardif han Toi, tu fermes ta le-gueu quand ça parle biff poh, poh Tu peux pas vesqui' l'paiement, si tu fais l'mort, ça te réveille à la pelle On fait la guerre, on fait pas d'appel à la paix, est-ce que tu la veux vraiment ? Faut qu'ça défile tous les jours, mon frère, faut pas qu'ça soit un évènement wouh Faut qu'ça défile tous les jours, mon frère, faut pas qu'ça soit un évènement wouh Tu peux pas vesqui' l'paiement, si tu fais l'mort, ça te réveille à la pelle On fait la guerre, on fait pas d'appel à la paix, est-ce que tu la veux vraiment ? Faut qu'ça défile tous les jours, mon frère, faut pas qu'ça soit un évènement brr Faut qu'ça défile tous les jours, mon frère, faut pas qu'ça soit un évènement brr</t>
+          <t>J'ai des reufs qui veulent me guider même si, ensemble, les interdits, on a bravé mais nan Nos liens, on a consolidé dans des vols aggravés, on n'a pas eu d'gravons mais nan J'fais semblant d'écouter quand cette pute, elle raconte sa vie, j'sais qu'j'vais rien mémoriser C'est pour péter l'salaire qu'on a dû salir, qu'est-ce que l'destin m'réserve après l'plavon ? On visser ta défonce on côtoie les camés On sait qu'on s'enfonce mais on continue quand même Les imite pas si tu veux pas finir comme eux J'mets tempête aux bacqueux, j'vais où le vent memmène Ça m'démange quand y a du papier à gratter, si t'es mon reuf, j'suis prêt à t'aider à grimper Dites à ces lopes-sa d'me lâcher la grappe uh, uh, j'peux pas acheter le temps à rattraper uh Tu peux pas vesqui' l'paiement, si tu fais l'mort, ça te réveille à la pelle On fait la guerre, on fait pas d'appel à la paix, est-ce que tu la veux vraiment ? Faut qu'ça défile tous les jours, mon frère, faut pas qu'ça soit un évènement wouh Faut qu'ça défile tous les jours, mon frère, faut pas qu'ça soit un évènement wouh Tu peux pas vesqui' l'paiement, si tu fais l'mort, ça te réveille à la pelle On fait la guerre, on fait pas d'appel à la paix, est-ce que tu la veux vraiment ? Faut qu'ça défile tous les jours, mon frère, faut pas qu'ça soit un évènement brr Faut qu'ça défile tous les jours, mon frère, faut pas qu'ça soit un évènement brr 9.2.1.4.0, 140-BRICKS, chez nous, la drill, c'est la mélodie du tieks ah bon J'vois les gyro' dans l'cavu, j'ai coffré un diez, nique la mère aux poucaves en diez-31-diez ah bon Tu t'rappelles à l'ancienne quand j'ai ouvert mon diez devant le pakat, j'les mettais tous en file indienne Ça défile tous les jours, mon frère, faire gonfler la paie quotidienne Elle a mouillé même si c'est une loc', ton son il est guez j'bouge même pas une locks Même pas une locks, t'as bossé deux semaines, t'as même pas eu d'loves han Bâtard, faut coffrer un billet et rebondir dessus, on tient le R, pas le mur, téma la posture Laisse pas traîner ton fils, sinon, il postule tes con si tu vois l'avenir dans la pe-stu Tu peux pas vesqui' l'paiement, si tu fais l'mort, ça te réveille à la pelle On fait la guerre, on fait pas d'appel à la paix, est-ce que tu la veux vraiment ? Faut qu'ça défile tous les jours, mon frère, faut pas qu'ça soit un évènement wouh Faut qu'ça défile tous les jours, mon frère, faut pas qu'ça soit un évènement wouh Tu peux pas vesqui' l'paiement, si tu fais l'mort, ça te réveille à la pelle On fait la guerre, on fait pas d'appel à la paix, est-ce que tu la veux vraiment ? Faut qu'ça défile tous les jours, mon frère, faut pas qu'ça soit un évènement brr Faut qu'ça défile tous les jours, mon frère, faut pas qu'ça soit un évènement brr On pense avoir gagné mais, quand on les tabasse, c'est des daronnes qui ré-pleu Quand j'y pense, je souris plus, enculé, tu l'as pas fermé poh quand t'aurais pu J'reçois d'l'amour mais j'ai plus d'attache poh, j'ressens plus rien pour ces pétasses poh T'as voulu brasser mais t'as bu la tasse brr, la tasse brr, miskine les victimes quon entasse brr 2-3 coups d'couteau, il est déjà coffré celui qu'a fait son taff emeuh On s'est servi quand on avait soif emeuh, bat les couilles de l'ancien qu'a fait son temps poh Tout ce temps, on a perdu à braver les interdits, chouara, on allait au moment tardif han Toi, tu fermes ta le-gueu quand ça parle biff poh, poh Tu peux pas vesqui' l'paiement, si tu fais l'mort, ça te réveille à la pelle On fait la guerre, on fait pas d'appel à la paix, est-ce que tu la veux vraiment ? Faut qu'ça défile tous les jours, mon frère, faut pas qu'ça soit un évènement wouh Faut qu'ça défile tous les jours, mon frère, faut pas qu'ça soit un évènement wouh Tu peux pas vesqui' l'paiement, si tu fais l'mort, ça te réveille à la pelle On fait la guerre, on fait pas d'appel à la paix, est-ce que tu la veux vraiment ? Faut qu'ça défile tous les jours, mon frère, faut pas qu'ça soit un évènement brr Faut qu'ça défile tous les jours, mon frère, faut pas qu'ça soit un évènement brr</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Franklin Vrai charo, c'est tout pour le khaliss Grah, la be-her, chez nous, ça la légalise Pah 140, on les baise, c'est rapide Ouh, dans la zone, que du réel, pas d'factice Grah C'est connu, en deux-deux, on rapplique Grah, toujours accompagné d'mes rates-pi Pah Sur l'terrain, titulaire comme Messi Pah, pah, pah, la sécu' est toujours prête à rer-ti Même sous l'trac, au calme, on t'fera pire Brr, sur moi, que d'la pure, tous les 'loss en rappel Brr On t'fait solo, sur personne on s'appuie, le cripteur kleh alors qu'ça commence à peine Poh Livrette dans l'excès, la tchop, elle pue l'pilon Ah, meh, Sur moi, j'ai l'ze-trei, Opi', j'ai pris l'plus long Ah, meh 1.4.0, la découpe est excellente, j'les vois s'mettre à cé-us quand ils ont pas l'filon J'veux sentir aucun manque, aller toucher cher Brr mais la peugeuf, pas peur d'la toucher chère Brr Si y a plus rien dans l'keus, j'me ressers, pour sortir la frappy, j'affine mes recherches Brr C'est l'monde à l'envers, la fierté vaut cher, la pudeur se perd, la pute bosse en se-per Han En solo sans sécu', cette pute tartine en paix Hum, hum, si j'rentre avec mon gava, on la f'ra ramper Uh Le p'tit voulait la vie d'Arjen Robben, il s'est levé tôt l'tin-ma, il a dérobé Uh Les mains faites pour l'or, j'leur mets des goldens Pah ou bien, j'dégaine la lame à la Yajirobee Brr Gros, plein phares, sur les appuis, sale pute, plus tard Ah, meh, fallait qu'la kich' s'empile Ah, meh Ça débite de ouf dans la même chambre Ouh, que des textes sombres pour que mon tiekson brille Ouh On débitait sa mère pendant la pandémie Grah, j'ai très peu d'amis, beaucoup d'ennemis Grah J'suis dans la villa, j'ai té-cla l'Hennessy Pah, millions d'vues, normal qu'elle est tactile Ouh J'ai toujours la dalle comme un reptile Grah, on les encule, soyez pas surpris Pah Fin d'soirée, ma pétasse, elle m'excite Pah, pah, tu dégaines mais tu vas pas re-ti PahPas du genre à faire confiance aux filles mais ma soirée, j'la finis avec Sophie Grah Pour la résine, tiens mon zéro-six, tu veux bosser, mes potos, ils font tapine Grah Sur l'terrain, c'est TN ou Asics Pah, j'ai l'démon, rendez-vous chez la SPIP Pah On les encule avec Maxbi Grah, ça bicrave du lundi au lundi T'sais qu'on peut pas s'arrêter, j'viens d'me réveiller, j'dois gérer l'P Grah, grah J'dois gérer l'P Grah, grah, j'relance ma SIM dans l'GLC Ouh, ouh J'ai pé-ta un neuf, vise la sécurité Pah, pah, j'ai fait d'ma mission ma priorité Pah, pah Clamart connu pour les remontées Pah, pah, relance WhatsApp, on fait ça en paix Pah, pah Allez, fonce t'habiller, rate pas l'clip, tu sais qu'faut faire ça bien Pah Tartin débite, clients téléguidés Pah, fume la frappe, ça s'voit qu'il est pas ien-b Pah Hum, ça sent bon, ton pilon, il sort d'où ?, la question qu'j'entends sans tabou Grah, grah J'entends sans tabou, j'écoutais SeklenLand 5, j'ai ché-cra dans sa bouche Pah À midi, ça push, après-midi, ça push Ouh, minuit, j'ai zappé d'enlever la cagoule Ouh, flow AK-4.7, ça l'sort comme à Kaboul Grah You might also like Vrai charo, c'est tout pour le khaliss Grah, la be-her, chez nous, ça la légalise Pah 140, on les baise, c'est rapide Ouh, dans la zone, que du réel, pas d'factice Grah C'est connu, en deux-deux, on rapplique Grah, toujours accompagné d'mes rates-pi Pah Sur l'terrain, titulaire comme Messi Pah, pah, pah, la sécu' est toujours prête à rer-ti Même sous l'trac, au calme, on t'fera pire Brr, sur moi, que d'la pure, tous les 'loss en rappel Brr On fait solo, sur personne on s'appuie, le cripteur kleh alors qu'ça commence à peine Poh Livrette dans l'excès, la tchop, elle pue l'pilon Ah, meh, Sur moi, j'ai l'ze-trei, Opi', j'ai pris l'plus long Ah, meh 1.4.0, la découpe est excellente, j'les vois s'mettre à cé-us quand ils ont pas l'filon</t>
+          <t>Franklin Vrai charo, c'est tout pour le khaliss Grah, la be-her, chez nous, ça la légalise Pah 140, on les baise, c'est rapide Ouh, dans la zone, que du réel, pas d'factice Grah C'est connu, en deux-deux, on rapplique Grah, toujours accompagné d'mes rates-pi Pah Sur l'terrain, titulaire comme Messi Pah, pah, pah, la sécu' est toujours prête à rer-ti Même sous l'trac, au calme, on t'fera pire Brr, sur moi, que d'la pure, tous les 'loss en rappel Brr On t'fait solo, sur personne on s'appuie, le cripteur kleh alors qu'ça commence à peine Poh Livrette dans l'excès, la tchop, elle pue l'pilon Ah, meh, Sur moi, j'ai l'ze-trei, Opi', j'ai pris l'plus long Ah, meh 1.4.0, la découpe est excellente, j'les vois s'mettre à cé-us quand ils ont pas l'filon J'veux sentir aucun manque, aller toucher cher Brr mais la peugeuf, pas peur d'la toucher chère Brr Si y a plus rien dans l'keus, j'me ressers, pour sortir la frappy, j'affine mes recherches Brr C'est l'monde à l'envers, la fierté vaut cher, la pudeur se perd, la pute bosse en se-per Han En solo sans sécu', cette pute tartine en paix Hum, hum, si j'rentre avec mon gava, on la f'ra ramper Uh Le p'tit voulait la vie d'Arjen Robben, il s'est levé tôt l'tin-ma, il a dérobé Uh Les mains faites pour l'or, j'leur mets des goldens Pah ou bien, j'dégaine la lame à la Yajirobee Brr Gros, plein phares, sur les appuis, sale pute, plus tard Ah, meh, fallait qu'la kich' s'empile Ah, meh Ça débite de ouf dans la même chambre Ouh, que des textes sombres pour que mon tiekson brille Ouh On débitait sa mère pendant la pandémie Grah, j'ai très peu d'amis, beaucoup d'ennemis Grah J'suis dans la villa, j'ai té-cla l'Hennessy Pah, millions d'vues, normal qu'elle est tactile Ouh J'ai toujours la dalle comme un reptile Grah, on les encule, soyez pas surpris Pah Fin d'soirée, ma pétasse, elle m'excite Pah, pah, tu dégaines mais tu vas pas re-ti PahPas du genre à faire confiance aux filles mais ma soirée, j'la finis avec Sophie Grah Pour la résine, tiens mon zéro-six, tu veux bosser, mes potos, ils font tapine Grah Sur l'terrain, c'est TN ou Asics Pah, j'ai l'démon, rendez-vous chez la SPIP Pah On les encule avec Maxbi Grah, ça bicrave du lundi au lundi T'sais qu'on peut pas s'arrêter, j'viens d'me réveiller, j'dois gérer l'P Grah, grah J'dois gérer l'P Grah, grah, j'relance ma SIM dans l'GLC Ouh, ouh J'ai pé-ta un neuf, vise la sécurité Pah, pah, j'ai fait d'ma mission ma priorité Pah, pah Clamart connu pour les remontées Pah, pah, relance WhatsApp, on fait ça en paix Pah, pah Allez, fonce t'habiller, rate pas l'clip, tu sais qu'faut faire ça bien Pah Tartin débite, clients téléguidés Pah, fume la frappe, ça s'voit qu'il est pas ien-b Pah Hum, ça sent bon, ton pilon, il sort d'où ?, la question qu'j'entends sans tabou Grah, grah J'entends sans tabou, j'écoutais SeklenLand 5, j'ai ché-cra dans sa bouche Pah À midi, ça push, après-midi, ça push Ouh, minuit, j'ai zappé d'enlever la cagoule Ouh, flow AK-4.7, ça l'sort comme à Kaboul Grah Vrai charo, c'est tout pour le khaliss Grah, la be-her, chez nous, ça la légalise Pah 140, on les baise, c'est rapide Ouh, dans la zone, que du réel, pas d'factice Grah C'est connu, en deux-deux, on rapplique Grah, toujours accompagné d'mes rates-pi Pah Sur l'terrain, titulaire comme Messi Pah, pah, pah, la sécu' est toujours prête à rer-ti Même sous l'trac, au calme, on t'fera pire Brr, sur moi, que d'la pure, tous les 'loss en rappel Brr On fait solo, sur personne on s'appuie, le cripteur kleh alors qu'ça commence à peine Poh Livrette dans l'excès, la tchop, elle pue l'pilon Ah, meh, Sur moi, j'ai l'ze-trei, Opi', j'ai pris l'plus long Ah, meh 1.4.0, la découpe est excellente, j'les vois s'mettre à cé-us quand ils ont pas l'filon</t>
         </is>
       </c>
     </row>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>On peut serrer ton cou pour des sommes Bâtard, nous oblige pas à descendre Le rrain-te sous CR, les keufs, ils m'ont dit ça On a sorti le pétard, j'vois tout l'monde qui sort T'entends l'bruit du tard-pé qui raisonne brr J'aime bien quand la mu-mu, elle cartonne brr J'aime pas quand elle ne-tour au quartier À minuit, j'suis ganté et j'vais pas regretter il y a des mecs qui montent sur des plans sans redescendre J'ai té-cla mon pet et j'ai fait tombr des cendres La tnsion est montée normal qu'on va descendre À la fin du charbon, j'vais péter Vanessa Au bigo un ien-cli qui m'appelle, il m'harcèle j'me sens obliger De répondrebah ouais, j'me sens obliger d'en reprendrebah ouais, quand y'a plus de taille-dé j'penses au tals toutes les secondes Le ien-cli y râle quand j'lui dit qu'il y'en a plus 5 minutes après y'a une bombonne remplie J'suis dans l'bâtiment pour faire un billet en plus Ils font pas de sous de mala ils sont remplis Une équipe de malades devant ta porte Si j'pète une grosse somme c'est pour ma famille d'abord Paw Paw Tu veux des sous t'a qu'a bosser, tu dois des sous tu va finir cabosser Paw Paw Les keufs veulent péter le terrain c'est impossibleah bon, ils connaissent pas le nom du bosseur Même si j'suis reconnu par la victimeah bon, j'fais que nier devant l'inspecteur Et les plavons on noirci mon cur j'ai vu des images noir j'ai aggraver mon cas L'ange de la mort te regarde tous les jours et quand on va pull-up il monte sur la bécane J'ai les mains faites pour l'or là j'suis en train de détaille Y'a pas que le 14 que les keufs rentrent au bercail Une 10 ou une 20 c'est comme ça qu'on t'accueil Si on dit ça vient d'où gros tu vas tout donner Fuck les condés, Fuck la caméra sur le plavon j'vais tout donné J'empile les billets j'veux brasser comme Madonna Si j'vend des barrettes c'est pour me barrer de là T'es un menteur, t'es pas dans les vrais trucs J'montais sur des plans j'men balek t'avoir le trac et toute la journée j'vois que les chickens nous traques, et toute la journée j'vois que les chickens nous traques On allais voler tous les soirs j'avais la dalle des sous et j'voulais pas rentrer Tant que l'argent est pas rentrée, c'est qu'une te-pu dans ma vie elle veut rentrer brrr You might also like On peut serrer ton cou pour des sommes Bâtard, nous oblige pas à descendre Le rrain-te sous CR, les keufs, ils m'ont dit ça On a sorti le pétard, j'vois tout l'monde qui sort T'entends l'bruit du tard-pé qui raisonne brr J'aime bien quand la mu-mu, elle cartonne brr J'aime pas quand elle ne-tour au quartier À minuit, j'suis ganté et j'vais pas regretter On peut serrer ton cou pour des sommes Bâtard, nous oblige pas à descendre Le rrain-te sous CR, les keufs, ils m'ont dit ça On a sorti le pétard, j'vois tout l'monde qui sort T'entends l'bruit du tard-pé qui raisonne brr J'aime bien quand la mu-mu, elle cartonne brr J'aime pas quand elle ne-tour au quartier À minuit, j'suis ganté et j'vais pas regretter Parle pas au 22 règle numéro 1 Règle numéro 2 vissère pas les te-schmi Règle numéro 3 met la boulette aux schmitts Règle numéro 4 sert pas la main aux schmet J'irai jamais chekem dans ma vie Fils de pute toi t'es même pas serein dans ta ville Y'a les keufs j'cherche un truc à jeter La miss c'est une pute j'crois qu'elle fait que d'meujeuter Là j'suis sur le terrain j'veux pas finir menotté Sur la puce les ien-clis y sont numérotés Askip les amis ne s'achètent pas le seul que j'vais acheter y s'appelle beretta Au quartier les tartineurs font partir la pure, au quartier les poucaves sont guidés par la peur Y'en a qui pète scalap en cassant des vitres, y'en a qui pète scalap y font partir des litres Y'en a qui enchaîne les plavons et les délits y peuvent cacher une liasse sous le canapé-lit une sse-lia sous l'canapé-lit Et vu que c'est d'la moula y font que dm'appeller C'fils de pute il a changer de pays c'est fini, c'est fini il va jamais te payé J'me fait courser j'fini au télo J'me sens dans GTA quand j'vois les 5 étoiles bah ouais J'visser capuché le ien-cli m'reconnais pas bah ouais Les keufs c'est des putes y sont monté sur le toit bah ouais Tu fais l'insolent est-ce-que t'es sûr de toi, tu fais l'insolent est-ce-que t'es sûr de toi ? Toute la journée on re-détaille, y'a toujours des ien-clis sur mon tel Alors les épreuves j'vais surmonter On est descendu ils ont peur de remonter brrr On peut serrer ton cou pour des sommes Bâtard, nous oblige pas à descendre Le rrain-te sous CR, les keufs, ils m'ont dit ça On a sorti le pétard, j'vois tout l'monde qui sort T'entends l'bruit du tard-pé qui raisonne brr J'aime bien quand la mu-mu, elle cartonne brr J'aime pas quand elle ne-tour au quartier À minuit, j'suis ganté et j'vais pas regretter On peut serrer ton cou pour des sommes Bâtard, nous oblige pas à descendre Le rrain-te sous CR, les keufs, ils m'ont dit ça On a sorti le pétard, j'vois tout l'monde qui sort T'entends l'bruit du tard-pé qui raisonne brr J'aime bien quand la mu-mu, elle cartonne brr J'aime pas quand elle ne-tour au quartier À minuit, j'suis ganté et j'vais pas regretter</t>
+          <t>On peut serrer ton cou pour des sommes Bâtard, nous oblige pas à descendre Le rrain-te sous CR, les keufs, ils m'ont dit ça On a sorti le pétard, j'vois tout l'monde qui sort T'entends l'bruit du tard-pé qui raisonne brr J'aime bien quand la mu-mu, elle cartonne brr J'aime pas quand elle ne-tour au quartier À minuit, j'suis ganté et j'vais pas regretter il y a des mecs qui montent sur des plans sans redescendre J'ai té-cla mon pet et j'ai fait tombr des cendres La tnsion est montée normal qu'on va descendre À la fin du charbon, j'vais péter Vanessa Au bigo un ien-cli qui m'appelle, il m'harcèle j'me sens obliger De répondrebah ouais, j'me sens obliger d'en reprendrebah ouais, quand y'a plus de taille-dé j'penses au tals toutes les secondes Le ien-cli y râle quand j'lui dit qu'il y'en a plus 5 minutes après y'a une bombonne remplie J'suis dans l'bâtiment pour faire un billet en plus Ils font pas de sous de mala ils sont remplis Une équipe de malades devant ta porte Si j'pète une grosse somme c'est pour ma famille d'abord Paw Paw Tu veux des sous t'a qu'a bosser, tu dois des sous tu va finir cabosser Paw Paw Les keufs veulent péter le terrain c'est impossibleah bon, ils connaissent pas le nom du bosseur Même si j'suis reconnu par la victimeah bon, j'fais que nier devant l'inspecteur Et les plavons on noirci mon cur j'ai vu des images noir j'ai aggraver mon cas L'ange de la mort te regarde tous les jours et quand on va pull-up il monte sur la bécane J'ai les mains faites pour l'or là j'suis en train de détaille Y'a pas que le 14 que les keufs rentrent au bercail Une 10 ou une 20 c'est comme ça qu'on t'accueil Si on dit ça vient d'où gros tu vas tout donner Fuck les condés, Fuck la caméra sur le plavon j'vais tout donné J'empile les billets j'veux brasser comme Madonna Si j'vend des barrettes c'est pour me barrer de là T'es un menteur, t'es pas dans les vrais trucs J'montais sur des plans j'men balek t'avoir le trac et toute la journée j'vois que les chickens nous traques, et toute la journée j'vois que les chickens nous traques On allais voler tous les soirs j'avais la dalle des sous et j'voulais pas rentrer Tant que l'argent est pas rentrée, c'est qu'une te-pu dans ma vie elle veut rentrer brrr On peut serrer ton cou pour des sommes Bâtard, nous oblige pas à descendre Le rrain-te sous CR, les keufs, ils m'ont dit ça On a sorti le pétard, j'vois tout l'monde qui sort T'entends l'bruit du tard-pé qui raisonne brr J'aime bien quand la mu-mu, elle cartonne brr J'aime pas quand elle ne-tour au quartier À minuit, j'suis ganté et j'vais pas regretter On peut serrer ton cou pour des sommes Bâtard, nous oblige pas à descendre Le rrain-te sous CR, les keufs, ils m'ont dit ça On a sorti le pétard, j'vois tout l'monde qui sort T'entends l'bruit du tard-pé qui raisonne brr J'aime bien quand la mu-mu, elle cartonne brr J'aime pas quand elle ne-tour au quartier À minuit, j'suis ganté et j'vais pas regretter Parle pas au 22 règle numéro 1 Règle numéro 2 vissère pas les te-schmi Règle numéro 3 met la boulette aux schmitts Règle numéro 4 sert pas la main aux schmet J'irai jamais chekem dans ma vie Fils de pute toi t'es même pas serein dans ta ville Y'a les keufs j'cherche un truc à jeter La miss c'est une pute j'crois qu'elle fait que d'meujeuter Là j'suis sur le terrain j'veux pas finir menotté Sur la puce les ien-clis y sont numérotés Askip les amis ne s'achètent pas le seul que j'vais acheter y s'appelle beretta Au quartier les tartineurs font partir la pure, au quartier les poucaves sont guidés par la peur Y'en a qui pète scalap en cassant des vitres, y'en a qui pète scalap y font partir des litres Y'en a qui enchaîne les plavons et les délits y peuvent cacher une liasse sous le canapé-lit une sse-lia sous l'canapé-lit Et vu que c'est d'la moula y font que dm'appeller C'fils de pute il a changer de pays c'est fini, c'est fini il va jamais te payé J'me fait courser j'fini au télo J'me sens dans GTA quand j'vois les 5 étoiles bah ouais J'visser capuché le ien-cli m'reconnais pas bah ouais Les keufs c'est des putes y sont monté sur le toit bah ouais Tu fais l'insolent est-ce-que t'es sûr de toi, tu fais l'insolent est-ce-que t'es sûr de toi ? Toute la journée on re-détaille, y'a toujours des ien-clis sur mon tel Alors les épreuves j'vais surmonter On est descendu ils ont peur de remonter brrr On peut serrer ton cou pour des sommes Bâtard, nous oblige pas à descendre Le rrain-te sous CR, les keufs, ils m'ont dit ça On a sorti le pétard, j'vois tout l'monde qui sort T'entends l'bruit du tard-pé qui raisonne brr J'aime bien quand la mu-mu, elle cartonne brr J'aime pas quand elle ne-tour au quartier À minuit, j'suis ganté et j'vais pas regretter On peut serrer ton cou pour des sommes Bâtard, nous oblige pas à descendre Le rrain-te sous CR, les keufs, ils m'ont dit ça On a sorti le pétard, j'vois tout l'monde qui sort T'entends l'bruit du tard-pé qui raisonne brr J'aime bien quand la mu-mu, elle cartonne brr J'aime pas quand elle ne-tour au quartier À minuit, j'suis ganté et j'vais pas regretter</t>
         </is>
       </c>
     </row>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Au quartier les keufs sont pas en sécurité quand ils descendent, ils sortent la bombe lacrymogène Sur la route du succès jaccélère jmets des chalba à toutes ces pédales qui me gênent Jme tue au shit mais jsais qujpeux mourir jeune, jfume tout ces jaloux et ça pue lseum Faut pas perdre ses cojo même si ils sont plusieurs,, si j'te rotte-ca c'est pour les sous, pas pour l'plaisir L'injustice cultive la haine, sur mon front le M Toute ma vida y m'faut de l'argent à mort, y peut s'passer tellement d'choses en une seule semaine Batard, obligé d'esquiver ces zehmel, j'remercie Dieu juste après les avoir semés 9.2.1.4.0 sur le pochton, à la tombée d'la nuit tu croises que des mecs jnounés On caresse la première patrouille, aucune bavure policière sera pardonnée Comme mes sons, j'veux les voir cartonner Arrogant sur chéra si tu veux pas donner Il faut qu'tu coopères si tu veux pas d'ennuis. Tant qu'j'ai pas fais rentrer, j'peux pas encore dormir Dans cette vie là rien n'est gratuit, belek si tu bé-tom personne pour amortir Mentalité anti keufs zéro bluff, aucuns d'mes gavas passent aux aveux J'ai jamais su c'que j'voulais faire dans la vie, j'allais péta, j'laissais mon coeur dans la ve-ca Tu parles de flappys comme si t'en avais, tu parles de plavons comme si t'en as fait Tu m'verras jamais retourner ma veste, on allume au mortier le camp adverse! Pour faire ce cash sur un souffert, que des idées sombres dans ma tête on m'a soufflé A part de la haine j'ai rien à t'offrir, comme mes sous, mes sentiments j'les ai coffrés Ta vie défile sur un coup d'fil devant les mes-ar, tout les méchants devient sages Ton avenir ne tient qu'à un fil, le plus dur c'est pas la chute mais l'atterrissage Ta vie défile sur un coup d'fil devant les mes-ar, tout les méchants devient sagesYou might also like1</t>
+          <t>Au quartier les keufs sont pas en sécurité quand ils descendent, ils sortent la bombe lacrymogène Sur la route du succès jaccélère jmets des chalba à toutes ces pédales qui me gênent Jme tue au shit mais jsais qujpeux mourir jeune, jfume tout ces jaloux et ça pue lseum Faut pas perdre ses cojo même si ils sont plusieurs,, si j'te rotte-ca c'est pour les sous, pas pour l'plaisir L'injustice cultive la haine, sur mon front le M Toute ma vida y m'faut de l'argent à mort, y peut s'passer tellement d'choses en une seule semaine Batard, obligé d'esquiver ces zehmel, j'remercie Dieu juste après les avoir semés 9.2.1.4.0 sur le pochton, à la tombée d'la nuit tu croises que des mecs jnounés On caresse la première patrouille, aucune bavure policière sera pardonnée Comme mes sons, j'veux les voir cartonner Arrogant sur chéra si tu veux pas donner Il faut qu'tu coopères si tu veux pas d'ennuis. Tant qu'j'ai pas fais rentrer, j'peux pas encore dormir Dans cette vie là rien n'est gratuit, belek si tu bé-tom personne pour amortir Mentalité anti keufs zéro bluff, aucuns d'mes gavas passent aux aveux J'ai jamais su c'que j'voulais faire dans la vie, j'allais péta, j'laissais mon coeur dans la ve-ca Tu parles de flappys comme si t'en avais, tu parles de plavons comme si t'en as fait Tu m'verras jamais retourner ma veste, on allume au mortier le camp adverse! Pour faire ce cash sur un souffert, que des idées sombres dans ma tête on m'a soufflé A part de la haine j'ai rien à t'offrir, comme mes sous, mes sentiments j'les ai coffrés Ta vie défile sur un coup d'fil devant les mes-ar, tout les méchants devient sages Ton avenir ne tient qu'à un fil, le plus dur c'est pas la chute mais l'atterrissage Ta vie défile sur un coup d'fil devant les mes-ar, tout les méchants devient sages1</t>
         </is>
       </c>
     </row>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>9-2-1-4-0 sur le pocheton 1pliké1-4-0 dans ton enceinte Première partie J'traîne avec des dealers, jtraîne avec des receleurs, des casseurs de porte, des casseurs de neiman Y en a qui s'démarquent sur le terrain comme Neymar, qu'enchainent les transactions, ne contrôlent plus leurs mains Cramponné au bitume pour dla nnaie-mo, ça vend la mort qui put que t'réanimer Elle s'habill mal, mais elle fait la bimbo, y aura toujours un charo pour venir l'abîmer C'que j'peux faire aujourd'hui, j'remets pas à demain Pour la rre-gue, on est méchant quand on sy met On y va à fond, igo, crois pas quon simule Remplir son ventre, c'est bien, remplir ses poches, cest mieux Bavure policière, y a l'quartier qui s'émeute, faut qu'tu sois des nôtres Plus dretour en arrière quand t'as les menottes, on peut t'mélanger même si t'es neutre J'suis serein comme d'hab', la cité me suit, t'es pas d'ici, Bâtard j'm'en ballek, millions d'vues j'm'en ballek J'veux des millions d'euros dans la mallette, qualité, quantité, on a les deux Tire sur la frappe, tu t'fais galette Partie 2 Nique toutes les poucaves, nique toutes les michtoneuses Tu manques de courages, tu manques de corones J'suis dans l'decoupage d'instru à la tronçonneuse J'met l'peu-ra en période de grossesse Si sa sort un fer c'est pas pour te crosser Igo tu vas rien faire à part négocier J'connais des grossistes qui allument les p'tits, j'connais des tis-peu qui soulèves tes grossistes La rue a ses règles faut qu'tu respectes ses consignes Pas pouki c'est l'premier conseil, ou tu seras l'premier qu'on saigne Le gratteur attend juste que tu signe Alors qu'ils sont filmés ils sont rempli d'ciné On cherche le cash, tu cherches ta dulcinée On t'fais du catch si payes pas la taxe C'est sois tu brasses ou sois tu bois la tasse J'ai mis la goule-ca j'me suis pas voilé la face Ça fait un moment que des dégâts on en fait 1-4-0 ça flingue dans ton quartier d'en face J'suis ps venu raconter les faits On fait du le-sa depuis l'époque, on veut brûler les porcs, on veut casser les portes Dans tous les cas la guerre on remporte J'ai rêvé qu'l'ennemi partait en rampant J'comptais pas gagner ma vie en rappant Sur l'instru j'dérape, j'passe les rapports 1 an qu'j'suis dans l'peu-ra mais j'baise tes rappeurs Ma voix reste dans ta tête comme si j'suis thérapeute Traînes pas avec nous gros si tu fais la pince, ou si tu fais la pute Si tu t'fais rott-ca tu meurs dans l'film et dans la pub L'instru elle m'a donner son cul j'l'ai tecla sans pot-ca comme d'hab j'suis dans l'abus 9-2-1-4-0 sur le pocheton sur l'rain-té y'a les vile-ci dans des tribunesYou might also like</t>
+          <t>9-2-1-4-0 sur le pocheton 1pliké1-4-0 dans ton enceinte Première partie J'traîne avec des dealers, jtraîne avec des receleurs, des casseurs de porte, des casseurs de neiman Y en a qui s'démarquent sur le terrain comme Neymar, qu'enchainent les transactions, ne contrôlent plus leurs mains Cramponné au bitume pour dla nnaie-mo, ça vend la mort qui put que t'réanimer Elle s'habill mal, mais elle fait la bimbo, y aura toujours un charo pour venir l'abîmer C'que j'peux faire aujourd'hui, j'remets pas à demain Pour la rre-gue, on est méchant quand on sy met On y va à fond, igo, crois pas quon simule Remplir son ventre, c'est bien, remplir ses poches, cest mieux Bavure policière, y a l'quartier qui s'émeute, faut qu'tu sois des nôtres Plus dretour en arrière quand t'as les menottes, on peut t'mélanger même si t'es neutre J'suis serein comme d'hab', la cité me suit, t'es pas d'ici, Bâtard j'm'en ballek, millions d'vues j'm'en ballek J'veux des millions d'euros dans la mallette, qualité, quantité, on a les deux Tire sur la frappe, tu t'fais galette Partie 2 Nique toutes les poucaves, nique toutes les michtoneuses Tu manques de courages, tu manques de corones J'suis dans l'decoupage d'instru à la tronçonneuse J'met l'peu-ra en période de grossesse Si sa sort un fer c'est pas pour te crosser Igo tu vas rien faire à part négocier J'connais des grossistes qui allument les p'tits, j'connais des tis-peu qui soulèves tes grossistes La rue a ses règles faut qu'tu respectes ses consignes Pas pouki c'est l'premier conseil, ou tu seras l'premier qu'on saigne Le gratteur attend juste que tu signe Alors qu'ils sont filmés ils sont rempli d'ciné On cherche le cash, tu cherches ta dulcinée On t'fais du catch si payes pas la taxe C'est sois tu brasses ou sois tu bois la tasse J'ai mis la goule-ca j'me suis pas voilé la face Ça fait un moment que des dégâts on en fait 1-4-0 ça flingue dans ton quartier d'en face J'suis ps venu raconter les faits On fait du le-sa depuis l'époque, on veut brûler les porcs, on veut casser les portes Dans tous les cas la guerre on remporte J'ai rêvé qu'l'ennemi partait en rampant J'comptais pas gagner ma vie en rappant Sur l'instru j'dérape, j'passe les rapports 1 an qu'j'suis dans l'peu-ra mais j'baise tes rappeurs Ma voix reste dans ta tête comme si j'suis thérapeute Traînes pas avec nous gros si tu fais la pince, ou si tu fais la pute Si tu t'fais rott-ca tu meurs dans l'film et dans la pub L'instru elle m'a donner son cul j'l'ai tecla sans pot-ca comme d'hab j'suis dans l'abus 9-2-1-4-0 sur le pocheton sur l'rain-té y'a les vile-ci dans des tribunes</t>
         </is>
       </c>
     </row>
@@ -1381,7 +1381,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Première part J'ai connu l'argent sale dans le vol de keusa J'ai appris à brasser avec paire de requins Tu fais la mala, tu mets tes derniers pe-sa T'es pas sur la liste, au final tu t'fais recale La hagra ça paie pas, la hasba ça paie J'en ai mis des rotte-ca comme Cenoura Toi, tu bombes le torse devant les p'tits Tu fais moins l'malin quand c'est nous, hein ? Moins l'malin quand c'est nous, hein ? Faut toujours donner à ceux qui ont besoin Une 10 ou une 20 apple moi en cas d'besoin Lopinl peut viser ton torse ou ta be-jam On est trop têtu alors on tabasse les gens Askip fumer tue pourtant on tabasse le joint Elle veut prendre mes thunes elle aura ma 3 eme jambe La miss elle mconnais bien mais pourtant elle fait genre Mes negros peuvent pull-up ta chaîne quand il fait jour Si ta un collier tu seras pas immunisé Mes negros peuvent pull-up ta chaîne quand il fait jour Jai les idées claires même quand jsuis alcoolisé Même si je revends toute la noche jdois encore mreveiller tôt le matin Les vil-ci, les poucaves, les faux frères, les te-trai sont dans mon collimateur J'tabasse toutes les prods jusquà qu'ils retiennent mon nom Je fais ça en deuspi après ça je retourne dans lombre Jcommence les mains vides, jdégaine si ils sont en nombre Jdégaine si ils sont en nombre You might also likeDeuxième partie Askip tes mon reufré mais jsens qutu manque dhonnêteté On a charbonner en hiver pour faire plus de cash en été Batard jsais bien qutu connais tchi Tas 0 connexion Dans le tier-quar tu peut chebran que les ptits Tas 0 connexion Dans le tier-quar tu peut chebran que les ptits Sur insta elle est gechar En vrai elle est squelettique Jgaz, jpietine jgaz, jpietine Putain jcrois bien qujai des tics Faut pas claquer faut investir Pour le plavon en noir je suis vêtue Et si tu me croises gantés cest pas pour la température Jparle à limpératif comme ça cest sure qu'tu donnes les thunes Jai jamais su ce que je voulais faire dans la vie Mais jme vois pas faire de longues études Dans ta cité y a que des acteurs de dormeurs mon négros le savais-tu ? Ça sent la perquis jsuis lever avant six heures On commet des péchés, on commet trop derreurs, mais on a pas perdu la foi Jpeux pas rater l'service comme Federer, mais y a les condes derrière moi Jme sens pisté, ça sent le bacon Si on sent un ke-tru, tu lâcheras ta bécane Le trafic c'est pour l'bien même si c'est pas légal Le trafic c'est pour l'bien même si c'est pas légal J'ai pas attendu d'fumer pour trouver d'l'inspi' J'écrivais mes textes sur une puce de ient-cli</t>
+          <t>Première part J'ai connu l'argent sale dans le vol de keusa J'ai appris à brasser avec paire de requins Tu fais la mala, tu mets tes derniers pe-sa T'es pas sur la liste, au final tu t'fais recale La hagra ça paie pas, la hasba ça paie J'en ai mis des rotte-ca comme Cenoura Toi, tu bombes le torse devant les p'tits Tu fais moins l'malin quand c'est nous, hein ? Moins l'malin quand c'est nous, hein ? Faut toujours donner à ceux qui ont besoin Une 10 ou une 20 apple moi en cas d'besoin Lopinl peut viser ton torse ou ta be-jam On est trop têtu alors on tabasse les gens Askip fumer tue pourtant on tabasse le joint Elle veut prendre mes thunes elle aura ma 3 eme jambe La miss elle mconnais bien mais pourtant elle fait genre Mes negros peuvent pull-up ta chaîne quand il fait jour Si ta un collier tu seras pas immunisé Mes negros peuvent pull-up ta chaîne quand il fait jour Jai les idées claires même quand jsuis alcoolisé Même si je revends toute la noche jdois encore mreveiller tôt le matin Les vil-ci, les poucaves, les faux frères, les te-trai sont dans mon collimateur J'tabasse toutes les prods jusquà qu'ils retiennent mon nom Je fais ça en deuspi après ça je retourne dans lombre Jcommence les mains vides, jdégaine si ils sont en nombre Jdégaine si ils sont en nombre Deuxième partie Askip tes mon reufré mais jsens qutu manque dhonnêteté On a charbonner en hiver pour faire plus de cash en été Batard jsais bien qutu connais tchi Tas 0 connexion Dans le tier-quar tu peut chebran que les ptits Tas 0 connexion Dans le tier-quar tu peut chebran que les ptits Sur insta elle est gechar En vrai elle est squelettique Jgaz, jpietine jgaz, jpietine Putain jcrois bien qujai des tics Faut pas claquer faut investir Pour le plavon en noir je suis vêtue Et si tu me croises gantés cest pas pour la température Jparle à limpératif comme ça cest sure qu'tu donnes les thunes Jai jamais su ce que je voulais faire dans la vie Mais jme vois pas faire de longues études Dans ta cité y a que des acteurs de dormeurs mon négros le savais-tu ? Ça sent la perquis jsuis lever avant six heures On commet des péchés, on commet trop derreurs, mais on a pas perdu la foi Jpeux pas rater l'service comme Federer, mais y a les condes derrière moi Jme sens pisté, ça sent le bacon Si on sent un ke-tru, tu lâcheras ta bécane Le trafic c'est pour l'bien même si c'est pas légal Le trafic c'est pour l'bien même si c'est pas légal J'ai pas attendu d'fumer pour trouver d'l'inspi' J'écrivais mes textes sur une puce de ient-cli</t>
         </is>
       </c>
     </row>
@@ -1398,7 +1398,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>9.2.1.4.0 sur le pocheton 9.2.1.4.0 sur le pocheton 9.2.1.4.0 sur le pocheton 9.2.1.4.0 sur le pocheton si l'argent rend beau on tenlève ta beauté T'es un chaud quand tu bois la pisse du diable, qu'est-ce tu fais si on tenlève ta bouteille? Cagoulé à chaque fois que j'tenais l'sac pour pas glisser sur l'terrain comme Boateng On s'promène chez eux avec des béquilles, ce soir tous les ennemis vont boîter Fin d'G.A.V on m'dit fais pas d'bêtises, niqu ta grand-mère jressors et jfais d'la d Pour un 100 muj de beuh il faut qu'tu cotises, on a toujours la peu-fra qui t'fait bader Gros ça vise pas les beuj' ça vise ton cochi, si on thagar on hagar ton pote aussi Que des liasses dans mon assiette j'ai bien grossi Le cur noirci le mal nous amochi C'est une kakala avec toi elle fait la timide, faut sortir la kichta pour la faire gémir Bâtard j'vais pas quitter l'trône comme Vladimir Tu vas cracher les tals j'te l'ai déjà dit mec Opinel 13 j'cours même pas devant 10 mecs Byakugan j'rodave les 22 à 10 mètres Skalape en moins d'une heure me fait changer d'humeur, mhh Faut qu'ça pète comme les tours jumelles J'repense au passé j'avais zéro pitié, est-ce que j'vais rembourser les curs que j'ai cassé ? La haine j'ai attisé Tout va bien tant qu'la puce est activée, sur ma mère que j'vais jamais pactiser Négro , bois pas si tu sais pas tiser, la teille j'la bois cul sec Que des têtes cramées sur le banc des accusés C'est pas en tenant l'sac que t'auras un Q7 Bâtard la brigade canine elle veut péter mon shit Bellek ta frangine veut péter mon chibre J'vide la cristalline et je remplis mon sheuf Les porcs ils veulent péter mon shit Zéro démocratie c'est la voyoucratie Si, j'mélange vodka-cassis c'est toi qui vas payer les pots cassés Charbon, argent sale j'suis bon qu'à ça Ceux qui descendent ne veulent plus repasser J'traine avec des 3arbi que des gueules cassées Mali, Côte d'Ivoire, Congo-Kinshasa, tous mes comoriens j'viens dédicacer On va te gonfler si t'es trop kassa J'fais gonfler ma liasse j'vesqui la casa J'aime trop l'argent donc j'esquive le casin' J'aime pas trop les jeux d'hasard Insolent depuis minot, fuck l'amour, fuck Juliette et Roméo, fuck Zemmour et tous ses idéaux Le regard est froid, viens t'péta si t'es chaud 3endek ça peut t'qué-cho J'suis pas seul dans la bine-ca mon cerveau il chauffe Comme d'habitude le guetteur il chouf On fait la guerre protége bien tes abdominaux Rafale, paw, impossible qu'on échoue Ils savent pas s'péta mais ils s'croient dans Ong-bak 2, Ong-bak 2 J'ai rêvé que j'me fais coursé par 11 bacqueux, 11 bacqueux Nique la juge elle joue trop avec ma queue, elle joue trop avec ma queue J'représente le 92 ma gueule, le 92 ma gueuleYou might also like</t>
+          <t>9.2.1.4.0 sur le pocheton 9.2.1.4.0 sur le pocheton 9.2.1.4.0 sur le pocheton 9.2.1.4.0 sur le pocheton si l'argent rend beau on tenlève ta beauté T'es un chaud quand tu bois la pisse du diable, qu'est-ce tu fais si on tenlève ta bouteille? Cagoulé à chaque fois que j'tenais l'sac pour pas glisser sur l'terrain comme Boateng On s'promène chez eux avec des béquilles, ce soir tous les ennemis vont boîter Fin d'G.A.V on m'dit fais pas d'bêtises, niqu ta grand-mère jressors et jfais d'la d Pour un 100 muj de beuh il faut qu'tu cotises, on a toujours la peu-fra qui t'fait bader Gros ça vise pas les beuj' ça vise ton cochi, si on thagar on hagar ton pote aussi Que des liasses dans mon assiette j'ai bien grossi Le cur noirci le mal nous amochi C'est une kakala avec toi elle fait la timide, faut sortir la kichta pour la faire gémir Bâtard j'vais pas quitter l'trône comme Vladimir Tu vas cracher les tals j'te l'ai déjà dit mec Opinel 13 j'cours même pas devant 10 mecs Byakugan j'rodave les 22 à 10 mètres Skalape en moins d'une heure me fait changer d'humeur, mhh Faut qu'ça pète comme les tours jumelles J'repense au passé j'avais zéro pitié, est-ce que j'vais rembourser les curs que j'ai cassé ? La haine j'ai attisé Tout va bien tant qu'la puce est activée, sur ma mère que j'vais jamais pactiser Négro , bois pas si tu sais pas tiser, la teille j'la bois cul sec Que des têtes cramées sur le banc des accusés C'est pas en tenant l'sac que t'auras un Q7 Bâtard la brigade canine elle veut péter mon shit Bellek ta frangine veut péter mon chibre J'vide la cristalline et je remplis mon sheuf Les porcs ils veulent péter mon shit Zéro démocratie c'est la voyoucratie Si, j'mélange vodka-cassis c'est toi qui vas payer les pots cassés Charbon, argent sale j'suis bon qu'à ça Ceux qui descendent ne veulent plus repasser J'traine avec des 3arbi que des gueules cassées Mali, Côte d'Ivoire, Congo-Kinshasa, tous mes comoriens j'viens dédicacer On va te gonfler si t'es trop kassa J'fais gonfler ma liasse j'vesqui la casa J'aime trop l'argent donc j'esquive le casin' J'aime pas trop les jeux d'hasard Insolent depuis minot, fuck l'amour, fuck Juliette et Roméo, fuck Zemmour et tous ses idéaux Le regard est froid, viens t'péta si t'es chaud 3endek ça peut t'qué-cho J'suis pas seul dans la bine-ca mon cerveau il chauffe Comme d'habitude le guetteur il chouf On fait la guerre protége bien tes abdominaux Rafale, paw, impossible qu'on échoue Ils savent pas s'péta mais ils s'croient dans Ong-bak 2, Ong-bak 2 J'ai rêvé que j'me fais coursé par 11 bacqueux, 11 bacqueux Nique la juge elle joue trop avec ma queue, elle joue trop avec ma queue J'représente le 92 ma gueule, le 92 ma gueule</t>
         </is>
       </c>
     </row>
@@ -1415,7 +1415,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Couplet 1 Quatre patrouilles, je m'évapore comme Joséphine T'as des trucs sur toi ? Renoi t'aurais dû filer Trop d'histoires de salades qui né-tour au vinaigre Elle voulait ton cash quand tu voulais la piner Ennemi dans le kamas même si c'est de la caille Une fois qu'j'ai roulé ça, obligé de calciner J'en veux pas mais elle m'envoie son tinier J'vis ma vida, j'en ai marre de l'imaginer J'ai quitté le rain-té sur un coup de tête comme Ziné J'ai quitté le rain-té sur un coup de tête comme Ziné En cas de pépin, j'appelle aucun grand T'inquiète pas gros, j'ramène que ma géné Pour skalap, ça peut t'masser comme le kiné J'suis zehef, mes démons ne veulent pas se confiner Rendre à Chicago si t'as du cran, ou si tu viens pour ton dîner Ça te pull up devant ta nana, y'a quoi faire courir la BAC et la NASS J'suis plutôt Menace, fuck Tony Montana-na J'gué-lar la Batman même si ils sont tenaces, bande de putes L'amour des hommes dans le tier-quar c'est devenu une maladie L'argent comble le bonheur des hommes, mon négro pourquoi t'as du mal à le dire, bande de putes Et on veut tous le paradis, billets bleus, oranges, vert Kichta arc-en-ciel pour faire la diff, bande de putes Et on veut tous le paradis, billets bleus, oranges, vert Kichta arc-en-ciel pour faire la diff, bande de putes Il était pas dans l'embrouille, il s'est fait mêlé On reste bre-som même en journée ensoleillée J'tire un trait sur les mecs ches-lou, on s'retrouvera si nos destins sont liés T'as déjà chaud mais on t'a pas ché-tou bâtard, si j'sors le truc c'est pour t'humilier Si je re-ti, gros je vais viser au milieu Si je re-ti, gros je vais viser au milieu Les iens-cli aiment la frappe du Rif, dans mon pochon, la frappe vient du Maroc J'connais des mecs bien déter qui visser pendant des concerts de Rock Pourquoi l'argent nous fascine autant? Pourquoi l'argent nous fascine autant? Sur le chemin du succès, je prends le virage sans mon clignotant Bientôt le feat l'histoire d'les grignoter Ici les keufs on les fait pivoter Quand j'prends le micro on dirait qu'j'suis opé C'est le peignerie mais j'suis encore opé Ils se font contrôlés sur le bas-côtés, tous mes négros ne sont pas contents Tu sais très bien qu'le temps c'est du seille-o, ici on déteste les pertes de temps You might also likeRefrain Sourire du Joker quand j'suis devant le Batman Y-a l'ta-ta si tu sais pas t'battre man Bâtard y-a du pilon tout jaune comme Pac-Man Et j'sers tout le monde comme si j'suis barman Couplet 2 Regarde dans les yeux quand tu m'serres la main En une journée, j'peux faire ton salaire man J'ai niqué des naiman, j'étais encore gamin Peu de temps après, j'ai revendu le Lemmon Les iens-cli ont faim, le bosseur les alimente Le terrain il ferme mais il reste des aliments À la base la racli c'était une meuf clean Aujourd'hui elle me dit Déshabille-moi J'essaye de bien conduire la mélo, j'en veux aux condés qui en veulent à mes loves On peut s'faire la guerre si tu veux prendre mes loves On peut s'faire la guerre si tu veux prendre mes loves Refrain Sourire du Joker quand j'suis devant le Batman, Batman Y-a l'ta-ta si tu sais pas t'battre man Bâtard y-a du pilon tout jaune comme Pac-Man, Pac-Man Et j'sers tout le monde comme si j'suis barman Sourire du Joker quand j'suis devant le Batman, Batman Y-a l'ta-ta si tu sais pas t'battre man Bâtard y-a du pilon tout jaune comme Pac-Man, Pac-Man Et j'sers tout le monde comme si j'suis barman</t>
+          <t>Couplet 1 Quatre patrouilles, je m'évapore comme Joséphine T'as des trucs sur toi ? Renoi t'aurais dû filer Trop d'histoires de salades qui né-tour au vinaigre Elle voulait ton cash quand tu voulais la piner Ennemi dans le kamas même si c'est de la caille Une fois qu'j'ai roulé ça, obligé de calciner J'en veux pas mais elle m'envoie son tinier J'vis ma vida, j'en ai marre de l'imaginer J'ai quitté le rain-té sur un coup de tête comme Ziné J'ai quitté le rain-té sur un coup de tête comme Ziné En cas de pépin, j'appelle aucun grand T'inquiète pas gros, j'ramène que ma géné Pour skalap, ça peut t'masser comme le kiné J'suis zehef, mes démons ne veulent pas se confiner Rendre à Chicago si t'as du cran, ou si tu viens pour ton dîner Ça te pull up devant ta nana, y'a quoi faire courir la BAC et la NASS J'suis plutôt Menace, fuck Tony Montana-na J'gué-lar la Batman même si ils sont tenaces, bande de putes L'amour des hommes dans le tier-quar c'est devenu une maladie L'argent comble le bonheur des hommes, mon négro pourquoi t'as du mal à le dire, bande de putes Et on veut tous le paradis, billets bleus, oranges, vert Kichta arc-en-ciel pour faire la diff, bande de putes Et on veut tous le paradis, billets bleus, oranges, vert Kichta arc-en-ciel pour faire la diff, bande de putes Il était pas dans l'embrouille, il s'est fait mêlé On reste bre-som même en journée ensoleillée J'tire un trait sur les mecs ches-lou, on s'retrouvera si nos destins sont liés T'as déjà chaud mais on t'a pas ché-tou bâtard, si j'sors le truc c'est pour t'humilier Si je re-ti, gros je vais viser au milieu Si je re-ti, gros je vais viser au milieu Les iens-cli aiment la frappe du Rif, dans mon pochon, la frappe vient du Maroc J'connais des mecs bien déter qui visser pendant des concerts de Rock Pourquoi l'argent nous fascine autant? Pourquoi l'argent nous fascine autant? Sur le chemin du succès, je prends le virage sans mon clignotant Bientôt le feat l'histoire d'les grignoter Ici les keufs on les fait pivoter Quand j'prends le micro on dirait qu'j'suis opé C'est le peignerie mais j'suis encore opé Ils se font contrôlés sur le bas-côtés, tous mes négros ne sont pas contents Tu sais très bien qu'le temps c'est du seille-o, ici on déteste les pertes de temps Refrain Sourire du Joker quand j'suis devant le Batman Y-a l'ta-ta si tu sais pas t'battre man Bâtard y-a du pilon tout jaune comme Pac-Man Et j'sers tout le monde comme si j'suis barman Couplet 2 Regarde dans les yeux quand tu m'serres la main En une journée, j'peux faire ton salaire man J'ai niqué des naiman, j'étais encore gamin Peu de temps après, j'ai revendu le Lemmon Les iens-cli ont faim, le bosseur les alimente Le terrain il ferme mais il reste des aliments À la base la racli c'était une meuf clean Aujourd'hui elle me dit Déshabille-moi J'essaye de bien conduire la mélo, j'en veux aux condés qui en veulent à mes loves On peut s'faire la guerre si tu veux prendre mes loves On peut s'faire la guerre si tu veux prendre mes loves Refrain Sourire du Joker quand j'suis devant le Batman, Batman Y-a l'ta-ta si tu sais pas t'battre man Bâtard y-a du pilon tout jaune comme Pac-Man, Pac-Man Et j'sers tout le monde comme si j'suis barman Sourire du Joker quand j'suis devant le Batman, Batman Y-a l'ta-ta si tu sais pas t'battre man Bâtard y-a du pilon tout jaune comme Pac-Man, Pac-Man Et j'sers tout le monde comme si j'suis barman</t>
         </is>
       </c>
     </row>
@@ -1432,7 +1432,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Paroles issues d'un extrait Action, réaction, déter' à 'boule un 9 Déboule en quatre anneaux, ça pue l'béné-né-néf J'espère qu't'as les nerfs, j'espère qu't'as l'énergie , c'est un bon élève Zéro fois deux, gros, c'est l'prix d'ta cassette J'sors un échant', fume le tant qu't'acceptes , toutes les portes, j'accède cinq doigts à la Jackson Zéro gestu', j'suis dans la gestion Pour te faire, juste un bouton, j'actionne Moi aussi quand j'ché-mar les cases s'allument mais j'fais aucun pas en arrièr à la JacksonYou might also like</t>
+          <t>Paroles issues d'un extrait Action, réaction, déter' à 'boule un 9 Déboule en quatre anneaux, ça pue l'béné-né-néf J'espère qu't'as les nerfs, j'espère qu't'as l'énergie , c'est un bon élève Zéro fois deux, gros, c'est l'prix d'ta cassette J'sors un échant', fume le tant qu't'acceptes , toutes les portes, j'accède cinq doigts à la Jackson Zéro gestu', j'suis dans la gestion Pour te faire, juste un bouton, j'actionne Moi aussi quand j'ché-mar les cases s'allument mais j'fais aucun pas en arrièr à la Jackson</t>
         </is>
       </c>
     </row>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Binks Beatz Myth Syzer Brr, brr, brr À 15 ans, il enfilait les gants pow, il arrachait des sacs, était méchant pow Avec ses reufs, il montait sur des plans, faisait couler le sang ou les larmes, ça dépend pow Il était loin quand y'avait les sirènes ouh mais il en avait rien à cirer ouh Il recommence même si ça a foiré brr, brr, pour pas rentrer bredouille cette soirée brr Il a rien à faire donc il va chouara, pas du genre à aller en soirée Quand il voit une sse-lia il sourit Il voit la bac il est prêt à courir Il traîne dans son quartier pas à Paris Quand y'a une embrouille il est préparé Il préfère agir, n'aime pas trop parler Vingt balle les ien-clis y'a des dix par là Au bigo un ien-cli qui appelle Il vend la beuh pour faire gonfler sa paye 16 ans il charbonne veut monter sa puce Il veut voir le monde, il veut voir gain de plus Il veut voir la vie, veut pas voir la mort Il veut la villa sur la mer Il sait que l'argent sale est éphémère Pourtant il peut pas s'arrêter d'en faire Et à 16 ans les billets il empile Et à 16 ans il goûtera au lon-pi A son âge les ien-clis il enchaîne Comme toujours lacostée est la dégaine Il a peur de personne l'opinel il dégaine ah bon Parfois il rentre avec des marques ah bon Sur le terrain il se démarque Parfois il se transforme en arnaqueur You might also like Et depuis le tit-pe a grandi Petit à petit est devenu un bandit, fuck Sa puce elle est remplie de ien-clis Sa mission est accomplie Il enchaîne les billets normal qu'il embellit Dans le quartier il commet des délits Il veut de la monnaie à l'infini Il est pas là à l'heure du dîner Et depuis le tit-pe a grandi Petit à petit est devenu un bandit, fuck Sa puce elle est remplie de ien-clis Sa mission est accomplie Il enchaîne les billets normal qu'il embellit Dans le quartier il commet des délits Il veut de la monnaie à l'infini Il est pas là à l'heure du dîner Même quand il a tord il se donne raison Parfois, il perd le chemin de la maison Il sait qu'il va pas rentrer ce soir C'est un lossa alors il pense qu'à ses sous Il s'éloigne des négros qui sont bons qu'a cer-su Parle lui d'un bon plan et il va monter dessus Cagoulé ganté il passe inaperçu Il vient à l'heure c'est un bosseur assidu Il s'éloigne du terrain quand il voit que c'est tendu De midi à minuit, il r'garde pas la pendule Il traîne pas avec des pédales Toute la journée il re-détaille Le temps c'est de l'argent, il aime pas les pertes de temps Il veut passer tout l'été en deux temps Ils font les grossistes mais ils sont endettés Lui il veut finir sur la plage en détente La nuit y'a les chickens ves-qui la batman Si y'a embrouilles ses négros déboulent en balle Son bigo il sonne en deuspi il s'habille Il te pull-up ta mère s'en fout de comment tu t'appelles Il a trop la haine quand les keufs ils viennent taper Y'a un conflit c'est normal qu'il vient équipé Toujours à l'affût quand y'a un billet à prendre Il sait faire des sous gros tu vas rien lui apprendre Même si les schmitts sont à ses trousses Il fait que de visser sans laisser aucune trace Tous les jours il vend la came Quand il déballe la 'quette il brûle le cellophane Rentre dans la cité, tu passes à la douane Souvent il se fait pister par la Mégane Jeune négro est matrixé par la bécane Il voit le monde en kilogramme Et depuis le tit-pe a grandi Petit à petit est devenu un bandit, fuck Sa puce elle est remplie de ien-clis Sa mission est accomplie Il enchaîne les billets normal qu'il embellit Dans le quartier il commet des délits Il veut de la monnaie à l'infini Il est pas là à l'heure du dîner Et depuis le tit-pe a grandi Petit à petit est devenu un bandit, fuck Sa puce elle est remplie de ien-clis Sa mission est accomplie Il enchaîne les billets normal qu'il embellit Dans le quartier il commet des délits Il veut de la monnaie à l'infini Il est pas là à l'heure du dîner Binks Beatz</t>
+          <t>Binks Beatz Myth Syzer Brr, brr, brr À 15 ans, il enfilait les gants pow, il arrachait des sacs, était méchant pow Avec ses reufs, il montait sur des plans, faisait couler le sang ou les larmes, ça dépend pow Il était loin quand y'avait les sirènes ouh mais il en avait rien à cirer ouh Il recommence même si ça a foiré brr, brr, pour pas rentrer bredouille cette soirée brr Il a rien à faire donc il va chouara, pas du genre à aller en soirée Quand il voit une sse-lia il sourit Il voit la bac il est prêt à courir Il traîne dans son quartier pas à Paris Quand y'a une embrouille il est préparé Il préfère agir, n'aime pas trop parler Vingt balle les ien-clis y'a des dix par là Au bigo un ien-cli qui appelle Il vend la beuh pour faire gonfler sa paye 16 ans il charbonne veut monter sa puce Il veut voir le monde, il veut voir gain de plus Il veut voir la vie, veut pas voir la mort Il veut la villa sur la mer Il sait que l'argent sale est éphémère Pourtant il peut pas s'arrêter d'en faire Et à 16 ans les billets il empile Et à 16 ans il goûtera au lon-pi A son âge les ien-clis il enchaîne Comme toujours lacostée est la dégaine Il a peur de personne l'opinel il dégaine ah bon Parfois il rentre avec des marques ah bon Sur le terrain il se démarque Parfois il se transforme en arnaqueur Et depuis le tit-pe a grandi Petit à petit est devenu un bandit, fuck Sa puce elle est remplie de ien-clis Sa mission est accomplie Il enchaîne les billets normal qu'il embellit Dans le quartier il commet des délits Il veut de la monnaie à l'infini Il est pas là à l'heure du dîner Et depuis le tit-pe a grandi Petit à petit est devenu un bandit, fuck Sa puce elle est remplie de ien-clis Sa mission est accomplie Il enchaîne les billets normal qu'il embellit Dans le quartier il commet des délits Il veut de la monnaie à l'infini Il est pas là à l'heure du dîner Même quand il a tord il se donne raison Parfois, il perd le chemin de la maison Il sait qu'il va pas rentrer ce soir C'est un lossa alors il pense qu'à ses sous Il s'éloigne des négros qui sont bons qu'a cer-su Parle lui d'un bon plan et il va monter dessus Cagoulé ganté il passe inaperçu Il vient à l'heure c'est un bosseur assidu Il s'éloigne du terrain quand il voit que c'est tendu De midi à minuit, il r'garde pas la pendule Il traîne pas avec des pédales Toute la journée il re-détaille Le temps c'est de l'argent, il aime pas les pertes de temps Il veut passer tout l'été en deux temps Ils font les grossistes mais ils sont endettés Lui il veut finir sur la plage en détente La nuit y'a les chickens ves-qui la batman Si y'a embrouilles ses négros déboulent en balle Son bigo il sonne en deuspi il s'habille Il te pull-up ta mère s'en fout de comment tu t'appelles Il a trop la haine quand les keufs ils viennent taper Y'a un conflit c'est normal qu'il vient équipé Toujours à l'affût quand y'a un billet à prendre Il sait faire des sous gros tu vas rien lui apprendre Même si les schmitts sont à ses trousses Il fait que de visser sans laisser aucune trace Tous les jours il vend la came Quand il déballe la 'quette il brûle le cellophane Rentre dans la cité, tu passes à la douane Souvent il se fait pister par la Mégane Jeune négro est matrixé par la bécane Il voit le monde en kilogramme Et depuis le tit-pe a grandi Petit à petit est devenu un bandit, fuck Sa puce elle est remplie de ien-clis Sa mission est accomplie Il enchaîne les billets normal qu'il embellit Dans le quartier il commet des délits Il veut de la monnaie à l'infini Il est pas là à l'heure du dîner Et depuis le tit-pe a grandi Petit à petit est devenu un bandit, fuck Sa puce elle est remplie de ien-clis Sa mission est accomplie Il enchaîne les billets normal qu'il embellit Dans le quartier il commet des délits Il veut de la monnaie à l'infini Il est pas là à l'heure du dîner Binks Beatz</t>
         </is>
       </c>
     </row>
@@ -1466,7 +1466,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>9 2 1 4 0 sur le pocheton Jai rempli mes poches, donc jai rempli ma mission Faut jamais lé-par à laudition, cagoulés, gantés on sincruste dans ta maison Et javoue qules femelles me lassent, jfais dla prévention pas des menaces Ya qules vrais lossa que jdédicace, on rentre, on prend tout et on scasse Jécris le texte sur le bigo a schlag, et toi tu tdemande comment on fait Tire sur lkamas, tire sur lkamas, et tu verras comment on fly Jlui donne ma be-teu, jlui offre pas des fleurs Vas-y, jvais tlaisser copier mon flow Cest une descente ou une mission commando ? Si on tcroise solo, dis-moi on fait comment gros ? En vérité, on fait comme on veut Jvais toublier vite, cest un peu comme mon feu Pour niquer les keufs, mes lossas sont en noir Tinquiète, on sait se camoufler Les condés vont repasser, jaime pas quand ils tournent à la plaine On est venu pour te masser, putain, jai encore oublié la crème Allez, fais tout ce quon ta demandé, belek à toi, batard, ça peut tamander Même si sur toi tas pas le fric, igo tu vas décoffrer Jsuis un salaud, elle trouve que jsuis frais Moi jsuis un lossa, jpense quà chiffrer Si tes mon reuf, pour toi, jy vais Dans ses yeux, dla peur, jai vu Jtire une ffe-ta, jperds la mémoire Est-ce que tu peux combattre la mort ? En vrai, faut rien laisser dans larmoire Cest pas sûr quelle va tenir ta porte A part ton cavu, quest-ce tu mapportes ? Tu la tej, elle a fini escorte, maintenant pour un illet-bi, elle scambre Jcacherais jamais ldétail dans ma chambre En vrai, jmen balec, si tas peté scal On revend la came devant la cam Elle a pas dcul, mais elle fait la Kim Si jmonte sur Paname habillé en jean Cest pas pour faire la fête, cest juste pour éviter les shmitts Pendant que jfais gonfler ma sim Pendant que jfais gonfler ma sim Comme dhabitude, jagresse le micro Et vu qule temps cest dlargent, cest fini, jarrête de faire des me-chro Jai dit qujarrêtais la criquette, cest ton problème, si tu me crois Ces négros mrapportent pas un rond, alors, sur eux, jai mis une croix Ya que largent qui mrend heureux Faut sbarrer à Las Vegas, au quartier, le secteur, il est trop quadrillé Jveux pas mfaire caner comme Tupac Jai vu lange de la mort rouler en Cadillac On rentre, on prend tout, et on scasse Eux, ils font les fous, mais ils se cachent La miss, elle est conne Elle saura jamais ya quoi dans ma sacoche Parfois, sur la playa, jmimagine Quand jouvre les yeux jsuis sur les R On sait gué-lar la BAC, sans regarder derrière Jai laissé les problèmes derrière moi Jte tamponne, si tu tmets sur ma route Largent fait pas lbonheur, cest des salades Malheur à toi si tu mcarottes, on vient cagoulé comme Sin Cara Et on pète ton carreau, si ta chaîne elle fait 24 carats 24 sur 24 jsuis disponible, pour les ceux-di cest en vente libre Tu prends en gros, jte passe mon num, mais jvais pas te donner mon nom Fuck la Bac qui déboule à tout moment Fuck la Bac qui déboule à tout momentYou might also like</t>
+          <t>9 2 1 4 0 sur le pocheton Jai rempli mes poches, donc jai rempli ma mission Faut jamais lé-par à laudition, cagoulés, gantés on sincruste dans ta maison Et javoue qules femelles me lassent, jfais dla prévention pas des menaces Ya qules vrais lossa que jdédicace, on rentre, on prend tout et on scasse Jécris le texte sur le bigo a schlag, et toi tu tdemande comment on fait Tire sur lkamas, tire sur lkamas, et tu verras comment on fly Jlui donne ma be-teu, jlui offre pas des fleurs Vas-y, jvais tlaisser copier mon flow Cest une descente ou une mission commando ? Si on tcroise solo, dis-moi on fait comment gros ? En vérité, on fait comme on veut Jvais toublier vite, cest un peu comme mon feu Pour niquer les keufs, mes lossas sont en noir Tinquiète, on sait se camoufler Les condés vont repasser, jaime pas quand ils tournent à la plaine On est venu pour te masser, putain, jai encore oublié la crème Allez, fais tout ce quon ta demandé, belek à toi, batard, ça peut tamander Même si sur toi tas pas le fric, igo tu vas décoffrer Jsuis un salaud, elle trouve que jsuis frais Moi jsuis un lossa, jpense quà chiffrer Si tes mon reuf, pour toi, jy vais Dans ses yeux, dla peur, jai vu Jtire une ffe-ta, jperds la mémoire Est-ce que tu peux combattre la mort ? En vrai, faut rien laisser dans larmoire Cest pas sûr quelle va tenir ta porte A part ton cavu, quest-ce tu mapportes ? Tu la tej, elle a fini escorte, maintenant pour un illet-bi, elle scambre Jcacherais jamais ldétail dans ma chambre En vrai, jmen balec, si tas peté scal On revend la came devant la cam Elle a pas dcul, mais elle fait la Kim Si jmonte sur Paname habillé en jean Cest pas pour faire la fête, cest juste pour éviter les shmitts Pendant que jfais gonfler ma sim Pendant que jfais gonfler ma sim Comme dhabitude, jagresse le micro Et vu qule temps cest dlargent, cest fini, jarrête de faire des me-chro Jai dit qujarrêtais la criquette, cest ton problème, si tu me crois Ces négros mrapportent pas un rond, alors, sur eux, jai mis une croix Ya que largent qui mrend heureux Faut sbarrer à Las Vegas, au quartier, le secteur, il est trop quadrillé Jveux pas mfaire caner comme Tupac Jai vu lange de la mort rouler en Cadillac On rentre, on prend tout, et on scasse Eux, ils font les fous, mais ils se cachent La miss, elle est conne Elle saura jamais ya quoi dans ma sacoche Parfois, sur la playa, jmimagine Quand jouvre les yeux jsuis sur les R On sait gué-lar la BAC, sans regarder derrière Jai laissé les problèmes derrière moi Jte tamponne, si tu tmets sur ma route Largent fait pas lbonheur, cest des salades Malheur à toi si tu mcarottes, on vient cagoulé comme Sin Cara Et on pète ton carreau, si ta chaîne elle fait 24 carats 24 sur 24 jsuis disponible, pour les ceux-di cest en vente libre Tu prends en gros, jte passe mon num, mais jvais pas te donner mon nom Fuck la Bac qui déboule à tout moment Fuck la Bac qui déboule à tout moment</t>
         </is>
       </c>
     </row>
@@ -1483,7 +1483,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Hey Castro, go crazy Binks Beatz Brr, brr Ils sont nés avec cuillère en or dans la bouche mais ils sinventent des problèmes imaginaires Jai pensé à cricket avant daller taffer 15 ans, j'prends des affaires même le ssiste-gro se demande comment jai fait Si on soulève ta cachette tout est à refaire 5 heures 59, je suis déjà levé Ma porte, je lai bien mée-fer au cas où les tes-shmi sont venus pour me faire J'tape dans sa ke-schne, elle m'dit Tarrête pas Elle entend la sonnerie elle sait pourquoi j'reste pas Combien d'fois j'suis rentré khabbat du charbon ? J'laisse tomber un pocheton quand je passe aux lettes-toi En G.A.V, j'm'amuse, j'insulte la lice-po uh, j'perds mon sourire, menotté dans le camion mais uh J'le r'gagne en sortant du dépôt Si tu res-ti, on tire, c'est la loi du talion uh Pour gagner, tu sais pas c'que j'ai dû perdre paw, j'suis écouté par des négros qui m'envient Par des gens qui m'en veulent, pas des anciens dus-per Y a qu'le passé pour me rattraper, toi, en vrai, j'sais même pas si tu peux À chaque fois qu'j'ai chouara, les keumés qui m'ont vu sont restés immobiles Ils ont fait les tipèrs Est-ce que j'peux rapper ma vie sans influencer les tits-pe ? You might also like Boîte automatique, les pneus qui patinent, ça tartine Dans l'gamos, j'me crois au karting brr, brr On n'est pas potos, j'ai pas changé ma team J'pose mon couplet, j'retourne dans l'futur comme Marty futur comme Marty, futur comme Marty J'pose mon couplet, j'retourne dans l'futur comme Marty Les keufs sont passés, j'suis resté présent Mon shit, j'l'ai fait partir paw, paw, paw Boîte automatique, les pneus qui patinent, ça tartine Dans l'gamos, j'me crois au karting brr, brr On n'est pas potos, j'ai pas changé ma team J'pose mon couplet, j'retourne dans l'futur comme Marty futur comme Marty, futur comme Marty J'pose mon couplet, j'retourne dans l'futur comme Marty Les keufs sont passés, j'suis resté présent Mon shit, j'l'ai fait partir paw, paw, paw Si t'es mon frérot, dans tous les cas, j'te suis J'te demande même pas il faut masser qui T'as musclé ton corps, t'as pas musclé tes couilles Moi, c'est mes cojones qui font ma sécu' Y a pas qu'le temps, y a d'la drogue qui s'écoule Le flow est saignant mais j'suis pas assez cru Cours vite et bien, pour l'instant, c'est cool Une fois qu'j'allume le fuego, pour vous, c'est cuit Jamais d'la vie on prend la fuite à part devant les flics Tu connais mes rafiks, on taillera jamais d'pipe Encore moins pour un feat', on laisse ça pour les putes sale pute Et pour les faire, pas b'soin d'une grosse équipe sale pute Renois, rebeus qu'empochent le liquide dans le dos d'la France Sans oublier qu'ils ont pillé l'Afrique, on avance Dans l'rap, j'ai fait la diff' avec mes textes d'avant brr J'ai pas peur de mourir, j'ai peur de finir avec une 'teille à la main ou bien l'équivalent brr, brr Y a ceux qui vont vite et y a ceux qui vont loin Pas d'repos, on s'enrichit en travaillant Donc tu m'vois au boulot en permanence J'ai compris qu'c'est pas l'honnêteté qui t'fait manger uh Zéro affiliation, zéro alliance La vérité blesse, demande à ceux qu'ont balancé uh Boîte automatique, les pneus qui patinent, ça tartine Dans l'gamos, j'me crois au karting brr, brr On n'est pas potos, j'ai pas changé ma team J'pose mon couplet, j'retourne dans l'futur comme Marty futur comme Marty, futur comme Marty J'pose mon couplet, j'retourne dans l'futur comme Marty Les keufs sont passés, j'suis resté présent Mon shit, j'l'ai fait partir paw, paw, paw Boîte automatique, les pneus qui patinent, ça tartine Dans l'gamos, j'me crois au karting brr, brr On n'est pas potos, j'ai pas changé ma team J'pose mon couplet, j'retourne dans l'futur comme Marty futur comme Marty, futur comme Marty J'pose mon couplet, j'retourne dans l'futur comme Marty Les keufs sont passés, j'suis resté présent Mon shit, j'l'ai fait partir paw, paw, paw Nan, nan, nan Uh, uh Uh, uh, uh Uh, uh Nan, nan, nan Uh, uh Uh, uh, uh Uh, uh, uh2</t>
+          <t>Hey Castro, go crazy Binks Beatz Brr, brr Ils sont nés avec cuillère en or dans la bouche mais ils sinventent des problèmes imaginaires Jai pensé à cricket avant daller taffer 15 ans, j'prends des affaires même le ssiste-gro se demande comment jai fait Si on soulève ta cachette tout est à refaire 5 heures 59, je suis déjà levé Ma porte, je lai bien mée-fer au cas où les tes-shmi sont venus pour me faire J'tape dans sa ke-schne, elle m'dit Tarrête pas Elle entend la sonnerie elle sait pourquoi j'reste pas Combien d'fois j'suis rentré khabbat du charbon ? J'laisse tomber un pocheton quand je passe aux lettes-toi En G.A.V, j'm'amuse, j'insulte la lice-po uh, j'perds mon sourire, menotté dans le camion mais uh J'le r'gagne en sortant du dépôt Si tu res-ti, on tire, c'est la loi du talion uh Pour gagner, tu sais pas c'que j'ai dû perdre paw, j'suis écouté par des négros qui m'envient Par des gens qui m'en veulent, pas des anciens dus-per Y a qu'le passé pour me rattraper, toi, en vrai, j'sais même pas si tu peux À chaque fois qu'j'ai chouara, les keumés qui m'ont vu sont restés immobiles Ils ont fait les tipèrs Est-ce que j'peux rapper ma vie sans influencer les tits-pe ? Boîte automatique, les pneus qui patinent, ça tartine Dans l'gamos, j'me crois au karting brr, brr On n'est pas potos, j'ai pas changé ma team J'pose mon couplet, j'retourne dans l'futur comme Marty futur comme Marty, futur comme Marty J'pose mon couplet, j'retourne dans l'futur comme Marty Les keufs sont passés, j'suis resté présent Mon shit, j'l'ai fait partir paw, paw, paw Boîte automatique, les pneus qui patinent, ça tartine Dans l'gamos, j'me crois au karting brr, brr On n'est pas potos, j'ai pas changé ma team J'pose mon couplet, j'retourne dans l'futur comme Marty futur comme Marty, futur comme Marty J'pose mon couplet, j'retourne dans l'futur comme Marty Les keufs sont passés, j'suis resté présent Mon shit, j'l'ai fait partir paw, paw, paw Si t'es mon frérot, dans tous les cas, j'te suis J'te demande même pas il faut masser qui T'as musclé ton corps, t'as pas musclé tes couilles Moi, c'est mes cojones qui font ma sécu' Y a pas qu'le temps, y a d'la drogue qui s'écoule Le flow est saignant mais j'suis pas assez cru Cours vite et bien, pour l'instant, c'est cool Une fois qu'j'allume le fuego, pour vous, c'est cuit Jamais d'la vie on prend la fuite à part devant les flics Tu connais mes rafiks, on taillera jamais d'pipe Encore moins pour un feat', on laisse ça pour les putes sale pute Et pour les faire, pas b'soin d'une grosse équipe sale pute Renois, rebeus qu'empochent le liquide dans le dos d'la France Sans oublier qu'ils ont pillé l'Afrique, on avance Dans l'rap, j'ai fait la diff' avec mes textes d'avant brr J'ai pas peur de mourir, j'ai peur de finir avec une 'teille à la main ou bien l'équivalent brr, brr Y a ceux qui vont vite et y a ceux qui vont loin Pas d'repos, on s'enrichit en travaillant Donc tu m'vois au boulot en permanence J'ai compris qu'c'est pas l'honnêteté qui t'fait manger uh Zéro affiliation, zéro alliance La vérité blesse, demande à ceux qu'ont balancé uh Boîte automatique, les pneus qui patinent, ça tartine Dans l'gamos, j'me crois au karting brr, brr On n'est pas potos, j'ai pas changé ma team J'pose mon couplet, j'retourne dans l'futur comme Marty futur comme Marty, futur comme Marty J'pose mon couplet, j'retourne dans l'futur comme Marty Les keufs sont passés, j'suis resté présent Mon shit, j'l'ai fait partir paw, paw, paw Boîte automatique, les pneus qui patinent, ça tartine Dans l'gamos, j'me crois au karting brr, brr On n'est pas potos, j'ai pas changé ma team J'pose mon couplet, j'retourne dans l'futur comme Marty futur comme Marty, futur comme Marty J'pose mon couplet, j'retourne dans l'futur comme Marty Les keufs sont passés, j'suis resté présent Mon shit, j'l'ai fait partir paw, paw, paw Nan, nan, nan Uh, uh Uh, uh, uh Uh, uh Nan, nan, nan Uh, uh Uh, uh, uh Uh, uh, uh2</t>
         </is>
       </c>
     </row>
@@ -1500,7 +1500,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Binks Beatz Si on t'encule ta mère, igo, fais passer l'message Batârd, écarte-toi du passage C'est une coquine pourtant elle fait la meuf sage J'reconnais l'vil-ci à son visage Y a les condés, j'suis passé par le grillage J'me casse en deuspi, j'suis pas grillé Le trafic s'arrête quand l'secteur est quadrillé J'vois des rappeurs qui se mettent à driller Mais est-ce que l'instru, ils peuvent la plier ? Ils aimeraient me voir les mains liées J'suis dans skalape, on est d'vant ton palier Et c'est la même chose si t'as pas nié J'rentre dans l'instru' comme dans une schneck J'ai té-cla le bédo, j'suis schner Faut qu'le pilon, il soit vert comme Shrek C'est pour voler si tu m'vois dans les quartiers chics J'recompte tous les soirs pourtant j'ai pas d'métier La monnaie m'attire, j'ai pas besoin d'amitié On s'fait contrôler et on est tous alignés Prêt à tenir le ceu-sa l'hiver Tellement l'argent sale nous fait saliver On m'appelle pour un plan, sans réfléchir j'y vais Si on t'tombe dessus, tu pourras pas t'relever Et pas la peine d'hausser la voix J'suis un laud-sa, j'veux pas respecter la loi J'veux la ken, j'veux pas lui passer l'anneau On allume les schmitts et puis la ville est à nous J'te raconte la réalité 9-2-1-4-0 sur le panneau On peut t'schlasser dans les points vitaux Batârd, t'étais pas invité donc on a pris ta sacoche Louis Vuitton J'ai les pieds dans le sale, les mains dans le sale Il m'faut d'l'argent à mort, j'm'en ballek d'faire du son Les schmitts, ils rentrent chez moi, j'ai grave des émotions Le bigo, il sonne alors j'enchaîne les missions On va t'amender, tu vas payer la caution Les keufs, ils sont à pattes, négro, fais attention Y a des kilos chez toi, on rentre dans ta maison Personne pour nous arrêter, on perd la raison Et les condés n'ont pas changé, comme d'habitude, ils veulent péter le réseau Comme d'habitude, ils veulent péter la résine J'ai cassé la SIM, j'entends ma voix qui résonne Et j'réponds pas quand l'OPJ, il me questionne Et j'réponds pas quand l'OPJ, il me questionne Putain, j'crois bien qu'la miss, elle est conne, elle croit que j'ai son temps, moi, j'veux soulever des tonnes Il te doit des sous, igo, il faut l'endetter C'est pas tes histoires, faut pas t'en mêler On t'pietine, on reste synchro, j'm'en ballek que tu finis en sanglots Même si le son, tu l'aimes pas, tu bouges la tête sur l'tempo Les bacqueux, ils déboulent comme la Gestapo, ils sont trop cons, ils sont rentrés dans l'guet-apens Même pas besoin d'une rafale, on déboule direct devant ta porte Si tu veux, j'te pousse du bédo, passe tes bijoux On croise un ennemi, ça l'pull-up sans dire bonjour Les condés, ils ont chaud, ils ont fait demi-tour Et toi, t'as rien fait donc arrête de mytho' J'suis toujours impliqué, me parle pas d'amour J'veux des billets, couleur végétaux Donc j'passe mon temps en bas d'la tour On va t'courser et tu vas crier au secours You might also like Il était gentil, il était du mauvais tieks J'ai vu les gyro' alors j'suis sorti du binks Et en deuspi j'ai mis la vitesse, rien a changé, le dépôt, il faut l'éviter Il veut voir l'argent, mais bon, il voit plus sa mère Plus il voit les sous et plus il voit où ça mène Mais lui, il pense qu'à débiter Il veut péter un salaire à la fin d'la semaine</t>
+          <t>Binks Beatz Si on t'encule ta mère, igo, fais passer l'message Batârd, écarte-toi du passage C'est une coquine pourtant elle fait la meuf sage J'reconnais l'vil-ci à son visage Y a les condés, j'suis passé par le grillage J'me casse en deuspi, j'suis pas grillé Le trafic s'arrête quand l'secteur est quadrillé J'vois des rappeurs qui se mettent à driller Mais est-ce que l'instru, ils peuvent la plier ? Ils aimeraient me voir les mains liées J'suis dans skalape, on est d'vant ton palier Et c'est la même chose si t'as pas nié J'rentre dans l'instru' comme dans une schneck J'ai té-cla le bédo, j'suis schner Faut qu'le pilon, il soit vert comme Shrek C'est pour voler si tu m'vois dans les quartiers chics J'recompte tous les soirs pourtant j'ai pas d'métier La monnaie m'attire, j'ai pas besoin d'amitié On s'fait contrôler et on est tous alignés Prêt à tenir le ceu-sa l'hiver Tellement l'argent sale nous fait saliver On m'appelle pour un plan, sans réfléchir j'y vais Si on t'tombe dessus, tu pourras pas t'relever Et pas la peine d'hausser la voix J'suis un laud-sa, j'veux pas respecter la loi J'veux la ken, j'veux pas lui passer l'anneau On allume les schmitts et puis la ville est à nous J'te raconte la réalité 9-2-1-4-0 sur le panneau On peut t'schlasser dans les points vitaux Batârd, t'étais pas invité donc on a pris ta sacoche Louis Vuitton J'ai les pieds dans le sale, les mains dans le sale Il m'faut d'l'argent à mort, j'm'en ballek d'faire du son Les schmitts, ils rentrent chez moi, j'ai grave des émotions Le bigo, il sonne alors j'enchaîne les missions On va t'amender, tu vas payer la caution Les keufs, ils sont à pattes, négro, fais attention Y a des kilos chez toi, on rentre dans ta maison Personne pour nous arrêter, on perd la raison Et les condés n'ont pas changé, comme d'habitude, ils veulent péter le réseau Comme d'habitude, ils veulent péter la résine J'ai cassé la SIM, j'entends ma voix qui résonne Et j'réponds pas quand l'OPJ, il me questionne Et j'réponds pas quand l'OPJ, il me questionne Putain, j'crois bien qu'la miss, elle est conne, elle croit que j'ai son temps, moi, j'veux soulever des tonnes Il te doit des sous, igo, il faut l'endetter C'est pas tes histoires, faut pas t'en mêler On t'pietine, on reste synchro, j'm'en ballek que tu finis en sanglots Même si le son, tu l'aimes pas, tu bouges la tête sur l'tempo Les bacqueux, ils déboulent comme la Gestapo, ils sont trop cons, ils sont rentrés dans l'guet-apens Même pas besoin d'une rafale, on déboule direct devant ta porte Si tu veux, j'te pousse du bédo, passe tes bijoux On croise un ennemi, ça l'pull-up sans dire bonjour Les condés, ils ont chaud, ils ont fait demi-tour Et toi, t'as rien fait donc arrête de mytho' J'suis toujours impliqué, me parle pas d'amour J'veux des billets, couleur végétaux Donc j'passe mon temps en bas d'la tour On va t'courser et tu vas crier au secours Il était gentil, il était du mauvais tieks J'ai vu les gyro' alors j'suis sorti du binks Et en deuspi j'ai mis la vitesse, rien a changé, le dépôt, il faut l'éviter Il veut voir l'argent, mais bon, il voit plus sa mère Plus il voit les sous et plus il voit où ça mène Mais lui, il pense qu'à débiter Il veut péter un salaire à la fin d'la semaine</t>
         </is>
       </c>
     </row>
@@ -1517,7 +1517,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Avant d'dave-bé, j'étais trop mobile mmh La fumée m'a détruit comme à Tchernobyl T'es fou si tu crois qu'on vient les mains vides T'es fou si t'as cru qu'on attend l'invit' Charbon dimanche, on n'attend pas lundi poh, poh J'retourne ta barraque, j'attends pas l'indice poh Ça fait les comptes sourire aux lèvres, si j'fais l'con, c'est les sous qui m'relèvent brr Cerveau bousillé par la monnaie, gros brr, que la monnaie, le reste, j'm'en bats les yeuks brr Continue d'lécher des 'euks, on fait pas d'somation han, pas d'tir en l'air han L'argnt rend beau, mais les pêchés rndent lég', j'récup' un colis piégé dans un point-relais poh, poh Si j'me fais kicker, j'm'en prends qu'à moi-même, une nouvelle journée commence, c'est encore la même Envoie la lame, j'te détaille huit cents balles, j'te fais ça en balle, t'inquiète, j'ai encore la main Manu Le Coq en voulait pas assez, Zé Pequ' en voulait trop, ils ont fini pareil T'as glissé, ça t'a remplacé quand tu sors, fais pas l'choqué, qu'c'est plus pareil Combien font les mecs pleins, genre ils veulent t'mettre bien bien ? Mais ils sont dans le paraître Si tu sais pas chiffrer, arrête arrête tellement j'les baise, j'sais pas si c'est un rêve uh Parano, j'fais avec, belek, il veut m'la mettre, qu'il a pas eu l'occas', j'sais pas si c'est un reuf Midi pile, j'ai pas d'retard, j'deviens Usain Bolt d'vant les shtars Sans faire crari, dans la crave-bi, j'ai pris des balles J'rigole quand j'vois ces gues-shla raconter nos vies brr On sait ouvrir les portes, fermer des bouches brr sans mettre de baffe Sans lâcher du biff salope J'mélange beuh dans le shit, pratique et théorie C'est l'Apocalypse, j'lâche un flow météorite j'lâche un flow météorite Guette la météo, il est temps qu'j'les terrorise bouh You might also like C'est comme ça qu'on extériorise bouh Comme ça qu'on extériorise C'est comme ça qu'on extériorise Comme ça qu'on extériorise Habitué au risque C'est comme ça qu'on extériorise C'est comme ça qu'on extériorise uh C'est comme ça qu'on extériorise uh Avant d'descendre, y a l'deux-roues qui localise, faut un kilo d'Cali, gros kamas pour faire les vocalises Elle a cru qu'c'était l'goro quand c'était l'calibre cette fois, c'est l'goro, elle croit qu'c'est l'calibre Donne-moi qu'du bir, t'as même pas coffré skalape, sale con, ça sort des lames en mode Excalibur oui Pas étonné d'voir ces putes galopent, sale con oui, t'entends la fale-ra mais pas l'cambu poh, poh J'reconnais les vrais et les falsches, parfois, j'les checke mais sans plus Ramène des plans à 10k ou vingt planches dans un keus et on sourit encore plus mmh En hiver, y a des trous sur l'bonnet, en été, c'est l'gator auquel j'suis abonné Sur un , j'ai fait pleurer ta mère, si j'me fais pét', j'fais pleurer la mienne, mon choix, tu le connais J'paie la caution, la vie, ou la loue, pour maman, j'te uer-t, après, j'me repentis 'tis, poh Le jour où l'soleil se lèvera à l'Ouest poh, ça s'ra trop tard pour jouer les bandits ah bon ? Impossible de roupiller quand j'suis en perte ou passer du bon temps Même quand, même quand j'vide mon esprit, garde le ffre-chi en tête Et j'crois qu'j'ai jamais réfléchi autant Sans faire crari, dans la crave-bi, j'ai pris des balles J'rigole quand j'vois ces gues-shla raconter nos vies brr On sait ouvrir les portes, fermer des bouches brr sans mettre de baffe Sans lâcher du biff salope J'mélange beuh dans le shit, pratique et théorie C'est l'Apocalypse, j'lâche un flow météorite j'lâche un flow météorite Guette la météo, il est temps qu'j'les terrorise bouh C'est comme ça qu'on extériorise bouh Comme ça qu'on extériorise C'est comme ça qu'on extériorise eh Comme ça qu'on extériorise eh Habitué au risque C'est comme ça qu'on extériorise C'est comme ça qu'on extériorise uh C'est comme ça qu'on extériorise uh C'est l'Glock qui lé-par, c'est pas Jacques a dit oui, la haine, on la noie pas dans la oui Zéro tête à part chez l'Paki', cette année, ça nehess pas, gros, j'envoie l'paquet paquet Fallait parler depuis l'début, imbécile, ça sent la fin la BAC t'a plaqué salope En deux-trois heures, j'me retrouve à BX eh à fond sur l'autoroute eh, allemande est la plaque eh Envoie un échant', j'en n'ai rien à foutre du tampon sur la plaquette Et on s'en fout qu'tu pètes un câble, si tu t'caches, on va retaper ta caisse poh J'les vois tous jouer brr les mecs en ce-pla brr, brr mais j'les connais, ces connards, ils sont pas prêts brr, pas prêts Quand la pute recompte le blé, j'suis pas con, poto, j'recompte juste après après, après, après</t>
+          <t>Avant d'dave-bé, j'étais trop mobile mmh La fumée m'a détruit comme à Tchernobyl T'es fou si tu crois qu'on vient les mains vides T'es fou si t'as cru qu'on attend l'invit' Charbon dimanche, on n'attend pas lundi poh, poh J'retourne ta barraque, j'attends pas l'indice poh Ça fait les comptes sourire aux lèvres, si j'fais l'con, c'est les sous qui m'relèvent brr Cerveau bousillé par la monnaie, gros brr, que la monnaie, le reste, j'm'en bats les yeuks brr Continue d'lécher des 'euks, on fait pas d'somation han, pas d'tir en l'air han L'argnt rend beau, mais les pêchés rndent lég', j'récup' un colis piégé dans un point-relais poh, poh Si j'me fais kicker, j'm'en prends qu'à moi-même, une nouvelle journée commence, c'est encore la même Envoie la lame, j'te détaille huit cents balles, j'te fais ça en balle, t'inquiète, j'ai encore la main Manu Le Coq en voulait pas assez, Zé Pequ' en voulait trop, ils ont fini pareil T'as glissé, ça t'a remplacé quand tu sors, fais pas l'choqué, qu'c'est plus pareil Combien font les mecs pleins, genre ils veulent t'mettre bien bien ? Mais ils sont dans le paraître Si tu sais pas chiffrer, arrête arrête tellement j'les baise, j'sais pas si c'est un rêve uh Parano, j'fais avec, belek, il veut m'la mettre, qu'il a pas eu l'occas', j'sais pas si c'est un reuf Midi pile, j'ai pas d'retard, j'deviens Usain Bolt d'vant les shtars Sans faire crari, dans la crave-bi, j'ai pris des balles J'rigole quand j'vois ces gues-shla raconter nos vies brr On sait ouvrir les portes, fermer des bouches brr sans mettre de baffe Sans lâcher du biff salope J'mélange beuh dans le shit, pratique et théorie C'est l'Apocalypse, j'lâche un flow météorite j'lâche un flow météorite Guette la météo, il est temps qu'j'les terrorise bouh C'est comme ça qu'on extériorise bouh Comme ça qu'on extériorise C'est comme ça qu'on extériorise Comme ça qu'on extériorise Habitué au risque C'est comme ça qu'on extériorise C'est comme ça qu'on extériorise uh C'est comme ça qu'on extériorise uh Avant d'descendre, y a l'deux-roues qui localise, faut un kilo d'Cali, gros kamas pour faire les vocalises Elle a cru qu'c'était l'goro quand c'était l'calibre cette fois, c'est l'goro, elle croit qu'c'est l'calibre Donne-moi qu'du bir, t'as même pas coffré skalape, sale con, ça sort des lames en mode Excalibur oui Pas étonné d'voir ces putes galopent, sale con oui, t'entends la fale-ra mais pas l'cambu poh, poh J'reconnais les vrais et les falsches, parfois, j'les checke mais sans plus Ramène des plans à 10k ou vingt planches dans un keus et on sourit encore plus mmh En hiver, y a des trous sur l'bonnet, en été, c'est l'gator auquel j'suis abonné Sur un , j'ai fait pleurer ta mère, si j'me fais pét', j'fais pleurer la mienne, mon choix, tu le connais J'paie la caution, la vie, ou la loue, pour maman, j'te uer-t, après, j'me repentis 'tis, poh Le jour où l'soleil se lèvera à l'Ouest poh, ça s'ra trop tard pour jouer les bandits ah bon ? Impossible de roupiller quand j'suis en perte ou passer du bon temps Même quand, même quand j'vide mon esprit, garde le ffre-chi en tête Et j'crois qu'j'ai jamais réfléchi autant Sans faire crari, dans la crave-bi, j'ai pris des balles J'rigole quand j'vois ces gues-shla raconter nos vies brr On sait ouvrir les portes, fermer des bouches brr sans mettre de baffe Sans lâcher du biff salope J'mélange beuh dans le shit, pratique et théorie C'est l'Apocalypse, j'lâche un flow météorite j'lâche un flow météorite Guette la météo, il est temps qu'j'les terrorise bouh C'est comme ça qu'on extériorise bouh Comme ça qu'on extériorise C'est comme ça qu'on extériorise eh Comme ça qu'on extériorise eh Habitué au risque C'est comme ça qu'on extériorise C'est comme ça qu'on extériorise uh C'est comme ça qu'on extériorise uh C'est l'Glock qui lé-par, c'est pas Jacques a dit oui, la haine, on la noie pas dans la oui Zéro tête à part chez l'Paki', cette année, ça nehess pas, gros, j'envoie l'paquet paquet Fallait parler depuis l'début, imbécile, ça sent la fin la BAC t'a plaqué salope En deux-trois heures, j'me retrouve à BX eh à fond sur l'autoroute eh, allemande est la plaque eh Envoie un échant', j'en n'ai rien à foutre du tampon sur la plaquette Et on s'en fout qu'tu pètes un câble, si tu t'caches, on va retaper ta caisse poh J'les vois tous jouer brr les mecs en ce-pla brr, brr mais j'les connais, ces connards, ils sont pas prêts brr, pas prêts Quand la pute recompte le blé, j'suis pas con, poto, j'recompte juste après après, après, après</t>
         </is>
       </c>
     </row>
@@ -1534,7 +1534,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Ça t'fait d'la, ça t'fait d'la Ça t'fait d'la drill, ça t'fait un sale boulot han, ça t'nique ta race, tes potes ont pas le temps de débouler Renoi, t'as pas honte t'as mis la boulette, la concu', j'la mange comme le Yassa poulet poh On esquive le fer, on s'bat contre les poulets, tu t'noies dans les ennuies, j'suis entrain de me la couler brr Arme blanche dans la main, j'annonce la couleur han, arme blanche dans la main, j'annonce la couleur han On s'en bat les couilles que t'es un mec cool ah bon ?, nique la mère aux condés qui fouillent mes couilles ah bon ? J'fais pas semblant quand j'ppe-ra, tout l'monde m'écoute, ça t'met en sang si tu sens pas les coups Que des négros dans l'gamos noir mat ouh, la BAC nous découpe à tous les coups ouh Le charbonneur est bon en maths, pourtant, rien qu'il v'-esqui les cours ouh Il a à peine 14 ans, il connait même pas la peine qu'il encourt uh Dans ton ghetto, y a grave du faux, comme au marché d'Clignancourt Tu fais le Pablo devant les tiperes, toi, askip, tu mets bien les tits-pe T'inquiète, j'dirais pas qu'ici ça t'visser, tu seras servi, attends un p'tit peu Tu veux faire rentrer, mais tu réfléchis pas, si tu dis que t'es dedans, mon négro, ne chie pas poh La vie des gens, j'en ai rien à foutre, encaisser, garder la santé c'est l'principal ph T'étais où quand on allait piller han ? T'étais où quand on allait dealer ? han Toujours des solutions tant qu'on a les billets, j'ai bicrave ma peine dans la bombonne d'hier J'ai pas claqué l'bénef' sous les cocotiers, askip, j'suis écouté dans la France entière Mais bon, j'crois qu'j'suis encore sous-côté, si on doit t'arroser, c'est pas à l'extinc, poh, poh On a plus l'temps d'papoter, on parle de plavon en comité restreint brr L'il des gens peut tout faire capoter brr, brr, brr, et si tu veux pas rembourser, ta vie, on peut la saboter salope You might also like Les dormeurs sont devenus démodés, les junkies défilent comme les top model Si cette tchaga envoie l'texto, ça t'mélange dans le Novotel uh Quand j'sors du comico, obligé d'aller per-ta un nouveau tel Tout les jours j'fais mes bails discrets, j'suis pas dans le relationnel J'gaze, j'piétine, j'gaze, j'piétine, ADN d'ennemis sous mes semelles Enquête, poucave, détonneur, saisie, j'vois le terrain qui bat de son aile T'es qu'un acteur, tes mensonges, j'vais pas gober, l'opinel leur fera danser le logobi Ils entendront mes sons même si j'suis boycoté, même si mes textes sont des photocopies T'étais où quand dans la veca, j'découpais ? Toi, t'es là que quand y a les groupies Il m'faut une Mitsubishi ou une Nissan coupée Tu veux suivre le train d'vie, igo, prends ton ticket, j'ai fais des trucs salasses, j'ai rien revendiqué Cette grosse pute, elle aime pas mon son, mais elle est prête à donner son cul pour s'impliquer Beaucoup d'jaloux, mais en vrai, ils ont cliqué pas d'interview, en vrai, j'suis bon qu'à kicker Ramène des prods, j'leur fais du sale boulot, j'arrive comme un bourreau pour les décapiter C'est pour bison, la mala, le J, Badem, mes refrés jusqu'à la muerte mmh Y a ibé, Croco, Gojos, Douma, et belek à toi si t'as merdé mmh Warrel, Yosko, DLF, Vito, la guerre, tu peux pas éviter Merka, Patch, TP, TP, tu dois un billet, ça peut t'amender mmh Nefast, , le T, merci pour la qualité Merci La moula, mapess', HLD, cette année, j'sens que ça va péter J'en place une pour Zack, pour tout mes sins-c' et les rates-pi qui tiennent le sac Ceux qui charbonnent dans l'sale, et même dans l'propre tout ceux qui m'écoute à la salle brr1</t>
+          <t>Ça t'fait d'la, ça t'fait d'la Ça t'fait d'la drill, ça t'fait un sale boulot han, ça t'nique ta race, tes potes ont pas le temps de débouler Renoi, t'as pas honte t'as mis la boulette, la concu', j'la mange comme le Yassa poulet poh On esquive le fer, on s'bat contre les poulets, tu t'noies dans les ennuies, j'suis entrain de me la couler brr Arme blanche dans la main, j'annonce la couleur han, arme blanche dans la main, j'annonce la couleur han On s'en bat les couilles que t'es un mec cool ah bon ?, nique la mère aux condés qui fouillent mes couilles ah bon ? J'fais pas semblant quand j'ppe-ra, tout l'monde m'écoute, ça t'met en sang si tu sens pas les coups Que des négros dans l'gamos noir mat ouh, la BAC nous découpe à tous les coups ouh Le charbonneur est bon en maths, pourtant, rien qu'il v'-esqui les cours ouh Il a à peine 14 ans, il connait même pas la peine qu'il encourt uh Dans ton ghetto, y a grave du faux, comme au marché d'Clignancourt Tu fais le Pablo devant les tiperes, toi, askip, tu mets bien les tits-pe T'inquiète, j'dirais pas qu'ici ça t'visser, tu seras servi, attends un p'tit peu Tu veux faire rentrer, mais tu réfléchis pas, si tu dis que t'es dedans, mon négro, ne chie pas poh La vie des gens, j'en ai rien à foutre, encaisser, garder la santé c'est l'principal ph T'étais où quand on allait piller han ? T'étais où quand on allait dealer ? han Toujours des solutions tant qu'on a les billets, j'ai bicrave ma peine dans la bombonne d'hier J'ai pas claqué l'bénef' sous les cocotiers, askip, j'suis écouté dans la France entière Mais bon, j'crois qu'j'suis encore sous-côté, si on doit t'arroser, c'est pas à l'extinc, poh, poh On a plus l'temps d'papoter, on parle de plavon en comité restreint brr L'il des gens peut tout faire capoter brr, brr, brr, et si tu veux pas rembourser, ta vie, on peut la saboter salope Les dormeurs sont devenus démodés, les junkies défilent comme les top model Si cette tchaga envoie l'texto, ça t'mélange dans le Novotel uh Quand j'sors du comico, obligé d'aller per-ta un nouveau tel Tout les jours j'fais mes bails discrets, j'suis pas dans le relationnel J'gaze, j'piétine, j'gaze, j'piétine, ADN d'ennemis sous mes semelles Enquête, poucave, détonneur, saisie, j'vois le terrain qui bat de son aile T'es qu'un acteur, tes mensonges, j'vais pas gober, l'opinel leur fera danser le logobi Ils entendront mes sons même si j'suis boycoté, même si mes textes sont des photocopies T'étais où quand dans la veca, j'découpais ? Toi, t'es là que quand y a les groupies Il m'faut une Mitsubishi ou une Nissan coupée Tu veux suivre le train d'vie, igo, prends ton ticket, j'ai fais des trucs salasses, j'ai rien revendiqué Cette grosse pute, elle aime pas mon son, mais elle est prête à donner son cul pour s'impliquer Beaucoup d'jaloux, mais en vrai, ils ont cliqué pas d'interview, en vrai, j'suis bon qu'à kicker Ramène des prods, j'leur fais du sale boulot, j'arrive comme un bourreau pour les décapiter C'est pour bison, la mala, le J, Badem, mes refrés jusqu'à la muerte mmh Y a ibé, Croco, Gojos, Douma, et belek à toi si t'as merdé mmh Warrel, Yosko, DLF, Vito, la guerre, tu peux pas éviter Merka, Patch, TP, TP, tu dois un billet, ça peut t'amender mmh Nefast, , le T, merci pour la qualité Merci La moula, mapess', HLD, cette année, j'sens que ça va péter J'en place une pour Zack, pour tout mes sins-c' et les rates-pi qui tiennent le sac Ceux qui charbonnent dans l'sale, et même dans l'propre tout ceux qui m'écoute à la salle brr1</t>
         </is>
       </c>
     </row>
@@ -1551,7 +1551,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Daddy Jo Nous, on t'sourit pas pour une pomme, j'ai du shit dans la paume, du shit dans la paume Sur l'terrain latéral, si j'tire, j'vais pas ter-ra Devant la que-ba, mon kamas, j'ai pété Askip, dans l'pe-ra, j'ai pété Deux-trois balles, est-ce qu'ils s'relèvent ? Là, j'suis en pétard Là, j'suis en pétard, y a qu'l'argent qu'j'épargne Ouh Tant qu'les menottes, j'ai pas Ouh Le passé, j'l'ai passé à bir' quand j'y pense t'es mort si t'agis pas J'me lève, j'cherche l'argent, j'mise pas sur les plans Poh, poh, poh, poh J'vois la ce-pu monter, la tension monter Poh, poh J'veux casser mon tête, les schmitts ont mon ADN, j'vis L'plavon, j'ai plus d'adré', j'me sappe et j'suis en bas d'l'adresse J'vais pas baiser une tain-p', ça fait longtemps qu'j'ai niqué la drill Ouais J'me fais ser-cour, un pied sur la grille Vol avec agre', quelques jours après, il m'arrive des dingueries Posé sur l'terrain, j'me faisais une puce Uh, j'm'en fous qu'l'oseille pue Poh, poh, poh, poh, uh J'veux peser plus, le poto, il ramasse une bouteille, il s'bute Poh, poh, poh, poh, poh, poh Belek, belek, belek, belek, tu vois le J cagoulé, y a boulé Le J cagoulé, le ient-cli attend pendant qu'j'suis en train d'rouler Brr, brr, brr Dans mes plus beaux rêves, j'vois le comico brûler, cité d'la ne-Plai, on piétine la paix À midi, j'ramasse un salaire sur un appel J'croise l'ennemi, il court J'remonte sur la selle, on repasse demain, t'façon, on n'a rien à perdre Y a du pilon re-ch', j'ai rien mis dans ma bre-ch', à tout moment, j'suis sté-pi, au bigo, j'abrège J'me réveille, j'roule un joint d'hasch', j'écoute du H Sur moi, j'ai un I, t'as fait tartin deux semaines, t'as pas mangé un K Ramène ton zinclar, il va s'manger un kick T'sais qu'à la se-ba, j'suis pas dans les clips dès qu'j'ai eu le déclic, j'allais rabattre des cli' Tah bekli Sur le bigo à clin's, v'là les textes, j'ai écrit, contrôle musclé, la G.A.V, j'y ai cru J'mange pas là-bas même si j'ai un creux, même si j'fais quantante-huit C'est San Andreas la porte d'chez toi, on crible R.A.F des caméras quand on crime R.A.S, zéro témoin quand ils crient Cuando habla dinero comprendro Toi-même, tu m'as compris Tu m'as compris J'sais pas l'jour où j'l'achète ou pas, j'vis au jour le jour, j'fais tout ti-par L'avocat gronde la juge, c'est sûr, j'vais ti-sor 1PLIKÉ C'est une pute, pour d'la cons', elle est moins réticente 1PLIKÉ Ma mentale dans mes sons y'a un obstacle, j'le saute 1PLIKÉ Mes plus grosses folies étant adolescent J'aurais pu aller loin, j'étais freiné par les autres Amour, bénéf', on confond pas les deux Bénéf' Bénéf', ils en font pas, ils font parler d'eux Bénéf' Période de gue-sh', le ciel est dégueu' Bénéf' Pour elle, j'suis son gars pour moi, c'est ambigu Poh, poh Sous beugeuh, boosté, j'rappe sur 2Pac ou Biggie Gros, faire du 1PLIKÉ, gros, c'est pas compliqué Longtemps que j'sais kicker, j'sais j'vais prendre chez qui, j'sais qui checker Mal au poignet, j'dois détailler l'kil' J'vois des dingueries, j'suis même plus choqué, ça fait longtemps que notre géné' part en vrille J'bosse solo, m'demande pas c'est l'tail-dé à qui Tu t'fais ter-sau au tel-hô, t'as pas l'temps d'la ken J'suis vers Chiraq, évidemment, j'suis no lackin' J'suis vers Chiraq, évidemment, j'suis no lackin' Le rap, c'est mon rrain-té, j'dois rester actif Comme Gucc', comme Gucc' Toujours des armes quand on bouge Quand on bouge On t'fait danser Sous la cagoule, c'est moi qui push Même si la CR fait des ricochets J'tte-j' un savon, pas l'éponge C'est des cons, j'les ramasse après, tu connais l'projet Avec ces connards, j'ai coupé les ponts 1PLIKÉ revient bouillant mais loin d'son apogée Failli ber-tom, j'me suis accroché J'voulais l'bifton, j'm'en suis approché Avant l'été, ça sort les bécs', faut qu'ça pète C'est bien, t'as pris du te-te, mais bon maintenant, faut qu'ça appelle Maintenant, faut qu'ça appelle You might also like Mal au poignet, j'dois détailler l'kil' J'bosse solo, m'demande pas c'est l'tail-dé à qui J'suis vers Chiraq, évidemment, j'suis no lackin'</t>
+          <t>Daddy Jo Nous, on t'sourit pas pour une pomme, j'ai du shit dans la paume, du shit dans la paume Sur l'terrain latéral, si j'tire, j'vais pas ter-ra Devant la que-ba, mon kamas, j'ai pété Askip, dans l'pe-ra, j'ai pété Deux-trois balles, est-ce qu'ils s'relèvent ? Là, j'suis en pétard Là, j'suis en pétard, y a qu'l'argent qu'j'épargne Ouh Tant qu'les menottes, j'ai pas Ouh Le passé, j'l'ai passé à bir' quand j'y pense t'es mort si t'agis pas J'me lève, j'cherche l'argent, j'mise pas sur les plans Poh, poh, poh, poh J'vois la ce-pu monter, la tension monter Poh, poh J'veux casser mon tête, les schmitts ont mon ADN, j'vis L'plavon, j'ai plus d'adré', j'me sappe et j'suis en bas d'l'adresse J'vais pas baiser une tain-p', ça fait longtemps qu'j'ai niqué la drill Ouais J'me fais ser-cour, un pied sur la grille Vol avec agre', quelques jours après, il m'arrive des dingueries Posé sur l'terrain, j'me faisais une puce Uh, j'm'en fous qu'l'oseille pue Poh, poh, poh, poh, uh J'veux peser plus, le poto, il ramasse une bouteille, il s'bute Poh, poh, poh, poh, poh, poh Belek, belek, belek, belek, tu vois le J cagoulé, y a boulé Le J cagoulé, le ient-cli attend pendant qu'j'suis en train d'rouler Brr, brr, brr Dans mes plus beaux rêves, j'vois le comico brûler, cité d'la ne-Plai, on piétine la paix À midi, j'ramasse un salaire sur un appel J'croise l'ennemi, il court J'remonte sur la selle, on repasse demain, t'façon, on n'a rien à perdre Y a du pilon re-ch', j'ai rien mis dans ma bre-ch', à tout moment, j'suis sté-pi, au bigo, j'abrège J'me réveille, j'roule un joint d'hasch', j'écoute du H Sur moi, j'ai un I, t'as fait tartin deux semaines, t'as pas mangé un K Ramène ton zinclar, il va s'manger un kick T'sais qu'à la se-ba, j'suis pas dans les clips dès qu'j'ai eu le déclic, j'allais rabattre des cli' Tah bekli Sur le bigo à clin's, v'là les textes, j'ai écrit, contrôle musclé, la G.A.V, j'y ai cru J'mange pas là-bas même si j'ai un creux, même si j'fais quantante-huit C'est San Andreas la porte d'chez toi, on crible R.A.F des caméras quand on crime R.A.S, zéro témoin quand ils crient Cuando habla dinero comprendro Toi-même, tu m'as compris Tu m'as compris J'sais pas l'jour où j'l'achète ou pas, j'vis au jour le jour, j'fais tout ti-par L'avocat gronde la juge, c'est sûr, j'vais ti-sor 1PLIKÉ C'est une pute, pour d'la cons', elle est moins réticente 1PLIKÉ Ma mentale dans mes sons y'a un obstacle, j'le saute 1PLIKÉ Mes plus grosses folies étant adolescent J'aurais pu aller loin, j'étais freiné par les autres Amour, bénéf', on confond pas les deux Bénéf' Bénéf', ils en font pas, ils font parler d'eux Bénéf' Période de gue-sh', le ciel est dégueu' Bénéf' Pour elle, j'suis son gars pour moi, c'est ambigu Poh, poh Sous beugeuh, boosté, j'rappe sur 2Pac ou Biggie Gros, faire du 1PLIKÉ, gros, c'est pas compliqué Longtemps que j'sais kicker, j'sais j'vais prendre chez qui, j'sais qui checker Mal au poignet, j'dois détailler l'kil' J'vois des dingueries, j'suis même plus choqué, ça fait longtemps que notre géné' part en vrille J'bosse solo, m'demande pas c'est l'tail-dé à qui Tu t'fais ter-sau au tel-hô, t'as pas l'temps d'la ken J'suis vers Chiraq, évidemment, j'suis no lackin' J'suis vers Chiraq, évidemment, j'suis no lackin' Le rap, c'est mon rrain-té, j'dois rester actif Comme Gucc', comme Gucc' Toujours des armes quand on bouge Quand on bouge On t'fait danser Sous la cagoule, c'est moi qui push Même si la CR fait des ricochets J'tte-j' un savon, pas l'éponge C'est des cons, j'les ramasse après, tu connais l'projet Avec ces connards, j'ai coupé les ponts 1PLIKÉ revient bouillant mais loin d'son apogée Failli ber-tom, j'me suis accroché J'voulais l'bifton, j'm'en suis approché Avant l'été, ça sort les bécs', faut qu'ça pète C'est bien, t'as pris du te-te, mais bon maintenant, faut qu'ça appelle Maintenant, faut qu'ça appelle Mal au poignet, j'dois détailler l'kil' J'bosse solo, m'demande pas c'est l'tail-dé à qui J'suis vers Chiraq, évidemment, j'suis no lackin'</t>
         </is>
       </c>
     </row>
@@ -1568,7 +1568,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Poh, poh, poh, poh Ton ness-bi' n'est pas durable comme mes relations, eux, c'est pas d'l'inspi', c'est d'l'imagination brr Ils s'inventent des vies, j'sais qu'ils sont pas dans l'action brr, brr, brr J'lui parle pour baiser, elle pense que j'veux m'poser brr Pétasse, y aura pas d'présentation, j'me nashave une fois qu'j'ai tout plié Tant mieux si j'finis aux oubliettes, y avait tout dans la ve-c', beugeuh, te-shi, deux-trois boulettes J'baraude avec le J, on est cagoulés, sans pitié, on a du l'être Normal, on t'serre la main même si on t'a boulé poh, poh, poh Ils savent qu'on déboulent que pour les uer-t mais bon, c'est des cons, j'sais qu'ils veulent pas s'l'avouer Tes plans tombent à l'eau, j'passe la bouée, j'v'-esqui l'ballon mais bon, j'ai pas savouré Sort l'opinel à tout va comme les chicanos uh Depuis l'pe-ra, la pute me trouve canon eh, j'la fais monter mais elle va pas snaper l'gamos eh, eh Côté Chicago, regarde le panneau, la hagra, ça paye pas mais nous, on dit pas non Jai des bonnes connexions et des bons gavas, tu vas hasba, mets-toi en cavale Pas moi qui est posté sur le R mais j'suis démarqué, envoie la balle T'aimes, avec une te-pu qui veut ken, elle doit s'mettre au boulot, putain, elle fait laquelle ? 1PLIKÉ J'pue la frappe, j'ai du étouffé la 'quette 1PLIKÉ , lassé par la paix, on a tous fait la guerre 1PLIKÉ Cest fini le temps des couches, j'tire sur l'O.G Kush, jsuis venu en découdre Lancien a raison, moi, en vrai, je men bas les couilles, on s'ra cool quand y aura l'million dans les fouilles Les pieds sur terre, ça perd pas la tête pour une fouffe mais en embrouille, ils savent qu'on est fous poh On vient marquer le coup, j'aime l'ennemi quand il souffre À midi, j'ai le kush, j'suis dans la finition poh Les balances, tu sais bien elles finissent où han, pour les deux définitions, j'débite hein, j'fais pas d'pause eh Quoiqu'il en coûte, j'sais qu'j'ai niqué l'instru', j'ai même pas fini l'son eh Ici, dans l'sous-sol, la ppe-fra, tu ramènes, quand tu sors d'la ve-ca, referme bien derrière Il est jamais loin celui qui veut t'la mettre, fais belek, gros, on sait jamais Pas assez détendus quand on est sobres poh, zéro mala, rien à foutre des sapes oui C'est quand tu crois qu'on a oublié, qu'on t'choppe, harbat, quand sa te-tê a tapé l'sol oui Point de côté, j'me revois compter sur le sable poh mais au final, j'ai pas compté sur ça brr Le plan où tu galères, on le trouve plutôt simple, viens pas nous kelerh, on a plus douze ans On manie les armes, on s'bat plus, désormais, j'ai vu l'ennemi din-din tapé l'deux-cent mètres La victime se plaint sans savoir la chance qu'elle a, j'espère qu'un jour, elle arrivera à s'en r'mettre Étant jeune, j'voulais pas que les plus grands m'cala poh, plus tard, c'est eux qui m'demandent si y a chose-quel C'est la reine des tain-p', zerma, personne te l'a dit j'la casse dans le bat' quand tu l'attends à l'hôtel Pour les faux négros, j'ai zéro empathie brr, pour les faux négros, j'ai zéro empathie brr T'étonnes pas qu'personne veut rester une fois qu'la balle elle est partie You might also like La nuit s'ra longue, j'ai tué l'pilon, dans ma 'bre, j'vois une ombre dans ma 'bre, j'vois une ombre J'm'en fous d'me faire un nom, j'veux faire que du nombre, j'veux faire que du nombre je veux faire que du nombre Igo, on s'en fout d'ta génération, on vient taper du monde poh, poh, poh, taper du monde 9.2.1.4.0 sur le pocheton Si tu veux passer, c'est l'fer qui dit non La nuit s'ra longue, j'ai tué l'pilon, dans ma 'bre, j'vois une ombre dans ma 'bre, j'vois une ombre J'm'en fous d'me faire un nom, j'veux faire que du nombre, j'veux faire que du nombre Igo, on s'en fout d'ta génération, on vient taper du monde poh, poh, poh, taper du monde 9.2.1.4.0 sur le pocheton Si tu veux passer, c'est l'fer qui dit non brr, brr, brr Y a pas que vous, les choy mont aussi sur écoute hein, jsouris quand le gérant se perd sur les comptes hein J'crois qu'au loin, j'aperçois les cond', tu nnais-co, leurs dit pas j't'ai donné quoi hein Elle est jeune mais c'est déjà une grosse tchaga, j'me demande Dans cinq ans, ça va donner quoi ? 1PLIKÉ Plus jamais j'reprends l'école, toujours précis, les bastos, on les colle 1PLIKÉ J'descends, j'détaille, j'redécolle, j'suis en détente, bientôt, j'vais jouer au golf Sur ton R, y a personne pour jouer au goal, j'ai vu que des mecs qui jouaient aux gols-mon brr C'est pour son cavu qu'j'la cala, salope, si t'as mal, t'as qu'à lâcher J'aime quand les tits-pe veulent tout arracher, madame la juge, il ne fait que la cheb La nuit s'ra longue, j'ai tué l'pilon, dans ma 'bre, j'vois une ombre dans ma 'bre, j'vois une ombre J'm'en fous d'me faire un nom, j'veux faire que du nombre, j'veux faire que du nombre je veux faire que du nombre Igo, on s'en fout d'ta génération, on vient taper du monde poh, poh, poh, taper du monde 9.2.1.4.0 sur le pocheton poh, poh Si tu veux passer, c'est l'fer qui dit non La nuit s'ra longue, j'ai tué l'pilon, dans ma 'bre, j'vois une ombre dans ma 'bre, j'vois une ombre J'm'en fous d'me faire un nom, j'veux faire que du nombre, j'veux faire que du nombre Igo, on s'en fout d'ta génération, on vient taper du monde poh, poh, poh, taper du monde 9.2.1.4.0 sur le pocheton eh Si tu veux passer, c'est l'fer qui dit non eh, eh, eh</t>
+          <t>Poh, poh, poh, poh Ton ness-bi' n'est pas durable comme mes relations, eux, c'est pas d'l'inspi', c'est d'l'imagination brr Ils s'inventent des vies, j'sais qu'ils sont pas dans l'action brr, brr, brr J'lui parle pour baiser, elle pense que j'veux m'poser brr Pétasse, y aura pas d'présentation, j'me nashave une fois qu'j'ai tout plié Tant mieux si j'finis aux oubliettes, y avait tout dans la ve-c', beugeuh, te-shi, deux-trois boulettes J'baraude avec le J, on est cagoulés, sans pitié, on a du l'être Normal, on t'serre la main même si on t'a boulé poh, poh, poh Ils savent qu'on déboulent que pour les uer-t mais bon, c'est des cons, j'sais qu'ils veulent pas s'l'avouer Tes plans tombent à l'eau, j'passe la bouée, j'v'-esqui l'ballon mais bon, j'ai pas savouré Sort l'opinel à tout va comme les chicanos uh Depuis l'pe-ra, la pute me trouve canon eh, j'la fais monter mais elle va pas snaper l'gamos eh, eh Côté Chicago, regarde le panneau, la hagra, ça paye pas mais nous, on dit pas non Jai des bonnes connexions et des bons gavas, tu vas hasba, mets-toi en cavale Pas moi qui est posté sur le R mais j'suis démarqué, envoie la balle T'aimes, avec une te-pu qui veut ken, elle doit s'mettre au boulot, putain, elle fait laquelle ? 1PLIKÉ J'pue la frappe, j'ai du étouffé la 'quette 1PLIKÉ , lassé par la paix, on a tous fait la guerre 1PLIKÉ Cest fini le temps des couches, j'tire sur l'O.G Kush, jsuis venu en découdre Lancien a raison, moi, en vrai, je men bas les couilles, on s'ra cool quand y aura l'million dans les fouilles Les pieds sur terre, ça perd pas la tête pour une fouffe mais en embrouille, ils savent qu'on est fous poh On vient marquer le coup, j'aime l'ennemi quand il souffre À midi, j'ai le kush, j'suis dans la finition poh Les balances, tu sais bien elles finissent où han, pour les deux définitions, j'débite hein, j'fais pas d'pause eh Quoiqu'il en coûte, j'sais qu'j'ai niqué l'instru', j'ai même pas fini l'son eh Ici, dans l'sous-sol, la ppe-fra, tu ramènes, quand tu sors d'la ve-ca, referme bien derrière Il est jamais loin celui qui veut t'la mettre, fais belek, gros, on sait jamais Pas assez détendus quand on est sobres poh, zéro mala, rien à foutre des sapes oui C'est quand tu crois qu'on a oublié, qu'on t'choppe, harbat, quand sa te-tê a tapé l'sol oui Point de côté, j'me revois compter sur le sable poh mais au final, j'ai pas compté sur ça brr Le plan où tu galères, on le trouve plutôt simple, viens pas nous kelerh, on a plus douze ans On manie les armes, on s'bat plus, désormais, j'ai vu l'ennemi din-din tapé l'deux-cent mètres La victime se plaint sans savoir la chance qu'elle a, j'espère qu'un jour, elle arrivera à s'en r'mettre Étant jeune, j'voulais pas que les plus grands m'cala poh, plus tard, c'est eux qui m'demandent si y a chose-quel C'est la reine des tain-p', zerma, personne te l'a dit j'la casse dans le bat' quand tu l'attends à l'hôtel Pour les faux négros, j'ai zéro empathie brr, pour les faux négros, j'ai zéro empathie brr T'étonnes pas qu'personne veut rester une fois qu'la balle elle est partie La nuit s'ra longue, j'ai tué l'pilon, dans ma 'bre, j'vois une ombre dans ma 'bre, j'vois une ombre J'm'en fous d'me faire un nom, j'veux faire que du nombre, j'veux faire que du nombre je veux faire que du nombre Igo, on s'en fout d'ta génération, on vient taper du monde poh, poh, poh, taper du monde 9.2.1.4.0 sur le pocheton Si tu veux passer, c'est l'fer qui dit non La nuit s'ra longue, j'ai tué l'pilon, dans ma 'bre, j'vois une ombre dans ma 'bre, j'vois une ombre J'm'en fous d'me faire un nom, j'veux faire que du nombre, j'veux faire que du nombre Igo, on s'en fout d'ta génération, on vient taper du monde poh, poh, poh, taper du monde 9.2.1.4.0 sur le pocheton Si tu veux passer, c'est l'fer qui dit non brr, brr, brr Y a pas que vous, les choy mont aussi sur écoute hein, jsouris quand le gérant se perd sur les comptes hein J'crois qu'au loin, j'aperçois les cond', tu nnais-co, leurs dit pas j't'ai donné quoi hein Elle est jeune mais c'est déjà une grosse tchaga, j'me demande Dans cinq ans, ça va donner quoi ? 1PLIKÉ Plus jamais j'reprends l'école, toujours précis, les bastos, on les colle 1PLIKÉ J'descends, j'détaille, j'redécolle, j'suis en détente, bientôt, j'vais jouer au golf Sur ton R, y a personne pour jouer au goal, j'ai vu que des mecs qui jouaient aux gols-mon brr C'est pour son cavu qu'j'la cala, salope, si t'as mal, t'as qu'à lâcher J'aime quand les tits-pe veulent tout arracher, madame la juge, il ne fait que la cheb La nuit s'ra longue, j'ai tué l'pilon, dans ma 'bre, j'vois une ombre dans ma 'bre, j'vois une ombre J'm'en fous d'me faire un nom, j'veux faire que du nombre, j'veux faire que du nombre je veux faire que du nombre Igo, on s'en fout d'ta génération, on vient taper du monde poh, poh, poh, taper du monde 9.2.1.4.0 sur le pocheton poh, poh Si tu veux passer, c'est l'fer qui dit non La nuit s'ra longue, j'ai tué l'pilon, dans ma 'bre, j'vois une ombre dans ma 'bre, j'vois une ombre J'm'en fous d'me faire un nom, j'veux faire que du nombre, j'veux faire que du nombre Igo, on s'en fout d'ta génération, on vient taper du monde poh, poh, poh, taper du monde 9.2.1.4.0 sur le pocheton eh Si tu veux passer, c'est l'fer qui dit non eh, eh, eh</t>
         </is>
       </c>
     </row>
@@ -1585,7 +1585,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>T'as même pas un client mais tu dis qu'ça part vite, y a heja, tu t'casses en mode tu reviens en de-spee Pourtant, dans la soirée, on t'a pas vu Eh, tu pars au soleil, tu retrouves ton appart' vide La première, on loba, la deuxième, on t'arrose, depuis qu'on est tit-pe, on v'-esqui les barreaux Aucun num' de salopes dans la puce Lebara, la sécu' est chromé, le single est doré La vérité blesse et fait tomber les masques, est-c que les mecs qu'j'ai crossé écoutnt mes sons ? On va t'pull up ton tieks mais y a aucun gars, devant l'Bulapi, plus aucun garsYou might also like</t>
+          <t>T'as même pas un client mais tu dis qu'ça part vite, y a heja, tu t'casses en mode tu reviens en de-spee Pourtant, dans la soirée, on t'a pas vu Eh, tu pars au soleil, tu retrouves ton appart' vide La première, on loba, la deuxième, on t'arrose, depuis qu'on est tit-pe, on v'-esqui les barreaux Aucun num' de salopes dans la puce Lebara, la sécu' est chromé, le single est doré La vérité blesse et fait tomber les masques, est-c que les mecs qu'j'ai crossé écoutnt mes sons ? On va t'pull up ton tieks mais y a aucun gars, devant l'Bulapi, plus aucun gars</t>
         </is>
       </c>
     </row>
@@ -1602,7 +1602,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Poh, poh, poh, poh Poh, poh, poh, poh Hein J'passe à la barre, j'laisse parler mon avocat hein, même si j'l'ai pas encore rincé hein Les ennemis déboulent, ils sont bukkake poh mais crois pas qu'ils vont pas danser poh Ils font pas d'argent, ils font des mises en scène J'ai pas attendu mes potes, j'me suis mis dans ça J'ai su brasser quand tu faisais la sieste drr, drr, drr C'est encore 1PLIKÉ-1.4 qui dead ça J'viens d'les remettre, tu veux déjà mes lacets Arrête ça, si on t'visser mal tu mérits ça ah bon ? On lance pas des piques, on fait coulr l'harissa ah bon ? À quoi bon parler ? T'façon, eux-mêmes, ils savent On commence tôt, bonbonne dans la raie du cul Le client à deux doigts d'l'arrêt du cur Passer toute ma vie dans la sique-mu poh, j'trouve ça ridicule poh, y penser, ça m'écure Ça peut t'faire ta 'pine, ta reum sans sécu', fuck l'OPJ qui veut que j'm'excuse Fuck l'il, à part si tu l'as sur l'textile, dommage si tu l'as sur l' C'est avec les billets qu'on t'estime, après les douze coups d'minuit, j'fais encore des thunes mmh Remballe tes lois ici, la vente est clandestine mmh Jamais j'donnerai mon cur à une pute en legging avec un corps de bus You might also like Rien qu'elle suce, elle veut tirer une taffe, elle mérite que le P4 Impossible que j'me déplace si l'billet qu'tu me proposes, il me plait as-p uh Parfois, j'ai d'la peine pour les opps uh, sur un mauvais coup, tu peux t'faire smoke drr Genre, tu vas rejoindre le Roi d'la pop drr, drr, drr, c'est dans un sale état qu'on rend l'appart' Dans un sale état, on laisse la tchop des porcs, on laisse la tchop des porcs, baw, baw C'est l'top départ, j'viens d'là où c'est l'pilon qui t'ouvre des portes Dans un sale état, on laisse la tchop des porcs mmh, on laisse la tchop des porcs mmh, baw, baw C'est l'top départ, j'viens d'là où c'est l'pilon qui t'ouvre des portes J'vais les baiser, baiser et rien leur donner mmh, me casser en balle, tu fais l'étonné mmh Mais tu me connais, j'ai des missions à faire, y'a du shit, de la beugeuh, il va bientôt neiger Mmh, mmh, on est des nes-jeu, hasba, on a mis pour péter l'ne-jau Pour péter le jaune, j'aurais jamais pensé casser mon jeûne Un jour, nan, j'le fais pas pour les gens, ces cons sont pas armés Je sais qu'ils font genre le jour où ils l'seront, ils viseront que les jambes J'ai connu mes démons, j'sortais du collège, hmm, hmm 1PLIKÉ Qui t'a dit qu'on est jeunes ? Les aléas d'la vie, on connait l'jeu 1PLIKÉ Remercie Dieu chaque fois qu'j'connais l'jour On gère le destin, les épreuves, on endure, bâtard De mettre le fuego, on va pas cesser, nous tends pas la main, on va jamais sucer L'affaire est classée, j'suis blanc comme neige J'ai rêvé qu'il pleuvait des boulettes de CC À l'idée d'bosser, ils sont craintifs, quel gâchis, ils s'en sortiront jamais en faisant aucun chiffre en faisant aucun chiffre Comment faire le bien quand le mal est lucratif ? Rien qu'elle suce, elle veut tirer une taffe, elle mérite que le P4 Impossible que j'me déplace si l'billet qu'tu me proposes, il me plait as-p uh Parfois, j'ai d'la peine pour les opps uh, sur un mauvais coup, tu peux t'faire smoke drr Genre, tu vas rejoindre le Roi d'la pop drr, drr, drr, c'est dans un sale état qu'on rend l'appart' Dans un sale état, on laisse la tchop des porcs, on laisse la tchop des porcs, baw, baw C'est l'top départ, j'viens d'là où c'est l'pilon qui t'ouvre des portes Dans un sale état, on laisse la tchop des porcs eh, on laisse la tchop des porcs eh, baw, baw C'est l'top départ, j'viens d'là où c'est l'pilon qui t'ouvre des portes 9.2.1.4.0 sur le pocheton, j'viens d'là où le pilon il t'ouvre des portes J'suis rentré avec des points, publiquement, on fait du sale, on oublie souvent que les tits-pe marchent sur nos pas Publiquement, on fait du sale mais on oublie souvent que les tits-pe marchent sur nos pas J'ai grandi, c'est le neuf qui assume mes pas Grah, normal tu t'en remets pas Grah, grah, grah, tu t'en remets pas 1PLIKÉ, 1.4.0 dans ton enceinte</t>
+          <t>Poh, poh, poh, poh Poh, poh, poh, poh Hein J'passe à la barre, j'laisse parler mon avocat hein, même si j'l'ai pas encore rincé hein Les ennemis déboulent, ils sont bukkake poh mais crois pas qu'ils vont pas danser poh Ils font pas d'argent, ils font des mises en scène J'ai pas attendu mes potes, j'me suis mis dans ça J'ai su brasser quand tu faisais la sieste drr, drr, drr C'est encore 1PLIKÉ-1.4 qui dead ça J'viens d'les remettre, tu veux déjà mes lacets Arrête ça, si on t'visser mal tu mérits ça ah bon ? On lance pas des piques, on fait coulr l'harissa ah bon ? À quoi bon parler ? T'façon, eux-mêmes, ils savent On commence tôt, bonbonne dans la raie du cul Le client à deux doigts d'l'arrêt du cur Passer toute ma vie dans la sique-mu poh, j'trouve ça ridicule poh, y penser, ça m'écure Ça peut t'faire ta 'pine, ta reum sans sécu', fuck l'OPJ qui veut que j'm'excuse Fuck l'il, à part si tu l'as sur l'textile, dommage si tu l'as sur l' C'est avec les billets qu'on t'estime, après les douze coups d'minuit, j'fais encore des thunes mmh Remballe tes lois ici, la vente est clandestine mmh Jamais j'donnerai mon cur à une pute en legging avec un corps de bus Rien qu'elle suce, elle veut tirer une taffe, elle mérite que le P4 Impossible que j'me déplace si l'billet qu'tu me proposes, il me plait as-p uh Parfois, j'ai d'la peine pour les opps uh, sur un mauvais coup, tu peux t'faire smoke drr Genre, tu vas rejoindre le Roi d'la pop drr, drr, drr, c'est dans un sale état qu'on rend l'appart' Dans un sale état, on laisse la tchop des porcs, on laisse la tchop des porcs, baw, baw C'est l'top départ, j'viens d'là où c'est l'pilon qui t'ouvre des portes Dans un sale état, on laisse la tchop des porcs mmh, on laisse la tchop des porcs mmh, baw, baw C'est l'top départ, j'viens d'là où c'est l'pilon qui t'ouvre des portes J'vais les baiser, baiser et rien leur donner mmh, me casser en balle, tu fais l'étonné mmh Mais tu me connais, j'ai des missions à faire, y'a du shit, de la beugeuh, il va bientôt neiger Mmh, mmh, on est des nes-jeu, hasba, on a mis pour péter l'ne-jau Pour péter le jaune, j'aurais jamais pensé casser mon jeûne Un jour, nan, j'le fais pas pour les gens, ces cons sont pas armés Je sais qu'ils font genre le jour où ils l'seront, ils viseront que les jambes J'ai connu mes démons, j'sortais du collège, hmm, hmm 1PLIKÉ Qui t'a dit qu'on est jeunes ? Les aléas d'la vie, on connait l'jeu 1PLIKÉ Remercie Dieu chaque fois qu'j'connais l'jour On gère le destin, les épreuves, on endure, bâtard De mettre le fuego, on va pas cesser, nous tends pas la main, on va jamais sucer L'affaire est classée, j'suis blanc comme neige J'ai rêvé qu'il pleuvait des boulettes de CC À l'idée d'bosser, ils sont craintifs, quel gâchis, ils s'en sortiront jamais en faisant aucun chiffre en faisant aucun chiffre Comment faire le bien quand le mal est lucratif ? Rien qu'elle suce, elle veut tirer une taffe, elle mérite que le P4 Impossible que j'me déplace si l'billet qu'tu me proposes, il me plait as-p uh Parfois, j'ai d'la peine pour les opps uh, sur un mauvais coup, tu peux t'faire smoke drr Genre, tu vas rejoindre le Roi d'la pop drr, drr, drr, c'est dans un sale état qu'on rend l'appart' Dans un sale état, on laisse la tchop des porcs, on laisse la tchop des porcs, baw, baw C'est l'top départ, j'viens d'là où c'est l'pilon qui t'ouvre des portes Dans un sale état, on laisse la tchop des porcs eh, on laisse la tchop des porcs eh, baw, baw C'est l'top départ, j'viens d'là où c'est l'pilon qui t'ouvre des portes 9.2.1.4.0 sur le pocheton, j'viens d'là où le pilon il t'ouvre des portes J'suis rentré avec des points, publiquement, on fait du sale, on oublie souvent que les tits-pe marchent sur nos pas Publiquement, on fait du sale mais on oublie souvent que les tits-pe marchent sur nos pas J'ai grandi, c'est le neuf qui assume mes pas Grah, normal tu t'en remets pas Grah, grah, grah, tu t'en remets pas 1PLIKÉ, 1.4.0 dans ton enceinte</t>
         </is>
       </c>
     </row>
@@ -1619,7 +1619,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Pah, pah, pah, pah Pah, pah, pah, pah Binks Beatz Ils s'font cher-bran par le ghetto Hein, ils s'mettent à bosser, ils font que des trous Hein Le poids d'mes péchés quand j'm'endors, j'ai rêvé de litrons, maintenant, je veux les ver-trou Hein J'ai pris des affaires, j'savais pas les mettre où Pah, j'te laisse choisir entre le neuf millimètres ou l'couteau papillon Pah Ça fait pas l'même trou Pah, j'suis marié à la street pour les papiers Pah Impossible d'la quitter, je sais qu'elle m'aim trop Brr, range-toi en deux-dux, c'est déjà plié Ouais On t'emprunte, on paie pas, c'est comme le métro et quand tu nous croises Brr, tu fais genre qu't'as oublié Brr Même dans la de-mer, on s'débrouille Eh, l'ambiance devient bre-som quand on déboule Eh Le temps, il est est compté, faut qu'j'me grouille Eh, soit j'empoche ou soit je dors debout Eh, eh Tu dois du liquide, t'esquives les rendez-vous, dans tous les cas, tu vas lâcher des coups D'arreter d'faire du sale, tous les jours, j'essaye mais bon, en vrai, y a que ça qui m'dégoûte En vrai Ça m'dégoûte, tout l'monde veut t'la mettre à croire qu'la vie, c'est un film de boule Oh Une ce-pu qui débite Oh, d'la frappe de fou pour fermer des bouches Oh, oh Pour la mi-f', j'suis prêt à tout laisser, j'dois me refaire, faut qu'j'me rachète J'repense aux conneries d'ma jeunesse, j'marche dans les rues où j'ai arraché Tous les jours, faut qu'ça vende, t'as vu, mes soucis j'ai attachés Pah Rien qu'elle fume, elle a perdu son cavu, le pilon l'a ravagée Pah You might also like Rien a changé dans mes textes, j'te raconte seulement l'implication L'implication Pour des dineros, j'déforme ta tête comme Pablo Picasso Comme Picasso Faut shooter les fédéraux, fédéraux, fédéraux, avant qu'ta porte, elle saute Ta porte, elle saute Charbon cramé, palpitations, on sait encaisser dans n'importe quelle zone Ton malheur, c'est l'dernier d'mes soucis Brr, nan, j'touche pas aux raclis sous C Brr J'ai zéro sensei, mental' zéro sucerie Brr, tu veux de l'inspi' ? Brr J'viens te ressourcer Brr Pour tuer la concu', il faut qu'j'me suicide, pour tuer la concu', il faut qu'j'me suicide Tu perds du temps Hein, sale imbécile Hein, même si tu fais des chichis, tu vas rembourser Sur la route du succès Pah, je reste lucide, lucide Pah, pah, pah, poussez-vous, j'vais éclabousser S'écarter du péché Hein, c'est presque impossible Hein, ici, même l'écolier, il finit par bosser Elle voulait pas ken, elle a fini par bosser Salope, elle trouve des chekems, faut qu'il finisse cabossé Salope Pour des tales, avec le me-cri, j'suis associé Hein et mes démons font que d'me saucer, mmh 1PLIKÉ, t'es trop boosté, boosté Boosté, dinero me gusta, casse toi avant qu'j'te shoote, tu vas pas goûter J'suis dans les dièses, j'visser des ges-shla en costard, costard Prends ton bout, bouge de là, connard, un faux pas, c'est le re-shta, re-shta Tu faisais pas un rond avant l'pe-ra, c'est pas l'moment d'nous faire la re-sta, re-sta Pour la mi-f', j'suis prêt à tout laisser, j'dois me refaire, faut qu'j'me rachète J'repense aux conneries d'ma jeunesse, j'marche dans les rues où j'ai arraché Tous les jours, faut qu'ça vende, t'as vu, mes soucis j'ai attachés Pah Rien qu'elle fume, elle a perdu son cavu, le pilon l'a ravagée Pah Rien n'a changé dans mes textes, j'te raconte seulement l'implication L'implication Pour des dineros, j'déforme ta tête comme Pablo Picasso Comme Picasso Faut shooter les fédéraux, fédéraux, fédéraux, avant qu'ta porte, elle saute Ta porte, elle saute Charbon cramé, palpitations, on sait encaisser dans n'importe quelle zone</t>
+          <t>Pah, pah, pah, pah Pah, pah, pah, pah Binks Beatz Ils s'font cher-bran par le ghetto Hein, ils s'mettent à bosser, ils font que des trous Hein Le poids d'mes péchés quand j'm'endors, j'ai rêvé de litrons, maintenant, je veux les ver-trou Hein J'ai pris des affaires, j'savais pas les mettre où Pah, j'te laisse choisir entre le neuf millimètres ou l'couteau papillon Pah Ça fait pas l'même trou Pah, j'suis marié à la street pour les papiers Pah Impossible d'la quitter, je sais qu'elle m'aim trop Brr, range-toi en deux-dux, c'est déjà plié Ouais On t'emprunte, on paie pas, c'est comme le métro et quand tu nous croises Brr, tu fais genre qu't'as oublié Brr Même dans la de-mer, on s'débrouille Eh, l'ambiance devient bre-som quand on déboule Eh Le temps, il est est compté, faut qu'j'me grouille Eh, soit j'empoche ou soit je dors debout Eh, eh Tu dois du liquide, t'esquives les rendez-vous, dans tous les cas, tu vas lâcher des coups D'arreter d'faire du sale, tous les jours, j'essaye mais bon, en vrai, y a que ça qui m'dégoûte En vrai Ça m'dégoûte, tout l'monde veut t'la mettre à croire qu'la vie, c'est un film de boule Oh Une ce-pu qui débite Oh, d'la frappe de fou pour fermer des bouches Oh, oh Pour la mi-f', j'suis prêt à tout laisser, j'dois me refaire, faut qu'j'me rachète J'repense aux conneries d'ma jeunesse, j'marche dans les rues où j'ai arraché Tous les jours, faut qu'ça vende, t'as vu, mes soucis j'ai attachés Pah Rien qu'elle fume, elle a perdu son cavu, le pilon l'a ravagée Pah Rien a changé dans mes textes, j'te raconte seulement l'implication L'implication Pour des dineros, j'déforme ta tête comme Pablo Picasso Comme Picasso Faut shooter les fédéraux, fédéraux, fédéraux, avant qu'ta porte, elle saute Ta porte, elle saute Charbon cramé, palpitations, on sait encaisser dans n'importe quelle zone Ton malheur, c'est l'dernier d'mes soucis Brr, nan, j'touche pas aux raclis sous C Brr J'ai zéro sensei, mental' zéro sucerie Brr, tu veux de l'inspi' ? Brr J'viens te ressourcer Brr Pour tuer la concu', il faut qu'j'me suicide, pour tuer la concu', il faut qu'j'me suicide Tu perds du temps Hein, sale imbécile Hein, même si tu fais des chichis, tu vas rembourser Sur la route du succès Pah, je reste lucide, lucide Pah, pah, pah, poussez-vous, j'vais éclabousser S'écarter du péché Hein, c'est presque impossible Hein, ici, même l'écolier, il finit par bosser Elle voulait pas ken, elle a fini par bosser Salope, elle trouve des chekems, faut qu'il finisse cabossé Salope Pour des tales, avec le me-cri, j'suis associé Hein et mes démons font que d'me saucer, mmh 1PLIKÉ, t'es trop boosté, boosté Boosté, dinero me gusta, casse toi avant qu'j'te shoote, tu vas pas goûter J'suis dans les dièses, j'visser des ges-shla en costard, costard Prends ton bout, bouge de là, connard, un faux pas, c'est le re-shta, re-shta Tu faisais pas un rond avant l'pe-ra, c'est pas l'moment d'nous faire la re-sta, re-sta Pour la mi-f', j'suis prêt à tout laisser, j'dois me refaire, faut qu'j'me rachète J'repense aux conneries d'ma jeunesse, j'marche dans les rues où j'ai arraché Tous les jours, faut qu'ça vende, t'as vu, mes soucis j'ai attachés Pah Rien qu'elle fume, elle a perdu son cavu, le pilon l'a ravagée Pah Rien n'a changé dans mes textes, j'te raconte seulement l'implication L'implication Pour des dineros, j'déforme ta tête comme Pablo Picasso Comme Picasso Faut shooter les fédéraux, fédéraux, fédéraux, avant qu'ta porte, elle saute Ta porte, elle saute Charbon cramé, palpitations, on sait encaisser dans n'importe quelle zone</t>
         </is>
       </c>
     </row>
@@ -1636,7 +1636,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Hi-hi Pah, pah, pah, pah Aïe, aïe, aïe, aïe Ouh-ouh Qui m'relève si j'perds ? Hein ? Qui m'relève si j'perds ? Pah Sur mon front des précieuses prières Pah, sur mon cou des précieuses pierres Grr, grr Y'a pas d'Shakespeare, j'rappe, un neiman j'pète Moi aussi j'étais là-bas mais bon, moi, j'me suis pas fait pét' J'suis rentré avec Kiki et j'ai pris des 3abets A-WAX, 1PLIKÉ, 140BRICKS Cours, ils ont réveillé la bête J'mets des distances, c'est la pute, elle rappelle, elle fait genre, elle savait pas que j'rappais Les caméras ont tout baisé, y'en aurait pas, on ferait des braquages en paix Combien, j't'ai dis on va galoper ? Combien d'bisons on a décalotté ? Elle fait la meuf riche mais elle dort à l'hôtel avec un vieux en train de la dorloter T'sais pas gérer tes affaires, j'reprends, fais pas semblant, toi-même tu m'comprends La lle-da du khal-ssi, toujours faim d'entreprendre, j'crame un vil-ci, il a une GoPro, GoPro Trop d'tours j'ai fait dans l'tieks, depuis jeune, ça fait du que-tro Brr de gue-dro Brr Dose bien, ça va rappeler sur la ce-pu, c'est jamais trop La barre, j'la mets trop haute, barjot dans l'métro, j'visser à Roosevelt Pas b'soin d'un métronome, la prod', j'l'ai ouverte Rappe à cur ouvert, j'chante quand y'a plus d'vers Pah, pah, pah C'est pas un coup d'vent, tous à couvert Pah, pah, pah On rappe la rue mais c'est pas ça qu'on veut, ils rappent la rue mais c'est pas ça qu'on voit Y'a trop d'cavus mais c'est pas ça qu'j'convoite, j'appelle une te-tê, faut qu'il m'sorte une boîte Dans ma tête, ça résonne mais c'est pas ma voix, j'savais pas qu'ces cons d'baqueux allaient m'avoir mes sons mais pas d'remords, j'suis dans l'convoi La pute veut mon buzz, mes thunes et même ma voiture, salope, ma haine, la vois-tu ? Coup d'bélier, 1PLIKÉ dans l'actu' et tu sais qu'c'est pour les thunes Ah bon ? Pah J'ai pas le choix, j'vais les faire, les voir titube, han j'garde l'attitude Nan, j'les piétine, nan, j'ai pitié, nan, j'les piétine, han, han, han Dans ton hall, y'a des han, j'ai trop donné, han, qui m'a donné ? Han 9.2.1.4 situé sur le, eh, sur toi tous mes macaques si t'es situé chez les dés-c' Pah, pah, pah, pah You might also like Remplis l'sac, j'ai pas l'temps, j'ai pas d'a-d'armes Pah Pas d'mi-temps, j'ai l'plein, baraude à 'dam J'mets un point sur l'ta-tard', j'ai pas vu, sur tata, j'prie Dieu Pas comme ces cons, j'tiens à l'préciser tôt, j'payais des mecs qui vont briser des teums Chemin traversé comme Olive et Tom, j'atteins mon but comme Olive et Tom Pas d'remords, pas d'remords Pah, pah, pah, pah J'suis d'vant la porte, pas d'remords, j'me lève, gros J'sors une kich' vu qu't'aimes bien Est-ce que t'aimes bien ? Est-ce que t'aimes bien ? Me gusta dinero también Ah</t>
+          <t>Hi-hi Pah, pah, pah, pah Aïe, aïe, aïe, aïe Ouh-ouh Qui m'relève si j'perds ? Hein ? Qui m'relève si j'perds ? Pah Sur mon front des précieuses prières Pah, sur mon cou des précieuses pierres Grr, grr Y'a pas d'Shakespeare, j'rappe, un neiman j'pète Moi aussi j'étais là-bas mais bon, moi, j'me suis pas fait pét' J'suis rentré avec Kiki et j'ai pris des 3abets A-WAX, 1PLIKÉ, 140BRICKS Cours, ils ont réveillé la bête J'mets des distances, c'est la pute, elle rappelle, elle fait genre, elle savait pas que j'rappais Les caméras ont tout baisé, y'en aurait pas, on ferait des braquages en paix Combien, j't'ai dis on va galoper ? Combien d'bisons on a décalotté ? Elle fait la meuf riche mais elle dort à l'hôtel avec un vieux en train de la dorloter T'sais pas gérer tes affaires, j'reprends, fais pas semblant, toi-même tu m'comprends La lle-da du khal-ssi, toujours faim d'entreprendre, j'crame un vil-ci, il a une GoPro, GoPro Trop d'tours j'ai fait dans l'tieks, depuis jeune, ça fait du que-tro Brr de gue-dro Brr Dose bien, ça va rappeler sur la ce-pu, c'est jamais trop La barre, j'la mets trop haute, barjot dans l'métro, j'visser à Roosevelt Pas b'soin d'un métronome, la prod', j'l'ai ouverte Rappe à cur ouvert, j'chante quand y'a plus d'vers Pah, pah, pah C'est pas un coup d'vent, tous à couvert Pah, pah, pah On rappe la rue mais c'est pas ça qu'on veut, ils rappent la rue mais c'est pas ça qu'on voit Y'a trop d'cavus mais c'est pas ça qu'j'convoite, j'appelle une te-tê, faut qu'il m'sorte une boîte Dans ma tête, ça résonne mais c'est pas ma voix, j'savais pas qu'ces cons d'baqueux allaient m'avoir mes sons mais pas d'remords, j'suis dans l'convoi La pute veut mon buzz, mes thunes et même ma voiture, salope, ma haine, la vois-tu ? Coup d'bélier, 1PLIKÉ dans l'actu' et tu sais qu'c'est pour les thunes Ah bon ? Pah J'ai pas le choix, j'vais les faire, les voir titube, han j'garde l'attitude Nan, j'les piétine, nan, j'ai pitié, nan, j'les piétine, han, han, han Dans ton hall, y'a des han, j'ai trop donné, han, qui m'a donné ? Han 9.2.1.4 situé sur le, eh, sur toi tous mes macaques si t'es situé chez les dés-c' Pah, pah, pah, pah Remplis l'sac, j'ai pas l'temps, j'ai pas d'a-d'armes Pah Pas d'mi-temps, j'ai l'plein, baraude à 'dam J'mets un point sur l'ta-tard', j'ai pas vu, sur tata, j'prie Dieu Pas comme ces cons, j'tiens à l'préciser tôt, j'payais des mecs qui vont briser des teums Chemin traversé comme Olive et Tom, j'atteins mon but comme Olive et Tom Pas d'remords, pas d'remords Pah, pah, pah, pah J'suis d'vant la porte, pas d'remords, j'me lève, gros J'sors une kich' vu qu't'aimes bien Est-ce que t'aimes bien ? Est-ce que t'aimes bien ? Me gusta dinero también Ah</t>
         </is>
       </c>
     </row>
@@ -1653,7 +1653,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Pch, pch, pch, pch Guette le peu-ra qu'on propose, t'es un floco, t'as pas tenu, t'as fait l'crapaud 1.4.0, viens lever l'drapeau, parano, ton cur palpite, t'entends l'Akrapo' On aime vendre la verte mais au doré, on s'cramponne han, han, han Même dans un champ d'beugeuh, ça roule un royal Elle veut s'promener sur les Champs mais j'vais pas y aller Enculé, t'as tenu l'keus' pour ta niaralé J'encaisse des points, putain ça va vite J'aime l'argent drr mais je sais qu'c'est pas ça la vie drr C'est pas pour ds futilités qu'faut s'en servir drr Y a deux ans d'ça drr, tu m'aurais pas rndu service drr Ils aiment mentir, ils aiment jouer du violon yih Quand on galère, nous, on joue avec la violence yih En manque d'adrénaline, j'joue avec le volant J'ai rechargé la SIM, faut gérer la relance Ça fait longtemps qu'on attend, c'est l'plata qu'on attaque Me parle pas d'bonbonne si tu m'parles de ballons Eux, ils s'enculent au tank Culotté, j'me d'mande pourquoi la ue-r les fascine autant Six heures, cauchemar, réveil en sursautant Au re-shta', on ira quand ? On tartine, on vesqui' les méras-ca Fuck la juge qui m'a prit pour une racaille You might also like T'iras pas loin si tu fais l'perso, c'est pas compliqué de citer personne C'est compliqué d'inciter personne, t'es mon frère, on est liés depuis l'berceau T'iras pas loin si tu fais l'perso, c'est pas compliqué de citer personne C'est compliqué d'inciter personne, t'es mon frère, on est liés depuis l'berceau Tu t'fais mêler pour ton pote eh, eh, eh, eh T'es un bonhomme si t'as pas lé-par eh, eh, eh, eh Publiquement, on fait du sale, on oublie souvent que les tits-pe marchent sur nos pas eh, eh, eh, eh Tu t'fais mêler pour ton pote eh, eh, eh, eh T'es un bonhomme si t'as pas lé-par Publiquement, on fait du sale, on oublie souvent que les tits-pe marchent sur nos pas eh, eh, eh, eh Visière teintée et T-max, qui t'es ? Tu peux vite nous quitter, y a que maman qui t'aime Mes rêves décapités, argent et grammes sous scellés Mentalité rate-pi sans capitaine Ils sont en larmes pendant qu'on célèbre Tarpé de shit, beugeuh dans le teum-teum À contre-temps, j'rappe à contre-thème sur une instru' dansante J'te parle de seum-seum Pour c'est dead, il t'invite à manger J'te porte dans mon cur, le tarot, j'vais t'arranger L'argent n'a pas d'odeur mais une mauvaise hygiène Ça c'est pour le bonheur, ça attend pas qu'il vienne Pas d'retournement d'veste, pas d'changement d'table uh Faut un que-sa rempli d'matos uh Salope, remballe tes ppes-sa, gros j'm'en tape uh, uh Pour la concu', j'ai grave des bastos Ça fait longtemps qu'on attend, c'est l'plata qu'on attaque Me parle pas d'bonbonne si tu m'parles de ballons Eux, ils s'enculent au tank Culotté, j'me d'mande pourquoi la ue-r les fascine autant Six heures, cauchemar, réveil en sursautant Au re-shta', on ira quand ? On tartine, on vesqui' les méras-ca Fuck la juge qui m'a prit pour une racaille T'iras pas loin si tu fais l'perso, c'est pas compliqué de citer personne C'est compliqué d'inciter personne, t'es mon frère, on est liés depuis l'berceau T'iras pas loin si tu fais l'perso, c'est pas compliqué de citer personne C'est compliqué d'inciter personne, t'es mon frère, on est liés depuis l'berceau Tu t'fais mêler pour ton pote eh, eh, eh, eh T'es un bonhomme si t'as pas lé-par eh, eh, eh, eh Publiquement, on fait du sale, on oublie souvent que les tits-pe marchent sur nos pas eh, eh, eh, eh Tu t'fais mêler pour ton pote eh, eh, eh, eh T'es un bonhomme si t'as pas lé-par Depuis l'temps, on fait du sale, on oublie souvent que les tits-pe marchent sur nos pas eh, eh, eh, eh T'iras pas loin si tu fais l'perso han, han, c'est pas compliqué de citer personne han, han C'est compliqué d'inciter personne han, han, t'es mon frère, on est liés depuis l'berceau poh T'iras pas loin si tu fais l'perso han, han, c'est pas compliqué de citer personne han, han C'est compliqué d'inciter personne han, han, t'es mon frère, on est liés depuis l'berceau Tu t'fais mêler pour ton pote eh, eh, eh, eh T'es un bonhomme si t'as pas lé-par eh, eh, eh, eh Publiquement, on fait du sale, on oublie souvent que les tits-pe marchent sur nos pas eh, eh, eh, eh Tu t'fais mêler pour ton pote han, han T'es un bonhomme si t'as pas lé-par han, han Depuis l'temps, on fait du sale han, han, on oublie souvent que les tits-pe marchent sur nos pas eh, eh, eh, eh Poh, poh, poh2</t>
+          <t>Pch, pch, pch, pch Guette le peu-ra qu'on propose, t'es un floco, t'as pas tenu, t'as fait l'crapaud 1.4.0, viens lever l'drapeau, parano, ton cur palpite, t'entends l'Akrapo' On aime vendre la verte mais au doré, on s'cramponne han, han, han Même dans un champ d'beugeuh, ça roule un royal Elle veut s'promener sur les Champs mais j'vais pas y aller Enculé, t'as tenu l'keus' pour ta niaralé J'encaisse des points, putain ça va vite J'aime l'argent drr mais je sais qu'c'est pas ça la vie drr C'est pas pour ds futilités qu'faut s'en servir drr Y a deux ans d'ça drr, tu m'aurais pas rndu service drr Ils aiment mentir, ils aiment jouer du violon yih Quand on galère, nous, on joue avec la violence yih En manque d'adrénaline, j'joue avec le volant J'ai rechargé la SIM, faut gérer la relance Ça fait longtemps qu'on attend, c'est l'plata qu'on attaque Me parle pas d'bonbonne si tu m'parles de ballons Eux, ils s'enculent au tank Culotté, j'me d'mande pourquoi la ue-r les fascine autant Six heures, cauchemar, réveil en sursautant Au re-shta', on ira quand ? On tartine, on vesqui' les méras-ca Fuck la juge qui m'a prit pour une racaille T'iras pas loin si tu fais l'perso, c'est pas compliqué de citer personne C'est compliqué d'inciter personne, t'es mon frère, on est liés depuis l'berceau T'iras pas loin si tu fais l'perso, c'est pas compliqué de citer personne C'est compliqué d'inciter personne, t'es mon frère, on est liés depuis l'berceau Tu t'fais mêler pour ton pote eh, eh, eh, eh T'es un bonhomme si t'as pas lé-par eh, eh, eh, eh Publiquement, on fait du sale, on oublie souvent que les tits-pe marchent sur nos pas eh, eh, eh, eh Tu t'fais mêler pour ton pote eh, eh, eh, eh T'es un bonhomme si t'as pas lé-par Publiquement, on fait du sale, on oublie souvent que les tits-pe marchent sur nos pas eh, eh, eh, eh Visière teintée et T-max, qui t'es ? Tu peux vite nous quitter, y a que maman qui t'aime Mes rêves décapités, argent et grammes sous scellés Mentalité rate-pi sans capitaine Ils sont en larmes pendant qu'on célèbre Tarpé de shit, beugeuh dans le teum-teum À contre-temps, j'rappe à contre-thème sur une instru' dansante J'te parle de seum-seum Pour c'est dead, il t'invite à manger J'te porte dans mon cur, le tarot, j'vais t'arranger L'argent n'a pas d'odeur mais une mauvaise hygiène Ça c'est pour le bonheur, ça attend pas qu'il vienne Pas d'retournement d'veste, pas d'changement d'table uh Faut un que-sa rempli d'matos uh Salope, remballe tes ppes-sa, gros j'm'en tape uh, uh Pour la concu', j'ai grave des bastos Ça fait longtemps qu'on attend, c'est l'plata qu'on attaque Me parle pas d'bonbonne si tu m'parles de ballons Eux, ils s'enculent au tank Culotté, j'me d'mande pourquoi la ue-r les fascine autant Six heures, cauchemar, réveil en sursautant Au re-shta', on ira quand ? On tartine, on vesqui' les méras-ca Fuck la juge qui m'a prit pour une racaille T'iras pas loin si tu fais l'perso, c'est pas compliqué de citer personne C'est compliqué d'inciter personne, t'es mon frère, on est liés depuis l'berceau T'iras pas loin si tu fais l'perso, c'est pas compliqué de citer personne C'est compliqué d'inciter personne, t'es mon frère, on est liés depuis l'berceau Tu t'fais mêler pour ton pote eh, eh, eh, eh T'es un bonhomme si t'as pas lé-par eh, eh, eh, eh Publiquement, on fait du sale, on oublie souvent que les tits-pe marchent sur nos pas eh, eh, eh, eh Tu t'fais mêler pour ton pote eh, eh, eh, eh T'es un bonhomme si t'as pas lé-par Depuis l'temps, on fait du sale, on oublie souvent que les tits-pe marchent sur nos pas eh, eh, eh, eh T'iras pas loin si tu fais l'perso han, han, c'est pas compliqué de citer personne han, han C'est compliqué d'inciter personne han, han, t'es mon frère, on est liés depuis l'berceau poh T'iras pas loin si tu fais l'perso han, han, c'est pas compliqué de citer personne han, han C'est compliqué d'inciter personne han, han, t'es mon frère, on est liés depuis l'berceau Tu t'fais mêler pour ton pote eh, eh, eh, eh T'es un bonhomme si t'as pas lé-par eh, eh, eh, eh Publiquement, on fait du sale, on oublie souvent que les tits-pe marchent sur nos pas eh, eh, eh, eh Tu t'fais mêler pour ton pote han, han T'es un bonhomme si t'as pas lé-par han, han Depuis l'temps, on fait du sale han, han, on oublie souvent que les tits-pe marchent sur nos pas eh, eh, eh, eh Poh, poh, poh2</t>
         </is>
       </c>
     </row>
@@ -1670,7 +1670,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Poh, poh, poh, poh poh, poh J'fais plus d'rêve, que des cauchemars, j'entends des gens qui pleurent des gens qui pleurent Cou-, couche-toi couche-toi, il fait jamais beau quand les coups pleuvent quand les coups pleuvent Coupe coupe, coupe, à ton âge, j'découpais à ton âge Si j'rentre si j'rentre, je, je prends la coupe C'est 1PLIKÉ ou c'est Awax ou c'est Awax qui découpe les couplets hin ? ? On est dans tout plan, t'inquiète, on a du toupet poh, poh Ls soirs, j'visser, j'vais pas zouker, sur l'pe-ra, j'ré-ti au bazooka Goule-ca, ganté drr, j'ai pas douté, deux joggings tout l'hiver, l'tartin s'passe au calme J'les vois taper des rails devant l'tram, j'crois que, de les niquer, j'suis en train De la niquer, j'ai mis deux coups en trop Rentre pas dans ma tête, c'est un deux contre un oui On l'fait, on pense pas à la peine, mais à l'argent qu'ça ramène Eh, j'me rappelle quand ça ramait, eh Avant d'sser-bra, j'ai pataugé tu t'rappelles, hein ? Avant d'sser-bra, j'ai dû faire un mec tu t'rappelles, hein ? Longtemps qu'j'vois la vie différemment dans la cité d'la plaine, la haine, on fait avec Y a un llet-bi qui dort, j'ai trop la veine Défonce la porte de ta vecs C'est nous, on défonce la porte de ta vecs C'est nous, on te donne la peur de ta vie C'est nous, la street, eux, ils ont R.A.V J'aime pas ce keuf, faut pas qu'je tombe sur sa fille sale pute Ils veulent pas faire de ce-pla, on s'affirme, pour scalape, on s'la fout, pour plus d'un K, on s'fume J'tartine, si j'm'arrête, j'suis mort dans l'film Trop d'sous dans l'sale qui sont partis en fumée oui Comme cette pute, ma frappe te prend la tête La miss me quitte, j'm'en bats les c', j'vide pas la 'teille brr, salope En cours, j'veux plus d'un médaillon, ça fait plus d'quatre heures qu'la ppe-fra me die uh C'est pas pour faire le tox' si j'passe vers Me-da uh tu t'rappelles d'avant ? J'arrangeais pas aux mecs d'ailleurs uh Si y a rien à tter-gra, j'me taille uh, uh, ça sort un brr, gros, y a plus d'muay-thaï Visage caché, ça tré-ren dans ton teum-teum On prend tout c'qui est bijoux, tout c'qui est high-tech poh, poh Belek, tu checkes le négro qu'a pé-ta ton shit han Bande pas sur les ttes-ch' qui veulent ton te-shi han Tu sais pas cher-ca, normal qu'on te chine han Tu sais pas cher-ca, normal qu'on te chine han Tous les jours, j'vide mon sac mais j'fais pas d'confidence On veut la paix, c'est la haine qu'on finance On veut la paix, c'est la haine qu'on finance J'donne pas un rond dans les caisses de l'Etat brr Ça sent l'coup d'bélier, je dors chez une 'tasse salope On cherche nos ennemis, tu cherches tes alliés salope Sur l'chemin, des traîtres, j'en ai lâché un tas salope Pendant qu'tu nehess, on coupe le pain salope, contre mes potos, je n'complote pas Monnaie, monnaie si tu veux qu'on parle, j'roule un avion si tu veux qu'on plane J'pensais arrêter quand, l'terrain, j'le fermais, le lendemain, j'pensais qu'à faire mieux ah ouais ? Dans l'tier-quar, on s'enferme ah ouais ?, dans l'tier-quar, on s'enferme J'ai pas vendu la mèche, nan, j'l'ai allumée, faire gonfler la kichta pour aller mieux Mon son c'est d'la pure, j'me dois d'les enfariner, j'pense qu'à la punition, crois pas qu'j'pense aux haineux nan C'est la ue-r, c'est les Hauts-d'Seine, y a d'la bicrave en masse et du recel J'vois l'baveux grossir à chaque procès, Coffre un max, attends pas l'été prochain Coffre un max, attends pas l'été prochain, une rotte-ca en trop, j'finis dans l'panier à salade J'aimerais pas qu'ma mère apprenne ça, y a qu'devant nos parents qu'on a l'air sages Même quand on dehek, on a l'air sah, même quand on est clean, on a l'air sales Ja-ja-jamais larsa, attends, j'ai pas capté, ils font les bonhommes, mais après, ils vont cafter Belek, la muerte, elle peut débouler casquée c'est chaud dans l're-fou drr, drr, y a des poulets cachés et des boulettes cachées drr Après l'plavon, on s'défoule sur celui qui a chié, ça vend d'la kush Pas des cachets, liasses sous le coussin, poto, j'dors pas sur du cash, l'week-end, ça défile, j'trouve ça trop fashion Encaisser, c'est l'défi, sans laisser de tales 1PLIKÉ, sans laisser de tales J'voulais la ter-j', j'vais attendre qu'elle se détache Ça t'pé-ta où ça fait mal, connard, t'es con, si l'te-shi, comble ton malheur Ça visser la mort gang, visser ta pierre tombale han, gang, j'prie pour que ma paie tombe à l'heure 1PLIKÉ J'prie pour que ma paie tombe à l'heure drr, pour moi, l'pe-ra, c'est tout balourd drr Quand j'débite, t'arrives plus à suivre l'allure, j'regarde plus l'horloge, j'arrive plus à suivre la leur You might also like 9.2.1.4.0 sur le pochton eh 9.2.1.4.0 sur le pochton eh 4.0 sur le pochton eh 4.0 sur le pochton 9.2.1.4.0 sur le pochton 9.2.1.4.0 sur le pochton 9.2.1.4.0 sur le pochton 4.0, 4.0 sur le pochton</t>
+          <t>Poh, poh, poh, poh poh, poh J'fais plus d'rêve, que des cauchemars, j'entends des gens qui pleurent des gens qui pleurent Cou-, couche-toi couche-toi, il fait jamais beau quand les coups pleuvent quand les coups pleuvent Coupe coupe, coupe, à ton âge, j'découpais à ton âge Si j'rentre si j'rentre, je, je prends la coupe C'est 1PLIKÉ ou c'est Awax ou c'est Awax qui découpe les couplets hin ? ? On est dans tout plan, t'inquiète, on a du toupet poh, poh Ls soirs, j'visser, j'vais pas zouker, sur l'pe-ra, j'ré-ti au bazooka Goule-ca, ganté drr, j'ai pas douté, deux joggings tout l'hiver, l'tartin s'passe au calme J'les vois taper des rails devant l'tram, j'crois que, de les niquer, j'suis en train De la niquer, j'ai mis deux coups en trop Rentre pas dans ma tête, c'est un deux contre un oui On l'fait, on pense pas à la peine, mais à l'argent qu'ça ramène Eh, j'me rappelle quand ça ramait, eh Avant d'sser-bra, j'ai pataugé tu t'rappelles, hein ? Avant d'sser-bra, j'ai dû faire un mec tu t'rappelles, hein ? Longtemps qu'j'vois la vie différemment dans la cité d'la plaine, la haine, on fait avec Y a un llet-bi qui dort, j'ai trop la veine Défonce la porte de ta vecs C'est nous, on défonce la porte de ta vecs C'est nous, on te donne la peur de ta vie C'est nous, la street, eux, ils ont R.A.V J'aime pas ce keuf, faut pas qu'je tombe sur sa fille sale pute Ils veulent pas faire de ce-pla, on s'affirme, pour scalape, on s'la fout, pour plus d'un K, on s'fume J'tartine, si j'm'arrête, j'suis mort dans l'film Trop d'sous dans l'sale qui sont partis en fumée oui Comme cette pute, ma frappe te prend la tête La miss me quitte, j'm'en bats les c', j'vide pas la 'teille brr, salope En cours, j'veux plus d'un médaillon, ça fait plus d'quatre heures qu'la ppe-fra me die uh C'est pas pour faire le tox' si j'passe vers Me-da uh tu t'rappelles d'avant ? J'arrangeais pas aux mecs d'ailleurs uh Si y a rien à tter-gra, j'me taille uh, uh, ça sort un brr, gros, y a plus d'muay-thaï Visage caché, ça tré-ren dans ton teum-teum On prend tout c'qui est bijoux, tout c'qui est high-tech poh, poh Belek, tu checkes le négro qu'a pé-ta ton shit han Bande pas sur les ttes-ch' qui veulent ton te-shi han Tu sais pas cher-ca, normal qu'on te chine han Tu sais pas cher-ca, normal qu'on te chine han Tous les jours, j'vide mon sac mais j'fais pas d'confidence On veut la paix, c'est la haine qu'on finance On veut la paix, c'est la haine qu'on finance J'donne pas un rond dans les caisses de l'Etat brr Ça sent l'coup d'bélier, je dors chez une 'tasse salope On cherche nos ennemis, tu cherches tes alliés salope Sur l'chemin, des traîtres, j'en ai lâché un tas salope Pendant qu'tu nehess, on coupe le pain salope, contre mes potos, je n'complote pas Monnaie, monnaie si tu veux qu'on parle, j'roule un avion si tu veux qu'on plane J'pensais arrêter quand, l'terrain, j'le fermais, le lendemain, j'pensais qu'à faire mieux ah ouais ? Dans l'tier-quar, on s'enferme ah ouais ?, dans l'tier-quar, on s'enferme J'ai pas vendu la mèche, nan, j'l'ai allumée, faire gonfler la kichta pour aller mieux Mon son c'est d'la pure, j'me dois d'les enfariner, j'pense qu'à la punition, crois pas qu'j'pense aux haineux nan C'est la ue-r, c'est les Hauts-d'Seine, y a d'la bicrave en masse et du recel J'vois l'baveux grossir à chaque procès, Coffre un max, attends pas l'été prochain Coffre un max, attends pas l'été prochain, une rotte-ca en trop, j'finis dans l'panier à salade J'aimerais pas qu'ma mère apprenne ça, y a qu'devant nos parents qu'on a l'air sages Même quand on dehek, on a l'air sah, même quand on est clean, on a l'air sales Ja-ja-jamais larsa, attends, j'ai pas capté, ils font les bonhommes, mais après, ils vont cafter Belek, la muerte, elle peut débouler casquée c'est chaud dans l're-fou drr, drr, y a des poulets cachés et des boulettes cachées drr Après l'plavon, on s'défoule sur celui qui a chié, ça vend d'la kush Pas des cachets, liasses sous le coussin, poto, j'dors pas sur du cash, l'week-end, ça défile, j'trouve ça trop fashion Encaisser, c'est l'défi, sans laisser de tales 1PLIKÉ, sans laisser de tales J'voulais la ter-j', j'vais attendre qu'elle se détache Ça t'pé-ta où ça fait mal, connard, t'es con, si l'te-shi, comble ton malheur Ça visser la mort gang, visser ta pierre tombale han, gang, j'prie pour que ma paie tombe à l'heure 1PLIKÉ J'prie pour que ma paie tombe à l'heure drr, pour moi, l'pe-ra, c'est tout balourd drr Quand j'débite, t'arrives plus à suivre l'allure, j'regarde plus l'horloge, j'arrive plus à suivre la leur 9.2.1.4.0 sur le pochton eh 9.2.1.4.0 sur le pochton eh 4.0 sur le pochton eh 4.0 sur le pochton 9.2.1.4.0 sur le pochton 9.2.1.4.0 sur le pochton 9.2.1.4.0 sur le pochton 4.0, 4.0 sur le pochton</t>
         </is>
       </c>
     </row>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>J'ai des reufs investis dans ldeal, y a pas d'Pacino, nan, pas d'ciné L'bigo, on l'met en sourdine juste avant d'aller chiner brr Quelques contrats à signer, l'argent sale dans la machine han Faut qu'j'm'investis dans l'dîn bien avant de calciner han C'est nous, on envoie l'poison mais on viendra les vacciner eh Quand on déboule dans ta zone, ta défense, on fait vaciller eh Les tchoys nous rajoutent des délits, veulent décorer mon casier han C'est nous, on envoi l'plavon han mais tu vas lâcher un billet han Trop souvent passé à l'act sans vraiment l'avoir voulu Pourtant, jamais d'la vie on rendra tout c'qu'on a volé pow Pour te faire, on attend juste que ton business, il évolue J'aime quand la kich' prend du volume, en vrai, moi, c'est tout c'que j'voulais Un mec en or, c'est cquelles veulent une femme en or, c'est tout cquelles veulent être Bécane, bijoux, téléphone, on allait chouara tout c'qu'on voyait Visage cramé comme mes frelons, trace de pilon sur les vres-lè Appelle si tu veux un filon eh, on vend la mort, on la frôlait eh Combien d'neimann on a dû casser ? J'vois qu'tu veux m'tendre la main mais tu m'l'aurais même tendue dans l'passé J'revends tout même mon flow dans l'rap, j'le bicrave pas cher J'la che-bran, j'veux la voir bosser mais elle, elle croit qu'j'la gère Brasse avant lsommeil éternel, la vie est passagère Prends l'volant d'la tienne, reste pas sur le coté passager passager Jpose mes couilles, et j'm'en bats les c' si ça gène Rien n't'appartient, on peut t'obliger à partager You might also like J'ai des reufs investis dans ldeal, y a pas d'Pacino, nan, pas d'ciné L'bigo, on l'met en sourdine juste avant d'aller chiner brr Quelques contrats à signer, l'argent sale dans la machine han Faut qu'j'm'investis dans l'dîn bien avant de calciner han C'est nous, on envoie l'poison mais on viendra les vacciner eh Quand on déboule dans ta zone, ta défense, on fait vaciller eh Les tchoys nous rajoutent des délits, veulent décorer mon casier han C'est nous, on envoie l'plavon han mais tu vas lâcher un billet han LÉtat, on connait son système donc on peut pas s'laisser faire J'me rappelle de mon changement d'SIM, jétais en mode SFR J'augmentais le taro, même si ça faisait les mêmes effets Toi, tu chenef devant les vrais, tu bombes seulement devant les faibles Envoie des prods à la chaine, dans tous les cas, j'vais les faire Jentends toutes leurs conneries, un peu comme sur BFM Pendant l'audition, j'gole-ri, j'reconnais pas les faits han Tu sais qu'ton équipe peut rien faire han, quand les mes-ar parlent FR Charbon sans congés, t'inquiète, c'est bon tant qu'on gère Bellec ta meuf monte avec un inconnu en chop étrangère salope Marre des lacets défaits mais j'peux pas être rangé pow Non, j'peux pas être en chien l'argent j'suis en train d'en faire J'pense au paradis en étant assis dans un train d'enfer J'vois des portes qui se ferment mais j'garde la forme, j'dois gérer les transferts J'ouvre la première 'quette, ça pue la beuh, il m'faut un litre en fait Cocktail sur la tchop des bleus, mets le quartier en fête On sait où t'as caché en deux minutes, on peut prendre tes affaires Je joue à Tenkaichi, j'savais pas qu'j'allais vendre la verte jvais faire pleuvoir les billets J'savais pas qu'j'allais prendre laverse tinquiète jme range une fois qucest plié J'savais pas qu'j'allais faire l'inverse Tu les connais depuis môme brr, ils sont là que dans les bons moments brr Quand les coups remplacent les mots brr, à quoi bon raconter tes romans brr ? On sen bat les couilles, gros, même si t'as des remords même si t'as des remords, même si t'as des remords J'ai des reufs investis dans ldeal, y a pas d'Pacino, nan, pas d'ciné L'bigo, on l'met en sourdine juste avant d'aller chiner brr Quelques contrats à signer, l'argent sale dans la machine han Faut qu'j'm'investis dans l'dîn bien avant de calciner han C'est nous, on envoie l'poison mais on viendra les vacciner eh Quand on déboule dans ta zone, ta défense, on fait vaciller eh Les tchoys nous rajoutent des délits, veulent décorer mon casier han C'est nous on envoie l'plavon han mais tu vas lâcher un billet han J'ai des reufs investis dans ldeal, y a pas d'Pacino, nan, pas d'ciné L'bigo, on l'met en sourdine juste avant d'aller chiner brr Quelques contrats à signer, l'argent sale dans la machine han Faut qu'j'm'investis dans l'dîn bien avant de calciner han C'est nous, on envoie l'poison mais on viendra les vacciner eh Quand on déboule dans ta zone, ta défense, on fait vaciller eh Les tchoys nous rajoutent des délits, veulent décorer mon casier han C'est nous, on envoie l'plavon han mais tu vas lâcher un billet han Brr, brr Han, han, han Eh, eh Han, han, han2</t>
+          <t>J'ai des reufs investis dans ldeal, y a pas d'Pacino, nan, pas d'ciné L'bigo, on l'met en sourdine juste avant d'aller chiner brr Quelques contrats à signer, l'argent sale dans la machine han Faut qu'j'm'investis dans l'dîn bien avant de calciner han C'est nous, on envoie l'poison mais on viendra les vacciner eh Quand on déboule dans ta zone, ta défense, on fait vaciller eh Les tchoys nous rajoutent des délits, veulent décorer mon casier han C'est nous, on envoi l'plavon han mais tu vas lâcher un billet han Trop souvent passé à l'act sans vraiment l'avoir voulu Pourtant, jamais d'la vie on rendra tout c'qu'on a volé pow Pour te faire, on attend juste que ton business, il évolue J'aime quand la kich' prend du volume, en vrai, moi, c'est tout c'que j'voulais Un mec en or, c'est cquelles veulent une femme en or, c'est tout cquelles veulent être Bécane, bijoux, téléphone, on allait chouara tout c'qu'on voyait Visage cramé comme mes frelons, trace de pilon sur les vres-lè Appelle si tu veux un filon eh, on vend la mort, on la frôlait eh Combien d'neimann on a dû casser ? J'vois qu'tu veux m'tendre la main mais tu m'l'aurais même tendue dans l'passé J'revends tout même mon flow dans l'rap, j'le bicrave pas cher J'la che-bran, j'veux la voir bosser mais elle, elle croit qu'j'la gère Brasse avant lsommeil éternel, la vie est passagère Prends l'volant d'la tienne, reste pas sur le coté passager passager Jpose mes couilles, et j'm'en bats les c' si ça gène Rien n't'appartient, on peut t'obliger à partager J'ai des reufs investis dans ldeal, y a pas d'Pacino, nan, pas d'ciné L'bigo, on l'met en sourdine juste avant d'aller chiner brr Quelques contrats à signer, l'argent sale dans la machine han Faut qu'j'm'investis dans l'dîn bien avant de calciner han C'est nous, on envoie l'poison mais on viendra les vacciner eh Quand on déboule dans ta zone, ta défense, on fait vaciller eh Les tchoys nous rajoutent des délits, veulent décorer mon casier han C'est nous, on envoie l'plavon han mais tu vas lâcher un billet han LÉtat, on connait son système donc on peut pas s'laisser faire J'me rappelle de mon changement d'SIM, jétais en mode SFR J'augmentais le taro, même si ça faisait les mêmes effets Toi, tu chenef devant les vrais, tu bombes seulement devant les faibles Envoie des prods à la chaine, dans tous les cas, j'vais les faire Jentends toutes leurs conneries, un peu comme sur BFM Pendant l'audition, j'gole-ri, j'reconnais pas les faits han Tu sais qu'ton équipe peut rien faire han, quand les mes-ar parlent FR Charbon sans congés, t'inquiète, c'est bon tant qu'on gère Bellec ta meuf monte avec un inconnu en chop étrangère salope Marre des lacets défaits mais j'peux pas être rangé pow Non, j'peux pas être en chien l'argent j'suis en train d'en faire J'pense au paradis en étant assis dans un train d'enfer J'vois des portes qui se ferment mais j'garde la forme, j'dois gérer les transferts J'ouvre la première 'quette, ça pue la beuh, il m'faut un litre en fait Cocktail sur la tchop des bleus, mets le quartier en fête On sait où t'as caché en deux minutes, on peut prendre tes affaires Je joue à Tenkaichi, j'savais pas qu'j'allais vendre la verte jvais faire pleuvoir les billets J'savais pas qu'j'allais prendre laverse tinquiète jme range une fois qucest plié J'savais pas qu'j'allais faire l'inverse Tu les connais depuis môme brr, ils sont là que dans les bons moments brr Quand les coups remplacent les mots brr, à quoi bon raconter tes romans brr ? On sen bat les couilles, gros, même si t'as des remords même si t'as des remords, même si t'as des remords J'ai des reufs investis dans ldeal, y a pas d'Pacino, nan, pas d'ciné L'bigo, on l'met en sourdine juste avant d'aller chiner brr Quelques contrats à signer, l'argent sale dans la machine han Faut qu'j'm'investis dans l'dîn bien avant de calciner han C'est nous, on envoie l'poison mais on viendra les vacciner eh Quand on déboule dans ta zone, ta défense, on fait vaciller eh Les tchoys nous rajoutent des délits, veulent décorer mon casier han C'est nous on envoie l'plavon han mais tu vas lâcher un billet han J'ai des reufs investis dans ldeal, y a pas d'Pacino, nan, pas d'ciné L'bigo, on l'met en sourdine juste avant d'aller chiner brr Quelques contrats à signer, l'argent sale dans la machine han Faut qu'j'm'investis dans l'dîn bien avant de calciner han C'est nous, on envoie l'poison mais on viendra les vacciner eh Quand on déboule dans ta zone, ta défense, on fait vaciller eh Les tchoys nous rajoutent des délits, veulent décorer mon casier han C'est nous, on envoie l'plavon han mais tu vas lâcher un billet han Brr, brr Han, han, han Eh, eh Han, han, han2</t>
         </is>
       </c>
     </row>
@@ -1704,7 +1704,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Poh, poh, poh, poh Poh, poh, poh, poh T'inquiète, j'm'en occupe Poh, poh, poh, poh T'inquiète, j'm'en occupe Poh, poh, poh, poh T'inquiète, j'm'en occupe Pour la mille-fa, t'inquiète, j'm'en occupe, c'est tout pour l'équipe, j'étais seul sur le kil', seul sur le quai, j'ai séché pour le liquide Fais belek, on vise bien, on fait tomber les quilles En fait, faut qu'on les kill, on fait ton bénéfice brr On a grandi, on s'en bat les c' tu connais qui brr Trop d'haine, trop d'haine, à croire qu'on est maudits brr, brr, brr Trop d'sale que dans mon texte, j'peux pas écrire Ça sort des trucs, quand je drill c'est d'la triche Je jump sur l'instru', gros, on n'est pas comme eux, pas d'idolâtrie J'aime pas quand ça s'enraye, j'achète nouveau truc J'suis sûr de ma team, y a pas qu'l'automatique J'bande quand ça parle de thunes, tu sais bien qu'ça m'attire Des sommes, j'ai compté donc j'peux plus être sympathique Deux payes dans la che-po, j'vais pas partir Ya plus dMMA, y'a l'que-tru dans les mains, j'ai pas l'million, l'amour, c'est pas ça qui me manque J'oublie les bons moments, du mal, j'me remémore Et quand y'a plus rien dans l'sac, je remonte J'ai du buzz, ma ce-pu sonne encore, j'me rappelle à l'époque quand j'pochtonnais en cours Embêtant, d'bétom en bécane, quand les condés tournent de ouf, tu sais ce quon encourt On pense vivre la misère, on regarde pas autour de nous, on est mouillés jusqu'au cou Jai changé mes plans en cours de route, pendant que ces cons se mettaient en couple C'est pas toi qu'on épargne, on sait que d'vant les coups tu ler-par Tétais chaud mais pourquoi tout dun coup tu les pas ? Je sais qui est qui, je sais qui est qui Tinquiète les vrais j'les oublies pas On baise tout et cest calculé depuis le départ Des euros, du produit mais j'suis déçu des parts Nan je quitte pas le tier-quar tant qu'j'suis pas plein Nan je quitte pas le tier-quar tant qu'j'suis pas plein You might also like Jmets tout dans le récit, jai zéro gestuelle 1.4 on découpe précis, 1.4 ils viennent pour décompresser Lamour des sommes, elle a rien compris là-celle, nan J'voulais pas l'devant d'la scène, nan Même pas les coulisses, jallumais l'zdeh dans les toilettes du lycée, histoire que les junkies réagissent Jnote tout dans le récit, jai zéro gestuelle 1.4 on découpe précis, 1.4 ils viennent pour décompresser Lamour des sommes, elle a rien compris là-celle, nan J'voulais pas l'devant d'la scène, nan Même pas les coulisses, jallumais l'zdeh dans les toilettes du lycée, histoire que les junkies réagissent Ya trop de trucs que j'pourrais jamais dire Si javais pas la foi, jaurais d'jà mes 10 leums Si j'la vois à fond, gros jaurais jamais dealé Comment marrêter ? Jsuis dans un sacré dilemme Est-ce que l'argent se trouve dans les sommes ? Cest soit le bonheur ou le seum Pourquoi tattend d'rencontrer les problèmes avant dlever les mains vers le ciel ? Va falloir méloigner d'mon côté malsain mais il m'rattrape à chaque fois Au bout d'200 mètres, les keufs te pètent à chaque fois Jai une nouvelle haine pour chaque voix, un nouveau pavé pour chaque voi-ture Jai mis la bague au doigt à la ue-r salope, pourvu qu'ça dure Cest pas une pute qui va m'faire flancher, me faire dépenser Ya que la maille qui hante mes pensées Hasba, extorsion, crave-bi Dans le me-cri, jai fais mes premiers pas Tu m'as croisé solo dans la lle-vi Jfaisais l'papier pendant que tu l'faisais pas C'est pas toi qu'on épargne, on sait que d'vant les coups tu ler-par Tétais chaud mais pourquoi tout dun coup tu les pas ? Je sais qui est qui, je sais qui est qui Tinquiète les vrais j'les oublies pas On baise tout et cest calculé depuis le départ Jmets tout dans le récit, jai zéro gestuelle 1.4 on découpe précis, 1.4 ils viennent pour décompresser Lamour des sommes, elle a rien compris là-celle, nan J'voulais pas l'devant d'la scène, nan Même pas les coulisses, jallumais l'zdeh dans les toilettes du lycée, histoire que les junkies réagissent Jnote tout dans le récit, jai zéro gestuelle 1.4 on découpe précis, 1.4 ils viennent pour décompresser Lamour des sommes, elle a rien compris là-celle, nan J'voulais pas l'devant d'la scène, nan Même pas les coulisses, jallumais l'zdeh dans les toilettes du lycée, histoire que les junkies réagissent</t>
+          <t>Poh, poh, poh, poh Poh, poh, poh, poh T'inquiète, j'm'en occupe Poh, poh, poh, poh T'inquiète, j'm'en occupe Poh, poh, poh, poh T'inquiète, j'm'en occupe Pour la mille-fa, t'inquiète, j'm'en occupe, c'est tout pour l'équipe, j'étais seul sur le kil', seul sur le quai, j'ai séché pour le liquide Fais belek, on vise bien, on fait tomber les quilles En fait, faut qu'on les kill, on fait ton bénéfice brr On a grandi, on s'en bat les c' tu connais qui brr Trop d'haine, trop d'haine, à croire qu'on est maudits brr, brr, brr Trop d'sale que dans mon texte, j'peux pas écrire Ça sort des trucs, quand je drill c'est d'la triche Je jump sur l'instru', gros, on n'est pas comme eux, pas d'idolâtrie J'aime pas quand ça s'enraye, j'achète nouveau truc J'suis sûr de ma team, y a pas qu'l'automatique J'bande quand ça parle de thunes, tu sais bien qu'ça m'attire Des sommes, j'ai compté donc j'peux plus être sympathique Deux payes dans la che-po, j'vais pas partir Ya plus dMMA, y'a l'que-tru dans les mains, j'ai pas l'million, l'amour, c'est pas ça qui me manque J'oublie les bons moments, du mal, j'me remémore Et quand y'a plus rien dans l'sac, je remonte J'ai du buzz, ma ce-pu sonne encore, j'me rappelle à l'époque quand j'pochtonnais en cours Embêtant, d'bétom en bécane, quand les condés tournent de ouf, tu sais ce quon encourt On pense vivre la misère, on regarde pas autour de nous, on est mouillés jusqu'au cou Jai changé mes plans en cours de route, pendant que ces cons se mettaient en couple C'est pas toi qu'on épargne, on sait que d'vant les coups tu ler-par Tétais chaud mais pourquoi tout dun coup tu les pas ? Je sais qui est qui, je sais qui est qui Tinquiète les vrais j'les oublies pas On baise tout et cest calculé depuis le départ Des euros, du produit mais j'suis déçu des parts Nan je quitte pas le tier-quar tant qu'j'suis pas plein Nan je quitte pas le tier-quar tant qu'j'suis pas plein Jmets tout dans le récit, jai zéro gestuelle 1.4 on découpe précis, 1.4 ils viennent pour décompresser Lamour des sommes, elle a rien compris là-celle, nan J'voulais pas l'devant d'la scène, nan Même pas les coulisses, jallumais l'zdeh dans les toilettes du lycée, histoire que les junkies réagissent Jnote tout dans le récit, jai zéro gestuelle 1.4 on découpe précis, 1.4 ils viennent pour décompresser Lamour des sommes, elle a rien compris là-celle, nan J'voulais pas l'devant d'la scène, nan Même pas les coulisses, jallumais l'zdeh dans les toilettes du lycée, histoire que les junkies réagissent Ya trop de trucs que j'pourrais jamais dire Si javais pas la foi, jaurais d'jà mes 10 leums Si j'la vois à fond, gros jaurais jamais dealé Comment marrêter ? Jsuis dans un sacré dilemme Est-ce que l'argent se trouve dans les sommes ? Cest soit le bonheur ou le seum Pourquoi tattend d'rencontrer les problèmes avant dlever les mains vers le ciel ? Va falloir méloigner d'mon côté malsain mais il m'rattrape à chaque fois Au bout d'200 mètres, les keufs te pètent à chaque fois Jai une nouvelle haine pour chaque voix, un nouveau pavé pour chaque voi-ture Jai mis la bague au doigt à la ue-r salope, pourvu qu'ça dure Cest pas une pute qui va m'faire flancher, me faire dépenser Ya que la maille qui hante mes pensées Hasba, extorsion, crave-bi Dans le me-cri, jai fais mes premiers pas Tu m'as croisé solo dans la lle-vi Jfaisais l'papier pendant que tu l'faisais pas C'est pas toi qu'on épargne, on sait que d'vant les coups tu ler-par Tétais chaud mais pourquoi tout dun coup tu les pas ? Je sais qui est qui, je sais qui est qui Tinquiète les vrais j'les oublies pas On baise tout et cest calculé depuis le départ Jmets tout dans le récit, jai zéro gestuelle 1.4 on découpe précis, 1.4 ils viennent pour décompresser Lamour des sommes, elle a rien compris là-celle, nan J'voulais pas l'devant d'la scène, nan Même pas les coulisses, jallumais l'zdeh dans les toilettes du lycée, histoire que les junkies réagissent Jnote tout dans le récit, jai zéro gestuelle 1.4 on découpe précis, 1.4 ils viennent pour décompresser Lamour des sommes, elle a rien compris là-celle, nan J'voulais pas l'devant d'la scène, nan Même pas les coulisses, jallumais l'zdeh dans les toilettes du lycée, histoire que les junkies réagissent</t>
         </is>
       </c>
     </row>
@@ -1721,7 +1721,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>You wanna focus, focus on this Focus on this Fuck tout faire péter, fuck le fair-play Poh, fuck leur faire plais' Poh, j'fais c'que j'ai envie Ouais Même le miroir, il khle3 du reflet Eh, voir le million au loin, c'est frais J'vois le million au loin, c'est vrai, j'v'-esqui les tchoïs Brr, oh, j'big up les réflexes Brr, oh Sur lui, t'as misé mais il t'la mise Brr, brr, fais c'que t'as à faire, te retourne pas, une fois qu'c'est fait Brr, brr Y a un plan cile-fa, c'est normal qu'on l'fait Fait, souvent khabat quand j'y vais Quand j'y vais J'ai pas bégayé quand j'l'ai vu Nan, j'ouvre une te-por, j'le maintiens en vie Brr En mode survie Brr, c'est en-dessous j'me demande si on vit Brr Les poches remplies, en moi, y a un vide Faut qu'j'prie, l'avenir, j'le trouve moyen vide Poh, poh, kamas au bec quand j'conduis Poh, poh La tchop, elle est jdid, la pute a un jean, jamais d'pénurie mais qui t'as dit ? Eh Si elle en veut, y a d'la beuh, y a du rab, si elle en veut, y a d'la beuh, y a du rab Fuck la pe-stu, l'rap, j'ai des produits durables, le p'tit grandit, dans un an, il postulera Uh Rentre sur l'T, fais crier l'stade Uh, criquets à midi pour t'lever à Cannes Uh Fais ton cash, évite le vacarme Poh, aller-retour, éviter la cam' Brr, brr Transactions d'vant les tantines et cles-on, roi est le client J'étais terre-pas, j'ai zolote un client, tu veux carna, j'mets l'tard-pé dans l'Clio Y a un canon, tu joues le philosophe Oui, j'l'ai filoche, j'tape, je file, le bras, j'allonge J'débloque les filons, plans sous j'arrose Poh c'est moi qu'a les tuyaux Poh Teh, massa, clope, sur moi, j'ai l'trio, j'me roule un p'tit Oh L'état du teum fait peur au proprio', normal qu'ça bosse d'lundi à lundi Oh Y a d'la ppe-f', t'apprécies l'odeur, il pense à pper-cho quand il est au taf La skung t'envoie en l'air, CM Punk Ah bon ? Y en a pour les skateurs et les hommes d'aff' Ah bon ?, je sé-cour, j'suis casqué comme un Daft Sale pute, ton passé, c'est pas du Velléda Salope, la victime s'est chouara, personne vient l'aider Ah bon ? Elle a plainté sous X, elle en veut à l'État Salope, j'sors d'un midi-minuit, j'dois d'jà faire une ssion-mi Le ient-cli est roi, ça fait une heure il câble, une heure du mat', j'suis devant les cages Trafic inarrêtable, sponso' par la Lyca', voiture allemande, j'suis vers Alicante Ah bon ? Les keufs sont cistes-ra, déboulent à cinquante Ah bon ?, cache ta cons', même une boulette, ça compte Brasser, c'est l'idée, c'est pour ça qu'on l'fait, casse pas d'bastos pour ces cons, ils sont traîtres Jamais, jamais You might also like Service précis, même si c'est miné d'flics Big up à mes réflexes, brr, brr, brr J'me dois d'protéger ma puce Sans elle, j'ai pas ma pièce Rien n'est gratis, on n'dort pas, on charbonne Y a des travaux dans toute la tess Tous les jours, j't'entends dire Cette fois, c'est la bonne Mais bon, au final, j'vois pas l'papel, 'pel, 'pel, 'pel Service précis, même si c'est miné d'flics Big up à mes réflexes, brr, brr, brr J'me dois d'protéger ma puce Sans elle, j'ai pas ma pièce Rien n'est gratis, on n'dort pas, on charbonne Y a des travaux dans toute la tess Tous les jours, j't'entends dire Cette fois, c'est la bonne Mais bon, au final, j'vois pas l'papel, 'pel, 'pel, 'pel Tout pour la mif', quitte à faire le crabe Mmh-mmh, avance sans gravons, c'est pas grave Mmh-mmh Nous trahis pas, j'oublie pas, même si j'bédave Jamais, il m'faut une nounou, j'pense à cher-bran une dame Et la noche, j'entends des voix comme Jeanne d'Arc Brr, j'ai besoin d'argent, besoin d'armes J'me targe avant le menottage Oui, sale con, t'es bé-tom pour un billet moutarde Oui Crique la bécane, j'entends les motards Han-han, crique la bécane, j'entends les motards J'débale en bas, j'détaille en bas Han-han mais ça pue jusqu'au dixième étage 1PLIKÉ, 1PLIKÉ 1PLIKÉ, attends un peu Oh, y a que la foi qui peut m'rattraper Oh Personne veut ma dépo', j'mets des pièces à l'OPJ, tout pour ma , j'ai placé l'P Le tour de ris-Pa, à fond sur l'riph'-pé, ris pas, après la rafale, c'est R.I.P Rien qu'tu parles de P, P, P, P, mais j'vois pas l'papel, eh Service précis, même si c'est miné d'flics Big up à mes réflexes, brr, brr, brr J'me dois d'protéger ma puce Sans elle, j'ai pas ma pièce, nan Rien n'est gratis, on n'dort pas, on charbonne Y a des travaux dans toute la tess Tous les jours, j't'entends dire Cette fois, c'est la bonne Mais bon, au final, j'vois pas l'papel, 'pel, 'pel, 'pel Service précis, même si c'est miné d'flics Big up à mes réflexes, brr, brr, brr J'me dois d'protéger ma puce Sans elle, j'ai pas ma pièce Rien n'est gratis, on n'dort pas, on charbonne Y a des travaux dans toute la tess Tous les jours, j't'entends dire Cette fois, c'est la bonne Mais bon, au final, j'vois pas l'papel, 'pel, 'pel, 'pel</t>
+          <t>You wanna focus, focus on this Focus on this Fuck tout faire péter, fuck le fair-play Poh, fuck leur faire plais' Poh, j'fais c'que j'ai envie Ouais Même le miroir, il khle3 du reflet Eh, voir le million au loin, c'est frais J'vois le million au loin, c'est vrai, j'v'-esqui les tchoïs Brr, oh, j'big up les réflexes Brr, oh Sur lui, t'as misé mais il t'la mise Brr, brr, fais c'que t'as à faire, te retourne pas, une fois qu'c'est fait Brr, brr Y a un plan cile-fa, c'est normal qu'on l'fait Fait, souvent khabat quand j'y vais Quand j'y vais J'ai pas bégayé quand j'l'ai vu Nan, j'ouvre une te-por, j'le maintiens en vie Brr En mode survie Brr, c'est en-dessous j'me demande si on vit Brr Les poches remplies, en moi, y a un vide Faut qu'j'prie, l'avenir, j'le trouve moyen vide Poh, poh, kamas au bec quand j'conduis Poh, poh La tchop, elle est jdid, la pute a un jean, jamais d'pénurie mais qui t'as dit ? Eh Si elle en veut, y a d'la beuh, y a du rab, si elle en veut, y a d'la beuh, y a du rab Fuck la pe-stu, l'rap, j'ai des produits durables, le p'tit grandit, dans un an, il postulera Uh Rentre sur l'T, fais crier l'stade Uh, criquets à midi pour t'lever à Cannes Uh Fais ton cash, évite le vacarme Poh, aller-retour, éviter la cam' Brr, brr Transactions d'vant les tantines et cles-on, roi est le client J'étais terre-pas, j'ai zolote un client, tu veux carna, j'mets l'tard-pé dans l'Clio Y a un canon, tu joues le philosophe Oui, j'l'ai filoche, j'tape, je file, le bras, j'allonge J'débloque les filons, plans sous j'arrose Poh c'est moi qu'a les tuyaux Poh Teh, massa, clope, sur moi, j'ai l'trio, j'me roule un p'tit Oh L'état du teum fait peur au proprio', normal qu'ça bosse d'lundi à lundi Oh Y a d'la ppe-f', t'apprécies l'odeur, il pense à pper-cho quand il est au taf La skung t'envoie en l'air, CM Punk Ah bon ? Y en a pour les skateurs et les hommes d'aff' Ah bon ?, je sé-cour, j'suis casqué comme un Daft Sale pute, ton passé, c'est pas du Velléda Salope, la victime s'est chouara, personne vient l'aider Ah bon ? Elle a plainté sous X, elle en veut à l'État Salope, j'sors d'un midi-minuit, j'dois d'jà faire une ssion-mi Le ient-cli est roi, ça fait une heure il câble, une heure du mat', j'suis devant les cages Trafic inarrêtable, sponso' par la Lyca', voiture allemande, j'suis vers Alicante Ah bon ? Les keufs sont cistes-ra, déboulent à cinquante Ah bon ?, cache ta cons', même une boulette, ça compte Brasser, c'est l'idée, c'est pour ça qu'on l'fait, casse pas d'bastos pour ces cons, ils sont traîtres Jamais, jamais Service précis, même si c'est miné d'flics Big up à mes réflexes, brr, brr, brr J'me dois d'protéger ma puce Sans elle, j'ai pas ma pièce Rien n'est gratis, on n'dort pas, on charbonne Y a des travaux dans toute la tess Tous les jours, j't'entends dire Cette fois, c'est la bonne Mais bon, au final, j'vois pas l'papel, 'pel, 'pel, 'pel Service précis, même si c'est miné d'flics Big up à mes réflexes, brr, brr, brr J'me dois d'protéger ma puce Sans elle, j'ai pas ma pièce Rien n'est gratis, on n'dort pas, on charbonne Y a des travaux dans toute la tess Tous les jours, j't'entends dire Cette fois, c'est la bonne Mais bon, au final, j'vois pas l'papel, 'pel, 'pel, 'pel Tout pour la mif', quitte à faire le crabe Mmh-mmh, avance sans gravons, c'est pas grave Mmh-mmh Nous trahis pas, j'oublie pas, même si j'bédave Jamais, il m'faut une nounou, j'pense à cher-bran une dame Et la noche, j'entends des voix comme Jeanne d'Arc Brr, j'ai besoin d'argent, besoin d'armes J'me targe avant le menottage Oui, sale con, t'es bé-tom pour un billet moutarde Oui Crique la bécane, j'entends les motards Han-han, crique la bécane, j'entends les motards J'débale en bas, j'détaille en bas Han-han mais ça pue jusqu'au dixième étage 1PLIKÉ, 1PLIKÉ 1PLIKÉ, attends un peu Oh, y a que la foi qui peut m'rattraper Oh Personne veut ma dépo', j'mets des pièces à l'OPJ, tout pour ma , j'ai placé l'P Le tour de ris-Pa, à fond sur l'riph'-pé, ris pas, après la rafale, c'est R.I.P Rien qu'tu parles de P, P, P, P, mais j'vois pas l'papel, eh Service précis, même si c'est miné d'flics Big up à mes réflexes, brr, brr, brr J'me dois d'protéger ma puce Sans elle, j'ai pas ma pièce, nan Rien n'est gratis, on n'dort pas, on charbonne Y a des travaux dans toute la tess Tous les jours, j't'entends dire Cette fois, c'est la bonne Mais bon, au final, j'vois pas l'papel, 'pel, 'pel, 'pel Service précis, même si c'est miné d'flics Big up à mes réflexes, brr, brr, brr J'me dois d'protéger ma puce Sans elle, j'ai pas ma pièce Rien n'est gratis, on n'dort pas, on charbonne Y a des travaux dans toute la tess Tous les jours, j't'entends dire Cette fois, c'est la bonne Mais bon, au final, j'vois pas l'papel, 'pel, 'pel, 'pel</t>
         </is>
       </c>
     </row>
@@ -1738,7 +1738,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Emeuh, emeuh C'est mon équipe qui vient dans ta fête et qui fait disparaître les objets On fait pas d'trous, on fait rentrer en scred, j'aimais pas quand l'gérant voulait voir les sous qu'j'ai On arrive violent, tu crois qu'on est sous 'she, si t'as pas mis un, crois pas qu'tu vas toucher Le .9 prêt à tirer, il s'en fout qu't'as poussé, t'as fumé, t'as toussé, tu rleh qu'on met tous ça Un billet à tter-gra, on y va tous, enculé, t'as chekem, tu veux pas tomber tout seul Un billet à tter-gra, on y va tous, quand les temps sont durs, ramène le mousseux En mode marathon, ils vont courir après l'coup d'feu, même si chez eux, ça m'écoute fort Ça pue la beuh, les voisins savent pas qu'j'découpe fort, nique la Focus Ford, à cause d'eux, mes coups foirent Cette pétasse veut qu'on s'voit, moi, j'veux la vue sur la costa sans même aller en cances-va On a caché nos tes-tê mais c'est pas la ce-fa qu'on s'voile et s'faire péter, c'est inconcevable Nos daronnes seront inconsolables, j'ai vécu des trucs qui sont pas racontables C'est pour l'appel du papier si on tarde, tu te caches, c'est dommage pour toi si on t'a J'suis sûr de les boire même en sirotant, on m'dit 1PLIKÉ, pourquoi t'es si hautain ? J'me suis fait seul, tu peux pas en dire autant, j'suis dans la renta', t'as fini terre-pa' Pourtant, avant, la beuh tu remontais, tu montres tes billets, nous, on les fait en s'débrouillant Quand t'étais à sec dans l'crime, j'étais mouillé, si on perd les nôtres, on s'refait en t'douillant Fais pas semblant, tu savais qu'j'étais bouillant, pour mon reuf, j'déboule en deux-deux Ça parle pas, y'a des pains à mort pourtant c'est pas la boulange', même des 50 de beuh pour les fils à papa Les 22 qui s'arrêtent, ne crois pas qu'ça papote, démarrage dans l'top, y a mortier et cailloux Tu veux pas donner les tales, tu sens la carotte, j'baraudais avec le ne-jeu qui t'met KO J'cassais la puce, j'avais les num' sur mon cahier, nous, on joue aucun rôle et tes rappeurs sont cailleux Cailleux, la solitude m'a accompagné, j'ai une lame tranchante donc j'suis en bonne compagnie On fout la de-mer donc ils veulent qu'on paye, pourtant, ils ont fait la même dans mon pays Viens pas faire la rre-gue si t'as peur de périr, j'voulais faire les choses propres, c'est l'sale qui a payé Pour une histoire de meuf, on descend pas, à part si cette pute, on la fait bosser Cace-déd' à celles qui baisent pas pour moins d'cent balles, j'sors d'un contrôle peinard, j'ai cent grammes dans l'boxer On t'a menti, y a pas d'paradis sur terre, tu traînes avec mais il a parlé sur toi J'ai plus d'amour, j'vois Cupidon ligoté, sous gros teh, y a que la haine que je côtoieYou might also like</t>
+          <t>Emeuh, emeuh C'est mon équipe qui vient dans ta fête et qui fait disparaître les objets On fait pas d'trous, on fait rentrer en scred, j'aimais pas quand l'gérant voulait voir les sous qu'j'ai On arrive violent, tu crois qu'on est sous 'she, si t'as pas mis un, crois pas qu'tu vas toucher Le .9 prêt à tirer, il s'en fout qu't'as poussé, t'as fumé, t'as toussé, tu rleh qu'on met tous ça Un billet à tter-gra, on y va tous, enculé, t'as chekem, tu veux pas tomber tout seul Un billet à tter-gra, on y va tous, quand les temps sont durs, ramène le mousseux En mode marathon, ils vont courir après l'coup d'feu, même si chez eux, ça m'écoute fort Ça pue la beuh, les voisins savent pas qu'j'découpe fort, nique la Focus Ford, à cause d'eux, mes coups foirent Cette pétasse veut qu'on s'voit, moi, j'veux la vue sur la costa sans même aller en cances-va On a caché nos tes-tê mais c'est pas la ce-fa qu'on s'voile et s'faire péter, c'est inconcevable Nos daronnes seront inconsolables, j'ai vécu des trucs qui sont pas racontables C'est pour l'appel du papier si on tarde, tu te caches, c'est dommage pour toi si on t'a J'suis sûr de les boire même en sirotant, on m'dit 1PLIKÉ, pourquoi t'es si hautain ? J'me suis fait seul, tu peux pas en dire autant, j'suis dans la renta', t'as fini terre-pa' Pourtant, avant, la beuh tu remontais, tu montres tes billets, nous, on les fait en s'débrouillant Quand t'étais à sec dans l'crime, j'étais mouillé, si on perd les nôtres, on s'refait en t'douillant Fais pas semblant, tu savais qu'j'étais bouillant, pour mon reuf, j'déboule en deux-deux Ça parle pas, y'a des pains à mort pourtant c'est pas la boulange', même des 50 de beuh pour les fils à papa Les 22 qui s'arrêtent, ne crois pas qu'ça papote, démarrage dans l'top, y a mortier et cailloux Tu veux pas donner les tales, tu sens la carotte, j'baraudais avec le ne-jeu qui t'met KO J'cassais la puce, j'avais les num' sur mon cahier, nous, on joue aucun rôle et tes rappeurs sont cailleux Cailleux, la solitude m'a accompagné, j'ai une lame tranchante donc j'suis en bonne compagnie On fout la de-mer donc ils veulent qu'on paye, pourtant, ils ont fait la même dans mon pays Viens pas faire la rre-gue si t'as peur de périr, j'voulais faire les choses propres, c'est l'sale qui a payé Pour une histoire de meuf, on descend pas, à part si cette pute, on la fait bosser Cace-déd' à celles qui baisent pas pour moins d'cent balles, j'sors d'un contrôle peinard, j'ai cent grammes dans l'boxer On t'a menti, y a pas d'paradis sur terre, tu traînes avec mais il a parlé sur toi J'ai plus d'amour, j'vois Cupidon ligoté, sous gros teh, y a que la haine que je côtoie</t>
         </is>
       </c>
     </row>
@@ -1755,7 +1755,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>1.4.0, 1.4.0 Eh, eh, eh C'est notre avenir qu'on dessine, c'est nos proches qui faut pas qu'on déçoive J'ai pas l'droit d'être indécis, j'suis toujours technique sur mes choix On perd pas tant qu'le but est pris pour cible, on n'a pas baissé les bras Mais lever la tête, poto, rien n'est impossible, reste sûr de toi poh, poh, poh, poh Pas l'temps d'chômer tant qu'on n'a pas vu le sommet Tu sens qu'j'suis déter' dans mes ceaux-mor Avance serein, n'écoute pas ces cons qui se moquent, à la fin, les doigts, ils se mordent On a su becter le destin, on le tord, on a supporté tous les mauvais temps uh On sort la tête de l'eau dès la première mi-temps, pour sortir du lot, faut pas les imiter En mode, j'suis un mutant, j'sors des ses-pha sans méditer J'rentre dans la bine-ca, le crime, il est prémédité Le succès, il faut le mériter, fais pas d'faux pas dans la zone Comme Neuer, tu sais qu'on a l'brassard depuis l'départ On encaisse des points brr, on mettra des virgules à ceux qui nous empêchent de brasser brr, brr, brr De personne on dépend On accomplira pas en rêvant, mais dites aux jeunes de garder leur rêves Lâche pas si t'as du talent a revendre han Ton espoir jamais on t'l'enlève han Je n'pense qu'à augmenter le level, qu'à voir la foule faire la ola Profite de ta vie y en a qui la veulent Brille comme les étoiles sur le lliot-ma paw You might also like Chaque saison, au top comme le Bayern, chaque saison, au top comme le Bayern poh Ils veulent savoir si j'suis encore dans les bails, eux, encore dans les bails, eux Chaque saison, au top comme le Bayern, chaque saison, au top comme le Bayern Ils veulent savoir si j'suis encore dans les bails, eux hein, encore dans les bails, eux hein 1.4.0</t>
+          <t>1.4.0, 1.4.0 Eh, eh, eh C'est notre avenir qu'on dessine, c'est nos proches qui faut pas qu'on déçoive J'ai pas l'droit d'être indécis, j'suis toujours technique sur mes choix On perd pas tant qu'le but est pris pour cible, on n'a pas baissé les bras Mais lever la tête, poto, rien n'est impossible, reste sûr de toi poh, poh, poh, poh Pas l'temps d'chômer tant qu'on n'a pas vu le sommet Tu sens qu'j'suis déter' dans mes ceaux-mor Avance serein, n'écoute pas ces cons qui se moquent, à la fin, les doigts, ils se mordent On a su becter le destin, on le tord, on a supporté tous les mauvais temps uh On sort la tête de l'eau dès la première mi-temps, pour sortir du lot, faut pas les imiter En mode, j'suis un mutant, j'sors des ses-pha sans méditer J'rentre dans la bine-ca, le crime, il est prémédité Le succès, il faut le mériter, fais pas d'faux pas dans la zone Comme Neuer, tu sais qu'on a l'brassard depuis l'départ On encaisse des points brr, on mettra des virgules à ceux qui nous empêchent de brasser brr, brr, brr De personne on dépend On accomplira pas en rêvant, mais dites aux jeunes de garder leur rêves Lâche pas si t'as du talent a revendre han Ton espoir jamais on t'l'enlève han Je n'pense qu'à augmenter le level, qu'à voir la foule faire la ola Profite de ta vie y en a qui la veulent Brille comme les étoiles sur le lliot-ma paw Chaque saison, au top comme le Bayern, chaque saison, au top comme le Bayern poh Ils veulent savoir si j'suis encore dans les bails, eux, encore dans les bails, eux Chaque saison, au top comme le Bayern, chaque saison, au top comme le Bayern Ils veulent savoir si j'suis encore dans les bails, eux hein, encore dans les bails, eux hein 1.4.0</t>
         </is>
       </c>
     </row>
@@ -1772,7 +1772,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Cocktail molotov, mortiers sur les keufs Joue pas les gros, t'as pété une to-ph' Hein, week-end sur un plav', j'vais pas péter une tte-ch' Hein J'vais péter une tête, pas que pour une 'quette, ni pour une branche de beuh De beuh La bicrave, le vol La bicrave, le vol, bien sûr, je branche les deux Faut les ken, tartine mais là, ça ken, l'instru' débite sa mère Eh, ça va se plaindre à un ce-m Eh Putain, c'est plus d'la came, tu vois bien c'est laquelle, juste un canon Brr, ça donne des blases Brr, ça lèche des queues Brr J'suis le ce-me qui peut le ressortir, recommencer Le ressortir Le drapeau est noir, ton sang est rouge, Milan AC Je sais où m'placer Amen, je sais où m'casser Amen, TP épicé, j'reste pas assis Amen Jamais changer d'équipe, j'ai vu sourire le baveux, j'sais qu'l'audience va bien s'passer Poh, poh, poh, poh, nonante Ients-cli fidèles Le client est roi ramènent toujours des intéressés Ma porte a pas pété, elle est belle, t'inquiète, l'avocat, y a de quoi l'rincer Bécane en i, sans casque Bécane en i, j'suis en roue libre J'suis en roue libre J'v'-esqui le trafic, j'suis dans le trafic, j'suis en roue libre J'suis en roue libre La journée, on livre, le soir, on livre, là, j'suis en roue libre Pa-pah Il reste des ffaires-a mais j'rajoute un tron-li, j'suis en roue libre Gros kamas en pilotant l'bolide, j'suis en roue libre Oui J'suis impliqué, recto verso Oui, oui, jamais hors-ligne Oui, nonante Chargeur camembert, chargeur entamé Chargeur camembert, po-po-po-poh J'attends l'échangeur, je remplis le chargeur Coupe, coupe, coupe, coupe Elle revient des îles, le ventre est rempli, j'suis à Orly CDG Un téléphone sans application, j'suis pas en ligne Sans application, coupe, coupe Contrôle du ballon dans la surface, Thierry Henry Numéro neuf J'v-'esqui le trafic, j'suis dans le trafic, j'suis en roue libre Au charbon même sous courbatures Hum, hum, j'ai l'produit qui traumatise 1PLIKÉ Avant que j'ai la VIP, pense à investir 1PLIKÉ, un pe-pom automatique, j'suis pas assez mature Brr Faut l'truc qui fait danser, j'pars de stup' au dio-stu, j'ai taffé que dans ça Taffé que dans ça, brr Tu réapparais quand y a plus trop d'tension Amen, toi, t'es pas trop dans l'sale Amen Quand c'est l'heure d'en découdre, c'est là qu'il faut faire du sale Coupe C'est là qu'il faut faire des sommes pour le réinvestir dans les armes Brr Le sers pas si sa tête, elle est zarre-b' Brr, mon gars, investis dans l'amnésia Amen J'recrute un ne-jeu Ouh qui fait mes missions sans phaser, j'peux dormir sur mes deux oreilles Ouh, ouh You might also like Bécane en i, sans casque Bécane en i, j'suis en roue libre J'suis en roue libre J'v'-esqui le trafic, j'suis dans le trafic, j'suis en roue libre La journée, on livre, le soir, on livre, là, j'suis en roue libre J'suis en roue libre Il reste des ffaires-a mais j'rajoute un tron-li J'suis en roue libre, j'suis en roue libre J'suis en roue libre Gros kamas en pilotant l'bolide Oui, j'suis en roue libre Oui J'suis impliqué, recto verso Oui, oui, jamais hors-ligne Jamais, jamais, jamais, jamais, jamais, jamais</t>
+          <t>Cocktail molotov, mortiers sur les keufs Joue pas les gros, t'as pété une to-ph' Hein, week-end sur un plav', j'vais pas péter une tte-ch' Hein J'vais péter une tête, pas que pour une 'quette, ni pour une branche de beuh De beuh La bicrave, le vol La bicrave, le vol, bien sûr, je branche les deux Faut les ken, tartine mais là, ça ken, l'instru' débite sa mère Eh, ça va se plaindre à un ce-m Eh Putain, c'est plus d'la came, tu vois bien c'est laquelle, juste un canon Brr, ça donne des blases Brr, ça lèche des queues Brr J'suis le ce-me qui peut le ressortir, recommencer Le ressortir Le drapeau est noir, ton sang est rouge, Milan AC Je sais où m'placer Amen, je sais où m'casser Amen, TP épicé, j'reste pas assis Amen Jamais changer d'équipe, j'ai vu sourire le baveux, j'sais qu'l'audience va bien s'passer Poh, poh, poh, poh, nonante Ients-cli fidèles Le client est roi ramènent toujours des intéressés Ma porte a pas pété, elle est belle, t'inquiète, l'avocat, y a de quoi l'rincer Bécane en i, sans casque Bécane en i, j'suis en roue libre J'suis en roue libre J'v'-esqui le trafic, j'suis dans le trafic, j'suis en roue libre J'suis en roue libre La journée, on livre, le soir, on livre, là, j'suis en roue libre Pa-pah Il reste des ffaires-a mais j'rajoute un tron-li, j'suis en roue libre Gros kamas en pilotant l'bolide, j'suis en roue libre Oui J'suis impliqué, recto verso Oui, oui, jamais hors-ligne Oui, nonante Chargeur camembert, chargeur entamé Chargeur camembert, po-po-po-poh J'attends l'échangeur, je remplis le chargeur Coupe, coupe, coupe, coupe Elle revient des îles, le ventre est rempli, j'suis à Orly CDG Un téléphone sans application, j'suis pas en ligne Sans application, coupe, coupe Contrôle du ballon dans la surface, Thierry Henry Numéro neuf J'v-'esqui le trafic, j'suis dans le trafic, j'suis en roue libre Au charbon même sous courbatures Hum, hum, j'ai l'produit qui traumatise 1PLIKÉ Avant que j'ai la VIP, pense à investir 1PLIKÉ, un pe-pom automatique, j'suis pas assez mature Brr Faut l'truc qui fait danser, j'pars de stup' au dio-stu, j'ai taffé que dans ça Taffé que dans ça, brr Tu réapparais quand y a plus trop d'tension Amen, toi, t'es pas trop dans l'sale Amen Quand c'est l'heure d'en découdre, c'est là qu'il faut faire du sale Coupe C'est là qu'il faut faire des sommes pour le réinvestir dans les armes Brr Le sers pas si sa tête, elle est zarre-b' Brr, mon gars, investis dans l'amnésia Amen J'recrute un ne-jeu Ouh qui fait mes missions sans phaser, j'peux dormir sur mes deux oreilles Ouh, ouh Bécane en i, sans casque Bécane en i, j'suis en roue libre J'suis en roue libre J'v'-esqui le trafic, j'suis dans le trafic, j'suis en roue libre La journée, on livre, le soir, on livre, là, j'suis en roue libre J'suis en roue libre Il reste des ffaires-a mais j'rajoute un tron-li J'suis en roue libre, j'suis en roue libre J'suis en roue libre Gros kamas en pilotant l'bolide Oui, j'suis en roue libre Oui J'suis impliqué, recto verso Oui, oui, jamais hors-ligne Jamais, jamais, jamais, jamais, jamais, jamais</t>
         </is>
       </c>
     </row>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Ça dit quoi ma beauté ? T'es mimi Hey, hey Hey, hey, hey Ouh eh Ouh, ouh Ça dit quoi ma beauté ? T'es mi- Hey, hey Hey, hey Brr, paw Brr, brr Ça dit quoi ma beauté ? T'es mimi, mimi, mimi, mimi, mimi, mimi, mimi Moi, j'viens de là où ça bibi, bibi, bibi, bibi, bibi, bibi, bibi J'sais qu'j'aurais pas l'salaire de Matuidi en revendant la matiti Mais l'argent facile me titille, mais l'argent facile me titille J'sais qu'j'aurais pas l'salaire de Matuidi en revendant la matiti Mais l'argent facile me titille, mais l'argent facile m titille On a fait le trajet, trajt, trajet, trajet Gue-dro dans l'sachet, sachet, sachet, sachet On connaît l'danger, danger, danger, danger Mais on veut manger, manger, manger, manger J'suis avec, il a caché l'fusil sous l'plancher Y a de la, pour animer tes soirées branchées On voulait brasser, bien avant de savoir nager Libérez tous ceux qui ont plongés J'me revois menotter sur le canapé Aujourd'hui, Negrito passe sur Booska-P J'ai dealé pour le papier, pas pour l'raper Si je t'ai donné, c'est pas pour t'le rappeler On m'a dit qu'il faut faire la guerre pour la paix Donc on fait la guerre aux gardiens de la paix Rancunier, tu m'as trahi, j'ai pas zappé La CC, faut la vendre, faut pas la taper Négro, négro, c'est Negrito hey, hey J'avais si j'récupère aussitôt hey, hey Igo, nous on fait pas les bandits hey, hey Mais crois-moi, on n'est pas des mythos hey, hey Négro, négro, c'est Negrito hey, hey J'avais si j'récupère aussitôt hey, hey Igo, nous on fait pas les bandits hey, hey Mais crois-moi, on n'est pas des mythos hey, hey Mon sin-cou Zaky, il vend le sel, pourtant, c'est pas un épicier hey, hey Si tu connais ton boug Negri, tu sais qu'il aime les filles métissées Mon sin-cou Zaky, il vend le sel, pourtant, c'est pas un épicier ouh Si tu connais ton boug Negri, tu sais qu'il aime les filles métissées You might also like Ça dit quoi ma beauté ? T'es mimi, mimi, mimi, mimi, mimi, mimi, mimi Moi, j'viens de là où ça bibi, bibi, bibi, bibi, bibi, bibi, bibi J'sais qu'j'aurais pas l'salaire de Matuidi en revendant la matiti Mais l'argent facile me titille, mais l'argent facile me titille J'sais qu'j'aurais pas l'salaire de Matuidi en revendant la matiti Mais l'argent facile me titille, mais l'argent facile me titille Kotazo eh, eh, ti na kotazo Kotazo eh, eh, ti na kotazo Kotazo eh, eh, ti na kotazo Kotazo Négro, négro, c'est Negrito Kotazo Igo, nous on fait pas les bandits Kotazo Négro, négro, c'est Negrito Kotazo Igo, nous on fait pas les bandits Ti na Kotazo On n'est pas des mythos</t>
+          <t>Ça dit quoi ma beauté ? T'es mimi Hey, hey Hey, hey, hey Ouh eh Ouh, ouh Ça dit quoi ma beauté ? T'es mi- Hey, hey Hey, hey Brr, paw Brr, brr Ça dit quoi ma beauté ? T'es mimi, mimi, mimi, mimi, mimi, mimi, mimi Moi, j'viens de là où ça bibi, bibi, bibi, bibi, bibi, bibi, bibi J'sais qu'j'aurais pas l'salaire de Matuidi en revendant la matiti Mais l'argent facile me titille, mais l'argent facile me titille J'sais qu'j'aurais pas l'salaire de Matuidi en revendant la matiti Mais l'argent facile me titille, mais l'argent facile m titille On a fait le trajet, trajt, trajet, trajet Gue-dro dans l'sachet, sachet, sachet, sachet On connaît l'danger, danger, danger, danger Mais on veut manger, manger, manger, manger J'suis avec, il a caché l'fusil sous l'plancher Y a de la, pour animer tes soirées branchées On voulait brasser, bien avant de savoir nager Libérez tous ceux qui ont plongés J'me revois menotter sur le canapé Aujourd'hui, Negrito passe sur Booska-P J'ai dealé pour le papier, pas pour l'raper Si je t'ai donné, c'est pas pour t'le rappeler On m'a dit qu'il faut faire la guerre pour la paix Donc on fait la guerre aux gardiens de la paix Rancunier, tu m'as trahi, j'ai pas zappé La CC, faut la vendre, faut pas la taper Négro, négro, c'est Negrito hey, hey J'avais si j'récupère aussitôt hey, hey Igo, nous on fait pas les bandits hey, hey Mais crois-moi, on n'est pas des mythos hey, hey Négro, négro, c'est Negrito hey, hey J'avais si j'récupère aussitôt hey, hey Igo, nous on fait pas les bandits hey, hey Mais crois-moi, on n'est pas des mythos hey, hey Mon sin-cou Zaky, il vend le sel, pourtant, c'est pas un épicier hey, hey Si tu connais ton boug Negri, tu sais qu'il aime les filles métissées Mon sin-cou Zaky, il vend le sel, pourtant, c'est pas un épicier ouh Si tu connais ton boug Negri, tu sais qu'il aime les filles métissées Ça dit quoi ma beauté ? T'es mimi, mimi, mimi, mimi, mimi, mimi, mimi Moi, j'viens de là où ça bibi, bibi, bibi, bibi, bibi, bibi, bibi J'sais qu'j'aurais pas l'salaire de Matuidi en revendant la matiti Mais l'argent facile me titille, mais l'argent facile me titille J'sais qu'j'aurais pas l'salaire de Matuidi en revendant la matiti Mais l'argent facile me titille, mais l'argent facile me titille Kotazo eh, eh, ti na kotazo Kotazo eh, eh, ti na kotazo Kotazo eh, eh, ti na kotazo Kotazo Négro, négro, c'est Negrito Kotazo Igo, nous on fait pas les bandits Kotazo Négro, négro, c'est Negrito Kotazo Igo, nous on fait pas les bandits Ti na Kotazo On n'est pas des mythos</t>
         </is>
       </c>
     </row>
@@ -1806,7 +1806,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Partie 1 H La Drogue H La Drogue SJ À mes 12 piges bâtard j'voulais d'jà un gros fer Bitches pécho casse-toi, y a pas d'dix balles offerts Pendant la chasse négro, stresse pas Les schmits c'est des mauviettes, dans la cellule j'fais mes 100 pas J'fume du pilon, il t'fait gamberge Dans ma click y a que des chacals Dans la capi' j'enchaîne livrette Ils racontent des trucs qu'ils font pas Ils m'ont claqué caché dans l'binks J'ai v'-esqui plus d'600 traquenards Ça vend d'la beuh à la sauvette T'as fait ton temps igo casse-toi T'es trop bizarre, t'enchaînes les dettes Malgré la défaite on y va On comme des p'tits frères J'suis à l'affût, j'me casse la voix Sur ma grandmère, ils vont rien pet' On va débar si tu fais l'roi Ils sont matrixés sous zipette Libérez Boubso au placard Cherche pas la merde si t'es pas prêt Parle-moi gent-ar ou bien casse-toi Dans ma te-té j'pense qu'à l'oseille J'viens d'récup' le clims ils m'géchar En trois minutes j'ai fait cinq checks Igo faut garder la mentale Gardav dépôt, j'suis trop keleh, c'est la rre-gue, on tourne chez oi-t Poto, il faut qu'j'les voie na3as, sur la quette-pla j'fais plus d'une balle Vrai charognard, j'm'en bats les steaks, bip, stringer pour d'l'Amnésia Ta go dans l'bât', gros, elle s'fait gma3 Ça veut m'te-j' au placard, j'répète, c'est nous les plus zahaf Quand j'guettais, toi, tu na3as, 9-2-1-4 dans ta grand-mère Mon poto gamberge, quand ça ré-ti, ça fait bang-bang On est pas trop dans l'din din, négro, tard l'bitume sa grand-mère Coyote posté jvisser des 10 Pas 7arag j'surveille la tess, en mode chimie j'découpe la S Dans l'gamos j'active mode S, sous pillave j'vois ses grosses fesses Si j'meurs, belek l'enfer, clims qui passe, direct j'vais l'faire , j'vends d'la beuh à des grand-pères Pas du genre à faire la paix, j'suis sur l'R, j'ramène les r En mode pirate j'vesqui la deb, elle veut d'l'amour, j'suis pas sincère You might also like Mme-gra d'pilon vendu à la sauvette, c'est trop bizarre, toutes ces baltringues se sont sauvées Mme-gra d'pilon vendu à la sauvette, c'est trop bizarre, toutes ces baltringues se sont sauvées HLD Partie 2 JRK Ouais MAV Hashtag trois Avenue Porte Brunet, c'est là qu'y a les gros bonnets Libérez l'équipe, hein Eh C'est Danube sale enfoiré 1-9, 1-9 Oh, yeah, oh boy, this shit bang Après avoir cassé un coup Ouais J'irais direct cassé un cul Tu veux la guerre ? Mais toi t'as pas d'armes Si on fait la guerre, on t'enlève ton âme Ils s'mettent en valeur après ils s'étonnent qu'ils s'attirent des voleurs Ouais, ouais J'm'amuse avec ma guitare, que des têtes cassées, y a pas de fêtards Eh, eh Et c'est dans la foule que j'm'engouffre Pour une R', ça t'étouffe Charismatique, elle a du charme J'vais serrer ton cou à l'aide de ton écharpe 22, Arthéna, faut qu'tu t'échappes Y a de la beuh et y a du shit Tu crois baroder dans les endroits chics ? C'est que j'ai filoché un bon plan, filoché un bon plan En tournant ta montre nous on la prend Y a pas plus combattantes que nos daronnes Toi t'es pas fiable, j'te crois pas sur paroles J'fais des une-deux avec Batama, tu parles de Ferza mais t'es pas dedans Nous on n'est MAV, m'appelle pas j'suis en mode avion En mode avion Dans le quatre-anneaux Dans le quatre-anneaux On est quatre re-nois On n'est quatre re-nois J'écoute les conseils de Ryoma Les conseils de Ryoma J'dois être la fierté du quartier La fierté du quartier Dans le quatre-anneaux Dans le quatre-anneaux On est quatre re-nois On n'est quatre re-nois J'écoute les conseils de Ryoma Les conseils de Ryoma J'dois être la fierté du quartier La fierté du quartier Libérez l'équipe, là c'est pas carré Pour une histoire de meufs, vous êtes séparés Elle aime les footballeurs et les voleurs C'est cette vie-là qu'on a voulue Pour une R', ça coupe ton bras Mes péchés sont encombrés Mon cur il est déchiré, tout l'équipage il a chaviré Ça dérobe ta R', ça dérobe ton collier Crois-moi, on n'est pas poli Avenue Porte Brunet, ouais c'est trop torride Ouais c'est trop torride Elle veut des câlins, elle veut des massages Elle me dit JRK, arrête tes mensonges Eh Elle veut des câlins, elle veut des massages Elle me dit JRK, arrête tes mensonges Eh Dans le quatre-anneaux Dans le quatre-anneaux On n'est quatre re-nois On n'est quatre re-nois J'écoute les conseils de Ryoma Les conseils de Ryoma J'dois être la fierté du quartier La fierté du quartier Dans le quatre-anneaux Dans le quatre-anneaux On n'est quatre re-nois On n'est quatre re-nois J'écoute les conseils de Ryoma Les conseils de Ryoma J'dois être la fierté du quartier La fierté du quartier Oh, yeah, oh boy Fierté du quartier ouais, ouais Fierté du quartier skrr, skrr Fierté du quartier ouais, ouais Skrr, skrr, MAV Libérez l'équipe, hein C'est pas fini Eh, 3, skrr, skrr Partie 3 Mapess Partie 4 1PLIKÉ140 J'ai connu l'argent sale dans le vol de keusa J'ai appris à brasser avec paire de requins Tu fais la mala, tu mets tes derniers pe-sa T'es pas sur la liste, au final tu t'fais recale La hagra ça paie pas, la hasba ça paie J'en ai mis des rotte-ca comme Cenoura Toi, tu bombes le torse devant les p'tits Tu fais moins l'malin quand c'est nous, hein ? Moins l'malin quand c'est nous, hein ? Faut toujours donner à ceux qui ont besoin Une 10 ou une 20 appele moi en cas d'besoin Lopinel peut viser ton torse ou ta be-jam On est trop têtu alors on tabasse les gens Askip fumer tue pourtant on tabasse le joint Elle veut prendre mes thunes elle aura ma 3 eme jambe La miss elle mconnais bien mais pourtant elle fait genre Mes negros peuvent pull-up ta chaîne quand il fait jour Si ta un collier tu seras pas immunisé Mes negros peuvent pull-up ta chaîne quand il fait jour Jai les idées claires même quand jsuis alcoolisé Même si je revends toute la noche jdois encore mreveiller tôt le matin Les vil-ci, les poucaves, les faux frères, les te-trai sont dans mon collimateur J'tabasse toutes les prods jusquà qu'ils retiennent mon nom Je fais ça en deuspi après ça je retourne dans lombre Jcommence les mains vides, jdégaine si ils sont en nombre Jdégaine si ils sont en nombre Partie 5 1PLIKÉ140 Askip tes mon reufré mais jsens qutu manque dhonnêteté On a charbonner en hiver pour faire plus de cash en été Batard jsais bien qutu connais tchi Tas 0 connexion Dans le tier-quar tu peut chebran que les ptits Tas 0 connexion Dans le tier-quar tu peut chebran que les ptits Sur insta elle est gechar En vrai elle est squelettique Jgaz, jpietine jgaz, jpietine Putain jcrois bien qujai des tics Faut pas claquer faut investir Pour le plavon en noir je suis vêtue Et si tu me croises gantés cest pas pour la température Jparle à limpératif comme ça cest sure qu'tu donnes les thunes Jai jamais su ce que je voulais faire dans la vie Mais jme vois pas faire de longues études Dans ta cité y a que des acteurs de dormeurs mon négros le savais-tu ? Ça sent la perquis jsuis lever avant six heures On commet des péchés, on commet trop derreurs, mais on a pas perdu la foi Jpeux pas rater l'service comme Federer, mais y a les condes derrière moi Jme sens pisté, ça sent le bacon Si on sent un ke-tru, tu lâcheras ta bécane Le trafic c'est pour l'bien même si c'est pas légal Le trafic c'est pour l'bien même si c'est pas légal J'ai pas attendu d'fumer pour trouver d'l'inspi' J'écrivais mes textes sur une puce de ient-cli</t>
+          <t>Partie 1 H La Drogue H La Drogue SJ À mes 12 piges bâtard j'voulais d'jà un gros fer Bitches pécho casse-toi, y a pas d'dix balles offerts Pendant la chasse négro, stresse pas Les schmits c'est des mauviettes, dans la cellule j'fais mes 100 pas J'fume du pilon, il t'fait gamberge Dans ma click y a que des chacals Dans la capi' j'enchaîne livrette Ils racontent des trucs qu'ils font pas Ils m'ont claqué caché dans l'binks J'ai v'-esqui plus d'600 traquenards Ça vend d'la beuh à la sauvette T'as fait ton temps igo casse-toi T'es trop bizarre, t'enchaînes les dettes Malgré la défaite on y va On comme des p'tits frères J'suis à l'affût, j'me casse la voix Sur ma grandmère, ils vont rien pet' On va débar si tu fais l'roi Ils sont matrixés sous zipette Libérez Boubso au placard Cherche pas la merde si t'es pas prêt Parle-moi gent-ar ou bien casse-toi Dans ma te-té j'pense qu'à l'oseille J'viens d'récup' le clims ils m'géchar En trois minutes j'ai fait cinq checks Igo faut garder la mentale Gardav dépôt, j'suis trop keleh, c'est la rre-gue, on tourne chez oi-t Poto, il faut qu'j'les voie na3as, sur la quette-pla j'fais plus d'une balle Vrai charognard, j'm'en bats les steaks, bip, stringer pour d'l'Amnésia Ta go dans l'bât', gros, elle s'fait gma3 Ça veut m'te-j' au placard, j'répète, c'est nous les plus zahaf Quand j'guettais, toi, tu na3as, 9-2-1-4 dans ta grand-mère Mon poto gamberge, quand ça ré-ti, ça fait bang-bang On est pas trop dans l'din din, négro, tard l'bitume sa grand-mère Coyote posté jvisser des 10 Pas 7arag j'surveille la tess, en mode chimie j'découpe la S Dans l'gamos j'active mode S, sous pillave j'vois ses grosses fesses Si j'meurs, belek l'enfer, clims qui passe, direct j'vais l'faire , j'vends d'la beuh à des grand-pères Pas du genre à faire la paix, j'suis sur l'R, j'ramène les r En mode pirate j'vesqui la deb, elle veut d'l'amour, j'suis pas sincère Mme-gra d'pilon vendu à la sauvette, c'est trop bizarre, toutes ces baltringues se sont sauvées Mme-gra d'pilon vendu à la sauvette, c'est trop bizarre, toutes ces baltringues se sont sauvées HLD Partie 2 JRK Ouais MAV Hashtag trois Avenue Porte Brunet, c'est là qu'y a les gros bonnets Libérez l'équipe, hein Eh C'est Danube sale enfoiré 1-9, 1-9 Oh, yeah, oh boy, this shit bang Après avoir cassé un coup Ouais J'irais direct cassé un cul Tu veux la guerre ? Mais toi t'as pas d'armes Si on fait la guerre, on t'enlève ton âme Ils s'mettent en valeur après ils s'étonnent qu'ils s'attirent des voleurs Ouais, ouais J'm'amuse avec ma guitare, que des têtes cassées, y a pas de fêtards Eh, eh Et c'est dans la foule que j'm'engouffre Pour une R', ça t'étouffe Charismatique, elle a du charme J'vais serrer ton cou à l'aide de ton écharpe 22, Arthéna, faut qu'tu t'échappes Y a de la beuh et y a du shit Tu crois baroder dans les endroits chics ? C'est que j'ai filoché un bon plan, filoché un bon plan En tournant ta montre nous on la prend Y a pas plus combattantes que nos daronnes Toi t'es pas fiable, j'te crois pas sur paroles J'fais des une-deux avec Batama, tu parles de Ferza mais t'es pas dedans Nous on n'est MAV, m'appelle pas j'suis en mode avion En mode avion Dans le quatre-anneaux Dans le quatre-anneaux On est quatre re-nois On n'est quatre re-nois J'écoute les conseils de Ryoma Les conseils de Ryoma J'dois être la fierté du quartier La fierté du quartier Dans le quatre-anneaux Dans le quatre-anneaux On est quatre re-nois On n'est quatre re-nois J'écoute les conseils de Ryoma Les conseils de Ryoma J'dois être la fierté du quartier La fierté du quartier Libérez l'équipe, là c'est pas carré Pour une histoire de meufs, vous êtes séparés Elle aime les footballeurs et les voleurs C'est cette vie-là qu'on a voulue Pour une R', ça coupe ton bras Mes péchés sont encombrés Mon cur il est déchiré, tout l'équipage il a chaviré Ça dérobe ta R', ça dérobe ton collier Crois-moi, on n'est pas poli Avenue Porte Brunet, ouais c'est trop torride Ouais c'est trop torride Elle veut des câlins, elle veut des massages Elle me dit JRK, arrête tes mensonges Eh Elle veut des câlins, elle veut des massages Elle me dit JRK, arrête tes mensonges Eh Dans le quatre-anneaux Dans le quatre-anneaux On n'est quatre re-nois On n'est quatre re-nois J'écoute les conseils de Ryoma Les conseils de Ryoma J'dois être la fierté du quartier La fierté du quartier Dans le quatre-anneaux Dans le quatre-anneaux On n'est quatre re-nois On n'est quatre re-nois J'écoute les conseils de Ryoma Les conseils de Ryoma J'dois être la fierté du quartier La fierté du quartier Oh, yeah, oh boy Fierté du quartier ouais, ouais Fierté du quartier skrr, skrr Fierté du quartier ouais, ouais Skrr, skrr, MAV Libérez l'équipe, hein C'est pas fini Eh, 3, skrr, skrr Partie 3 Mapess Partie 4 1PLIKÉ140 J'ai connu l'argent sale dans le vol de keusa J'ai appris à brasser avec paire de requins Tu fais la mala, tu mets tes derniers pe-sa T'es pas sur la liste, au final tu t'fais recale La hagra ça paie pas, la hasba ça paie J'en ai mis des rotte-ca comme Cenoura Toi, tu bombes le torse devant les p'tits Tu fais moins l'malin quand c'est nous, hein ? Moins l'malin quand c'est nous, hein ? Faut toujours donner à ceux qui ont besoin Une 10 ou une 20 appele moi en cas d'besoin Lopinel peut viser ton torse ou ta be-jam On est trop têtu alors on tabasse les gens Askip fumer tue pourtant on tabasse le joint Elle veut prendre mes thunes elle aura ma 3 eme jambe La miss elle mconnais bien mais pourtant elle fait genre Mes negros peuvent pull-up ta chaîne quand il fait jour Si ta un collier tu seras pas immunisé Mes negros peuvent pull-up ta chaîne quand il fait jour Jai les idées claires même quand jsuis alcoolisé Même si je revends toute la noche jdois encore mreveiller tôt le matin Les vil-ci, les poucaves, les faux frères, les te-trai sont dans mon collimateur J'tabasse toutes les prods jusquà qu'ils retiennent mon nom Je fais ça en deuspi après ça je retourne dans lombre Jcommence les mains vides, jdégaine si ils sont en nombre Jdégaine si ils sont en nombre Partie 5 1PLIKÉ140 Askip tes mon reufré mais jsens qutu manque dhonnêteté On a charbonner en hiver pour faire plus de cash en été Batard jsais bien qutu connais tchi Tas 0 connexion Dans le tier-quar tu peut chebran que les ptits Tas 0 connexion Dans le tier-quar tu peut chebran que les ptits Sur insta elle est gechar En vrai elle est squelettique Jgaz, jpietine jgaz, jpietine Putain jcrois bien qujai des tics Faut pas claquer faut investir Pour le plavon en noir je suis vêtue Et si tu me croises gantés cest pas pour la température Jparle à limpératif comme ça cest sure qu'tu donnes les thunes Jai jamais su ce que je voulais faire dans la vie Mais jme vois pas faire de longues études Dans ta cité y a que des acteurs de dormeurs mon négros le savais-tu ? Ça sent la perquis jsuis lever avant six heures On commet des péchés, on commet trop derreurs, mais on a pas perdu la foi Jpeux pas rater l'service comme Federer, mais y a les condes derrière moi Jme sens pisté, ça sent le bacon Si on sent un ke-tru, tu lâcheras ta bécane Le trafic c'est pour l'bien même si c'est pas légal Le trafic c'est pour l'bien même si c'est pas légal J'ai pas attendu d'fumer pour trouver d'l'inspi' J'écrivais mes textes sur une puce de ient-cli</t>
         </is>
       </c>
     </row>
@@ -1823,7 +1823,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Mapess He, he Le keu-sa j'ai déballé Le keu-sa j'ai déballé Le keu-sa j'ai déballé Double 7 cartel Okay, he, he Le keu-sa j'ai déballé, j'suis tombé sur d'la ppe-fra, t'as pas idée, j'envoie un snap pour régaler La tête du rrain-té, j'appelle mon sin-cou, est-ce que la zone est quadrillée ? Mexico sur le tampon, c'est bien au cartel, qu'il devait s'écouler Grâce à ceux qui m'connaissent, pour soulever j'ai pas eu besoin d'passer mon CACES Pour faire honneur à la tess, donc j'rappe le quartier et sans aucune maladresse C'est en sortant son fer qu'on t'prendra au sérieux, j'comprendrai jamais l'problème des envieux Décale-toi d'eux t'avanceras mieux sans eux Décale-toi d'eux t'avanceras mieux sans eux Dans nos champs d'mort y a la méchante drogue, faut monter le degrés de fêlance Pour s'faire respecter, sécuriser l'bail, peu importe le nombre de mecs qu'on a en face de nous Fils de pute, on court pas, j'allais voler à Franprix après l'cours de maths, wAllah qu'j'révisais pas Diplômé pour ma daronne, j'l'ai aidée, j'ai fini à la barre juste avant l'été J'pensais qu'on allait jamais m'péter, j'baise la PJ, la mumu et la Sûreté Moi, j'ai pas retourné ma ste-vé, j'ai confiance qu'en mes reufs et chiffres sur ma balance J'baise toujours le proc', 100 grammes, ça j'laisais en avance he, he Dans la street c'est les vrais négros qui s'en sortent, c'est pas vers les raclis que j'trouve du réconfort Ils paient la mort pour revivre, après le meuj ils se croient tous super forts Si j'écoute mon coeur, c'est une peine à deux chiffres qui m'attend ma gueuleYou might also like</t>
+          <t>Mapess He, he Le keu-sa j'ai déballé Le keu-sa j'ai déballé Le keu-sa j'ai déballé Double 7 cartel Okay, he, he Le keu-sa j'ai déballé, j'suis tombé sur d'la ppe-fra, t'as pas idée, j'envoie un snap pour régaler La tête du rrain-té, j'appelle mon sin-cou, est-ce que la zone est quadrillée ? Mexico sur le tampon, c'est bien au cartel, qu'il devait s'écouler Grâce à ceux qui m'connaissent, pour soulever j'ai pas eu besoin d'passer mon CACES Pour faire honneur à la tess, donc j'rappe le quartier et sans aucune maladresse C'est en sortant son fer qu'on t'prendra au sérieux, j'comprendrai jamais l'problème des envieux Décale-toi d'eux t'avanceras mieux sans eux Décale-toi d'eux t'avanceras mieux sans eux Dans nos champs d'mort y a la méchante drogue, faut monter le degrés de fêlance Pour s'faire respecter, sécuriser l'bail, peu importe le nombre de mecs qu'on a en face de nous Fils de pute, on court pas, j'allais voler à Franprix après l'cours de maths, wAllah qu'j'révisais pas Diplômé pour ma daronne, j'l'ai aidée, j'ai fini à la barre juste avant l'été J'pensais qu'on allait jamais m'péter, j'baise la PJ, la mumu et la Sûreté Moi, j'ai pas retourné ma ste-vé, j'ai confiance qu'en mes reufs et chiffres sur ma balance J'baise toujours le proc', 100 grammes, ça j'laisais en avance he, he Dans la street c'est les vrais négros qui s'en sortent, c'est pas vers les raclis que j'trouve du réconfort Ils paient la mort pour revivre, après le meuj ils se croient tous super forts Si j'écoute mon coeur, c'est une peine à deux chiffres qui m'attend ma gueule</t>
         </is>
       </c>
     </row>
@@ -1840,7 +1840,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Fxnder J'allume, j'tire deux taffes, pour dix balles, j't'étouffe chez toi dans ta bre-cham La pétassé que tu kiff, nous on peut la brancher, Opinel 12 en servir pour trancher MIG trop chaud depuis ne-jeu, dans mes couilles, ne-jau quand il neigeait Jai aussi dla beuh, bien sec, bien verte, j'té-cla mon pét', tu pètes ta tête Rabats les gues-shla, ramène-les par là, si jamais ça pète, faudra pas parler La vie ne tient quà une saisi, besoin dargent toutes ls saisons Dix-huit mois d'sursis, non, c'est pas carré, j'ai trop niqué des mères, j'me suis trop bagarré Les keufs se sont garés, j'suis en train d'me barrer, ils préparent une attaque pour trouver des barrettes Personne va séparer si jamais on tape, son du 401, j'leur ai mis que des tartes J'ai toujours été déter' pour niquer des mères ou pour voler des tels Le succès doit venir mais ça prend du temps, j'suis l'boss de la ville, faut surtout pas douter Le succès doit venir mais ça prend du temps, j'suis l'boss de la ville, faut surtout pas douter C'est nous, on déboule, on casse tout, tout en noir, capuché, masqué J'te sors un plis et une odeur mystique, ils vendent de la caille toute l'année, miskine Mon briquet éclaire idées bres-som, elle va sucer, pas faire d'suçon J'était prêt avant de faire du son, on faisait déjà couler du sang Fier de mon équipe et tous mes collègues, j'ai fait un collage, j'ai roulé quatre couleurs J'en suis sûr, tu connais, tu veux faire une collab', y a qu'devant les gens qu'tu fais des accolades J'fais peur comme les Djoku ou comme Oyass quand il est sous Jacky ah Quand on arrive, on est beaucoup, quand la flicaille arrive, on a d'jà kill Ça fait des années qu'tu suces, crari, maintenant, tu veux changer genre, tu veux changer toi ? Ferme ta gueule, tu vas encore sucer, sucer, sucer, t'es bon qu'à ça J'récupère des colis depuis gamin, on va la couper si tu la tends ta main Le bénéfice, il est pas mal, sept-cents sur une 'quette, j'vais rien claquer sur Paname Fxnder C'est inconcevable de finir à terre parce que t'as fait des belles passes dans tous les sens du terme Nos vies se résument à faire du mal pour être bien, pourquoi la vie est ainsi faite ? J'aime pas les pipelettes, j'aime pas ceux qui parlent, cent meujs au détail, en deux jours, fais dix baffes Si cest fermé, on va péter les deux portes Tu réplique, t'es mort, ils font que d'chantonner, c'est pas des rappeurs Billets colorés comme un sapeur, on va prendre sa paire, on va l'taper Dans son regard, j'ai senti sa peur, MIG, moulaYou might also like</t>
+          <t>Fxnder J'allume, j'tire deux taffes, pour dix balles, j't'étouffe chez toi dans ta bre-cham La pétassé que tu kiff, nous on peut la brancher, Opinel 12 en servir pour trancher MIG trop chaud depuis ne-jeu, dans mes couilles, ne-jau quand il neigeait Jai aussi dla beuh, bien sec, bien verte, j'té-cla mon pét', tu pètes ta tête Rabats les gues-shla, ramène-les par là, si jamais ça pète, faudra pas parler La vie ne tient quà une saisi, besoin dargent toutes ls saisons Dix-huit mois d'sursis, non, c'est pas carré, j'ai trop niqué des mères, j'me suis trop bagarré Les keufs se sont garés, j'suis en train d'me barrer, ils préparent une attaque pour trouver des barrettes Personne va séparer si jamais on tape, son du 401, j'leur ai mis que des tartes J'ai toujours été déter' pour niquer des mères ou pour voler des tels Le succès doit venir mais ça prend du temps, j'suis l'boss de la ville, faut surtout pas douter Le succès doit venir mais ça prend du temps, j'suis l'boss de la ville, faut surtout pas douter C'est nous, on déboule, on casse tout, tout en noir, capuché, masqué J'te sors un plis et une odeur mystique, ils vendent de la caille toute l'année, miskine Mon briquet éclaire idées bres-som, elle va sucer, pas faire d'suçon J'était prêt avant de faire du son, on faisait déjà couler du sang Fier de mon équipe et tous mes collègues, j'ai fait un collage, j'ai roulé quatre couleurs J'en suis sûr, tu connais, tu veux faire une collab', y a qu'devant les gens qu'tu fais des accolades J'fais peur comme les Djoku ou comme Oyass quand il est sous Jacky ah Quand on arrive, on est beaucoup, quand la flicaille arrive, on a d'jà kill Ça fait des années qu'tu suces, crari, maintenant, tu veux changer genre, tu veux changer toi ? Ferme ta gueule, tu vas encore sucer, sucer, sucer, t'es bon qu'à ça J'récupère des colis depuis gamin, on va la couper si tu la tends ta main Le bénéfice, il est pas mal, sept-cents sur une 'quette, j'vais rien claquer sur Paname Fxnder C'est inconcevable de finir à terre parce que t'as fait des belles passes dans tous les sens du terme Nos vies se résument à faire du mal pour être bien, pourquoi la vie est ainsi faite ? J'aime pas les pipelettes, j'aime pas ceux qui parlent, cent meujs au détail, en deux jours, fais dix baffes Si cest fermé, on va péter les deux portes Tu réplique, t'es mort, ils font que d'chantonner, c'est pas des rappeurs Billets colorés comme un sapeur, on va prendre sa paire, on va l'taper Dans son regard, j'ai senti sa peur, MIG, moula</t>
         </is>
       </c>
     </row>
@@ -1857,7 +1857,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Deux-trois pains, j'fais tout ti-par, ça va vite alors j'vais tout découper C'est la crave-bi qui nous maintient, j'pète la forme depuis qu'j'ai tout découpé T'es mon ennemi c'est pour la vie J'me lève déchiré, mais tu connais, j'garde la tate-pa comme C hiro han ? Dans l'teum, ça sent la frappe et la baise, la kich dort pas avec les kilos han ? Guette la météo, il est temps qu'j'les terrorise en un couplet, j'vais les ventilo poh Joue pas l'escroc, t'as douillé un p'tit poh, douillé un p'tit Bientôt, j'clippe sur un bateau comme Lil Yachty ouh Pas l'te-shi mais le cash qu'adoucit abruti, j'suis en période de chiffres Faut tu lui fait à deux chiffres, ta pote cheum a la mort, ça veut pas la toucher brr 140BRICKS, j'vais bih ou j'vais barber, des solutions, y en a pas quatre cent mille uh J'me fais contrôle, j'guette ses formes dans l'uniforme uh, uh, uh, j'veux la voir soumise comme Katsuni J'vois déboule la mu'-mu', le samu-mu, ça sent la tate-pa, ça crie toutes les cinq minutes han ? J'rentre sur le R, tape dans la lulu han ?, la BAC veut m'éteindre pendant qu'le joint, j'allu-llume salope Déconnecté, tu peux m'voir sur la Lu-Lune, j'vais pas à fond mais bon, j'dois gérer l'allu-lure On baise tout, fuck la loi j'vais jamais la li-lire Surement un fait divers, si je passe sur la une, menotté, j'sors une version qu'personne n'a eue L'amour du papel donc j'le claque pas pour un ul-c J'ai l'cro-mi, le pe-ra, j'le pose sur ma eue-qu On pochetonne le 'te-'te, on pochetonne la euh-b La rue, c'est cru donc c'est sûrement pas eux Ils ont pas un eu', ils ont pas d'couilles, c'est des litchis On les voit pas quand y a litiges, des coups ils ont reup De la niquer j'suis en train, deux coups en trop elle veut m'présenter son re-p' Le bigo sonne quand j'la r'ken Marcel, le babtou du XVI mmh, j'décale, j'suis vers Sevran Marcel brr J'oublie pas l'premier qui m'a avancé uh, pas besoin d'chekem son blase, t'façon lui-même, il sait uh Je sais où sont placés les Glock uh, je sais où sont placés les Glock Elle, j'connais son passé elle gobe putain, qu'est-c'qu'il est gore J'roule à deux pots, j'suis dans le Golf, y a d'quoi finir au shtar dans la gov' Le truc dans les mains peut faire tomber les masques Peut nous ouvrir les portes, te faire donner le Max poh J'm'en fous d'savoir y a quoi dans tes poches salope, j'sais qu'tu vas donner le max Lumière éteinte, j'suis dans mon élément salope, j'fais péter l'sin-cou, on va parler maths poh Les bleus, j'sais bien qu'ils ont le mort brr, brr, brr, deux semaines qu'ils pètent rien donc on domine le match You might also like J'deviens relou quand c'est pas carré, tu l'vois dans l'regard Pas pour une tte-ch' qu'on s'bagarre J'me fais courser par l'placard, j'me fais courser par l'placard J'ai l'mort, les keufs ils ont entouré ma piaule, quand ça toque, j'suis chez une mra Marre de baiser faut qu'j'me rie-ma, nan, j'dehek, j'dis ça pour rimer J'ai l'coeur pourri mec, font les Toto Rina mais j'vois que des remakes ou des intérimaires J'ai une ce-pla à faire, j'vais la faire, j'm'en fous si j'suis dans un périmètre Vie de baisé mais j'ai fait l'con j'ai fait l'con, dans l'pochtar, la dynamo La frappe de Shevchenko Shevchenko Les los-ki, on sait qui les coffre eh, les tes-bi, on sait qui les gobe eh Sur moi, y a d'quoi prendre deux-trois ans mais en vrai, j'm'en bats les cojo' Tu veux encaisser en croisant les bras, gros, t'es trop nia t'es trop nia J'pense qu'à brasser, pas assez d'bras brr, brr, brr, j'finis l'couplet en de-spee, faut qu'on y aille Mentalité arnaqueur, bicraveur, on donnera tant qu'il y aura d'la demande uh Tu t'rappelles, on prenait c'qui t'tenait à cur uh Pour nous c'était que d'la merde à revendre Que d'la de-mer à revendre pah J'deviens relou quand c'est pas carré, tu l'vois dans l'regard Pas pour une tte-ch' qu'on s'bagarre J'me fais courser par l'placard, j'me fais courser par l'placard Y a deux-trois piges, j'étais bloqué en bas Pilon d'beuh, j'te débloquais en balle D'la ppe-f', y en a peu qui en donnent, peu qui en donnent J'me dois d'ramasser à croire qu'on m'ordonne J'deviens relou quand c'est pas carré, tu l'vois dans l'regard Pas pour une tte-ch' qu'on s'bagarre J'me fais courser par l'placard, j'me fais courser par l'placard Y a deux-trois piges, j'étais bloqué en bas Pilon d'beuh, j'te débloquais en balle D'la ppe-f', y en a peu qui en donnent, peu qui en donnent J'me dois d'ramasser à croire qu'on m'ordonne</t>
+          <t>Deux-trois pains, j'fais tout ti-par, ça va vite alors j'vais tout découper C'est la crave-bi qui nous maintient, j'pète la forme depuis qu'j'ai tout découpé T'es mon ennemi c'est pour la vie J'me lève déchiré, mais tu connais, j'garde la tate-pa comme C hiro han ? Dans l'teum, ça sent la frappe et la baise, la kich dort pas avec les kilos han ? Guette la météo, il est temps qu'j'les terrorise en un couplet, j'vais les ventilo poh Joue pas l'escroc, t'as douillé un p'tit poh, douillé un p'tit Bientôt, j'clippe sur un bateau comme Lil Yachty ouh Pas l'te-shi mais le cash qu'adoucit abruti, j'suis en période de chiffres Faut tu lui fait à deux chiffres, ta pote cheum a la mort, ça veut pas la toucher brr 140BRICKS, j'vais bih ou j'vais barber, des solutions, y en a pas quatre cent mille uh J'me fais contrôle, j'guette ses formes dans l'uniforme uh, uh, uh, j'veux la voir soumise comme Katsuni J'vois déboule la mu'-mu', le samu-mu, ça sent la tate-pa, ça crie toutes les cinq minutes han ? J'rentre sur le R, tape dans la lulu han ?, la BAC veut m'éteindre pendant qu'le joint, j'allu-llume salope Déconnecté, tu peux m'voir sur la Lu-Lune, j'vais pas à fond mais bon, j'dois gérer l'allu-lure On baise tout, fuck la loi j'vais jamais la li-lire Surement un fait divers, si je passe sur la une, menotté, j'sors une version qu'personne n'a eue L'amour du papel donc j'le claque pas pour un ul-c J'ai l'cro-mi, le pe-ra, j'le pose sur ma eue-qu On pochetonne le 'te-'te, on pochetonne la euh-b La rue, c'est cru donc c'est sûrement pas eux Ils ont pas un eu', ils ont pas d'couilles, c'est des litchis On les voit pas quand y a litiges, des coups ils ont reup De la niquer j'suis en train, deux coups en trop elle veut m'présenter son re-p' Le bigo sonne quand j'la r'ken Marcel, le babtou du XVI mmh, j'décale, j'suis vers Sevran Marcel brr J'oublie pas l'premier qui m'a avancé uh, pas besoin d'chekem son blase, t'façon lui-même, il sait uh Je sais où sont placés les Glock uh, je sais où sont placés les Glock Elle, j'connais son passé elle gobe putain, qu'est-c'qu'il est gore J'roule à deux pots, j'suis dans le Golf, y a d'quoi finir au shtar dans la gov' Le truc dans les mains peut faire tomber les masques Peut nous ouvrir les portes, te faire donner le Max poh J'm'en fous d'savoir y a quoi dans tes poches salope, j'sais qu'tu vas donner le max Lumière éteinte, j'suis dans mon élément salope, j'fais péter l'sin-cou, on va parler maths poh Les bleus, j'sais bien qu'ils ont le mort brr, brr, brr, deux semaines qu'ils pètent rien donc on domine le match J'deviens relou quand c'est pas carré, tu l'vois dans l'regard Pas pour une tte-ch' qu'on s'bagarre J'me fais courser par l'placard, j'me fais courser par l'placard J'ai l'mort, les keufs ils ont entouré ma piaule, quand ça toque, j'suis chez une mra Marre de baiser faut qu'j'me rie-ma, nan, j'dehek, j'dis ça pour rimer J'ai l'coeur pourri mec, font les Toto Rina mais j'vois que des remakes ou des intérimaires J'ai une ce-pla à faire, j'vais la faire, j'm'en fous si j'suis dans un périmètre Vie de baisé mais j'ai fait l'con j'ai fait l'con, dans l'pochtar, la dynamo La frappe de Shevchenko Shevchenko Les los-ki, on sait qui les coffre eh, les tes-bi, on sait qui les gobe eh Sur moi, y a d'quoi prendre deux-trois ans mais en vrai, j'm'en bats les cojo' Tu veux encaisser en croisant les bras, gros, t'es trop nia t'es trop nia J'pense qu'à brasser, pas assez d'bras brr, brr, brr, j'finis l'couplet en de-spee, faut qu'on y aille Mentalité arnaqueur, bicraveur, on donnera tant qu'il y aura d'la demande uh Tu t'rappelles, on prenait c'qui t'tenait à cur uh Pour nous c'était que d'la merde à revendre Que d'la de-mer à revendre pah J'deviens relou quand c'est pas carré, tu l'vois dans l'regard Pas pour une tte-ch' qu'on s'bagarre J'me fais courser par l'placard, j'me fais courser par l'placard Y a deux-trois piges, j'étais bloqué en bas Pilon d'beuh, j'te débloquais en balle D'la ppe-f', y en a peu qui en donnent, peu qui en donnent J'me dois d'ramasser à croire qu'on m'ordonne J'deviens relou quand c'est pas carré, tu l'vois dans l'regard Pas pour une tte-ch' qu'on s'bagarre J'me fais courser par l'placard, j'me fais courser par l'placard Y a deux-trois piges, j'étais bloqué en bas Pilon d'beuh, j'te débloquais en balle D'la ppe-f', y en a peu qui en donnent, peu qui en donnent J'me dois d'ramasser à croire qu'on m'ordonne</t>
         </is>
       </c>
     </row>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Poh, poh, poh Kazza Mmh, mmh, mmh, mmh, mmh, mmh, mmh Mmh, mmh, mmh, mmh, mmh, mmh, mmh Mmh, mmh, mmh, mmh, mmh, mmh, mmh Mmh, mmh, mmh, mmh, mmh, mmh, mmh Tu sais qu'jarrive déter' et que jamais j'renonce poh Y a plus rien, tinquiète, j'débloque du teh, j'attends pas qu'tu m'relances brr Met la Y, poumons encrassés brr, je gère l'endurance, y a d'l'argent qui rentre brr Jfinis dplavonner mon butin, j'lai caché, j'entends l'ambulance, j'entends lambulance J'suis un bon, j'sais pas faire la re-sta, j'ai visser des skaters et des rastas uh C'est pour ma ce-pu, si tu m'vois accoster, c'est pas l'te-shi qui m'a faya uh Mon khey, j'ai passé la journé ganté, maintenant, c'est d'la flicaille qui jou les gangsters hey She-ca pour celui qui sait pas quand s'taire hey J'vendais solo dans mon coin hey, en face, j'voyais personne pour riposter han Les p'tits s'font engrainer han, dans la rue, ils s'sont élancés han Comme un missile, impossible de faire demi-tour Au charbon même quand c'est difficile, même quand y a que des patrouilles qui tournent Impossible qu'tu m'vois raconter des mythos han ou bien tenir le sac juste une mi-temps han J'ai braqué l'bonheur, il veut plus m'voir oui, askip, tu cherches une sécu', toi oui Tu fais semblant oui mais tu sais qu'tu m'dois oui You might also like J'aurais pu tout donner pour toi, on m'dit qu'c'est pas la peine c'est pas la peine J'me rappelle même plus d'l'époque où j'connaissais pas la haine j'connaissais pas la haine J'aurais pu tout donner pour toi, on m'dit qu'c'est pas la peine c'est pas la peine J'me rappelle même plus d'l'époque où j'connaissais pas la haine j'connaissais pas la haine Du dépôt j'ressors penard, au pénave, j'entends ma voix qui résonne han Tu peux t'débattre pendant des heures, le tarpé a raison han J'vendais que d'la weed, j'faisais pas crari quand l'bigo sonnait J'ai charbonné, j'voyais plus l'soleil, que d'grimper sans voir le sommet J'pense qu'à brasser, poto, j'sens plus l'sommeil tous les jours, faut d'la renta' J'sens plus l'sommeil tous les jours, faut qu'je rentre tard J'pense qu'à brasser, poto, j'sens plus l'sommeil que des business rentables J'sens plus l'sommeil Millions d'vues j'en ai rien à foutre, j'vends d'la foutre, j'attire la foudre J'sais qu'tu mens mais j'attends qu't'avoues, tu t'plains, c'est toi qui tends ta joue Toujours pas dans les I love you, j'suis pas dans les menaces et l'chantage Maintenant qu'la kichta, elle a vu, elle en veut, c'est trop contagieux Y a qu'les montagnes qui s'croisent pas, on retombe sur celui qu'on a mêlé Quitte à prendre une grosse peine, on poucave pas han, elle t'préserve d'aucun mal, ton amulette Pour encaisser assidus on a dû l'être, y a que Dieu qu'on peut aduler J'ai vu des mecs prendre des kilos genre ils pèsent mais c'est que du léger Tu fais chier pendant qu'on fait l'chiffre, au culot, on fonce sans réfléchir 1PLIKÉ Front au sol, le monde est figé, j'veux zéro poster à mon effigie 1PLIKÉ Tu rappes la street mais t'as pas d'QG, j'dis pas tout c'que j'vis, j'vis c'que j'dis uh Tu sais pas tous les soucis qu'j'ai, j'm'en fous d'la juge qui met sous CJ uh J'étais d'vant pour visser même si c'était pas mon lycée J'vois qu'les loux-ja s'prolifèrent, pourtant, d'la maille, j'en n'ai pas assez Plaquettes sous blister, Llah y ster, mes pêchés, j'peux pas lister Mon cur pour les sous han, nan, t'es pas la seule, j'rêve d'un palace han J'veux vivre, pas seulement exister han J'aurais pu tout donner pour toi, on m'dit qu'c'est pas la peine c'est pas la peine J'me rappelle même plus d'l'époque où j'connaissais pas la haine j'connaissais pas la haine J'aurais pu tout donner pour toi, on m'dit qu'c'est pas la peine c'est pas la peine J'me rappelle même plus d'l'époque où j'connaissais pas la haine j'connaissais pas la haine Du dépôt j'ressors penard, au pénave, j'entends ma voix qui résonne han Tu peux débattre pendant des heures, le tarpé a raison han J'vendais que d'la weed, j'faisais pas crari quand l'bigo sonnait J'ai charbonné, j'voyais plus l'soleil, que d'grimper sans voir le sommet J'pense qu'à brasser, poto, j'sens plus l'sommeil tous les jours, faut d'la renta' J'sens plus l'sommeil tous les jours, faut qu'je rentre tard J'pense qu'à brasser, poto, j'sens plus l'sommeil que des business rentables J'sens plus l'sommeil Mmh, mmh, mmh, mmh, mmh, mmh, mmh Mmh, mmh, mmh, mmh, mmh, mmh, mmh Mmh, mmh, mmh, mmh, mmh, mmh, mmh Mmh, mmh, mmh, mmh, mmh, mmh, mmh</t>
+          <t>Poh, poh, poh Kazza Mmh, mmh, mmh, mmh, mmh, mmh, mmh Mmh, mmh, mmh, mmh, mmh, mmh, mmh Mmh, mmh, mmh, mmh, mmh, mmh, mmh Mmh, mmh, mmh, mmh, mmh, mmh, mmh Tu sais qu'jarrive déter' et que jamais j'renonce poh Y a plus rien, tinquiète, j'débloque du teh, j'attends pas qu'tu m'relances brr Met la Y, poumons encrassés brr, je gère l'endurance, y a d'l'argent qui rentre brr Jfinis dplavonner mon butin, j'lai caché, j'entends l'ambulance, j'entends lambulance J'suis un bon, j'sais pas faire la re-sta, j'ai visser des skaters et des rastas uh C'est pour ma ce-pu, si tu m'vois accoster, c'est pas l'te-shi qui m'a faya uh Mon khey, j'ai passé la journé ganté, maintenant, c'est d'la flicaille qui jou les gangsters hey She-ca pour celui qui sait pas quand s'taire hey J'vendais solo dans mon coin hey, en face, j'voyais personne pour riposter han Les p'tits s'font engrainer han, dans la rue, ils s'sont élancés han Comme un missile, impossible de faire demi-tour Au charbon même quand c'est difficile, même quand y a que des patrouilles qui tournent Impossible qu'tu m'vois raconter des mythos han ou bien tenir le sac juste une mi-temps han J'ai braqué l'bonheur, il veut plus m'voir oui, askip, tu cherches une sécu', toi oui Tu fais semblant oui mais tu sais qu'tu m'dois oui J'aurais pu tout donner pour toi, on m'dit qu'c'est pas la peine c'est pas la peine J'me rappelle même plus d'l'époque où j'connaissais pas la haine j'connaissais pas la haine J'aurais pu tout donner pour toi, on m'dit qu'c'est pas la peine c'est pas la peine J'me rappelle même plus d'l'époque où j'connaissais pas la haine j'connaissais pas la haine Du dépôt j'ressors penard, au pénave, j'entends ma voix qui résonne han Tu peux t'débattre pendant des heures, le tarpé a raison han J'vendais que d'la weed, j'faisais pas crari quand l'bigo sonnait J'ai charbonné, j'voyais plus l'soleil, que d'grimper sans voir le sommet J'pense qu'à brasser, poto, j'sens plus l'sommeil tous les jours, faut d'la renta' J'sens plus l'sommeil tous les jours, faut qu'je rentre tard J'pense qu'à brasser, poto, j'sens plus l'sommeil que des business rentables J'sens plus l'sommeil Millions d'vues j'en ai rien à foutre, j'vends d'la foutre, j'attire la foudre J'sais qu'tu mens mais j'attends qu't'avoues, tu t'plains, c'est toi qui tends ta joue Toujours pas dans les I love you, j'suis pas dans les menaces et l'chantage Maintenant qu'la kichta, elle a vu, elle en veut, c'est trop contagieux Y a qu'les montagnes qui s'croisent pas, on retombe sur celui qu'on a mêlé Quitte à prendre une grosse peine, on poucave pas han, elle t'préserve d'aucun mal, ton amulette Pour encaisser assidus on a dû l'être, y a que Dieu qu'on peut aduler J'ai vu des mecs prendre des kilos genre ils pèsent mais c'est que du léger Tu fais chier pendant qu'on fait l'chiffre, au culot, on fonce sans réfléchir 1PLIKÉ Front au sol, le monde est figé, j'veux zéro poster à mon effigie 1PLIKÉ Tu rappes la street mais t'as pas d'QG, j'dis pas tout c'que j'vis, j'vis c'que j'dis uh Tu sais pas tous les soucis qu'j'ai, j'm'en fous d'la juge qui met sous CJ uh J'étais d'vant pour visser même si c'était pas mon lycée J'vois qu'les loux-ja s'prolifèrent, pourtant, d'la maille, j'en n'ai pas assez Plaquettes sous blister, Llah y ster, mes pêchés, j'peux pas lister Mon cur pour les sous han, nan, t'es pas la seule, j'rêve d'un palace han J'veux vivre, pas seulement exister han J'aurais pu tout donner pour toi, on m'dit qu'c'est pas la peine c'est pas la peine J'me rappelle même plus d'l'époque où j'connaissais pas la haine j'connaissais pas la haine J'aurais pu tout donner pour toi, on m'dit qu'c'est pas la peine c'est pas la peine J'me rappelle même plus d'l'époque où j'connaissais pas la haine j'connaissais pas la haine Du dépôt j'ressors penard, au pénave, j'entends ma voix qui résonne han Tu peux débattre pendant des heures, le tarpé a raison han J'vendais que d'la weed, j'faisais pas crari quand l'bigo sonnait J'ai charbonné, j'voyais plus l'soleil, que d'grimper sans voir le sommet J'pense qu'à brasser, poto, j'sens plus l'sommeil tous les jours, faut d'la renta' J'sens plus l'sommeil tous les jours, faut qu'je rentre tard J'pense qu'à brasser, poto, j'sens plus l'sommeil que des business rentables J'sens plus l'sommeil Mmh, mmh, mmh, mmh, mmh, mmh, mmh Mmh, mmh, mmh, mmh, mmh, mmh, mmh Mmh, mmh, mmh, mmh, mmh, mmh, mmh Mmh, mmh, mmh, mmh, mmh, mmh, mmh</t>
         </is>
       </c>
     </row>
@@ -1891,7 +1891,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Les bécanes sont de sortie Donc le bendo crie Escroquerie, les gamins ont les crocs Ils se mettent bien avec les biens d'autrui Po, po, po pow Ramène des P38, ça défouraille comme à Crenshaw Pow Ramène un million huit, sur la ble-ta j'me fais l'crâne chauve Pow Charbon l'hiver c'est le stress qui tient chaud Hm hm Ok tu veux la guerre mais bon dis-moi Est-ce que tu tiens le choc ? Ok Ça te té-plan ça te souhaite un bon dimanche Le lundi tente ta chance Ok Ils comprendront que je suis harr une fois que js'rai mort À la X-Tentacion, Hm hm Belek c'est un attentat l'son Brr C'est la mélo' du tard-pé qui t'fait valser, Brr Coeur d'acier, Brr Mental sombre, Brr Anxieux quand j'relis des versets, Hein? J'allume le zdeh à 1h du mat dans l'bat, Orh? Quand vont-ils bouger ? Orh? Lâcher les conneries j'ai grave du mal Orh? Pourtant j'mapproche de ma vingtième bougie Pow J'sors tôt avec le ventre vide Hm? J'fais un billet saumon pour le p'tit déjeuner Hm? J'aime l'argent du rap mais j'veux pas de cette vie, Hm? Pas, harag depuis que j'suis né, Ehh Avant de fumer j'étais déjà chneh, Ehh Ramasse les que-chè pas les cke-schne Ehh Tu vois pas comment l'temps s'accélère ? Ehh Se repentir c'est maintenant que c'est l'heure Te fais pas de ciné on a touché l'or Eh mais Entre les mains j'avais ton pendentif Eh mais Ok, ils dorment pendant que j'dors Mais pourquoi ils nehess pendant que j'deal ? Eh mais Enculé faut salir pour faire un bon salaire Toute ma carrière j'vais clipper dans la caille 1pliké Netflix c'est la quali' J'suis pas sukali poto Eh, eh, eh, eh J'suis sous calibre Askip j'suis pas dans les temps j'suis trop bien calé Eh, eh, eh, ehYou might also like</t>
+          <t>Les bécanes sont de sortie Donc le bendo crie Escroquerie, les gamins ont les crocs Ils se mettent bien avec les biens d'autrui Po, po, po pow Ramène des P38, ça défouraille comme à Crenshaw Pow Ramène un million huit, sur la ble-ta j'me fais l'crâne chauve Pow Charbon l'hiver c'est le stress qui tient chaud Hm hm Ok tu veux la guerre mais bon dis-moi Est-ce que tu tiens le choc ? Ok Ça te té-plan ça te souhaite un bon dimanche Le lundi tente ta chance Ok Ils comprendront que je suis harr une fois que js'rai mort À la X-Tentacion, Hm hm Belek c'est un attentat l'son Brr C'est la mélo' du tard-pé qui t'fait valser, Brr Coeur d'acier, Brr Mental sombre, Brr Anxieux quand j'relis des versets, Hein? J'allume le zdeh à 1h du mat dans l'bat, Orh? Quand vont-ils bouger ? Orh? Lâcher les conneries j'ai grave du mal Orh? Pourtant j'mapproche de ma vingtième bougie Pow J'sors tôt avec le ventre vide Hm? J'fais un billet saumon pour le p'tit déjeuner Hm? J'aime l'argent du rap mais j'veux pas de cette vie, Hm? Pas, harag depuis que j'suis né, Ehh Avant de fumer j'étais déjà chneh, Ehh Ramasse les que-chè pas les cke-schne Ehh Tu vois pas comment l'temps s'accélère ? Ehh Se repentir c'est maintenant que c'est l'heure Te fais pas de ciné on a touché l'or Eh mais Entre les mains j'avais ton pendentif Eh mais Ok, ils dorment pendant que j'dors Mais pourquoi ils nehess pendant que j'deal ? Eh mais Enculé faut salir pour faire un bon salaire Toute ma carrière j'vais clipper dans la caille 1pliké Netflix c'est la quali' J'suis pas sukali poto Eh, eh, eh, eh J'suis sous calibre Askip j'suis pas dans les temps j'suis trop bien calé Eh, eh, eh, eh</t>
         </is>
       </c>
     </row>
@@ -1908,7 +1908,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Bow Bow Le ent-cli a la veine Grr, bow Faut qu'j'arrive chargé, là il m'reste que des vingt Et en cas d'embrouille j'suis devant J'attends d'avoir l'pétard pour reprendre c'qui m'devait J'ai roulé un kamas, y'a des plaquettes empilées sur la table J'cours après les tals tout l'temps j've-esqui la taule La drogue c'est rentable, maintenant qu'jai vu les sous bah j'vois plus mon avenir à l'école Donné c'est donné, reprendre c'est volé, alors j'me la donne pendant l'cambriolage Grr, bow J'ai grandi, j'fais des sous, j'embelli et vu qu'jai d'la money elle demande pas mon âge Midi-minuit j'charbonne, midi-minuit j'tartinne Sheesh J'arrache un c-sa et j'enchaîne Sheesh J'arrache une chaîne, j'fais que ça j'calcule pas les filles, y'a qu'des ents-cli sur ma SIM Bow, bow Toute ma vie j'veux d'l'argent à mort J'veux une arme à feu bien cachée dans l'armoire La meuf elle est gée-char donc j'la tire par les veux-ch' Grr, bow Pourtant elle voulait que j'lui fasse l'amour Rien qu'j'encaisse, j'ai un sommeil profond quand j'recompte ma liasse Bow, bow Personne s'inquiète quand y'a la police Ils sont remplis de bavures, c'est normal qu'on caillasse À minuit ça plavonne, à minuit ça plavonne Ça plavonne À midi l'ouverture du terrain Du terrain J'veux pas qu'l'OPJ m'interroge, y'a des dix et des vingt, viens si ça t'intéresse Sur mon bigo y'a des échos Y'a un ennemi, on l'a pas checker J'rap pour le tie-quar et pas pour les chicas À deux sur la bécane, on esquive les chickens Y'a mes gars derrière oi-m, les ents-cli que j'ai vi'-ser, j'lai ait mis dans les Waves Crache la fumée, t'es dans les vapes Si t'entend le T-max faut chahed, ça va vite J'suis ganté, j'rentre dans la planque Y'a la MH qui passe, j'ai reconnu la plaque On fait partir la blanche Y'a d'la ppe-fra en bloc On a dépouille un blanc mais la tenue est black Faut qu'le terrain il tourne comme la roue On ta jamais vu donc ne raconte pas la rue Bow, bow Arthéna y'a les keufs à l'arrêt, met la boulette en speed juste avant qu'ils arrivent À ce qui'p le savoir est une arme Tu sais pas comment on est armé On re-ti, re-ti et laisse ta mère en larme Et pour qu'ça débite sur l'terrain j'ramène d'la beuh Ta perdu la vie en essayant d'la gagner Il m'faut des llets-bi, j'pense qu'a remplir ma cagnotte Le temps c'est d'largent, j'veux qu'la caissière prend son temps Il a fait l'ancien ce batard, on l'a sauté Batard Et l'argent fais pas l'bonheur Mais l'ent-clibarrive à la bonne heure Pour pécho sa dix J'ai les pieds dans l'trafic donc mes mains se salissent À la cité d'La Plaine toutes nos rues sont salass Midi 22 ça visère Midi 23 ça visère Midi 24 ça visère Ça débite sur l'terrain jsui seul Vaut mieux être seul que mal accompagné Donc j'ai ajouté un tard-pé dans mon panier Y'a embrouille on est d'vant ton palier Y'a aucune issue si la rue ta condamné You might also likeMidi 22 ça visère Midi 23 ça visère Midi 24 ça visère Ça débite sur l'terrain jsui seul Vaut mieux être seul que mal accompagné Donc j'ai ajouté un tard-pé dans mon panier Y'a embrouille on est d'vant ton palier Y'a aucune issue si la rue ta condamné J'en place une pour tout ceux qu'j'ai chouara Le détail dans la poche ou dans la Quechua A midi le vil-ci veulent pécho leurs me-ca Passe ton tour dans l're-fou On stock dans la ve-ca Y'a d'la moula du jaune gros dis moi tu veux quoi J'ai pété c'gars là pour payer l'avocat Ouais j'sui un vrai lossa Et tous les vrais le savent Pour m'habiller propre j'fai que du le-sa Dans la guenda jsui en or mais penser aussi faut des billets J'encaisse la liasse à Sosa Si j'cours après une meuf c'est pour ché-ra son sac Sur le terrain les 10 balles sont à 2 grammes 5 Tu bouges ta tête sur le clip J'finis l'couplet j'ai té-cla ma clope C'est qu'une pute et en plus elle est conne Pour maman j'te canne fils de pute j'en ai qu'une Woo ! Midi 22 ça visère Woo ! Midi 23 ça visère Woo ! Midi 24 ça visère Woo ! Ça débite sur l'terrain jsui seul Vaut mieux être seul que mal accompagné Donc j'ai ajouté un tard-pé dans mon panier Y'a embrouille on est d'vant ton palier Y'a aucune issue si la rue ta condamné Midi 22 ça visère Midi 23 ça visère Midi 24 ça visère Ça débite sur l'terrain jsui seul Vaut mieux être seul que mal accompagné Donc j'ai ajouté un tard-pé dans mon panier Y'a embrouille on est d'vant ton palier Y'a aucune issue si la rue ta condamné</t>
+          <t>Bow Bow Le ent-cli a la veine Grr, bow Faut qu'j'arrive chargé, là il m'reste que des vingt Et en cas d'embrouille j'suis devant J'attends d'avoir l'pétard pour reprendre c'qui m'devait J'ai roulé un kamas, y'a des plaquettes empilées sur la table J'cours après les tals tout l'temps j've-esqui la taule La drogue c'est rentable, maintenant qu'jai vu les sous bah j'vois plus mon avenir à l'école Donné c'est donné, reprendre c'est volé, alors j'me la donne pendant l'cambriolage Grr, bow J'ai grandi, j'fais des sous, j'embelli et vu qu'jai d'la money elle demande pas mon âge Midi-minuit j'charbonne, midi-minuit j'tartinne Sheesh J'arrache un c-sa et j'enchaîne Sheesh J'arrache une chaîne, j'fais que ça j'calcule pas les filles, y'a qu'des ents-cli sur ma SIM Bow, bow Toute ma vie j'veux d'l'argent à mort J'veux une arme à feu bien cachée dans l'armoire La meuf elle est gée-char donc j'la tire par les veux-ch' Grr, bow Pourtant elle voulait que j'lui fasse l'amour Rien qu'j'encaisse, j'ai un sommeil profond quand j'recompte ma liasse Bow, bow Personne s'inquiète quand y'a la police Ils sont remplis de bavures, c'est normal qu'on caillasse À minuit ça plavonne, à minuit ça plavonne Ça plavonne À midi l'ouverture du terrain Du terrain J'veux pas qu'l'OPJ m'interroge, y'a des dix et des vingt, viens si ça t'intéresse Sur mon bigo y'a des échos Y'a un ennemi, on l'a pas checker J'rap pour le tie-quar et pas pour les chicas À deux sur la bécane, on esquive les chickens Y'a mes gars derrière oi-m, les ents-cli que j'ai vi'-ser, j'lai ait mis dans les Waves Crache la fumée, t'es dans les vapes Si t'entend le T-max faut chahed, ça va vite J'suis ganté, j'rentre dans la planque Y'a la MH qui passe, j'ai reconnu la plaque On fait partir la blanche Y'a d'la ppe-fra en bloc On a dépouille un blanc mais la tenue est black Faut qu'le terrain il tourne comme la roue On ta jamais vu donc ne raconte pas la rue Bow, bow Arthéna y'a les keufs à l'arrêt, met la boulette en speed juste avant qu'ils arrivent À ce qui'p le savoir est une arme Tu sais pas comment on est armé On re-ti, re-ti et laisse ta mère en larme Et pour qu'ça débite sur l'terrain j'ramène d'la beuh Ta perdu la vie en essayant d'la gagner Il m'faut des llets-bi, j'pense qu'a remplir ma cagnotte Le temps c'est d'largent, j'veux qu'la caissière prend son temps Il a fait l'ancien ce batard, on l'a sauté Batard Et l'argent fais pas l'bonheur Mais l'ent-clibarrive à la bonne heure Pour pécho sa dix J'ai les pieds dans l'trafic donc mes mains se salissent À la cité d'La Plaine toutes nos rues sont salass Midi 22 ça visère Midi 23 ça visère Midi 24 ça visère Ça débite sur l'terrain jsui seul Vaut mieux être seul que mal accompagné Donc j'ai ajouté un tard-pé dans mon panier Y'a embrouille on est d'vant ton palier Y'a aucune issue si la rue ta condamné Midi 22 ça visère Midi 23 ça visère Midi 24 ça visère Ça débite sur l'terrain jsui seul Vaut mieux être seul que mal accompagné Donc j'ai ajouté un tard-pé dans mon panier Y'a embrouille on est d'vant ton palier Y'a aucune issue si la rue ta condamné J'en place une pour tout ceux qu'j'ai chouara Le détail dans la poche ou dans la Quechua A midi le vil-ci veulent pécho leurs me-ca Passe ton tour dans l're-fou On stock dans la ve-ca Y'a d'la moula du jaune gros dis moi tu veux quoi J'ai pété c'gars là pour payer l'avocat Ouais j'sui un vrai lossa Et tous les vrais le savent Pour m'habiller propre j'fai que du le-sa Dans la guenda jsui en or mais penser aussi faut des billets J'encaisse la liasse à Sosa Si j'cours après une meuf c'est pour ché-ra son sac Sur le terrain les 10 balles sont à 2 grammes 5 Tu bouges ta tête sur le clip J'finis l'couplet j'ai té-cla ma clope C'est qu'une pute et en plus elle est conne Pour maman j'te canne fils de pute j'en ai qu'une Woo ! Midi 22 ça visère Woo ! Midi 23 ça visère Woo ! Midi 24 ça visère Woo ! Ça débite sur l'terrain jsui seul Vaut mieux être seul que mal accompagné Donc j'ai ajouté un tard-pé dans mon panier Y'a embrouille on est d'vant ton palier Y'a aucune issue si la rue ta condamné Midi 22 ça visère Midi 23 ça visère Midi 24 ça visère Ça débite sur l'terrain jsui seul Vaut mieux être seul que mal accompagné Donc j'ai ajouté un tard-pé dans mon panier Y'a embrouille on est d'vant ton palier Y'a aucune issue si la rue ta condamné</t>
         </is>
       </c>
     </row>
@@ -1925,7 +1925,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Binks Beats Zéro mala, j'suis pas là pour la frime, j'vais pas te montrer mon fric Même si je sais que tu sais que jen fais Et si un jour je suis amené à prendre 10 ans ferme Cest que mes démons sont vénères, igo, y faut que je les enferme Chaque euro me rapproche du bonheur, chaque euro me rapproche de lenfer Et si je dégaine un que-tru en embrouille t'étonnes pas si je men sers Dédicace les charbonneurs et les guetteurs qui bossent même quand cest corsé J'te raconte la réalité du ghetto pourtant toi tas envie ddanser Zéro mala, jsuis pas là pour la frime, jvais pas te montrer mon fric Même si je sais que tu sais que jen fais Et si un jour je suis amené à prendre 10 ans ferme Cest que mes démons sont vénères, igo, y faut que je les enferme Chaque euro me rapproche du bonheur, chaque euro me rapproche de lenfer Et si je dégaine un que-tru en embrouille, t'étonnes pas si je men sers Dédicace les charbonneurs et les guetteurs qui bossent même quand cest corsé J'te raconte la réalité du ghetto pourtant toi tas envie ddanser Plus y fait tard plus la scène sera sombre Jaime quand mon équipe se rassemble Et si y descendent dans le tieks, est-ce que y vont repartir en sang ? On a grandi avec lamour de largent, jusquà oublier nos rêves Jsuis avec la Mala, Bizon, le J, Baddem, jpeux pas oublier mes reufs La vie est injuste, la vie est injuste Les condés te passent les menottes sans preuve Si tu veux faire la re-gué avec nous, mon gars faut que tu sois prêt Et c'est bien beau dparler sur le net, mais quest-ce que tu vas faire après ? Enchaîner les plavons lunettes sur le nez Tant qui voit pas tes yeux y connaît pas ta tête salope Et le premier qui veut rotca au tieks, obligé dle patater salope C'est le son qui mdonne envie dcasser des bouches Jme balade sur linstru avec délicatesse On fait la regué aux gardiens dla paix Et les faux négros sont bon quà snapper Jsors de GAV jentend même pas les échos, mais jvais quand même casser la puce Ils ont pas un rond mais y font les mecs de tess Ya un plavon tes gars y sont sur répondeur, pourtant y faisaient les mecs déter Cest des acteurs ils sont bon quà rouler des teh Jai pas perdu mes habitudes jprend un 100g, jfais ti-par sur le bitume Écrasement de tête tu vas manger le béton Si tas poucave tu vas quitter le ghetto Jai fini dgaspiller ma salive narvalo, aujourdhui tu vas cracher mes thunes Jte raconte ma réalité zéro mytho J'lève un doigt à ceux qui mimportunent Pour arracher jattend le moment opportun La rue elle est vide pourtant tas crié mayday 10 négros dans ton tieks, et ya personne pour taider Quest ce quon ferait pour de la money Jte laisse mon numéro mais taura pas mon name Tu veux un truc tu peux me téléphoner Non jai pas le temps découter tes problèmes Jai un RDV jme promène avec une lame Au cas où la scène elle peut tourner au drame Jme suis éloigné de tous ceux qui me ralentissent, alors jai tourné le dos aux femmes Jdisparais à la vue des gyrophares Jen place une pour tous mes dealers, mes voleurs, qui sfont péter zéro fois Fait belek largent, lossa, ça porte malheur, négro est-ce que tu me reçois ? Le ghetto cest réel quand ya plus dissue À cette vie-là ne tattache pas, sinon tu seras déçu Lange de la mort fait le premier pas, quand ton heure a sonnée y te sautera dessus Bicrave, vol, escroquerie, les plus petits respecte la tradition Extinct, batte, tu perds léquilibre, paire de TN soccupe de la finition Les embrouilles de tiekar ne sarrêtent jamais, faut sortir un brolique si tu veux finir ça Jmempresse de faire rentrer de largent propre La mort ça vient vite et je veux pas finir sale ah bon ? Avec toi elle fait la sainte, pourtant avec moi elle fait du sale ah bon ? Avec moi elle veut samuser, pourtant avec toi elle veut du sah ah bon ? 1pliké140 jmimpressionne chaque fois que je fini un son You might also like Zéro mala, j'suis pas là pour la frime, j'vais pas te montrer mon fric Même si je sais que tu sais que jen fais Et si un jour je suis amené à prendre 10 ans ferme Cest que mes démons sont vénères, igo, y faut que je les enferme Chaque euro me rapproche du bonheur, chaque euro me rapproche de lenfer Et si je dégaine un que-tru en embrouille t'étonnes pas si je men sers Dédicace les charbonneurs et les guetteurs qui bossent même quand cest corsé J'te raconte la réalité du ghetto pourtant toi tas envie ddanser Zéro mala, jsuis pas là pour la frime, jvais pas te montrer mon fric Même si je sais que tu sais que jen fais Et si un jour je suis amené à prendre 10 ans ferme Cest que mes démons sont vénères, igo, y faut que je les enferme Chaque euro me rapproche du bonheur, chaque euro me rapproche de lenfer Et si je dégaine un que-tru en embrouille, t'étonnes pas si je men sers Dédicace les charbonneurs et les guetteurs qui bossent même quand cest corsé J'te raconte la réalité du ghetto pourtant toi tas envie ddanser Zéro mala Zéro mala Baw, baw</t>
+          <t>Binks Beats Zéro mala, j'suis pas là pour la frime, j'vais pas te montrer mon fric Même si je sais que tu sais que jen fais Et si un jour je suis amené à prendre 10 ans ferme Cest que mes démons sont vénères, igo, y faut que je les enferme Chaque euro me rapproche du bonheur, chaque euro me rapproche de lenfer Et si je dégaine un que-tru en embrouille t'étonnes pas si je men sers Dédicace les charbonneurs et les guetteurs qui bossent même quand cest corsé J'te raconte la réalité du ghetto pourtant toi tas envie ddanser Zéro mala, jsuis pas là pour la frime, jvais pas te montrer mon fric Même si je sais que tu sais que jen fais Et si un jour je suis amené à prendre 10 ans ferme Cest que mes démons sont vénères, igo, y faut que je les enferme Chaque euro me rapproche du bonheur, chaque euro me rapproche de lenfer Et si je dégaine un que-tru en embrouille, t'étonnes pas si je men sers Dédicace les charbonneurs et les guetteurs qui bossent même quand cest corsé J'te raconte la réalité du ghetto pourtant toi tas envie ddanser Plus y fait tard plus la scène sera sombre Jaime quand mon équipe se rassemble Et si y descendent dans le tieks, est-ce que y vont repartir en sang ? On a grandi avec lamour de largent, jusquà oublier nos rêves Jsuis avec la Mala, Bizon, le J, Baddem, jpeux pas oublier mes reufs La vie est injuste, la vie est injuste Les condés te passent les menottes sans preuve Si tu veux faire la re-gué avec nous, mon gars faut que tu sois prêt Et c'est bien beau dparler sur le net, mais quest-ce que tu vas faire après ? Enchaîner les plavons lunettes sur le nez Tant qui voit pas tes yeux y connaît pas ta tête salope Et le premier qui veut rotca au tieks, obligé dle patater salope C'est le son qui mdonne envie dcasser des bouches Jme balade sur linstru avec délicatesse On fait la regué aux gardiens dla paix Et les faux négros sont bon quà snapper Jsors de GAV jentend même pas les échos, mais jvais quand même casser la puce Ils ont pas un rond mais y font les mecs de tess Ya un plavon tes gars y sont sur répondeur, pourtant y faisaient les mecs déter Cest des acteurs ils sont bon quà rouler des teh Jai pas perdu mes habitudes jprend un 100g, jfais ti-par sur le bitume Écrasement de tête tu vas manger le béton Si tas poucave tu vas quitter le ghetto Jai fini dgaspiller ma salive narvalo, aujourdhui tu vas cracher mes thunes Jte raconte ma réalité zéro mytho J'lève un doigt à ceux qui mimportunent Pour arracher jattend le moment opportun La rue elle est vide pourtant tas crié mayday 10 négros dans ton tieks, et ya personne pour taider Quest ce quon ferait pour de la money Jte laisse mon numéro mais taura pas mon name Tu veux un truc tu peux me téléphoner Non jai pas le temps découter tes problèmes Jai un RDV jme promène avec une lame Au cas où la scène elle peut tourner au drame Jme suis éloigné de tous ceux qui me ralentissent, alors jai tourné le dos aux femmes Jdisparais à la vue des gyrophares Jen place une pour tous mes dealers, mes voleurs, qui sfont péter zéro fois Fait belek largent, lossa, ça porte malheur, négro est-ce que tu me reçois ? Le ghetto cest réel quand ya plus dissue À cette vie-là ne tattache pas, sinon tu seras déçu Lange de la mort fait le premier pas, quand ton heure a sonnée y te sautera dessus Bicrave, vol, escroquerie, les plus petits respecte la tradition Extinct, batte, tu perds léquilibre, paire de TN soccupe de la finition Les embrouilles de tiekar ne sarrêtent jamais, faut sortir un brolique si tu veux finir ça Jmempresse de faire rentrer de largent propre La mort ça vient vite et je veux pas finir sale ah bon ? Avec toi elle fait la sainte, pourtant avec moi elle fait du sale ah bon ? Avec moi elle veut samuser, pourtant avec toi elle veut du sah ah bon ? 1pliké140 jmimpressionne chaque fois que je fini un son Zéro mala, j'suis pas là pour la frime, j'vais pas te montrer mon fric Même si je sais que tu sais que jen fais Et si un jour je suis amené à prendre 10 ans ferme Cest que mes démons sont vénères, igo, y faut que je les enferme Chaque euro me rapproche du bonheur, chaque euro me rapproche de lenfer Et si je dégaine un que-tru en embrouille t'étonnes pas si je men sers Dédicace les charbonneurs et les guetteurs qui bossent même quand cest corsé J'te raconte la réalité du ghetto pourtant toi tas envie ddanser Zéro mala, jsuis pas là pour la frime, jvais pas te montrer mon fric Même si je sais que tu sais que jen fais Et si un jour je suis amené à prendre 10 ans ferme Cest que mes démons sont vénères, igo, y faut que je les enferme Chaque euro me rapproche du bonheur, chaque euro me rapproche de lenfer Et si je dégaine un que-tru en embrouille, t'étonnes pas si je men sers Dédicace les charbonneurs et les guetteurs qui bossent même quand cest corsé J'te raconte la réalité du ghetto pourtant toi tas envie ddanser Zéro mala Zéro mala Baw, baw</t>
         </is>
       </c>
     </row>

</xml_diff>